<commit_message>
added dependencies and eam/edit scripts
</commit_message>
<xml_diff>
--- a/edit_eam/crosscheck.xlsx
+++ b/edit_eam/crosscheck.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="237" uniqueCount="204">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="235" uniqueCount="223">
   <si>
     <t>Nombre</t>
   </si>
@@ -178,9 +178,6 @@
     <t>%ACTI Sobre total trabajadores</t>
   </si>
   <si>
-    <t>Capital humano</t>
-  </si>
-  <si>
     <t>Primaria/Bachillerato</t>
   </si>
   <si>
@@ -367,9 +364,6 @@
     <t>I1R4C2M</t>
   </si>
   <si>
-    <t>IR3C2M &gt; 0 | I1R3C2N &gt; 0</t>
-  </si>
-  <si>
     <t>Dummys Tipo de empresa innovadora</t>
   </si>
   <si>
@@ -385,18 +379,9 @@
     <t>No innova? 1=Si</t>
   </si>
   <si>
-    <t>IR2C2M &gt; 0 | I1R2C2N &gt; 0</t>
-  </si>
-  <si>
-    <t>Else de las demas</t>
-  </si>
-  <si>
     <t>II1R4C1 &gt; 0 | II1R4C2 &gt; 0</t>
   </si>
   <si>
-    <t>I6R1C1 == 1</t>
-  </si>
-  <si>
     <t>Dummys Networking innovacion</t>
   </si>
   <si>
@@ -415,15 +400,6 @@
     <t>EDIT</t>
   </si>
   <si>
-    <t>Hay una similar</t>
-  </si>
-  <si>
-    <t>No esta en EDIT, de pronto EAM</t>
-  </si>
-  <si>
-    <t>CIIU4 Se puede mutar a 2 Digitos</t>
-  </si>
-  <si>
     <t>EAM</t>
   </si>
   <si>
@@ -433,30 +409,12 @@
     <t>Total</t>
   </si>
   <si>
-    <t>Total &lt;=10</t>
-  </si>
-  <si>
-    <t>Total &gt; 10 &amp; Total &lt;=50</t>
-  </si>
-  <si>
-    <t>Total &gt; 50 &amp; Total &lt;=200</t>
-  </si>
-  <si>
-    <t>Total &gt; 200</t>
-  </si>
-  <si>
-    <t>(IV1R11C3 + IV1R11C4)/2</t>
-  </si>
-  <si>
     <t>Total ACTI / Total</t>
   </si>
   <si>
     <t>Total ACTI</t>
   </si>
   <si>
-    <t>EDIT Tiene de los que estan en ACTI, EAM de pronto tiene mas</t>
-  </si>
-  <si>
     <t>IV4R4C3/Total</t>
   </si>
   <si>
@@ -469,33 +427,15 @@
     <t>IV4R3C3/Total</t>
   </si>
   <si>
-    <t>III1R1C1 + III1R1C2</t>
-  </si>
-  <si>
     <t>No se puede desagregar x trabajador. Mas bien =1 si emplea mujeres? O Hacer ratio de mujeres en cada division</t>
   </si>
   <si>
-    <t>III1R2C1 + III1R2C2</t>
-  </si>
-  <si>
-    <t>III1R3C1 + III1R3C2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">III1R4C1 + III1R4C2 + III1R4C3 + III1R4C4 </t>
-  </si>
-  <si>
-    <t>III1R5C1 + III1R5C2 + III1R5C3 + III1R5C4</t>
-  </si>
-  <si>
     <t>Otras Empresas</t>
   </si>
   <si>
     <t>Otras fuentes</t>
   </si>
   <si>
-    <t xml:space="preserve">III1R6C1 + III1R6C2 + III1R6C3 + III1R6C4 +  III1R7C1 + III1R7C2 + III1R7C3 + III1R7C4 </t>
-  </si>
-  <si>
     <t>Ampliar info</t>
   </si>
   <si>
@@ -520,84 +460,27 @@
     <t>V2R15C1 == 1</t>
   </si>
   <si>
-    <t>V2R7C1 == 1 Ojo no discrimina por publicas</t>
-  </si>
-  <si>
     <t>No veo</t>
   </si>
   <si>
-    <t>No veo pero hay workaround con III2R1C1 &gt; 0 | III2R1C2 &gt; 0</t>
-  </si>
-  <si>
     <t>Escases de recursos propios</t>
   </si>
   <si>
-    <t>I10R1C1 == 1 | I10R1C1 == 2</t>
-  </si>
-  <si>
-    <t>I10R10C1 == 1 | I10R10C1 == 2</t>
-  </si>
-  <si>
-    <t>I10R12C1 == 1 | I10R12C1 == 2</t>
-  </si>
-  <si>
-    <t>I10R7C1 == 1 | I10R7C1 == 2</t>
-  </si>
-  <si>
-    <t>I10R8C1 == 1 | I10R8C1 == 2</t>
-  </si>
-  <si>
-    <t>I10R11C1 == 1 | I10R11C1 == 2</t>
-  </si>
-  <si>
-    <t>III4R6C1 == 1 | III4R6C1 == 2</t>
-  </si>
-  <si>
-    <t>III4R3C1 == 1 | III4R3C1 == 2</t>
-  </si>
-  <si>
-    <t>I10R3C1 == 1 | I10R3C1 == 2</t>
-  </si>
-  <si>
-    <t>I10R6C1 == 1 | I10R6C1 == 2</t>
-  </si>
-  <si>
-    <t>I10R14C1 == 1 | I10R14C1 == 2</t>
-  </si>
-  <si>
-    <t>I10R13C1 == 1 | I10R13C1 == 2</t>
-  </si>
-  <si>
-    <t>III4R4C1 == 1 | III4R4C1 == 2</t>
-  </si>
-  <si>
     <t>Frente a rentabilidad</t>
   </si>
   <si>
     <t>Condiciones de financiacion poco atractivas</t>
   </si>
   <si>
-    <t>III4R5C1 == 1 | III4R5C1 == 2</t>
-  </si>
-  <si>
-    <t>I10R2C1 == 1 | I10R2C1 == 2</t>
-  </si>
-  <si>
     <t>Else de todo lo demas</t>
   </si>
   <si>
-    <t>(I10R4C1 == 1 | I10R4C1 == 2) &amp; (I10R5C1 == 1 | I10R5C1 == 2)</t>
-  </si>
-  <si>
     <t>Falta de informacion sobre apoyo publico</t>
   </si>
   <si>
     <t>Falta informacion mercados o tecnologia</t>
   </si>
   <si>
-    <t>I10R9C1 == 1 | I10R9C1 == 2</t>
-  </si>
-  <si>
     <t>VIII12R5C1 != 1</t>
   </si>
   <si>
@@ -626,6 +509,180 @@
   </si>
   <si>
     <t>PORCVT</t>
+  </si>
+  <si>
+    <t>Mejora de calidad B/S</t>
+  </si>
+  <si>
+    <t>Aumenta gama B/S</t>
+  </si>
+  <si>
+    <t>Mantener posicion de mercado o ingresar a otro</t>
+  </si>
+  <si>
+    <t>Aumentos de productividad</t>
+  </si>
+  <si>
+    <t>Reduccion de costos de factores</t>
+  </si>
+  <si>
+    <t>Reduccion de costos de transporte, comunicacion o reparacion</t>
+  </si>
+  <si>
+    <t>Otros</t>
+  </si>
+  <si>
+    <t>V2R7C1 == 1</t>
+  </si>
+  <si>
+    <t>I10R1C1 &lt; 3</t>
+  </si>
+  <si>
+    <t>I10R10C1 &lt; 3</t>
+  </si>
+  <si>
+    <t>I10R6C1 &lt; 3</t>
+  </si>
+  <si>
+    <t>I10R2C1 &lt; 3</t>
+  </si>
+  <si>
+    <t>I10R3C1 &lt; 3</t>
+  </si>
+  <si>
+    <t>I10R11C1 &lt; 3</t>
+  </si>
+  <si>
+    <t>I10R13C1 &lt; 3</t>
+  </si>
+  <si>
+    <t>I10R14C1 &lt; 3</t>
+  </si>
+  <si>
+    <t>III4R4C1 &lt; 3</t>
+  </si>
+  <si>
+    <t>III4R6C1 &lt; 3</t>
+  </si>
+  <si>
+    <t>III4R3C1 &lt; 3</t>
+  </si>
+  <si>
+    <t>III4R5C1 &lt; 3</t>
+  </si>
+  <si>
+    <t>I10R7C1 &lt; 3</t>
+  </si>
+  <si>
+    <t>I10R8C1 &lt; 3</t>
+  </si>
+  <si>
+    <t>I10R12C1 &lt; 3</t>
+  </si>
+  <si>
+    <t>I10R9C1 &lt; 3</t>
+  </si>
+  <si>
+    <t>(I10R4C1 &lt; 3) | (I10R5C1 &lt; 3)</t>
+  </si>
+  <si>
+    <t>I2R1C1 &lt; 3</t>
+  </si>
+  <si>
+    <t>I2R2C1 &lt; 3</t>
+  </si>
+  <si>
+    <t>I2R3C1 &lt; 3 | I2R4C1 &lt; 3</t>
+  </si>
+  <si>
+    <t>I2R5C1 &lt; 3</t>
+  </si>
+  <si>
+    <t>I2R6C1 &lt; 3 | I2R7C1 &lt; 3 | I2R8C1 &lt; 3 | I2R9C1 &lt; 3</t>
+  </si>
+  <si>
+    <t>I2R10C1 &lt; 3 | I2R11C1 &lt; 3 | I2R12C1 &lt; 3</t>
+  </si>
+  <si>
+    <t>I2R13C1 &lt; 3 | I2R14C1 &lt; 3 | I2R15C1 &lt; 3</t>
+  </si>
+  <si>
+    <t>III2R1C1 &gt; 0 | III2R1C2 &gt; 0</t>
+  </si>
+  <si>
+    <t>Total 2017 == IV1R11C1;        Total 2018 == IV1R11C2</t>
+  </si>
+  <si>
+    <t>Totales &lt;=10</t>
+  </si>
+  <si>
+    <t>Totales &gt; 10 &amp; Totales &lt;=50</t>
+  </si>
+  <si>
+    <t>Totales &gt; 50 &amp; Totales &lt;=200</t>
+  </si>
+  <si>
+    <t>Totales &gt; 200</t>
+  </si>
+  <si>
+    <t>CIIU4 (mutar a 2 digitos)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2017 == IV1R7C1 + IV1R8C1,          2018 == IV1R7C2 + IV1R8C2  </t>
+  </si>
+  <si>
+    <t>2017 == IV1R1C1 + IV1R2C1 + IV1R3C1,           2018 == IV1R1C2 + IV1R2C2 + IV1R3C2</t>
+  </si>
+  <si>
+    <t>2017 == IV1R10C1,         2018 == IV1R10C2</t>
+  </si>
+  <si>
+    <t>Capital humano (promedio)</t>
+  </si>
+  <si>
+    <t>2017 == IV1R11C1, 2018 == IV1R11C2</t>
+  </si>
+  <si>
+    <t>2017 ==  IV1R4C1 + IV1R5C1 + IV1R6C1 + IV1R9C1,          2018 == IV1R4C2 + IV1R5C2 + IV1R6C2 + IV1R9C2</t>
+  </si>
+  <si>
+    <t>2017 == IV1R11C3, 2018 == IV1R11C4</t>
+  </si>
+  <si>
+    <t>Ojo no se calcula con IPP</t>
+  </si>
+  <si>
+    <t>VA == ?,  Empleados == Total Capital Humano</t>
+  </si>
+  <si>
+    <t>ACTI2017 == II1R10C1, ACTI2018 == II1R10C2,                   VA == ?</t>
+  </si>
+  <si>
+    <t>EAM/EDIT</t>
+  </si>
+  <si>
+    <t>TIPOLO</t>
+  </si>
+  <si>
+    <t>Otro (else)</t>
+  </si>
+  <si>
+    <t>2017 == III1R1C1, 2018 == III1R1C2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2017 == III1R4C1 + III1R4C2,            2018 == III1R4C3 + III1R4C4 </t>
+  </si>
+  <si>
+    <t>2017 == III1R2C1 , 2018 == III1R2C2</t>
+  </si>
+  <si>
+    <t>2017 == III1R3C1,  2018 == III1R3C2</t>
+  </si>
+  <si>
+    <t>2017 == III1R5C1 + III1R5C2,           2018 ==  III1R5C3 + III1R5C4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2017 == III1R6C1 + III1R6C2  +  III1R7C1 + III1R7C2           2018 == III1R6C3 + III1R6C4  + III1R7C3 + III1R7C4 </t>
   </si>
 </sst>
 </file>
@@ -797,7 +854,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -851,9 +908,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -863,43 +917,49 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1206,10 +1266,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="C2:I102"/>
+  <dimension ref="C2:I108"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="E40" sqref="E40"/>
+    <sheetView tabSelected="1" topLeftCell="A55" workbookViewId="0">
+      <selection activeCell="F100" sqref="F100"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="15.05" x14ac:dyDescent="0.3"/>
@@ -1217,7 +1277,7 @@
     <col min="3" max="3" width="23.21875" style="1" customWidth="1"/>
     <col min="4" max="4" width="20.77734375" style="2" customWidth="1"/>
     <col min="5" max="5" width="14" style="13" customWidth="1"/>
-    <col min="6" max="6" width="18.44140625" style="1" customWidth="1"/>
+    <col min="6" max="6" width="15.6640625" style="1" customWidth="1"/>
     <col min="7" max="7" width="15.33203125" style="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1229,13 +1289,13 @@
         <v>8</v>
       </c>
       <c r="E2" s="14" t="s">
-        <v>131</v>
+        <v>126</v>
       </c>
       <c r="F2" s="16" t="s">
         <v>1</v>
       </c>
       <c r="G2" s="14" t="s">
-        <v>137</v>
+        <v>129</v>
       </c>
       <c r="H2" s="17" t="s">
         <v>2</v>
@@ -1251,8 +1311,8 @@
       <c r="D3" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="E3" s="5" t="s">
-        <v>132</v>
+      <c r="E3" s="25" t="s">
+        <v>127</v>
       </c>
       <c r="F3" s="9" t="s">
         <v>5</v>
@@ -1268,1362 +1328,1405 @@
       <c r="D4" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="E4" s="5" t="s">
-        <v>132</v>
-      </c>
-      <c r="F4" s="10" t="s">
-        <v>111</v>
+      <c r="E4" s="26"/>
+      <c r="F4" s="12" t="s">
+        <v>110</v>
       </c>
       <c r="G4" s="6"/>
       <c r="H4" s="4"/>
       <c r="I4" s="4"/>
     </row>
     <row r="5" spans="3:9" x14ac:dyDescent="0.3">
-      <c r="C5" s="30" t="s">
+      <c r="C5" s="28" t="s">
         <v>7</v>
       </c>
       <c r="D5" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="E5" s="24" t="s">
-        <v>132</v>
-      </c>
+      <c r="E5" s="26"/>
       <c r="F5" s="9" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="G5" s="6"/>
       <c r="H5" s="4"/>
       <c r="I5" s="4"/>
     </row>
     <row r="6" spans="3:9" x14ac:dyDescent="0.3">
-      <c r="C6" s="30"/>
+      <c r="C6" s="28"/>
       <c r="D6" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="E6" s="25"/>
-      <c r="F6" s="31" t="s">
-        <v>114</v>
+      <c r="E6" s="26"/>
+      <c r="F6" s="35" t="s">
+        <v>113</v>
       </c>
       <c r="G6" s="6"/>
       <c r="H6" s="4"/>
       <c r="I6" s="4"/>
     </row>
     <row r="7" spans="3:9" x14ac:dyDescent="0.3">
-      <c r="C7" s="30"/>
+      <c r="C7" s="28"/>
       <c r="D7" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="E7" s="25"/>
-      <c r="F7" s="32"/>
+      <c r="E7" s="26"/>
+      <c r="F7" s="36"/>
       <c r="G7" s="6"/>
       <c r="H7" s="4"/>
       <c r="I7" s="4"/>
     </row>
     <row r="8" spans="3:9" x14ac:dyDescent="0.3">
-      <c r="C8" s="30"/>
+      <c r="C8" s="28"/>
       <c r="D8" s="7" t="s">
         <v>12</v>
       </c>
       <c r="E8" s="26"/>
       <c r="F8" s="11" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="G8" s="6"/>
       <c r="H8" s="4"/>
       <c r="I8" s="4"/>
     </row>
     <row r="9" spans="3:9" x14ac:dyDescent="0.3">
-      <c r="C9" s="30" t="s">
+      <c r="C9" s="28" t="s">
         <v>13</v>
       </c>
       <c r="D9" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="E9" s="5"/>
-      <c r="F9" s="27" t="s">
-        <v>133</v>
+        <v>165</v>
+      </c>
+      <c r="E9" s="26"/>
+      <c r="F9" s="24" t="s">
+        <v>190</v>
       </c>
       <c r="G9" s="6"/>
       <c r="H9" s="4"/>
       <c r="I9" s="4"/>
     </row>
     <row r="10" spans="3:9" x14ac:dyDescent="0.3">
-      <c r="C10" s="30"/>
+      <c r="C10" s="28"/>
       <c r="D10" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="E10" s="5"/>
-      <c r="F10" s="28"/>
+        <v>166</v>
+      </c>
+      <c r="E10" s="26"/>
+      <c r="F10" s="24" t="s">
+        <v>191</v>
+      </c>
       <c r="G10" s="6"/>
       <c r="H10" s="4"/>
       <c r="I10" s="4"/>
     </row>
-    <row r="11" spans="3:9" x14ac:dyDescent="0.3">
-      <c r="C11" s="30"/>
+    <row r="11" spans="3:9" ht="34.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C11" s="28"/>
       <c r="D11" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="E11" s="5"/>
-      <c r="F11" s="28"/>
+        <v>167</v>
+      </c>
+      <c r="E11" s="26"/>
+      <c r="F11" s="24" t="s">
+        <v>192</v>
+      </c>
       <c r="G11" s="6"/>
       <c r="H11" s="4"/>
       <c r="I11" s="4"/>
     </row>
-    <row r="12" spans="3:9" x14ac:dyDescent="0.3">
-      <c r="C12" s="30"/>
+    <row r="12" spans="3:9" ht="34.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C12" s="28"/>
       <c r="D12" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="E12" s="5"/>
-      <c r="F12" s="29"/>
+        <v>168</v>
+      </c>
+      <c r="E12" s="26"/>
+      <c r="F12" s="24" t="s">
+        <v>193</v>
+      </c>
       <c r="G12" s="6"/>
       <c r="H12" s="4"/>
       <c r="I12" s="4"/>
     </row>
-    <row r="13" spans="3:9" x14ac:dyDescent="0.3">
-      <c r="C13" s="30" t="s">
-        <v>14</v>
-      </c>
+    <row r="13" spans="3:9" ht="65.45" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C13" s="28"/>
       <c r="D13" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="E13" s="24" t="s">
-        <v>132</v>
-      </c>
-      <c r="F13" s="9" t="s">
-        <v>115</v>
+        <v>169</v>
+      </c>
+      <c r="E13" s="26"/>
+      <c r="F13" s="24" t="s">
+        <v>194</v>
       </c>
       <c r="G13" s="6"/>
       <c r="H13" s="4"/>
       <c r="I13" s="4"/>
     </row>
-    <row r="14" spans="3:9" x14ac:dyDescent="0.3">
-      <c r="C14" s="30"/>
+    <row r="14" spans="3:9" ht="46.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C14" s="28"/>
       <c r="D14" s="7" t="s">
-        <v>16</v>
+        <v>170</v>
       </c>
       <c r="E14" s="26"/>
-      <c r="F14" s="9" t="s">
-        <v>116</v>
+      <c r="F14" s="24" t="s">
+        <v>195</v>
       </c>
       <c r="G14" s="6"/>
       <c r="H14" s="4"/>
       <c r="I14" s="4"/>
     </row>
-    <row r="15" spans="3:9" ht="30.15" x14ac:dyDescent="0.3">
-      <c r="C15" s="30" t="s">
-        <v>118</v>
-      </c>
+    <row r="15" spans="3:9" ht="66.150000000000006" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C15" s="28"/>
       <c r="D15" s="7" t="s">
-        <v>119</v>
-      </c>
-      <c r="E15" s="24" t="s">
-        <v>132</v>
-      </c>
-      <c r="F15" s="9" t="s">
-        <v>117</v>
+        <v>171</v>
+      </c>
+      <c r="E15" s="26"/>
+      <c r="F15" s="24" t="s">
+        <v>196</v>
       </c>
       <c r="G15" s="6"/>
       <c r="H15" s="4"/>
       <c r="I15" s="4"/>
     </row>
-    <row r="16" spans="3:9" ht="30.15" x14ac:dyDescent="0.3">
-      <c r="C16" s="30"/>
+    <row r="16" spans="3:9" x14ac:dyDescent="0.3">
+      <c r="C16" s="28" t="s">
+        <v>14</v>
+      </c>
       <c r="D16" s="7" t="s">
-        <v>120</v>
-      </c>
-      <c r="E16" s="25"/>
+        <v>15</v>
+      </c>
+      <c r="E16" s="26"/>
       <c r="F16" s="9" t="s">
-        <v>123</v>
+        <v>114</v>
       </c>
       <c r="G16" s="6"/>
       <c r="H16" s="4"/>
       <c r="I16" s="4"/>
     </row>
     <row r="17" spans="3:9" x14ac:dyDescent="0.3">
-      <c r="C17" s="30"/>
+      <c r="C17" s="28"/>
       <c r="D17" s="7" t="s">
-        <v>121</v>
-      </c>
-      <c r="E17" s="25"/>
+        <v>16</v>
+      </c>
+      <c r="E17" s="26"/>
       <c r="F17" s="9" t="s">
-        <v>126</v>
+        <v>115</v>
       </c>
       <c r="G17" s="6"/>
       <c r="H17" s="4"/>
       <c r="I17" s="4"/>
     </row>
-    <row r="18" spans="3:9" x14ac:dyDescent="0.3">
-      <c r="C18" s="30"/>
+    <row r="18" spans="3:9" ht="15.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C18" s="25" t="s">
+        <v>116</v>
+      </c>
       <c r="D18" s="7" t="s">
-        <v>122</v>
+        <v>117</v>
       </c>
       <c r="E18" s="26"/>
-      <c r="F18" s="9" t="s">
-        <v>124</v>
+      <c r="F18" s="25" t="s">
+        <v>215</v>
       </c>
       <c r="G18" s="6"/>
       <c r="H18" s="4"/>
       <c r="I18" s="4"/>
     </row>
-    <row r="19" spans="3:9" ht="30.15" x14ac:dyDescent="0.3">
-      <c r="C19" s="3" t="s">
-        <v>17</v>
-      </c>
+    <row r="19" spans="3:9" x14ac:dyDescent="0.3">
+      <c r="C19" s="26"/>
       <c r="D19" s="7" t="s">
-        <v>63</v>
-      </c>
-      <c r="E19" s="5" t="s">
-        <v>132</v>
-      </c>
-      <c r="F19" s="9" t="s">
-        <v>125</v>
-      </c>
+        <v>118</v>
+      </c>
+      <c r="E19" s="26"/>
+      <c r="F19" s="26"/>
       <c r="G19" s="6"/>
       <c r="H19" s="4"/>
       <c r="I19" s="4"/>
     </row>
     <row r="20" spans="3:9" x14ac:dyDescent="0.3">
-      <c r="C20" s="30" t="s">
-        <v>127</v>
-      </c>
+      <c r="C20" s="26"/>
       <c r="D20" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="E20" s="24" t="s">
-        <v>132</v>
-      </c>
-      <c r="F20" s="12" t="s">
-        <v>129</v>
-      </c>
+        <v>119</v>
+      </c>
+      <c r="E20" s="26"/>
+      <c r="F20" s="26"/>
       <c r="G20" s="6"/>
       <c r="H20" s="4"/>
       <c r="I20" s="4"/>
     </row>
-    <row r="21" spans="3:9" ht="30.15" x14ac:dyDescent="0.3">
-      <c r="C21" s="30"/>
+    <row r="21" spans="3:9" x14ac:dyDescent="0.3">
+      <c r="C21" s="26"/>
       <c r="D21" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="E21" s="25"/>
-      <c r="F21" s="12" t="s">
-        <v>130</v>
-      </c>
+        <v>120</v>
+      </c>
+      <c r="E21" s="26"/>
+      <c r="F21" s="26"/>
       <c r="G21" s="6"/>
       <c r="H21" s="4"/>
       <c r="I21" s="4"/>
     </row>
-    <row r="22" spans="3:9" ht="30.15" x14ac:dyDescent="0.3">
-      <c r="C22" s="30"/>
-      <c r="D22" s="8" t="s">
-        <v>20</v>
+    <row r="22" spans="3:9" x14ac:dyDescent="0.3">
+      <c r="C22" s="27"/>
+      <c r="D22" s="7" t="s">
+        <v>216</v>
       </c>
       <c r="E22" s="26"/>
-      <c r="F22" s="12" t="s">
-        <v>128</v>
-      </c>
+      <c r="F22" s="27"/>
       <c r="G22" s="6"/>
       <c r="H22" s="4"/>
       <c r="I22" s="4"/>
     </row>
-    <row r="23" spans="3:9" x14ac:dyDescent="0.3">
-      <c r="C23" s="30" t="s">
-        <v>23</v>
+    <row r="23" spans="3:9" ht="30.15" x14ac:dyDescent="0.3">
+      <c r="C23" s="3" t="s">
+        <v>17</v>
       </c>
       <c r="D23" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="E23" s="5"/>
-      <c r="F23" s="27" t="s">
-        <v>134</v>
+        <v>62</v>
+      </c>
+      <c r="E23" s="26"/>
+      <c r="F23" s="9" t="s">
+        <v>121</v>
       </c>
       <c r="G23" s="6"/>
       <c r="H23" s="4"/>
       <c r="I23" s="4"/>
     </row>
     <row r="24" spans="3:9" x14ac:dyDescent="0.3">
-      <c r="C24" s="30"/>
+      <c r="C24" s="28" t="s">
+        <v>122</v>
+      </c>
       <c r="D24" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="E24" s="5"/>
-      <c r="F24" s="28"/>
+        <v>18</v>
+      </c>
+      <c r="E24" s="26"/>
+      <c r="F24" s="12" t="s">
+        <v>124</v>
+      </c>
       <c r="G24" s="6"/>
       <c r="H24" s="4"/>
       <c r="I24" s="4"/>
     </row>
-    <row r="25" spans="3:9" x14ac:dyDescent="0.3">
-      <c r="C25" s="30" t="s">
-        <v>24</v>
-      </c>
+    <row r="25" spans="3:9" ht="30.15" x14ac:dyDescent="0.3">
+      <c r="C25" s="28"/>
       <c r="D25" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="E25" s="5"/>
-      <c r="F25" s="28"/>
+        <v>19</v>
+      </c>
+      <c r="E25" s="26"/>
+      <c r="F25" s="12" t="s">
+        <v>125</v>
+      </c>
       <c r="G25" s="6"/>
       <c r="H25" s="4"/>
       <c r="I25" s="4"/>
     </row>
-    <row r="26" spans="3:9" x14ac:dyDescent="0.3">
-      <c r="C26" s="30"/>
-      <c r="D26" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="E26" s="5"/>
-      <c r="F26" s="28"/>
+    <row r="26" spans="3:9" ht="30.15" x14ac:dyDescent="0.3">
+      <c r="C26" s="28"/>
+      <c r="D26" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="E26" s="27"/>
+      <c r="F26" s="12" t="s">
+        <v>123</v>
+      </c>
       <c r="G26" s="6"/>
       <c r="H26" s="4"/>
       <c r="I26" s="4"/>
     </row>
     <row r="27" spans="3:9" x14ac:dyDescent="0.3">
-      <c r="C27" s="30"/>
+      <c r="C27" s="28" t="s">
+        <v>23</v>
+      </c>
       <c r="D27" s="7" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="E27" s="5"/>
-      <c r="F27" s="29"/>
+      <c r="F27" s="29" t="s">
+        <v>148</v>
+      </c>
       <c r="G27" s="6"/>
       <c r="H27" s="4"/>
       <c r="I27" s="4"/>
     </row>
-    <row r="28" spans="3:9" ht="60.25" x14ac:dyDescent="0.3">
-      <c r="C28" s="24" t="s">
-        <v>28</v>
-      </c>
+    <row r="28" spans="3:9" x14ac:dyDescent="0.3">
+      <c r="C28" s="28"/>
       <c r="D28" s="7" t="s">
-        <v>138</v>
-      </c>
-      <c r="E28" s="24" t="s">
-        <v>132</v>
-      </c>
-      <c r="F28" s="23" t="s">
-        <v>146</v>
-      </c>
+        <v>22</v>
+      </c>
+      <c r="E28" s="5"/>
+      <c r="F28" s="30"/>
       <c r="G28" s="6"/>
       <c r="H28" s="4"/>
       <c r="I28" s="4"/>
     </row>
-    <row r="29" spans="3:9" ht="30.15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C29" s="25"/>
-      <c r="D29" s="7">
-        <v>10</v>
-      </c>
-      <c r="E29" s="25"/>
-      <c r="F29" s="18" t="s">
-        <v>139</v>
-      </c>
-      <c r="G29" s="22"/>
+    <row r="29" spans="3:9" x14ac:dyDescent="0.3">
+      <c r="C29" s="28" t="s">
+        <v>24</v>
+      </c>
+      <c r="D29" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="E29" s="5"/>
+      <c r="F29" s="30"/>
+      <c r="G29" s="6"/>
       <c r="H29" s="4"/>
       <c r="I29" s="4"/>
     </row>
-    <row r="30" spans="3:9" ht="30.15" x14ac:dyDescent="0.3">
-      <c r="C30" s="25"/>
+    <row r="30" spans="3:9" x14ac:dyDescent="0.3">
+      <c r="C30" s="28"/>
       <c r="D30" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="E30" s="25"/>
-      <c r="F30" s="18" t="s">
-        <v>140</v>
-      </c>
-      <c r="G30" s="22"/>
+        <v>26</v>
+      </c>
+      <c r="E30" s="5"/>
+      <c r="F30" s="30"/>
+      <c r="G30" s="6"/>
       <c r="H30" s="4"/>
       <c r="I30" s="4"/>
     </row>
-    <row r="31" spans="3:9" ht="30.15" x14ac:dyDescent="0.3">
-      <c r="C31" s="25"/>
+    <row r="31" spans="3:9" x14ac:dyDescent="0.3">
+      <c r="C31" s="28"/>
       <c r="D31" s="7" t="s">
-        <v>30</v>
-      </c>
-      <c r="E31" s="25"/>
-      <c r="F31" s="18" t="s">
-        <v>141</v>
-      </c>
-      <c r="G31" s="22"/>
+        <v>27</v>
+      </c>
+      <c r="E31" s="5"/>
+      <c r="F31" s="31"/>
+      <c r="G31" s="6"/>
       <c r="H31" s="4"/>
       <c r="I31" s="4"/>
     </row>
-    <row r="32" spans="3:9" x14ac:dyDescent="0.3">
-      <c r="C32" s="26"/>
+    <row r="32" spans="3:9" ht="60.25" x14ac:dyDescent="0.3">
+      <c r="C32" s="25" t="s">
+        <v>28</v>
+      </c>
       <c r="D32" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="E32" s="26"/>
-      <c r="F32" s="18" t="s">
-        <v>142</v>
-      </c>
-      <c r="G32" s="22"/>
+        <v>130</v>
+      </c>
+      <c r="E32" s="25" t="s">
+        <v>127</v>
+      </c>
+      <c r="F32" s="22" t="s">
+        <v>198</v>
+      </c>
+      <c r="G32" s="6"/>
       <c r="H32" s="4"/>
       <c r="I32" s="4"/>
     </row>
-    <row r="33" spans="3:9" ht="30.15" x14ac:dyDescent="0.3">
-      <c r="C33" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="D33" s="7" t="s">
-        <v>33</v>
-      </c>
-      <c r="E33" s="5" t="s">
-        <v>132</v>
-      </c>
-      <c r="F33" s="12" t="s">
-        <v>135</v>
-      </c>
-      <c r="G33" s="6"/>
+    <row r="33" spans="3:9" ht="30.15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C33" s="26"/>
+      <c r="D33" s="7">
+        <v>10</v>
+      </c>
+      <c r="E33" s="26"/>
+      <c r="F33" s="18" t="s">
+        <v>199</v>
+      </c>
+      <c r="G33" s="21"/>
       <c r="H33" s="4"/>
       <c r="I33" s="4"/>
     </row>
-    <row r="34" spans="3:9" x14ac:dyDescent="0.3">
-      <c r="C34" s="3" t="s">
-        <v>34</v>
-      </c>
+    <row r="34" spans="3:9" ht="30.15" x14ac:dyDescent="0.3">
+      <c r="C34" s="26"/>
       <c r="D34" s="7" t="s">
-        <v>35</v>
-      </c>
-      <c r="E34" s="5" t="s">
-        <v>136</v>
-      </c>
-      <c r="F34" s="12" t="s">
+        <v>29</v>
+      </c>
+      <c r="E34" s="26"/>
+      <c r="F34" s="18" t="s">
         <v>200</v>
       </c>
-      <c r="G34" s="6"/>
+      <c r="G34" s="21"/>
       <c r="H34" s="4"/>
       <c r="I34" s="4"/>
     </row>
-    <row r="35" spans="3:9" x14ac:dyDescent="0.3">
-      <c r="C35" s="30" t="s">
-        <v>36</v>
-      </c>
+    <row r="35" spans="3:9" ht="30.15" x14ac:dyDescent="0.3">
+      <c r="C35" s="26"/>
       <c r="D35" s="7" t="s">
-        <v>37</v>
-      </c>
-      <c r="E35" s="24" t="s">
-        <v>136</v>
-      </c>
-      <c r="F35" s="33" t="s">
+        <v>30</v>
+      </c>
+      <c r="E35" s="26"/>
+      <c r="F35" s="18" t="s">
         <v>201</v>
       </c>
-      <c r="G35" s="6"/>
+      <c r="G35" s="21"/>
       <c r="H35" s="4"/>
       <c r="I35" s="4"/>
     </row>
     <row r="36" spans="3:9" x14ac:dyDescent="0.3">
-      <c r="C36" s="30"/>
+      <c r="C36" s="27"/>
       <c r="D36" s="7" t="s">
-        <v>38</v>
-      </c>
-      <c r="E36" s="25"/>
-      <c r="F36" s="34"/>
-      <c r="G36" s="6"/>
+        <v>31</v>
+      </c>
+      <c r="E36" s="26"/>
+      <c r="F36" s="18" t="s">
+        <v>202</v>
+      </c>
+      <c r="G36" s="21"/>
       <c r="H36" s="4"/>
       <c r="I36" s="4"/>
     </row>
-    <row r="37" spans="3:9" x14ac:dyDescent="0.3">
-      <c r="C37" s="30"/>
+    <row r="37" spans="3:9" ht="30.15" x14ac:dyDescent="0.3">
+      <c r="C37" s="3" t="s">
+        <v>32</v>
+      </c>
       <c r="D37" s="7" t="s">
-        <v>39</v>
-      </c>
-      <c r="E37" s="25"/>
-      <c r="F37" s="34"/>
+        <v>33</v>
+      </c>
+      <c r="E37" s="27"/>
+      <c r="F37" s="12" t="s">
+        <v>203</v>
+      </c>
       <c r="G37" s="6"/>
       <c r="H37" s="4"/>
       <c r="I37" s="4"/>
     </row>
     <row r="38" spans="3:9" x14ac:dyDescent="0.3">
-      <c r="C38" s="30"/>
+      <c r="C38" s="3" t="s">
+        <v>34</v>
+      </c>
       <c r="D38" s="7" t="s">
-        <v>40</v>
-      </c>
-      <c r="E38" s="25"/>
-      <c r="F38" s="34"/>
+        <v>35</v>
+      </c>
+      <c r="E38" s="28" t="s">
+        <v>128</v>
+      </c>
+      <c r="F38" s="12" t="s">
+        <v>161</v>
+      </c>
       <c r="G38" s="6"/>
       <c r="H38" s="4"/>
       <c r="I38" s="4"/>
     </row>
     <row r="39" spans="3:9" x14ac:dyDescent="0.3">
-      <c r="C39" s="30"/>
+      <c r="C39" s="28" t="s">
+        <v>36</v>
+      </c>
       <c r="D39" s="7" t="s">
-        <v>41</v>
-      </c>
-      <c r="E39" s="26"/>
-      <c r="F39" s="35"/>
+        <v>37</v>
+      </c>
+      <c r="E39" s="28"/>
+      <c r="F39" s="32" t="s">
+        <v>162</v>
+      </c>
       <c r="G39" s="6"/>
       <c r="H39" s="4"/>
       <c r="I39" s="4"/>
     </row>
-    <row r="40" spans="3:9" ht="30.15" x14ac:dyDescent="0.3">
-      <c r="C40" s="3" t="s">
-        <v>42</v>
-      </c>
+    <row r="40" spans="3:9" x14ac:dyDescent="0.3">
+      <c r="C40" s="28"/>
       <c r="D40" s="7" t="s">
-        <v>43</v>
-      </c>
-      <c r="E40" s="5" t="s">
-        <v>136</v>
-      </c>
-      <c r="F40" s="10" t="s">
-        <v>136</v>
-      </c>
+        <v>38</v>
+      </c>
+      <c r="E40" s="28"/>
+      <c r="F40" s="33"/>
       <c r="G40" s="6"/>
       <c r="H40" s="4"/>
       <c r="I40" s="4"/>
     </row>
     <row r="41" spans="3:9" x14ac:dyDescent="0.3">
-      <c r="C41" s="3" t="s">
-        <v>44</v>
-      </c>
+      <c r="C41" s="28"/>
       <c r="D41" s="7" t="s">
-        <v>45</v>
-      </c>
-      <c r="E41" s="5" t="s">
-        <v>136</v>
-      </c>
-      <c r="F41" s="10" t="s">
-        <v>136</v>
-      </c>
+        <v>39</v>
+      </c>
+      <c r="E41" s="28"/>
+      <c r="F41" s="33"/>
       <c r="G41" s="6"/>
       <c r="H41" s="4"/>
       <c r="I41" s="4"/>
     </row>
     <row r="42" spans="3:9" x14ac:dyDescent="0.3">
-      <c r="C42" s="3" t="s">
-        <v>46</v>
-      </c>
+      <c r="C42" s="28"/>
       <c r="D42" s="7" t="s">
-        <v>48</v>
-      </c>
-      <c r="E42" s="5" t="s">
-        <v>136</v>
-      </c>
-      <c r="F42" s="12" t="s">
-        <v>203</v>
-      </c>
+        <v>40</v>
+      </c>
+      <c r="E42" s="28"/>
+      <c r="F42" s="33"/>
       <c r="G42" s="6"/>
       <c r="H42" s="4"/>
       <c r="I42" s="4"/>
     </row>
-    <row r="43" spans="3:9" ht="30.15" x14ac:dyDescent="0.3">
-      <c r="C43" s="3" t="s">
-        <v>47</v>
-      </c>
+    <row r="43" spans="3:9" x14ac:dyDescent="0.3">
+      <c r="C43" s="28"/>
       <c r="D43" s="7" t="s">
-        <v>49</v>
-      </c>
-      <c r="E43" s="5" t="s">
-        <v>136</v>
-      </c>
-      <c r="F43" s="12" t="s">
-        <v>202</v>
-      </c>
+        <v>41</v>
+      </c>
+      <c r="E43" s="28"/>
+      <c r="F43" s="34"/>
       <c r="G43" s="6"/>
       <c r="H43" s="4"/>
       <c r="I43" s="4"/>
     </row>
-    <row r="44" spans="3:9" x14ac:dyDescent="0.3">
+    <row r="44" spans="3:9" ht="30.15" x14ac:dyDescent="0.3">
       <c r="C44" s="3" t="s">
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="D44" s="7" t="s">
-        <v>51</v>
-      </c>
-      <c r="E44" s="5" t="s">
-        <v>136</v>
-      </c>
+        <v>43</v>
+      </c>
+      <c r="E44" s="28"/>
       <c r="F44" s="10" t="s">
-        <v>136</v>
+        <v>211</v>
       </c>
       <c r="G44" s="6"/>
       <c r="H44" s="4"/>
       <c r="I44" s="4"/>
     </row>
-    <row r="45" spans="3:9" ht="30.15" x14ac:dyDescent="0.3">
-      <c r="C45" s="24" t="s">
-        <v>52</v>
+    <row r="45" spans="3:9" ht="60.25" x14ac:dyDescent="0.3">
+      <c r="C45" s="3" t="s">
+        <v>44</v>
       </c>
       <c r="D45" s="7" t="s">
-        <v>145</v>
-      </c>
-      <c r="E45" s="24" t="s">
-        <v>132</v>
-      </c>
-      <c r="F45" s="19" t="s">
-        <v>143</v>
+        <v>45</v>
+      </c>
+      <c r="E45" s="28"/>
+      <c r="F45" s="12" t="s">
+        <v>212</v>
       </c>
       <c r="G45" s="6"/>
       <c r="H45" s="4"/>
       <c r="I45" s="4"/>
     </row>
-    <row r="46" spans="3:9" ht="30.15" x14ac:dyDescent="0.3">
-      <c r="C46" s="26"/>
+    <row r="46" spans="3:9" x14ac:dyDescent="0.3">
+      <c r="C46" s="3" t="s">
+        <v>46</v>
+      </c>
       <c r="D46" s="7" t="s">
-        <v>53</v>
-      </c>
-      <c r="E46" s="26"/>
-      <c r="F46" s="20" t="s">
-        <v>144</v>
+        <v>48</v>
+      </c>
+      <c r="E46" s="28"/>
+      <c r="F46" s="12" t="s">
+        <v>164</v>
       </c>
       <c r="G46" s="6"/>
       <c r="H46" s="4"/>
       <c r="I46" s="4"/>
     </row>
-    <row r="47" spans="3:9" ht="60.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C47" s="24" t="s">
-        <v>54</v>
+    <row r="47" spans="3:9" ht="30.15" x14ac:dyDescent="0.3">
+      <c r="C47" s="3" t="s">
+        <v>47</v>
       </c>
       <c r="D47" s="7" t="s">
-        <v>55</v>
-      </c>
-      <c r="E47" s="5"/>
-      <c r="F47" s="27" t="s">
-        <v>146</v>
+        <v>49</v>
+      </c>
+      <c r="E47" s="28"/>
+      <c r="F47" s="12" t="s">
+        <v>163</v>
       </c>
       <c r="G47" s="6"/>
       <c r="H47" s="4"/>
       <c r="I47" s="4"/>
     </row>
-    <row r="48" spans="3:9" x14ac:dyDescent="0.3">
-      <c r="C48" s="25"/>
+    <row r="48" spans="3:9" ht="75.3" x14ac:dyDescent="0.3">
+      <c r="C48" s="3" t="s">
+        <v>50</v>
+      </c>
       <c r="D48" s="7" t="s">
-        <v>56</v>
-      </c>
-      <c r="E48" s="5"/>
-      <c r="F48" s="28"/>
+        <v>51</v>
+      </c>
+      <c r="E48" s="23" t="s">
+        <v>214</v>
+      </c>
+      <c r="F48" s="12" t="s">
+        <v>213</v>
+      </c>
       <c r="G48" s="6"/>
       <c r="H48" s="4"/>
       <c r="I48" s="4"/>
     </row>
-    <row r="49" spans="3:9" x14ac:dyDescent="0.3">
-      <c r="C49" s="26"/>
+    <row r="49" spans="3:9" ht="30.15" x14ac:dyDescent="0.3">
+      <c r="C49" s="25" t="s">
+        <v>52</v>
+      </c>
       <c r="D49" s="7" t="s">
-        <v>57</v>
-      </c>
-      <c r="E49" s="5"/>
-      <c r="F49" s="29"/>
+        <v>132</v>
+      </c>
+      <c r="E49" s="25" t="s">
+        <v>127</v>
+      </c>
+      <c r="F49" s="19" t="s">
+        <v>210</v>
+      </c>
       <c r="G49" s="6"/>
       <c r="H49" s="4"/>
       <c r="I49" s="4"/>
     </row>
-    <row r="50" spans="3:9" ht="30.15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C50" s="30" t="s">
-        <v>94</v>
-      </c>
+    <row r="50" spans="3:9" ht="30.15" x14ac:dyDescent="0.3">
+      <c r="C50" s="27"/>
       <c r="D50" s="7" t="s">
-        <v>58</v>
-      </c>
-      <c r="E50" s="24" t="s">
-        <v>132</v>
-      </c>
-      <c r="F50" s="9" t="s">
-        <v>147</v>
+        <v>53</v>
+      </c>
+      <c r="E50" s="26"/>
+      <c r="F50" s="19" t="s">
+        <v>131</v>
       </c>
       <c r="G50" s="6"/>
       <c r="H50" s="4"/>
       <c r="I50" s="4"/>
     </row>
-    <row r="51" spans="3:9" x14ac:dyDescent="0.3">
-      <c r="C51" s="30"/>
+    <row r="51" spans="3:9" ht="30.15" x14ac:dyDescent="0.3">
+      <c r="C51" s="25" t="s">
+        <v>207</v>
+      </c>
       <c r="D51" s="7" t="s">
-        <v>59</v>
-      </c>
-      <c r="E51" s="25"/>
-      <c r="F51" s="9" t="s">
-        <v>148</v>
+        <v>130</v>
+      </c>
+      <c r="E51" s="26"/>
+      <c r="F51" s="19" t="s">
+        <v>208</v>
       </c>
       <c r="G51" s="6"/>
       <c r="H51" s="4"/>
       <c r="I51" s="4"/>
     </row>
-    <row r="52" spans="3:9" ht="45.2" x14ac:dyDescent="0.3">
-      <c r="C52" s="30"/>
+    <row r="52" spans="3:9" ht="60.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C52" s="26"/>
       <c r="D52" s="7" t="s">
-        <v>60</v>
-      </c>
-      <c r="E52" s="25"/>
-      <c r="F52" s="9" t="s">
-        <v>149</v>
+        <v>54</v>
+      </c>
+      <c r="E52" s="26"/>
+      <c r="F52" s="24" t="s">
+        <v>204</v>
       </c>
       <c r="G52" s="6"/>
       <c r="H52" s="4"/>
       <c r="I52" s="4"/>
     </row>
-    <row r="53" spans="3:9" x14ac:dyDescent="0.3">
-      <c r="C53" s="30"/>
+    <row r="53" spans="3:9" ht="120.45" x14ac:dyDescent="0.3">
+      <c r="C53" s="26"/>
       <c r="D53" s="7" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="E53" s="26"/>
-      <c r="F53" s="9" t="s">
-        <v>150</v>
+      <c r="F53" s="24" t="s">
+        <v>209</v>
       </c>
       <c r="G53" s="6"/>
       <c r="H53" s="4"/>
       <c r="I53" s="4"/>
     </row>
-    <row r="54" spans="3:9" ht="105.4" x14ac:dyDescent="0.3">
-      <c r="C54" s="3" t="s">
-        <v>62</v>
-      </c>
+    <row r="54" spans="3:9" ht="90.35" x14ac:dyDescent="0.3">
+      <c r="C54" s="26"/>
       <c r="D54" s="7" t="s">
-        <v>64</v>
-      </c>
-      <c r="E54" s="5"/>
-      <c r="F54" s="10" t="s">
-        <v>152</v>
+        <v>56</v>
+      </c>
+      <c r="E54" s="26"/>
+      <c r="F54" s="24" t="s">
+        <v>205</v>
       </c>
       <c r="G54" s="6"/>
       <c r="H54" s="4"/>
       <c r="I54" s="4"/>
     </row>
     <row r="55" spans="3:9" ht="30.15" x14ac:dyDescent="0.3">
-      <c r="C55" s="30" t="s">
-        <v>65</v>
-      </c>
+      <c r="C55" s="27"/>
       <c r="D55" s="7" t="s">
-        <v>66</v>
-      </c>
-      <c r="E55" s="24" t="s">
-        <v>132</v>
-      </c>
-      <c r="F55" s="9" t="s">
-        <v>151</v>
+        <v>69</v>
+      </c>
+      <c r="E55" s="26"/>
+      <c r="F55" s="12" t="s">
+        <v>206</v>
       </c>
       <c r="G55" s="6"/>
       <c r="H55" s="4"/>
       <c r="I55" s="4"/>
     </row>
-    <row r="56" spans="3:9" ht="60.25" x14ac:dyDescent="0.3">
-      <c r="C56" s="30"/>
+    <row r="56" spans="3:9" ht="30.15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C56" s="28" t="s">
+        <v>93</v>
+      </c>
       <c r="D56" s="7" t="s">
-        <v>67</v>
-      </c>
-      <c r="E56" s="25"/>
+        <v>57</v>
+      </c>
+      <c r="E56" s="26"/>
       <c r="F56" s="9" t="s">
-        <v>155</v>
+        <v>133</v>
       </c>
       <c r="G56" s="6"/>
       <c r="H56" s="4"/>
       <c r="I56" s="4"/>
     </row>
-    <row r="57" spans="3:9" ht="30.15" x14ac:dyDescent="0.3">
-      <c r="C57" s="30"/>
+    <row r="57" spans="3:9" x14ac:dyDescent="0.3">
+      <c r="C57" s="28"/>
       <c r="D57" s="7" t="s">
-        <v>68</v>
-      </c>
-      <c r="E57" s="25"/>
+        <v>58</v>
+      </c>
+      <c r="E57" s="26"/>
       <c r="F57" s="9" t="s">
-        <v>153</v>
+        <v>134</v>
       </c>
       <c r="G57" s="6"/>
       <c r="H57" s="4"/>
       <c r="I57" s="4"/>
     </row>
-    <row r="58" spans="3:9" ht="30.15" x14ac:dyDescent="0.3">
-      <c r="C58" s="30"/>
+    <row r="58" spans="3:9" ht="52.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C58" s="28"/>
       <c r="D58" s="7" t="s">
-        <v>69</v>
-      </c>
-      <c r="E58" s="25"/>
+        <v>59</v>
+      </c>
+      <c r="E58" s="26"/>
       <c r="F58" s="9" t="s">
-        <v>154</v>
+        <v>135</v>
       </c>
       <c r="G58" s="6"/>
       <c r="H58" s="4"/>
       <c r="I58" s="4"/>
     </row>
-    <row r="59" spans="3:9" ht="60.25" x14ac:dyDescent="0.3">
-      <c r="C59" s="30"/>
+    <row r="59" spans="3:9" x14ac:dyDescent="0.3">
+      <c r="C59" s="28"/>
       <c r="D59" s="7" t="s">
-        <v>157</v>
-      </c>
-      <c r="E59" s="25"/>
+        <v>60</v>
+      </c>
+      <c r="E59" s="27"/>
       <c r="F59" s="9" t="s">
-        <v>156</v>
+        <v>136</v>
       </c>
       <c r="G59" s="6"/>
       <c r="H59" s="4"/>
       <c r="I59" s="4"/>
     </row>
-    <row r="60" spans="3:9" ht="120.45" x14ac:dyDescent="0.3">
-      <c r="C60" s="30"/>
-      <c r="D60" s="2" t="s">
-        <v>158</v>
-      </c>
-      <c r="E60" s="26"/>
-      <c r="F60" s="9" t="s">
-        <v>159</v>
+    <row r="60" spans="3:9" ht="105.4" x14ac:dyDescent="0.3">
+      <c r="C60" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="D60" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="E60" s="5"/>
+      <c r="F60" s="10" t="s">
+        <v>137</v>
       </c>
       <c r="G60" s="6"/>
       <c r="H60" s="4"/>
       <c r="I60" s="4"/>
     </row>
-    <row r="61" spans="3:9" x14ac:dyDescent="0.3">
-      <c r="C61" s="3" t="s">
-        <v>71</v>
+    <row r="61" spans="3:9" ht="30.15" x14ac:dyDescent="0.3">
+      <c r="C61" s="28" t="s">
+        <v>64</v>
       </c>
       <c r="D61" s="7" t="s">
-        <v>72</v>
-      </c>
-      <c r="E61" s="5"/>
-      <c r="F61" s="10" t="s">
-        <v>160</v>
+        <v>65</v>
+      </c>
+      <c r="E61" s="25" t="s">
+        <v>127</v>
+      </c>
+      <c r="F61" s="9" t="s">
+        <v>217</v>
       </c>
       <c r="G61" s="6"/>
       <c r="H61" s="4"/>
       <c r="I61" s="4"/>
     </row>
-    <row r="62" spans="3:9" ht="30.15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C62" s="30" t="s">
-        <v>73</v>
-      </c>
+    <row r="62" spans="3:9" ht="60.25" x14ac:dyDescent="0.3">
+      <c r="C62" s="28"/>
       <c r="D62" s="7" t="s">
-        <v>74</v>
-      </c>
-      <c r="E62" s="5"/>
+        <v>66</v>
+      </c>
+      <c r="E62" s="26"/>
       <c r="F62" s="9" t="s">
-        <v>161</v>
+        <v>218</v>
       </c>
       <c r="G62" s="6"/>
       <c r="H62" s="4"/>
       <c r="I62" s="4"/>
     </row>
     <row r="63" spans="3:9" ht="30.15" x14ac:dyDescent="0.3">
-      <c r="C63" s="30"/>
+      <c r="C63" s="28"/>
       <c r="D63" s="7" t="s">
-        <v>75</v>
-      </c>
-      <c r="E63" s="5"/>
+        <v>67</v>
+      </c>
+      <c r="E63" s="26"/>
       <c r="F63" s="9" t="s">
-        <v>167</v>
+        <v>219</v>
       </c>
       <c r="G63" s="6"/>
       <c r="H63" s="4"/>
       <c r="I63" s="4"/>
     </row>
-    <row r="64" spans="3:9" x14ac:dyDescent="0.3">
-      <c r="C64" s="30"/>
+    <row r="64" spans="3:9" ht="30.15" x14ac:dyDescent="0.3">
+      <c r="C64" s="28"/>
       <c r="D64" s="7" t="s">
-        <v>76</v>
-      </c>
-      <c r="E64" s="5"/>
+        <v>68</v>
+      </c>
+      <c r="E64" s="26"/>
       <c r="F64" s="9" t="s">
-        <v>163</v>
+        <v>220</v>
       </c>
       <c r="G64" s="6"/>
       <c r="H64" s="4"/>
       <c r="I64" s="4"/>
     </row>
-    <row r="65" spans="3:9" ht="45.2" x14ac:dyDescent="0.3">
-      <c r="C65" s="30"/>
+    <row r="65" spans="3:9" ht="60.25" x14ac:dyDescent="0.3">
+      <c r="C65" s="28"/>
       <c r="D65" s="7" t="s">
-        <v>77</v>
-      </c>
-      <c r="E65" s="5"/>
-      <c r="F65" s="10" t="s">
-        <v>168</v>
+        <v>138</v>
+      </c>
+      <c r="E65" s="26"/>
+      <c r="F65" s="9" t="s">
+        <v>221</v>
       </c>
       <c r="G65" s="6"/>
       <c r="H65" s="4"/>
       <c r="I65" s="4"/>
     </row>
-    <row r="66" spans="3:9" x14ac:dyDescent="0.3">
-      <c r="C66" s="30"/>
-      <c r="D66" s="7" t="s">
-        <v>78</v>
-      </c>
-      <c r="E66" s="5"/>
+    <row r="66" spans="3:9" ht="90.35" x14ac:dyDescent="0.3">
+      <c r="C66" s="28"/>
+      <c r="D66" s="2" t="s">
+        <v>139</v>
+      </c>
+      <c r="E66" s="26"/>
       <c r="F66" s="9" t="s">
-        <v>164</v>
+        <v>222</v>
       </c>
       <c r="G66" s="6"/>
       <c r="H66" s="4"/>
       <c r="I66" s="4"/>
     </row>
     <row r="67" spans="3:9" x14ac:dyDescent="0.3">
-      <c r="C67" s="30"/>
+      <c r="C67" s="3" t="s">
+        <v>70</v>
+      </c>
       <c r="D67" s="7" t="s">
-        <v>79</v>
-      </c>
-      <c r="E67" s="5"/>
-      <c r="F67" s="9" t="s">
-        <v>162</v>
+        <v>71</v>
+      </c>
+      <c r="E67" s="26"/>
+      <c r="F67" s="10" t="s">
+        <v>140</v>
       </c>
       <c r="G67" s="6"/>
       <c r="H67" s="4"/>
       <c r="I67" s="4"/>
     </row>
-    <row r="68" spans="3:9" x14ac:dyDescent="0.3">
-      <c r="C68" s="30"/>
+    <row r="68" spans="3:9" ht="30.15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C68" s="28" t="s">
+        <v>72</v>
+      </c>
       <c r="D68" s="7" t="s">
-        <v>80</v>
-      </c>
-      <c r="E68" s="5"/>
+        <v>73</v>
+      </c>
+      <c r="E68" s="26"/>
       <c r="F68" s="9" t="s">
-        <v>166</v>
+        <v>141</v>
       </c>
       <c r="G68" s="6"/>
       <c r="H68" s="4"/>
       <c r="I68" s="4"/>
     </row>
-    <row r="69" spans="3:9" x14ac:dyDescent="0.3">
-      <c r="C69" s="30"/>
+    <row r="69" spans="3:9" ht="30.15" x14ac:dyDescent="0.3">
+      <c r="C69" s="28"/>
       <c r="D69" s="7" t="s">
-        <v>81</v>
-      </c>
-      <c r="E69" s="5"/>
+        <v>74</v>
+      </c>
+      <c r="E69" s="26"/>
       <c r="F69" s="9" t="s">
-        <v>165</v>
+        <v>147</v>
       </c>
       <c r="G69" s="6"/>
       <c r="H69" s="4"/>
       <c r="I69" s="4"/>
     </row>
-    <row r="70" spans="3:9" ht="60.25" x14ac:dyDescent="0.3">
-      <c r="C70" s="30"/>
+    <row r="70" spans="3:9" x14ac:dyDescent="0.3">
+      <c r="C70" s="28"/>
       <c r="D70" s="7" t="s">
-        <v>82</v>
-      </c>
-      <c r="E70" s="5"/>
-      <c r="F70" s="10" t="s">
-        <v>170</v>
+        <v>75</v>
+      </c>
+      <c r="E70" s="26"/>
+      <c r="F70" s="9" t="s">
+        <v>143</v>
       </c>
       <c r="G70" s="6"/>
       <c r="H70" s="4"/>
       <c r="I70" s="4"/>
     </row>
-    <row r="71" spans="3:9" ht="30.15" x14ac:dyDescent="0.3">
-      <c r="C71" s="30"/>
+    <row r="71" spans="3:9" x14ac:dyDescent="0.3">
+      <c r="C71" s="28"/>
       <c r="D71" s="7" t="s">
-        <v>83</v>
-      </c>
-      <c r="E71" s="5"/>
-      <c r="F71" s="10" t="s">
-        <v>169</v>
+        <v>76</v>
+      </c>
+      <c r="E71" s="26"/>
+      <c r="F71" s="12" t="s">
+        <v>172</v>
       </c>
       <c r="G71" s="6"/>
       <c r="H71" s="4"/>
       <c r="I71" s="4"/>
     </row>
     <row r="72" spans="3:9" x14ac:dyDescent="0.3">
-      <c r="C72" s="24" t="s">
-        <v>86</v>
-      </c>
+      <c r="C72" s="28"/>
       <c r="D72" s="7" t="s">
-        <v>84</v>
-      </c>
-      <c r="E72" s="24" t="s">
-        <v>132</v>
-      </c>
-      <c r="F72" s="10" t="s">
-        <v>169</v>
+        <v>77</v>
+      </c>
+      <c r="E72" s="26"/>
+      <c r="F72" s="9" t="s">
+        <v>144</v>
       </c>
       <c r="G72" s="6"/>
       <c r="H72" s="4"/>
       <c r="I72" s="4"/>
     </row>
-    <row r="73" spans="3:9" ht="30.15" x14ac:dyDescent="0.3">
-      <c r="C73" s="25"/>
+    <row r="73" spans="3:9" x14ac:dyDescent="0.3">
+      <c r="C73" s="28"/>
       <c r="D73" s="7" t="s">
-        <v>171</v>
-      </c>
-      <c r="E73" s="25"/>
+        <v>78</v>
+      </c>
+      <c r="E73" s="26"/>
       <c r="F73" s="9" t="s">
-        <v>172</v>
+        <v>142</v>
       </c>
       <c r="G73" s="6"/>
       <c r="H73" s="4"/>
       <c r="I73" s="4"/>
     </row>
-    <row r="74" spans="3:9" ht="30.15" x14ac:dyDescent="0.3">
-      <c r="C74" s="25"/>
+    <row r="74" spans="3:9" x14ac:dyDescent="0.3">
+      <c r="C74" s="28"/>
       <c r="D74" s="7" t="s">
-        <v>85</v>
-      </c>
-      <c r="E74" s="25"/>
+        <v>79</v>
+      </c>
+      <c r="E74" s="26"/>
       <c r="F74" s="9" t="s">
-        <v>173</v>
+        <v>146</v>
       </c>
       <c r="G74" s="6"/>
       <c r="H74" s="4"/>
       <c r="I74" s="4"/>
     </row>
-    <row r="75" spans="3:9" ht="30.15" x14ac:dyDescent="0.3">
-      <c r="C75" s="24" t="s">
-        <v>87</v>
-      </c>
+    <row r="75" spans="3:9" x14ac:dyDescent="0.3">
+      <c r="C75" s="28"/>
       <c r="D75" s="7" t="s">
-        <v>191</v>
-      </c>
-      <c r="E75" s="25"/>
+        <v>80</v>
+      </c>
+      <c r="E75" s="26"/>
       <c r="F75" s="9" t="s">
-        <v>181</v>
+        <v>145</v>
       </c>
       <c r="G75" s="6"/>
       <c r="H75" s="4"/>
       <c r="I75" s="4"/>
     </row>
-    <row r="76" spans="3:9" ht="69.400000000000006" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C76" s="25"/>
+    <row r="76" spans="3:9" ht="30.15" x14ac:dyDescent="0.3">
+      <c r="C76" s="28"/>
       <c r="D76" s="7" t="s">
-        <v>192</v>
-      </c>
-      <c r="E76" s="25"/>
-      <c r="F76" s="9" t="s">
-        <v>190</v>
+        <v>81</v>
+      </c>
+      <c r="E76" s="26"/>
+      <c r="F76" s="12" t="s">
+        <v>197</v>
       </c>
       <c r="G76" s="6"/>
       <c r="H76" s="4"/>
       <c r="I76" s="4"/>
     </row>
-    <row r="77" spans="3:9" x14ac:dyDescent="0.3">
-      <c r="C77" s="25"/>
+    <row r="77" spans="3:9" ht="30.15" x14ac:dyDescent="0.3">
+      <c r="C77" s="28"/>
       <c r="D77" s="7" t="s">
-        <v>88</v>
-      </c>
-      <c r="E77" s="25"/>
+        <v>82</v>
+      </c>
+      <c r="E77" s="26"/>
       <c r="F77" s="10" t="s">
-        <v>169</v>
+        <v>148</v>
       </c>
       <c r="G77" s="6"/>
       <c r="H77" s="4"/>
       <c r="I77" s="4"/>
     </row>
-    <row r="78" spans="3:9" ht="30.15" x14ac:dyDescent="0.3">
-      <c r="C78" s="25"/>
+    <row r="78" spans="3:9" x14ac:dyDescent="0.3">
+      <c r="C78" s="25" t="s">
+        <v>85</v>
+      </c>
       <c r="D78" s="7" t="s">
-        <v>89</v>
-      </c>
-      <c r="E78" s="25"/>
-      <c r="F78" s="9" t="s">
-        <v>188</v>
+        <v>83</v>
+      </c>
+      <c r="E78" s="26"/>
+      <c r="F78" s="10" t="s">
+        <v>148</v>
       </c>
       <c r="G78" s="6"/>
       <c r="H78" s="4"/>
       <c r="I78" s="4"/>
     </row>
     <row r="79" spans="3:9" ht="30.15" x14ac:dyDescent="0.3">
-      <c r="C79" s="25"/>
+      <c r="C79" s="26"/>
       <c r="D79" s="7" t="s">
-        <v>90</v>
-      </c>
-      <c r="E79" s="25"/>
+        <v>149</v>
+      </c>
+      <c r="E79" s="26"/>
       <c r="F79" s="9" t="s">
-        <v>180</v>
+        <v>173</v>
       </c>
       <c r="G79" s="6"/>
       <c r="H79" s="4"/>
       <c r="I79" s="4"/>
     </row>
     <row r="80" spans="3:9" ht="30.15" x14ac:dyDescent="0.3">
-      <c r="C80" s="25"/>
+      <c r="C80" s="26"/>
       <c r="D80" s="7" t="s">
-        <v>91</v>
-      </c>
-      <c r="E80" s="25"/>
+        <v>84</v>
+      </c>
+      <c r="E80" s="26"/>
       <c r="F80" s="9" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="G80" s="6"/>
       <c r="H80" s="4"/>
       <c r="I80" s="4"/>
     </row>
     <row r="81" spans="3:9" ht="30.15" x14ac:dyDescent="0.3">
-      <c r="C81" s="25"/>
+      <c r="C81" s="25" t="s">
+        <v>86</v>
+      </c>
       <c r="D81" s="7" t="s">
-        <v>92</v>
-      </c>
-      <c r="E81" s="25"/>
+        <v>153</v>
+      </c>
+      <c r="E81" s="26"/>
       <c r="F81" s="9" t="s">
-        <v>183</v>
+        <v>175</v>
       </c>
       <c r="G81" s="6"/>
       <c r="H81" s="4"/>
       <c r="I81" s="4"/>
     </row>
-    <row r="82" spans="3:9" ht="30.15" x14ac:dyDescent="0.3">
-      <c r="C82" s="25"/>
+    <row r="82" spans="3:9" ht="69.400000000000006" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C82" s="26"/>
       <c r="D82" s="7" t="s">
-        <v>93</v>
-      </c>
-      <c r="E82" s="25"/>
+        <v>154</v>
+      </c>
+      <c r="E82" s="26"/>
       <c r="F82" s="9" t="s">
-        <v>182</v>
+        <v>189</v>
       </c>
       <c r="G82" s="6"/>
       <c r="H82" s="4"/>
       <c r="I82" s="4"/>
     </row>
     <row r="83" spans="3:9" x14ac:dyDescent="0.3">
-      <c r="C83" s="25"/>
+      <c r="C83" s="26"/>
       <c r="D83" s="7" t="s">
-        <v>100</v>
-      </c>
-      <c r="E83" s="25"/>
+        <v>87</v>
+      </c>
+      <c r="E83" s="26"/>
       <c r="F83" s="10" t="s">
-        <v>169</v>
+        <v>148</v>
       </c>
       <c r="G83" s="6"/>
       <c r="H83" s="4"/>
       <c r="I83" s="4"/>
     </row>
-    <row r="84" spans="3:9" ht="30.15" x14ac:dyDescent="0.3">
-      <c r="C84" s="25"/>
+    <row r="84" spans="3:9" x14ac:dyDescent="0.3">
+      <c r="C84" s="26"/>
       <c r="D84" s="7" t="s">
-        <v>101</v>
-      </c>
-      <c r="E84" s="25"/>
+        <v>88</v>
+      </c>
+      <c r="E84" s="26"/>
       <c r="F84" s="9" t="s">
-        <v>184</v>
+        <v>176</v>
       </c>
       <c r="G84" s="6"/>
       <c r="H84" s="4"/>
       <c r="I84" s="4"/>
     </row>
     <row r="85" spans="3:9" ht="30.15" x14ac:dyDescent="0.3">
-      <c r="C85" s="25"/>
+      <c r="C85" s="26"/>
       <c r="D85" s="7" t="s">
-        <v>102</v>
-      </c>
-      <c r="E85" s="25"/>
+        <v>89</v>
+      </c>
+      <c r="E85" s="26"/>
       <c r="F85" s="9" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="G85" s="6"/>
       <c r="H85" s="4"/>
       <c r="I85" s="4"/>
     </row>
     <row r="86" spans="3:9" ht="30.15" x14ac:dyDescent="0.3">
-      <c r="C86" s="25"/>
+      <c r="C86" s="26"/>
       <c r="D86" s="7" t="s">
-        <v>103</v>
-      </c>
-      <c r="E86" s="25"/>
+        <v>90</v>
+      </c>
+      <c r="E86" s="26"/>
       <c r="F86" s="9" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="G86" s="6"/>
       <c r="H86" s="4"/>
       <c r="I86" s="4"/>
     </row>
-    <row r="87" spans="3:9" ht="45.2" x14ac:dyDescent="0.3">
-      <c r="C87" s="25"/>
+    <row r="87" spans="3:9" x14ac:dyDescent="0.3">
+      <c r="C87" s="26"/>
       <c r="D87" s="7" t="s">
-        <v>186</v>
-      </c>
-      <c r="E87" s="25"/>
+        <v>91</v>
+      </c>
+      <c r="E87" s="26"/>
       <c r="F87" s="9" t="s">
-        <v>187</v>
+        <v>179</v>
       </c>
       <c r="G87" s="6"/>
       <c r="H87" s="4"/>
       <c r="I87" s="4"/>
     </row>
-    <row r="88" spans="3:9" ht="30.15" x14ac:dyDescent="0.3">
-      <c r="C88" s="24" t="s">
-        <v>95</v>
-      </c>
+    <row r="88" spans="3:9" x14ac:dyDescent="0.3">
+      <c r="C88" s="26"/>
       <c r="D88" s="7" t="s">
-        <v>96</v>
-      </c>
-      <c r="E88" s="25"/>
+        <v>92</v>
+      </c>
+      <c r="E88" s="26"/>
       <c r="F88" s="9" t="s">
-        <v>175</v>
+        <v>180</v>
       </c>
       <c r="G88" s="6"/>
       <c r="H88" s="4"/>
       <c r="I88" s="4"/>
     </row>
-    <row r="89" spans="3:9" ht="30.15" x14ac:dyDescent="0.3">
-      <c r="C89" s="25"/>
+    <row r="89" spans="3:9" x14ac:dyDescent="0.3">
+      <c r="C89" s="26"/>
       <c r="D89" s="7" t="s">
-        <v>97</v>
-      </c>
-      <c r="E89" s="25"/>
-      <c r="F89" s="9" t="s">
-        <v>176</v>
+        <v>99</v>
+      </c>
+      <c r="E89" s="26"/>
+      <c r="F89" s="10" t="s">
+        <v>148</v>
       </c>
       <c r="G89" s="6"/>
       <c r="H89" s="4"/>
       <c r="I89" s="4"/>
     </row>
     <row r="90" spans="3:9" x14ac:dyDescent="0.3">
-      <c r="C90" s="25"/>
+      <c r="C90" s="26"/>
       <c r="D90" s="7" t="s">
-        <v>98</v>
-      </c>
-      <c r="E90" s="25"/>
-      <c r="F90" s="10" t="s">
-        <v>169</v>
+        <v>100</v>
+      </c>
+      <c r="E90" s="26"/>
+      <c r="F90" s="9" t="s">
+        <v>181</v>
       </c>
       <c r="G90" s="6"/>
       <c r="H90" s="4"/>
       <c r="I90" s="4"/>
     </row>
-    <row r="91" spans="3:9" ht="30.15" x14ac:dyDescent="0.3">
-      <c r="C91" s="25"/>
+    <row r="91" spans="3:9" x14ac:dyDescent="0.3">
+      <c r="C91" s="26"/>
       <c r="D91" s="7" t="s">
-        <v>99</v>
-      </c>
-      <c r="E91" s="25"/>
+        <v>101</v>
+      </c>
+      <c r="E91" s="26"/>
       <c r="F91" s="9" t="s">
-        <v>174</v>
+        <v>182</v>
       </c>
       <c r="G91" s="6"/>
       <c r="H91" s="4"/>
       <c r="I91" s="4"/>
     </row>
     <row r="92" spans="3:9" ht="30.15" x14ac:dyDescent="0.3">
-      <c r="C92" s="25"/>
+      <c r="C92" s="26"/>
       <c r="D92" s="7" t="s">
-        <v>185</v>
-      </c>
-      <c r="E92" s="25"/>
+        <v>102</v>
+      </c>
+      <c r="E92" s="26"/>
       <c r="F92" s="9" t="s">
-        <v>193</v>
+        <v>183</v>
       </c>
       <c r="G92" s="6"/>
       <c r="H92" s="4"/>
       <c r="I92" s="4"/>
     </row>
-    <row r="93" spans="3:9" ht="30.15" x14ac:dyDescent="0.3">
+    <row r="93" spans="3:9" ht="45.2" x14ac:dyDescent="0.3">
       <c r="C93" s="26"/>
-      <c r="D93" s="2" t="s">
-        <v>70</v>
+      <c r="D93" s="7" t="s">
+        <v>151</v>
       </c>
       <c r="E93" s="26"/>
       <c r="F93" s="9" t="s">
-        <v>189</v>
+        <v>184</v>
       </c>
       <c r="G93" s="6"/>
       <c r="H93" s="4"/>
       <c r="I93" s="4"/>
     </row>
     <row r="94" spans="3:9" x14ac:dyDescent="0.3">
-      <c r="C94" s="30" t="s">
-        <v>110</v>
+      <c r="C94" s="25" t="s">
+        <v>94</v>
       </c>
       <c r="D94" s="7" t="s">
-        <v>104</v>
-      </c>
-      <c r="E94" s="24" t="s">
-        <v>132</v>
-      </c>
+        <v>95</v>
+      </c>
+      <c r="E94" s="26"/>
       <c r="F94" s="9" t="s">
-        <v>195</v>
+        <v>185</v>
       </c>
       <c r="G94" s="6"/>
       <c r="H94" s="4"/>
       <c r="I94" s="4"/>
     </row>
     <row r="95" spans="3:9" ht="30.15" x14ac:dyDescent="0.3">
-      <c r="C95" s="30"/>
+      <c r="C95" s="26"/>
       <c r="D95" s="7" t="s">
-        <v>105</v>
-      </c>
-      <c r="E95" s="25"/>
+        <v>96</v>
+      </c>
+      <c r="E95" s="26"/>
       <c r="F95" s="9" t="s">
-        <v>194</v>
+        <v>186</v>
       </c>
       <c r="G95" s="6"/>
       <c r="H95" s="4"/>
       <c r="I95" s="4"/>
     </row>
     <row r="96" spans="3:9" x14ac:dyDescent="0.3">
-      <c r="C96" s="30"/>
+      <c r="C96" s="26"/>
       <c r="D96" s="7" t="s">
-        <v>106</v>
-      </c>
-      <c r="E96" s="25"/>
-      <c r="F96" s="9" t="s">
-        <v>197</v>
+        <v>97</v>
+      </c>
+      <c r="E96" s="26"/>
+      <c r="F96" s="10" t="s">
+        <v>148</v>
       </c>
       <c r="G96" s="6"/>
       <c r="H96" s="4"/>
       <c r="I96" s="4"/>
     </row>
-    <row r="97" spans="3:9" ht="30.15" x14ac:dyDescent="0.3">
-      <c r="C97" s="30"/>
+    <row r="97" spans="3:9" x14ac:dyDescent="0.3">
+      <c r="C97" s="26"/>
       <c r="D97" s="7" t="s">
-        <v>107</v>
-      </c>
-      <c r="E97" s="25"/>
+        <v>98</v>
+      </c>
+      <c r="E97" s="26"/>
       <c r="F97" s="9" t="s">
-        <v>196</v>
+        <v>187</v>
       </c>
       <c r="G97" s="6"/>
       <c r="H97" s="4"/>
       <c r="I97" s="4"/>
     </row>
     <row r="98" spans="3:9" x14ac:dyDescent="0.3">
-      <c r="C98" s="30"/>
+      <c r="C98" s="26"/>
       <c r="D98" s="7" t="s">
-        <v>108</v>
-      </c>
-      <c r="E98" s="25"/>
+        <v>150</v>
+      </c>
+      <c r="E98" s="26"/>
       <c r="F98" s="9" t="s">
-        <v>198</v>
+        <v>188</v>
       </c>
       <c r="G98" s="6"/>
       <c r="H98" s="4"/>
       <c r="I98" s="4"/>
     </row>
     <row r="99" spans="3:9" ht="30.15" x14ac:dyDescent="0.3">
-      <c r="C99" s="30"/>
-      <c r="D99" s="8" t="s">
-        <v>109</v>
+      <c r="C99" s="27"/>
+      <c r="D99" s="2" t="s">
+        <v>69</v>
       </c>
       <c r="E99" s="26"/>
       <c r="F99" s="9" t="s">
-        <v>199</v>
+        <v>152</v>
       </c>
       <c r="G99" s="6"/>
       <c r="H99" s="4"/>
       <c r="I99" s="4"/>
     </row>
     <row r="100" spans="3:9" x14ac:dyDescent="0.3">
-      <c r="E100" s="21"/>
-    </row>
-    <row r="101" spans="3:9" x14ac:dyDescent="0.3">
-      <c r="E101" s="21"/>
+      <c r="C100" s="28" t="s">
+        <v>109</v>
+      </c>
+      <c r="D100" s="7" t="s">
+        <v>103</v>
+      </c>
+      <c r="E100" s="26"/>
+      <c r="F100" s="9" t="s">
+        <v>156</v>
+      </c>
+      <c r="G100" s="6"/>
+      <c r="H100" s="4"/>
+      <c r="I100" s="4"/>
+    </row>
+    <row r="101" spans="3:9" ht="30.15" x14ac:dyDescent="0.3">
+      <c r="C101" s="28"/>
+      <c r="D101" s="7" t="s">
+        <v>104</v>
+      </c>
+      <c r="E101" s="26"/>
+      <c r="F101" s="9" t="s">
+        <v>155</v>
+      </c>
+      <c r="G101" s="6"/>
+      <c r="H101" s="4"/>
+      <c r="I101" s="4"/>
     </row>
     <row r="102" spans="3:9" x14ac:dyDescent="0.3">
-      <c r="E102" s="21"/>
+      <c r="C102" s="28"/>
+      <c r="D102" s="7" t="s">
+        <v>105</v>
+      </c>
+      <c r="E102" s="26"/>
+      <c r="F102" s="9" t="s">
+        <v>158</v>
+      </c>
+      <c r="G102" s="6"/>
+      <c r="H102" s="4"/>
+      <c r="I102" s="4"/>
+    </row>
+    <row r="103" spans="3:9" ht="30.15" x14ac:dyDescent="0.3">
+      <c r="C103" s="28"/>
+      <c r="D103" s="7" t="s">
+        <v>106</v>
+      </c>
+      <c r="E103" s="26"/>
+      <c r="F103" s="9" t="s">
+        <v>157</v>
+      </c>
+      <c r="G103" s="6"/>
+      <c r="H103" s="4"/>
+      <c r="I103" s="4"/>
+    </row>
+    <row r="104" spans="3:9" x14ac:dyDescent="0.3">
+      <c r="C104" s="28"/>
+      <c r="D104" s="7" t="s">
+        <v>107</v>
+      </c>
+      <c r="E104" s="26"/>
+      <c r="F104" s="9" t="s">
+        <v>159</v>
+      </c>
+      <c r="G104" s="6"/>
+      <c r="H104" s="4"/>
+      <c r="I104" s="4"/>
+    </row>
+    <row r="105" spans="3:9" ht="30.15" x14ac:dyDescent="0.3">
+      <c r="C105" s="28"/>
+      <c r="D105" s="8" t="s">
+        <v>108</v>
+      </c>
+      <c r="E105" s="27"/>
+      <c r="F105" s="9" t="s">
+        <v>160</v>
+      </c>
+      <c r="G105" s="6"/>
+      <c r="H105" s="4"/>
+      <c r="I105" s="4"/>
+    </row>
+    <row r="106" spans="3:9" x14ac:dyDescent="0.3">
+      <c r="E106" s="20"/>
+    </row>
+    <row r="107" spans="3:9" x14ac:dyDescent="0.3">
+      <c r="E107" s="20"/>
+    </row>
+    <row r="108" spans="3:9" x14ac:dyDescent="0.3">
+      <c r="E108" s="20"/>
     </row>
   </sheetData>
-  <mergeCells count="34">
-    <mergeCell ref="F9:F12"/>
-    <mergeCell ref="F23:F27"/>
-    <mergeCell ref="F35:F39"/>
+  <mergeCells count="27">
+    <mergeCell ref="F27:F31"/>
+    <mergeCell ref="F39:F43"/>
     <mergeCell ref="F6:F7"/>
-    <mergeCell ref="E15:E18"/>
-    <mergeCell ref="E13:E14"/>
-    <mergeCell ref="E5:E8"/>
-    <mergeCell ref="E28:E32"/>
-    <mergeCell ref="E20:E22"/>
-    <mergeCell ref="C55:C60"/>
+    <mergeCell ref="E3:E26"/>
+    <mergeCell ref="E32:E37"/>
+    <mergeCell ref="E38:E47"/>
+    <mergeCell ref="F18:F22"/>
+    <mergeCell ref="C61:C66"/>
     <mergeCell ref="C5:C8"/>
-    <mergeCell ref="C9:C12"/>
-    <mergeCell ref="C13:C14"/>
-    <mergeCell ref="C15:C18"/>
-    <mergeCell ref="C20:C22"/>
-    <mergeCell ref="C23:C24"/>
-    <mergeCell ref="C25:C27"/>
-    <mergeCell ref="C35:C39"/>
-    <mergeCell ref="C47:C49"/>
-    <mergeCell ref="C50:C53"/>
-    <mergeCell ref="C28:C32"/>
-    <mergeCell ref="C45:C46"/>
-    <mergeCell ref="C62:C71"/>
-    <mergeCell ref="C72:C74"/>
-    <mergeCell ref="C75:C87"/>
-    <mergeCell ref="C88:C93"/>
+    <mergeCell ref="C9:C15"/>
+    <mergeCell ref="C16:C17"/>
+    <mergeCell ref="C24:C26"/>
+    <mergeCell ref="C27:C28"/>
+    <mergeCell ref="C29:C31"/>
+    <mergeCell ref="C39:C43"/>
+    <mergeCell ref="C56:C59"/>
+    <mergeCell ref="C32:C36"/>
+    <mergeCell ref="C49:C50"/>
+    <mergeCell ref="C51:C55"/>
+    <mergeCell ref="C18:C22"/>
+    <mergeCell ref="C68:C77"/>
+    <mergeCell ref="C78:C80"/>
+    <mergeCell ref="C81:C93"/>
     <mergeCell ref="C94:C99"/>
-    <mergeCell ref="E94:E99"/>
-    <mergeCell ref="F47:F49"/>
-    <mergeCell ref="E35:E39"/>
-    <mergeCell ref="E55:E60"/>
-    <mergeCell ref="E50:E53"/>
-    <mergeCell ref="E72:E93"/>
-    <mergeCell ref="E45:E46"/>
+    <mergeCell ref="C100:C105"/>
+    <mergeCell ref="E49:E59"/>
+    <mergeCell ref="E61:E105"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
more mutates until human capital distribution ratios
</commit_message>
<xml_diff>
--- a/edit_eam/crosscheck.xlsx
+++ b/edit_eam/crosscheck.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="317" uniqueCount="226">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="318" uniqueCount="226">
   <si>
     <t>Nombre</t>
   </si>
@@ -403,9 +403,6 @@
     <t>IV4R4C3/Total</t>
   </si>
   <si>
-    <t>IV4R6C3/Total</t>
-  </si>
-  <si>
     <t>(IV4R5C3 + IV4R2C3 + IV4R1C3)/Total</t>
   </si>
   <si>
@@ -692,6 +689,9 @@
   </si>
   <si>
     <t>Capital humano educacion</t>
+  </si>
+  <si>
+    <t>IV4R11C3/Total</t>
   </si>
 </sst>
 </file>
@@ -984,6 +984,51 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
@@ -999,51 +1044,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1352,8 +1352,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="C2:I108"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B50" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C57" sqref="C57:C60"/>
+    <sheetView tabSelected="1" topLeftCell="B55" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C62" sqref="C62:C67"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="15.05" x14ac:dyDescent="0.3"/>
@@ -1396,7 +1396,7 @@
       <c r="D3" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="E3" s="56" t="s">
+      <c r="E3" s="39" t="s">
         <v>122</v>
       </c>
       <c r="F3" s="9" t="s">
@@ -1404,7 +1404,7 @@
       </c>
       <c r="G3" s="6"/>
       <c r="H3" s="27" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="I3" s="4"/>
     </row>
@@ -1415,7 +1415,7 @@
       <c r="D4" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="E4" s="57"/>
+      <c r="E4" s="40"/>
       <c r="F4" s="12" t="s">
         <v>108</v>
       </c>
@@ -1424,262 +1424,262 @@
       <c r="I4" s="4"/>
     </row>
     <row r="5" spans="3:9" x14ac:dyDescent="0.3">
-      <c r="C5" s="59" t="s">
+      <c r="C5" s="42" t="s">
         <v>7</v>
       </c>
       <c r="D5" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="E5" s="57"/>
+      <c r="E5" s="40"/>
       <c r="F5" s="9" t="s">
         <v>109</v>
       </c>
       <c r="G5" s="6"/>
       <c r="H5" s="27" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="I5" s="4"/>
     </row>
     <row r="6" spans="3:9" x14ac:dyDescent="0.3">
-      <c r="C6" s="59"/>
+      <c r="C6" s="42"/>
       <c r="D6" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="E6" s="57"/>
-      <c r="F6" s="54" t="s">
+      <c r="E6" s="40"/>
+      <c r="F6" s="52" t="s">
         <v>111</v>
       </c>
-      <c r="G6" s="42"/>
-      <c r="H6" s="39" t="s">
-        <v>212</v>
-      </c>
-      <c r="I6" s="45"/>
+      <c r="G6" s="57"/>
+      <c r="H6" s="54" t="s">
+        <v>211</v>
+      </c>
+      <c r="I6" s="43"/>
     </row>
     <row r="7" spans="3:9" x14ac:dyDescent="0.3">
-      <c r="C7" s="59"/>
+      <c r="C7" s="42"/>
       <c r="D7" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="E7" s="57"/>
-      <c r="F7" s="55"/>
-      <c r="G7" s="44"/>
-      <c r="H7" s="41"/>
-      <c r="I7" s="46"/>
+      <c r="E7" s="40"/>
+      <c r="F7" s="53"/>
+      <c r="G7" s="59"/>
+      <c r="H7" s="56"/>
+      <c r="I7" s="44"/>
     </row>
     <row r="8" spans="3:9" x14ac:dyDescent="0.3">
-      <c r="C8" s="59"/>
+      <c r="C8" s="42"/>
       <c r="D8" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="E8" s="57"/>
+      <c r="E8" s="40"/>
       <c r="F8" s="11" t="s">
         <v>110</v>
       </c>
       <c r="G8" s="6"/>
       <c r="H8" s="27" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="I8" s="4"/>
     </row>
     <row r="9" spans="3:9" x14ac:dyDescent="0.3">
-      <c r="C9" s="59" t="s">
+      <c r="C9" s="42" t="s">
         <v>13</v>
       </c>
       <c r="D9" s="7" t="s">
-        <v>158</v>
-      </c>
-      <c r="E9" s="57"/>
+        <v>157</v>
+      </c>
+      <c r="E9" s="40"/>
       <c r="F9" s="24" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="G9" s="6"/>
       <c r="H9" s="27" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="I9" s="4"/>
     </row>
     <row r="10" spans="3:9" x14ac:dyDescent="0.3">
-      <c r="C10" s="59"/>
+      <c r="C10" s="42"/>
       <c r="D10" s="7" t="s">
-        <v>159</v>
-      </c>
-      <c r="E10" s="57"/>
+        <v>158</v>
+      </c>
+      <c r="E10" s="40"/>
       <c r="F10" s="24" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="G10" s="6"/>
       <c r="H10" s="27" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="I10" s="4"/>
     </row>
     <row r="11" spans="3:9" ht="34.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C11" s="59"/>
+      <c r="C11" s="42"/>
       <c r="D11" s="7" t="s">
-        <v>160</v>
-      </c>
-      <c r="E11" s="57"/>
+        <v>159</v>
+      </c>
+      <c r="E11" s="40"/>
       <c r="F11" s="24" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="G11" s="6"/>
       <c r="H11" s="27" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="I11" s="4"/>
     </row>
     <row r="12" spans="3:9" ht="34.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C12" s="59"/>
+      <c r="C12" s="42"/>
       <c r="D12" s="7" t="s">
-        <v>161</v>
-      </c>
-      <c r="E12" s="57"/>
+        <v>160</v>
+      </c>
+      <c r="E12" s="40"/>
       <c r="F12" s="24" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="G12" s="6"/>
       <c r="H12" s="27" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="I12" s="4"/>
     </row>
     <row r="13" spans="3:9" ht="65.45" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C13" s="59"/>
+      <c r="C13" s="42"/>
       <c r="D13" s="7" t="s">
-        <v>162</v>
-      </c>
-      <c r="E13" s="57"/>
+        <v>161</v>
+      </c>
+      <c r="E13" s="40"/>
       <c r="F13" s="24" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="G13" s="6"/>
       <c r="H13" s="27" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="I13" s="4"/>
     </row>
     <row r="14" spans="3:9" ht="46.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C14" s="59"/>
+      <c r="C14" s="42"/>
       <c r="D14" s="7" t="s">
-        <v>163</v>
-      </c>
-      <c r="E14" s="57"/>
+        <v>162</v>
+      </c>
+      <c r="E14" s="40"/>
       <c r="F14" s="24" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="G14" s="6"/>
       <c r="H14" s="27" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="I14" s="4"/>
     </row>
     <row r="15" spans="3:9" ht="66.150000000000006" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C15" s="59"/>
+      <c r="C15" s="42"/>
       <c r="D15" s="7" t="s">
-        <v>164</v>
-      </c>
-      <c r="E15" s="57"/>
+        <v>163</v>
+      </c>
+      <c r="E15" s="40"/>
       <c r="F15" s="24" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="G15" s="6"/>
       <c r="H15" s="27" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="I15" s="4"/>
     </row>
     <row r="16" spans="3:9" x14ac:dyDescent="0.3">
-      <c r="C16" s="59" t="s">
+      <c r="C16" s="42" t="s">
         <v>14</v>
       </c>
       <c r="D16" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="E16" s="57"/>
+      <c r="E16" s="40"/>
       <c r="F16" s="9" t="s">
         <v>112</v>
       </c>
       <c r="G16" s="6"/>
       <c r="H16" s="27" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="I16" s="4"/>
     </row>
     <row r="17" spans="3:9" x14ac:dyDescent="0.3">
-      <c r="C17" s="59"/>
+      <c r="C17" s="42"/>
       <c r="D17" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="E17" s="57"/>
+      <c r="E17" s="40"/>
       <c r="F17" s="9" t="s">
         <v>113</v>
       </c>
       <c r="G17" s="6"/>
       <c r="H17" s="27" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="I17" s="4"/>
     </row>
     <row r="18" spans="3:9" ht="15.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C18" s="56" t="s">
+      <c r="C18" s="39" t="s">
         <v>114</v>
       </c>
       <c r="D18" s="7" t="s">
         <v>115</v>
       </c>
-      <c r="E18" s="57"/>
-      <c r="F18" s="56" t="s">
-        <v>203</v>
-      </c>
-      <c r="G18" s="42"/>
-      <c r="H18" s="39" t="s">
-        <v>212</v>
-      </c>
-      <c r="I18" s="45"/>
+      <c r="E18" s="40"/>
+      <c r="F18" s="39" t="s">
+        <v>202</v>
+      </c>
+      <c r="G18" s="57"/>
+      <c r="H18" s="54" t="s">
+        <v>211</v>
+      </c>
+      <c r="I18" s="43"/>
     </row>
     <row r="19" spans="3:9" x14ac:dyDescent="0.3">
-      <c r="C19" s="57"/>
+      <c r="C19" s="40"/>
       <c r="D19" s="7" t="s">
         <v>116</v>
       </c>
-      <c r="E19" s="57"/>
-      <c r="F19" s="57"/>
-      <c r="G19" s="43"/>
-      <c r="H19" s="40"/>
-      <c r="I19" s="47"/>
+      <c r="E19" s="40"/>
+      <c r="F19" s="40"/>
+      <c r="G19" s="58"/>
+      <c r="H19" s="55"/>
+      <c r="I19" s="45"/>
     </row>
     <row r="20" spans="3:9" x14ac:dyDescent="0.3">
-      <c r="C20" s="57"/>
+      <c r="C20" s="40"/>
       <c r="D20" s="7" t="s">
         <v>117</v>
       </c>
-      <c r="E20" s="57"/>
-      <c r="F20" s="57"/>
-      <c r="G20" s="43"/>
-      <c r="H20" s="40"/>
-      <c r="I20" s="47"/>
+      <c r="E20" s="40"/>
+      <c r="F20" s="40"/>
+      <c r="G20" s="58"/>
+      <c r="H20" s="55"/>
+      <c r="I20" s="45"/>
     </row>
     <row r="21" spans="3:9" x14ac:dyDescent="0.3">
-      <c r="C21" s="57"/>
+      <c r="C21" s="40"/>
       <c r="D21" s="7" t="s">
         <v>118</v>
       </c>
-      <c r="E21" s="57"/>
-      <c r="F21" s="57"/>
-      <c r="G21" s="43"/>
-      <c r="H21" s="40"/>
-      <c r="I21" s="47"/>
+      <c r="E21" s="40"/>
+      <c r="F21" s="40"/>
+      <c r="G21" s="58"/>
+      <c r="H21" s="55"/>
+      <c r="I21" s="45"/>
     </row>
     <row r="22" spans="3:9" x14ac:dyDescent="0.3">
-      <c r="C22" s="58"/>
+      <c r="C22" s="41"/>
       <c r="D22" s="7" t="s">
-        <v>204</v>
-      </c>
-      <c r="E22" s="57"/>
-      <c r="F22" s="58"/>
-      <c r="G22" s="44"/>
-      <c r="H22" s="41"/>
-      <c r="I22" s="46"/>
+        <v>203</v>
+      </c>
+      <c r="E22" s="40"/>
+      <c r="F22" s="41"/>
+      <c r="G22" s="59"/>
+      <c r="H22" s="56"/>
+      <c r="I22" s="44"/>
     </row>
     <row r="23" spans="3:9" ht="30.15" x14ac:dyDescent="0.3">
       <c r="C23" s="3" t="s">
@@ -1688,213 +1688,215 @@
       <c r="D23" s="7" t="s">
         <v>62</v>
       </c>
-      <c r="E23" s="57"/>
+      <c r="E23" s="40"/>
       <c r="F23" s="9" t="s">
         <v>119</v>
       </c>
       <c r="G23" s="6"/>
       <c r="H23" s="27" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="I23" s="4"/>
     </row>
     <row r="24" spans="3:9" x14ac:dyDescent="0.3">
-      <c r="C24" s="59" t="s">
+      <c r="C24" s="42" t="s">
         <v>120</v>
       </c>
       <c r="D24" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="E24" s="57"/>
+      <c r="E24" s="40"/>
       <c r="F24" s="12" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="G24" s="6"/>
       <c r="H24" s="27" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="I24" s="4"/>
     </row>
     <row r="25" spans="3:9" ht="135.5" x14ac:dyDescent="0.3">
-      <c r="C25" s="59"/>
+      <c r="C25" s="42"/>
       <c r="D25" s="7" t="s">
-        <v>223</v>
-      </c>
-      <c r="E25" s="57"/>
+        <v>222</v>
+      </c>
+      <c r="E25" s="40"/>
       <c r="F25" s="12" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="G25" s="6"/>
-      <c r="H25" s="27"/>
+      <c r="H25" s="27" t="s">
+        <v>211</v>
+      </c>
       <c r="I25" s="4"/>
     </row>
     <row r="26" spans="3:9" ht="45.2" x14ac:dyDescent="0.3">
-      <c r="C26" s="59"/>
+      <c r="C26" s="42"/>
       <c r="D26" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="E26" s="57"/>
+      <c r="E26" s="40"/>
       <c r="F26" s="12" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="G26" s="6"/>
       <c r="H26" s="27" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="I26" s="4"/>
     </row>
     <row r="27" spans="3:9" ht="45.2" x14ac:dyDescent="0.3">
-      <c r="C27" s="59"/>
+      <c r="C27" s="42"/>
       <c r="D27" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="E27" s="58"/>
+      <c r="E27" s="41"/>
       <c r="F27" s="12" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="G27" s="6"/>
       <c r="H27" s="27" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="I27" s="4"/>
     </row>
     <row r="28" spans="3:9" x14ac:dyDescent="0.3">
-      <c r="C28" s="59" t="s">
+      <c r="C28" s="42" t="s">
         <v>23</v>
       </c>
       <c r="D28" s="7" t="s">
         <v>21</v>
       </c>
       <c r="E28" s="5"/>
-      <c r="F28" s="48" t="s">
-        <v>217</v>
+      <c r="F28" s="46" t="s">
+        <v>216</v>
       </c>
       <c r="G28" s="36"/>
       <c r="H28" s="37"/>
       <c r="I28" s="38"/>
     </row>
     <row r="29" spans="3:9" x14ac:dyDescent="0.3">
-      <c r="C29" s="59"/>
+      <c r="C29" s="42"/>
       <c r="D29" s="7" t="s">
         <v>22</v>
       </c>
       <c r="E29" s="5"/>
-      <c r="F29" s="49"/>
+      <c r="F29" s="47"/>
       <c r="G29" s="36"/>
       <c r="H29" s="37"/>
       <c r="I29" s="38"/>
     </row>
     <row r="30" spans="3:9" x14ac:dyDescent="0.3">
-      <c r="C30" s="59" t="s">
+      <c r="C30" s="42" t="s">
         <v>24</v>
       </c>
       <c r="D30" s="7" t="s">
         <v>25</v>
       </c>
       <c r="E30" s="5"/>
-      <c r="F30" s="49"/>
+      <c r="F30" s="47"/>
       <c r="G30" s="36"/>
       <c r="H30" s="37"/>
       <c r="I30" s="38"/>
     </row>
     <row r="31" spans="3:9" x14ac:dyDescent="0.3">
-      <c r="C31" s="59"/>
+      <c r="C31" s="42"/>
       <c r="D31" s="7" t="s">
         <v>26</v>
       </c>
       <c r="E31" s="5"/>
-      <c r="F31" s="49"/>
+      <c r="F31" s="47"/>
       <c r="G31" s="36"/>
       <c r="H31" s="37"/>
       <c r="I31" s="38"/>
     </row>
     <row r="32" spans="3:9" x14ac:dyDescent="0.3">
-      <c r="C32" s="59"/>
+      <c r="C32" s="42"/>
       <c r="D32" s="7" t="s">
         <v>27</v>
       </c>
       <c r="E32" s="5"/>
-      <c r="F32" s="50"/>
+      <c r="F32" s="48"/>
       <c r="G32" s="36"/>
       <c r="H32" s="37"/>
       <c r="I32" s="38"/>
     </row>
     <row r="33" spans="3:9" ht="60.25" x14ac:dyDescent="0.3">
-      <c r="C33" s="56" t="s">
+      <c r="C33" s="39" t="s">
         <v>28</v>
       </c>
       <c r="D33" s="7" t="s">
         <v>125</v>
       </c>
-      <c r="E33" s="56" t="s">
+      <c r="E33" s="39" t="s">
         <v>122</v>
       </c>
       <c r="F33" s="22" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="G33" s="6"/>
       <c r="H33" s="27" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="I33" s="4"/>
     </row>
     <row r="34" spans="3:9" ht="30.15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C34" s="57"/>
+      <c r="C34" s="40"/>
       <c r="D34" s="7">
         <v>10</v>
       </c>
-      <c r="E34" s="57"/>
+      <c r="E34" s="40"/>
       <c r="F34" s="18" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="G34" s="21"/>
       <c r="H34" s="27" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="I34" s="4"/>
     </row>
     <row r="35" spans="3:9" ht="30.15" x14ac:dyDescent="0.3">
-      <c r="C35" s="57"/>
+      <c r="C35" s="40"/>
       <c r="D35" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="E35" s="57"/>
+      <c r="E35" s="40"/>
       <c r="F35" s="18" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="G35" s="21"/>
       <c r="H35" s="27" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="I35" s="4"/>
     </row>
     <row r="36" spans="3:9" ht="30.15" x14ac:dyDescent="0.3">
-      <c r="C36" s="57"/>
+      <c r="C36" s="40"/>
       <c r="D36" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="E36" s="57"/>
+      <c r="E36" s="40"/>
       <c r="F36" s="18" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="G36" s="21"/>
       <c r="H36" s="27" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="I36" s="4"/>
     </row>
     <row r="37" spans="3:9" x14ac:dyDescent="0.3">
-      <c r="C37" s="58"/>
+      <c r="C37" s="41"/>
       <c r="D37" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="E37" s="57"/>
+      <c r="E37" s="40"/>
       <c r="F37" s="18" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="G37" s="21"/>
       <c r="H37" s="27" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="I37" s="4"/>
     </row>
@@ -1905,13 +1907,13 @@
       <c r="D38" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="E38" s="58"/>
+      <c r="E38" s="41"/>
       <c r="F38" s="12" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="G38" s="6"/>
       <c r="H38" s="27" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="I38" s="4"/>
     </row>
@@ -1922,77 +1924,77 @@
       <c r="D39" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="E39" s="59" t="s">
+      <c r="E39" s="42" t="s">
         <v>123</v>
       </c>
       <c r="F39" s="12" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="G39" s="6"/>
       <c r="H39" s="27" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="I39" s="4"/>
     </row>
     <row r="40" spans="3:9" x14ac:dyDescent="0.3">
-      <c r="C40" s="59" t="s">
+      <c r="C40" s="42" t="s">
         <v>36</v>
       </c>
       <c r="D40" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="E40" s="59"/>
-      <c r="F40" s="51" t="s">
-        <v>156</v>
+      <c r="E40" s="42"/>
+      <c r="F40" s="49" t="s">
+        <v>155</v>
       </c>
       <c r="G40" s="6"/>
-      <c r="H40" s="39" t="s">
-        <v>212</v>
+      <c r="H40" s="54" t="s">
+        <v>211</v>
       </c>
       <c r="I40" s="4"/>
     </row>
     <row r="41" spans="3:9" x14ac:dyDescent="0.3">
-      <c r="C41" s="59"/>
+      <c r="C41" s="42"/>
       <c r="D41" s="7" t="s">
         <v>38</v>
       </c>
-      <c r="E41" s="59"/>
-      <c r="F41" s="52"/>
+      <c r="E41" s="42"/>
+      <c r="F41" s="50"/>
       <c r="G41" s="6"/>
-      <c r="H41" s="40"/>
+      <c r="H41" s="55"/>
       <c r="I41" s="4"/>
     </row>
     <row r="42" spans="3:9" x14ac:dyDescent="0.3">
-      <c r="C42" s="59"/>
+      <c r="C42" s="42"/>
       <c r="D42" s="7" t="s">
         <v>39</v>
       </c>
-      <c r="E42" s="59"/>
-      <c r="F42" s="52"/>
+      <c r="E42" s="42"/>
+      <c r="F42" s="50"/>
       <c r="G42" s="6"/>
-      <c r="H42" s="40"/>
+      <c r="H42" s="55"/>
       <c r="I42" s="4"/>
     </row>
     <row r="43" spans="3:9" x14ac:dyDescent="0.3">
-      <c r="C43" s="59"/>
+      <c r="C43" s="42"/>
       <c r="D43" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="E43" s="59"/>
-      <c r="F43" s="52"/>
+      <c r="E43" s="42"/>
+      <c r="F43" s="50"/>
       <c r="G43" s="6"/>
-      <c r="H43" s="40"/>
+      <c r="H43" s="55"/>
       <c r="I43" s="4"/>
     </row>
     <row r="44" spans="3:9" x14ac:dyDescent="0.3">
-      <c r="C44" s="59"/>
+      <c r="C44" s="42"/>
       <c r="D44" s="7" t="s">
         <v>41</v>
       </c>
-      <c r="E44" s="59"/>
-      <c r="F44" s="53"/>
+      <c r="E44" s="42"/>
+      <c r="F44" s="51"/>
       <c r="G44" s="6"/>
-      <c r="H44" s="41"/>
+      <c r="H44" s="56"/>
       <c r="I44" s="4"/>
     </row>
     <row r="45" spans="3:9" ht="60.25" x14ac:dyDescent="0.3">
@@ -2002,13 +2004,13 @@
       <c r="D45" s="7" t="s">
         <v>43</v>
       </c>
-      <c r="E45" s="59"/>
+      <c r="E45" s="42"/>
       <c r="F45" s="25" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="G45" s="6"/>
       <c r="H45" s="27" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="I45" s="4"/>
     </row>
@@ -2019,13 +2021,13 @@
       <c r="D46" s="7" t="s">
         <v>45</v>
       </c>
-      <c r="E46" s="59"/>
+      <c r="E46" s="42"/>
       <c r="F46" s="12" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="G46" s="6"/>
       <c r="H46" s="27" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="I46" s="4"/>
     </row>
@@ -2036,13 +2038,13 @@
       <c r="D47" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="E47" s="59"/>
+      <c r="E47" s="42"/>
       <c r="F47" s="12" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="G47" s="6"/>
       <c r="H47" s="27" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="I47" s="4"/>
     </row>
@@ -2053,13 +2055,13 @@
       <c r="D48" s="7" t="s">
         <v>49</v>
       </c>
-      <c r="E48" s="59"/>
+      <c r="E48" s="42"/>
       <c r="F48" s="12" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="G48" s="6"/>
       <c r="H48" s="27" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="I48" s="4"/>
     </row>
@@ -2071,187 +2073,187 @@
         <v>51</v>
       </c>
       <c r="E49" s="23" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="F49" s="12" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="G49" s="6"/>
       <c r="H49" s="27" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="I49" s="4"/>
     </row>
     <row r="50" spans="3:9" ht="45.2" x14ac:dyDescent="0.3">
-      <c r="C50" s="56" t="s">
+      <c r="C50" s="39" t="s">
         <v>52</v>
       </c>
       <c r="D50" s="7" t="s">
         <v>127</v>
       </c>
-      <c r="E50" s="56" t="s">
+      <c r="E50" s="39" t="s">
         <v>122</v>
       </c>
       <c r="F50" s="19" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="G50" s="6"/>
       <c r="H50" s="27" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="I50" s="4"/>
     </row>
     <row r="51" spans="3:9" ht="30.15" x14ac:dyDescent="0.3">
-      <c r="C51" s="58"/>
+      <c r="C51" s="41"/>
       <c r="D51" s="7" t="s">
         <v>53</v>
       </c>
-      <c r="E51" s="57"/>
+      <c r="E51" s="40"/>
       <c r="F51" s="19" t="s">
         <v>126</v>
       </c>
       <c r="G51" s="6"/>
       <c r="H51" s="27" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="I51" s="4"/>
     </row>
     <row r="52" spans="3:9" ht="60.25" x14ac:dyDescent="0.3">
-      <c r="C52" s="56" t="s">
-        <v>225</v>
+      <c r="C52" s="39" t="s">
+        <v>224</v>
       </c>
       <c r="D52" s="7" t="s">
         <v>125</v>
       </c>
-      <c r="E52" s="57"/>
+      <c r="E52" s="40"/>
       <c r="F52" s="19" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="G52" s="6"/>
       <c r="H52" s="27" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="I52" s="4"/>
     </row>
     <row r="53" spans="3:9" ht="60.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C53" s="57"/>
+      <c r="C53" s="40"/>
       <c r="D53" s="7" t="s">
         <v>54</v>
       </c>
-      <c r="E53" s="57"/>
+      <c r="E53" s="40"/>
       <c r="F53" s="24" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="G53" s="6"/>
       <c r="H53" s="27" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="I53" s="4"/>
     </row>
     <row r="54" spans="3:9" ht="120.45" x14ac:dyDescent="0.3">
-      <c r="C54" s="57"/>
+      <c r="C54" s="40"/>
       <c r="D54" s="7" t="s">
         <v>55</v>
       </c>
-      <c r="E54" s="57"/>
+      <c r="E54" s="40"/>
       <c r="F54" s="24" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="G54" s="6"/>
       <c r="H54" s="27" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="I54" s="4"/>
     </row>
     <row r="55" spans="3:9" ht="90.35" x14ac:dyDescent="0.3">
-      <c r="C55" s="57"/>
+      <c r="C55" s="40"/>
       <c r="D55" s="7" t="s">
         <v>56</v>
       </c>
-      <c r="E55" s="57"/>
+      <c r="E55" s="40"/>
       <c r="F55" s="24" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="G55" s="6"/>
       <c r="H55" s="27" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="I55" s="4"/>
     </row>
     <row r="56" spans="3:9" ht="45.2" x14ac:dyDescent="0.3">
-      <c r="C56" s="58"/>
+      <c r="C56" s="41"/>
       <c r="D56" s="7" t="s">
         <v>69</v>
       </c>
-      <c r="E56" s="57"/>
+      <c r="E56" s="40"/>
       <c r="F56" s="12" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="G56" s="6"/>
       <c r="H56" s="27" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="I56" s="4"/>
     </row>
     <row r="57" spans="3:9" ht="30.15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C57" s="59" t="s">
+      <c r="C57" s="42" t="s">
         <v>91</v>
       </c>
       <c r="D57" s="7" t="s">
         <v>57</v>
       </c>
-      <c r="E57" s="57"/>
+      <c r="E57" s="40"/>
       <c r="F57" s="9" t="s">
         <v>128</v>
       </c>
       <c r="G57" s="6"/>
       <c r="H57" s="27" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="I57" s="4"/>
     </row>
     <row r="58" spans="3:9" x14ac:dyDescent="0.3">
-      <c r="C58" s="59"/>
+      <c r="C58" s="42"/>
       <c r="D58" s="7" t="s">
         <v>58</v>
       </c>
-      <c r="E58" s="57"/>
+      <c r="E58" s="40"/>
       <c r="F58" s="9" t="s">
-        <v>129</v>
+        <v>225</v>
       </c>
       <c r="G58" s="6"/>
       <c r="H58" s="27" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="I58" s="4"/>
     </row>
     <row r="59" spans="3:9" ht="52.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C59" s="59"/>
+      <c r="C59" s="42"/>
       <c r="D59" s="7" t="s">
         <v>59</v>
       </c>
-      <c r="E59" s="57"/>
+      <c r="E59" s="40"/>
       <c r="F59" s="9" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="G59" s="6"/>
       <c r="H59" s="27" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="I59" s="4"/>
     </row>
     <row r="60" spans="3:9" x14ac:dyDescent="0.3">
-      <c r="C60" s="59"/>
+      <c r="C60" s="42"/>
       <c r="D60" s="7" t="s">
         <v>60</v>
       </c>
-      <c r="E60" s="58"/>
+      <c r="E60" s="41"/>
       <c r="F60" s="9" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="G60" s="6"/>
       <c r="H60" s="27" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="I60" s="4"/>
     </row>
@@ -2264,103 +2266,103 @@
       </c>
       <c r="E61" s="5"/>
       <c r="F61" s="10" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="G61" s="36"/>
       <c r="H61" s="37"/>
       <c r="I61" s="38"/>
     </row>
     <row r="62" spans="3:9" ht="30.15" x14ac:dyDescent="0.3">
-      <c r="C62" s="59" t="s">
+      <c r="C62" s="42" t="s">
         <v>64</v>
       </c>
       <c r="D62" s="7" t="s">
         <v>65</v>
       </c>
-      <c r="E62" s="56" t="s">
+      <c r="E62" s="39" t="s">
         <v>122</v>
       </c>
       <c r="F62" s="9" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="G62" s="6"/>
       <c r="H62" s="27" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="I62" s="4"/>
     </row>
     <row r="63" spans="3:9" ht="60.25" x14ac:dyDescent="0.3">
-      <c r="C63" s="59"/>
+      <c r="C63" s="42"/>
       <c r="D63" s="7" t="s">
         <v>66</v>
       </c>
-      <c r="E63" s="57"/>
+      <c r="E63" s="40"/>
       <c r="F63" s="9" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="G63" s="6"/>
       <c r="H63" s="27" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="I63" s="4"/>
     </row>
     <row r="64" spans="3:9" ht="30.15" x14ac:dyDescent="0.3">
-      <c r="C64" s="59"/>
+      <c r="C64" s="42"/>
       <c r="D64" s="7" t="s">
         <v>67</v>
       </c>
-      <c r="E64" s="57"/>
+      <c r="E64" s="40"/>
       <c r="F64" s="9" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="G64" s="6"/>
       <c r="H64" s="27" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="I64" s="4"/>
     </row>
     <row r="65" spans="3:9" ht="30.15" x14ac:dyDescent="0.3">
-      <c r="C65" s="59"/>
+      <c r="C65" s="42"/>
       <c r="D65" s="7" t="s">
         <v>68</v>
       </c>
-      <c r="E65" s="57"/>
+      <c r="E65" s="40"/>
       <c r="F65" s="9" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="G65" s="6"/>
       <c r="H65" s="27" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="I65" s="4"/>
     </row>
     <row r="66" spans="3:9" ht="60.25" x14ac:dyDescent="0.3">
-      <c r="C66" s="59"/>
+      <c r="C66" s="42"/>
       <c r="D66" s="7" t="s">
-        <v>133</v>
-      </c>
-      <c r="E66" s="57"/>
+        <v>132</v>
+      </c>
+      <c r="E66" s="40"/>
       <c r="F66" s="9" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="G66" s="6"/>
       <c r="H66" s="27" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="I66" s="4"/>
     </row>
     <row r="67" spans="3:9" ht="120.45" x14ac:dyDescent="0.3">
-      <c r="C67" s="59"/>
+      <c r="C67" s="42"/>
       <c r="D67" s="2" t="s">
-        <v>134</v>
-      </c>
-      <c r="E67" s="57"/>
+        <v>133</v>
+      </c>
+      <c r="E67" s="40"/>
       <c r="F67" s="9" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="G67" s="6"/>
       <c r="H67" s="27" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="I67" s="4"/>
     </row>
@@ -2371,570 +2373,570 @@
       <c r="D68" s="7" t="s">
         <v>71</v>
       </c>
-      <c r="E68" s="57"/>
+      <c r="E68" s="40"/>
       <c r="F68" s="25" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="G68" s="6"/>
       <c r="H68" s="27" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="I68" s="4"/>
     </row>
     <row r="69" spans="3:9" ht="30.15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C69" s="59" t="s">
+      <c r="C69" s="42" t="s">
         <v>72</v>
       </c>
       <c r="D69" s="7" t="s">
         <v>73</v>
       </c>
-      <c r="E69" s="57"/>
+      <c r="E69" s="40"/>
       <c r="F69" s="9" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="G69" s="6"/>
       <c r="H69" s="27" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="I69" s="4"/>
     </row>
     <row r="70" spans="3:9" ht="30.15" x14ac:dyDescent="0.3">
-      <c r="C70" s="59"/>
+      <c r="C70" s="42"/>
       <c r="D70" s="7" t="s">
         <v>74</v>
       </c>
-      <c r="E70" s="57"/>
+      <c r="E70" s="40"/>
       <c r="F70" s="9" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="G70" s="6"/>
       <c r="H70" s="27" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="I70" s="4"/>
     </row>
     <row r="71" spans="3:9" x14ac:dyDescent="0.3">
-      <c r="C71" s="59"/>
+      <c r="C71" s="42"/>
       <c r="D71" s="7" t="s">
         <v>75</v>
       </c>
-      <c r="E71" s="57"/>
+      <c r="E71" s="40"/>
       <c r="F71" s="9" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="G71" s="6"/>
       <c r="H71" s="27" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="I71" s="4"/>
     </row>
     <row r="72" spans="3:9" ht="30.15" x14ac:dyDescent="0.3">
-      <c r="C72" s="59"/>
+      <c r="C72" s="42"/>
       <c r="D72" s="7" t="s">
-        <v>220</v>
-      </c>
-      <c r="E72" s="57"/>
+        <v>219</v>
+      </c>
+      <c r="E72" s="40"/>
       <c r="F72" s="12" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="G72" s="6"/>
       <c r="H72" s="27" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="I72" s="4"/>
     </row>
     <row r="73" spans="3:9" x14ac:dyDescent="0.3">
-      <c r="C73" s="59"/>
+      <c r="C73" s="42"/>
       <c r="D73" s="7" t="s">
         <v>76</v>
       </c>
-      <c r="E73" s="57"/>
+      <c r="E73" s="40"/>
       <c r="F73" s="9" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="G73" s="6"/>
       <c r="H73" s="27" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="I73" s="4"/>
     </row>
     <row r="74" spans="3:9" x14ac:dyDescent="0.3">
-      <c r="C74" s="59"/>
+      <c r="C74" s="42"/>
       <c r="D74" s="7" t="s">
         <v>77</v>
       </c>
-      <c r="E74" s="57"/>
+      <c r="E74" s="40"/>
       <c r="F74" s="9" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="G74" s="6"/>
       <c r="H74" s="27" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="I74" s="4"/>
     </row>
     <row r="75" spans="3:9" x14ac:dyDescent="0.3">
-      <c r="C75" s="59"/>
+      <c r="C75" s="42"/>
       <c r="D75" s="7" t="s">
         <v>78</v>
       </c>
-      <c r="E75" s="57"/>
+      <c r="E75" s="40"/>
       <c r="F75" s="9" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="G75" s="6"/>
       <c r="H75" s="27" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="I75" s="4"/>
     </row>
     <row r="76" spans="3:9" x14ac:dyDescent="0.3">
-      <c r="C76" s="59"/>
+      <c r="C76" s="42"/>
       <c r="D76" s="7" t="s">
         <v>79</v>
       </c>
-      <c r="E76" s="57"/>
+      <c r="E76" s="40"/>
       <c r="F76" s="9" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="G76" s="6"/>
       <c r="H76" s="27" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="I76" s="4"/>
     </row>
     <row r="77" spans="3:9" ht="30.15" x14ac:dyDescent="0.3">
-      <c r="C77" s="59"/>
+      <c r="C77" s="42"/>
       <c r="D77" s="7" t="s">
         <v>80</v>
       </c>
-      <c r="E77" s="57"/>
+      <c r="E77" s="40"/>
       <c r="F77" s="12" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="G77" s="6"/>
       <c r="H77" s="27" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="I77" s="4"/>
     </row>
     <row r="78" spans="3:9" ht="30.15" x14ac:dyDescent="0.3">
-      <c r="C78" s="59"/>
+      <c r="C78" s="42"/>
       <c r="D78" s="7" t="s">
         <v>81</v>
       </c>
-      <c r="E78" s="57"/>
+      <c r="E78" s="40"/>
       <c r="F78" s="26" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="G78" s="33"/>
       <c r="H78" s="34"/>
       <c r="I78" s="35"/>
     </row>
     <row r="79" spans="3:9" ht="30.15" x14ac:dyDescent="0.3">
-      <c r="C79" s="57" t="s">
+      <c r="C79" s="40" t="s">
         <v>83</v>
       </c>
       <c r="D79" s="7" t="s">
-        <v>143</v>
-      </c>
-      <c r="E79" s="57"/>
+        <v>142</v>
+      </c>
+      <c r="E79" s="40"/>
       <c r="F79" s="9" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="G79" s="6"/>
       <c r="H79" s="27" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="I79" s="4"/>
     </row>
     <row r="80" spans="3:9" ht="30.15" x14ac:dyDescent="0.3">
-      <c r="C80" s="57"/>
+      <c r="C80" s="40"/>
       <c r="D80" s="7" t="s">
         <v>82</v>
       </c>
-      <c r="E80" s="57"/>
+      <c r="E80" s="40"/>
       <c r="F80" s="9" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="G80" s="6"/>
       <c r="H80" s="27" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="I80" s="4"/>
     </row>
     <row r="81" spans="3:9" ht="30.15" x14ac:dyDescent="0.3">
-      <c r="C81" s="56" t="s">
+      <c r="C81" s="39" t="s">
         <v>84</v>
       </c>
       <c r="D81" s="7" t="s">
-        <v>147</v>
-      </c>
-      <c r="E81" s="57"/>
+        <v>146</v>
+      </c>
+      <c r="E81" s="40"/>
       <c r="F81" s="9" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="G81" s="6"/>
       <c r="H81" s="27" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="I81" s="4"/>
     </row>
     <row r="82" spans="3:9" ht="69.400000000000006" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C82" s="57"/>
+      <c r="C82" s="40"/>
       <c r="D82" s="7" t="s">
-        <v>148</v>
-      </c>
-      <c r="E82" s="57"/>
+        <v>147</v>
+      </c>
+      <c r="E82" s="40"/>
       <c r="F82" s="9" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="G82" s="6"/>
       <c r="H82" s="27" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="I82" s="4"/>
     </row>
     <row r="83" spans="3:9" x14ac:dyDescent="0.3">
-      <c r="C83" s="57"/>
+      <c r="C83" s="40"/>
       <c r="D83" s="7" t="s">
         <v>85</v>
       </c>
-      <c r="E83" s="57"/>
+      <c r="E83" s="40"/>
       <c r="F83" s="26" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="G83" s="33"/>
       <c r="H83" s="34"/>
       <c r="I83" s="35"/>
     </row>
     <row r="84" spans="3:9" x14ac:dyDescent="0.3">
-      <c r="C84" s="57"/>
+      <c r="C84" s="40"/>
       <c r="D84" s="7" t="s">
         <v>86</v>
       </c>
-      <c r="E84" s="57"/>
+      <c r="E84" s="40"/>
       <c r="F84" s="9" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="G84" s="6"/>
       <c r="H84" s="27" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="I84" s="4"/>
     </row>
     <row r="85" spans="3:9" ht="30.15" x14ac:dyDescent="0.3">
-      <c r="C85" s="57"/>
+      <c r="C85" s="40"/>
       <c r="D85" s="7" t="s">
         <v>87</v>
       </c>
-      <c r="E85" s="57"/>
+      <c r="E85" s="40"/>
       <c r="F85" s="9" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="G85" s="6"/>
       <c r="H85" s="27" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="I85" s="4"/>
     </row>
     <row r="86" spans="3:9" ht="30.15" x14ac:dyDescent="0.3">
-      <c r="C86" s="57"/>
+      <c r="C86" s="40"/>
       <c r="D86" s="7" t="s">
         <v>88</v>
       </c>
-      <c r="E86" s="57"/>
+      <c r="E86" s="40"/>
       <c r="F86" s="9" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="G86" s="6"/>
       <c r="H86" s="27" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="I86" s="4"/>
     </row>
     <row r="87" spans="3:9" x14ac:dyDescent="0.3">
-      <c r="C87" s="57"/>
+      <c r="C87" s="40"/>
       <c r="D87" s="7" t="s">
         <v>89</v>
       </c>
-      <c r="E87" s="57"/>
+      <c r="E87" s="40"/>
       <c r="F87" s="9" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="G87" s="6"/>
       <c r="H87" s="27" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="I87" s="4"/>
     </row>
     <row r="88" spans="3:9" x14ac:dyDescent="0.3">
-      <c r="C88" s="57"/>
+      <c r="C88" s="40"/>
       <c r="D88" s="7" t="s">
         <v>90</v>
       </c>
-      <c r="E88" s="57"/>
+      <c r="E88" s="40"/>
       <c r="F88" s="9" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="G88" s="6"/>
       <c r="H88" s="27" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="I88" s="4"/>
     </row>
     <row r="89" spans="3:9" x14ac:dyDescent="0.3">
-      <c r="C89" s="57"/>
+      <c r="C89" s="40"/>
       <c r="D89" s="7" t="s">
         <v>97</v>
       </c>
-      <c r="E89" s="57"/>
+      <c r="E89" s="40"/>
       <c r="F89" s="26" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="G89" s="33"/>
       <c r="H89" s="34"/>
       <c r="I89" s="35"/>
     </row>
     <row r="90" spans="3:9" x14ac:dyDescent="0.3">
-      <c r="C90" s="57"/>
+      <c r="C90" s="40"/>
       <c r="D90" s="7" t="s">
         <v>98</v>
       </c>
-      <c r="E90" s="57"/>
+      <c r="E90" s="40"/>
       <c r="F90" s="9" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="G90" s="6"/>
       <c r="H90" s="27" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="I90" s="4"/>
     </row>
     <row r="91" spans="3:9" x14ac:dyDescent="0.3">
-      <c r="C91" s="57"/>
+      <c r="C91" s="40"/>
       <c r="D91" s="7" t="s">
         <v>99</v>
       </c>
-      <c r="E91" s="57"/>
+      <c r="E91" s="40"/>
       <c r="F91" s="9" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="G91" s="6"/>
       <c r="H91" s="27" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="I91" s="4"/>
     </row>
     <row r="92" spans="3:9" ht="30.15" x14ac:dyDescent="0.3">
-      <c r="C92" s="57"/>
+      <c r="C92" s="40"/>
       <c r="D92" s="7" t="s">
         <v>100</v>
       </c>
-      <c r="E92" s="57"/>
+      <c r="E92" s="40"/>
       <c r="F92" s="9" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="G92" s="6"/>
       <c r="H92" s="27" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="I92" s="4"/>
     </row>
     <row r="93" spans="3:9" ht="45.2" x14ac:dyDescent="0.3">
-      <c r="C93" s="57"/>
+      <c r="C93" s="40"/>
       <c r="D93" s="7" t="s">
-        <v>145</v>
-      </c>
-      <c r="E93" s="57"/>
+        <v>144</v>
+      </c>
+      <c r="E93" s="40"/>
       <c r="F93" s="9" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="G93" s="6"/>
       <c r="H93" s="27" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="I93" s="4"/>
     </row>
     <row r="94" spans="3:9" x14ac:dyDescent="0.3">
-      <c r="C94" s="56" t="s">
+      <c r="C94" s="39" t="s">
         <v>92</v>
       </c>
       <c r="D94" s="7" t="s">
         <v>93</v>
       </c>
-      <c r="E94" s="57"/>
+      <c r="E94" s="40"/>
       <c r="F94" s="9" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="G94" s="6"/>
       <c r="H94" s="27" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="I94" s="4"/>
     </row>
     <row r="95" spans="3:9" ht="30.15" x14ac:dyDescent="0.3">
-      <c r="C95" s="57"/>
+      <c r="C95" s="40"/>
       <c r="D95" s="7" t="s">
         <v>94</v>
       </c>
-      <c r="E95" s="57"/>
+      <c r="E95" s="40"/>
       <c r="F95" s="9" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="G95" s="6"/>
       <c r="H95" s="27" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="I95" s="4"/>
     </row>
     <row r="96" spans="3:9" x14ac:dyDescent="0.3">
-      <c r="C96" s="57"/>
+      <c r="C96" s="40"/>
       <c r="D96" s="7" t="s">
         <v>95</v>
       </c>
-      <c r="E96" s="57"/>
+      <c r="E96" s="40"/>
       <c r="F96" s="29" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="G96" s="30"/>
       <c r="H96" s="31"/>
       <c r="I96" s="32"/>
     </row>
     <row r="97" spans="3:9" x14ac:dyDescent="0.3">
-      <c r="C97" s="57"/>
+      <c r="C97" s="40"/>
       <c r="D97" s="7" t="s">
         <v>96</v>
       </c>
-      <c r="E97" s="57"/>
+      <c r="E97" s="40"/>
       <c r="F97" s="9" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="G97" s="6"/>
       <c r="H97" s="27" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="I97" s="4"/>
     </row>
     <row r="98" spans="3:9" x14ac:dyDescent="0.3">
-      <c r="C98" s="57"/>
+      <c r="C98" s="40"/>
       <c r="D98" s="7" t="s">
-        <v>144</v>
-      </c>
-      <c r="E98" s="57"/>
+        <v>143</v>
+      </c>
+      <c r="E98" s="40"/>
       <c r="F98" s="9" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="G98" s="6"/>
       <c r="H98" s="27" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="I98" s="4"/>
     </row>
     <row r="99" spans="3:9" ht="30.15" x14ac:dyDescent="0.3">
-      <c r="C99" s="58"/>
+      <c r="C99" s="41"/>
       <c r="D99" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="E99" s="57"/>
+      <c r="E99" s="40"/>
       <c r="F99" s="9" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="G99" s="6"/>
       <c r="H99" s="27" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="I99" s="4"/>
     </row>
     <row r="100" spans="3:9" x14ac:dyDescent="0.3">
-      <c r="C100" s="59" t="s">
+      <c r="C100" s="42" t="s">
         <v>107</v>
       </c>
       <c r="D100" s="7" t="s">
         <v>101</v>
       </c>
-      <c r="E100" s="57"/>
+      <c r="E100" s="40"/>
       <c r="F100" s="9" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="G100" s="6"/>
       <c r="H100" s="27" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="I100" s="4"/>
     </row>
     <row r="101" spans="3:9" ht="30.15" x14ac:dyDescent="0.3">
-      <c r="C101" s="59"/>
+      <c r="C101" s="42"/>
       <c r="D101" s="7" t="s">
         <v>102</v>
       </c>
-      <c r="E101" s="57"/>
+      <c r="E101" s="40"/>
       <c r="F101" s="9" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="G101" s="6"/>
       <c r="H101" s="27" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="I101" s="4"/>
     </row>
     <row r="102" spans="3:9" x14ac:dyDescent="0.3">
-      <c r="C102" s="59"/>
+      <c r="C102" s="42"/>
       <c r="D102" s="7" t="s">
         <v>103</v>
       </c>
-      <c r="E102" s="57"/>
+      <c r="E102" s="40"/>
       <c r="F102" s="9" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="G102" s="6"/>
       <c r="H102" s="27" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="I102" s="4"/>
     </row>
     <row r="103" spans="3:9" ht="30.15" x14ac:dyDescent="0.3">
-      <c r="C103" s="59"/>
+      <c r="C103" s="42"/>
       <c r="D103" s="7" t="s">
         <v>104</v>
       </c>
-      <c r="E103" s="57"/>
+      <c r="E103" s="40"/>
       <c r="F103" s="9" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="G103" s="6"/>
       <c r="H103" s="27" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="I103" s="4"/>
     </row>
     <row r="104" spans="3:9" x14ac:dyDescent="0.3">
-      <c r="C104" s="59"/>
+      <c r="C104" s="42"/>
       <c r="D104" s="7" t="s">
         <v>105</v>
       </c>
-      <c r="E104" s="57"/>
+      <c r="E104" s="40"/>
       <c r="F104" s="9" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="G104" s="6"/>
       <c r="H104" s="27" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="I104" s="4"/>
     </row>
     <row r="105" spans="3:9" ht="30.15" x14ac:dyDescent="0.3">
-      <c r="C105" s="59"/>
+      <c r="C105" s="42"/>
       <c r="D105" s="8" t="s">
         <v>106</v>
       </c>
-      <c r="E105" s="58"/>
+      <c r="E105" s="41"/>
       <c r="F105" s="9" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="G105" s="6"/>
       <c r="H105" s="27" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="I105" s="4"/>
     </row>
@@ -2949,30 +2951,6 @@
     </row>
   </sheetData>
   <mergeCells count="34">
-    <mergeCell ref="E50:E60"/>
-    <mergeCell ref="E62:E105"/>
-    <mergeCell ref="C69:C78"/>
-    <mergeCell ref="C79:C80"/>
-    <mergeCell ref="C81:C93"/>
-    <mergeCell ref="C94:C99"/>
-    <mergeCell ref="C100:C105"/>
-    <mergeCell ref="C62:C67"/>
-    <mergeCell ref="C57:C60"/>
-    <mergeCell ref="C33:C37"/>
-    <mergeCell ref="C50:C51"/>
-    <mergeCell ref="C52:C56"/>
-    <mergeCell ref="C5:C8"/>
-    <mergeCell ref="C9:C15"/>
-    <mergeCell ref="C16:C17"/>
-    <mergeCell ref="C24:C27"/>
-    <mergeCell ref="C28:C29"/>
-    <mergeCell ref="C18:C22"/>
-    <mergeCell ref="E3:E27"/>
-    <mergeCell ref="E33:E38"/>
-    <mergeCell ref="E39:E48"/>
-    <mergeCell ref="F18:F22"/>
-    <mergeCell ref="C30:C32"/>
-    <mergeCell ref="C40:C44"/>
     <mergeCell ref="I6:I7"/>
     <mergeCell ref="I18:I22"/>
     <mergeCell ref="F28:F32"/>
@@ -2983,6 +2961,30 @@
     <mergeCell ref="H18:H22"/>
     <mergeCell ref="G18:G22"/>
     <mergeCell ref="G6:G7"/>
+    <mergeCell ref="E3:E27"/>
+    <mergeCell ref="E33:E38"/>
+    <mergeCell ref="E39:E48"/>
+    <mergeCell ref="F18:F22"/>
+    <mergeCell ref="C30:C32"/>
+    <mergeCell ref="C40:C44"/>
+    <mergeCell ref="C33:C37"/>
+    <mergeCell ref="C50:C51"/>
+    <mergeCell ref="C52:C56"/>
+    <mergeCell ref="C5:C8"/>
+    <mergeCell ref="C9:C15"/>
+    <mergeCell ref="C16:C17"/>
+    <mergeCell ref="C24:C27"/>
+    <mergeCell ref="C28:C29"/>
+    <mergeCell ref="C18:C22"/>
+    <mergeCell ref="E50:E60"/>
+    <mergeCell ref="E62:E105"/>
+    <mergeCell ref="C69:C78"/>
+    <mergeCell ref="C79:C80"/>
+    <mergeCell ref="C81:C93"/>
+    <mergeCell ref="C94:C99"/>
+    <mergeCell ref="C100:C105"/>
+    <mergeCell ref="C62:C67"/>
+    <mergeCell ref="C57:C60"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
more mutates almost finishing edit
</commit_message>
<xml_diff>
--- a/edit_eam/crosscheck.xlsx
+++ b/edit_eam/crosscheck.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="318" uniqueCount="226">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="377" uniqueCount="283">
   <si>
     <t>Nombre</t>
   </si>
@@ -692,6 +692,177 @@
   </si>
   <si>
     <t>IV4R11C3/Total</t>
+  </si>
+  <si>
+    <t>innProceso</t>
+  </si>
+  <si>
+    <t>innProducto</t>
+  </si>
+  <si>
+    <t>innOrganizacional</t>
+  </si>
+  <si>
+    <t>mejoraBS</t>
+  </si>
+  <si>
+    <t>aumentaBS</t>
+  </si>
+  <si>
+    <t>mantienePosicion</t>
+  </si>
+  <si>
+    <t>aumentaProductividad</t>
+  </si>
+  <si>
+    <t>reduceCostoFactores</t>
+  </si>
+  <si>
+    <t>reduceCostoLogistico</t>
+  </si>
+  <si>
+    <t>reduceCostoOtros</t>
+  </si>
+  <si>
+    <t>innRadical</t>
+  </si>
+  <si>
+    <t>innIncremental</t>
+  </si>
+  <si>
+    <t>innovadorAmplio</t>
+  </si>
+  <si>
+    <t>noInnovadora</t>
+  </si>
+  <si>
+    <t>innovadorEstricto</t>
+  </si>
+  <si>
+    <t>innovadorPotencial</t>
+  </si>
+  <si>
+    <t>otroTipo</t>
+  </si>
+  <si>
+    <t>usaTICs</t>
+  </si>
+  <si>
+    <t>networkNoEmpresa</t>
+  </si>
+  <si>
+    <t>networkEmpresas</t>
+  </si>
+  <si>
+    <t>modificaOtros</t>
+  </si>
+  <si>
+    <t>sinNetwork</t>
+  </si>
+  <si>
+    <t>catOcupados2017, catOcupados2018</t>
+  </si>
+  <si>
+    <t>totOcupados2017, totOcupados2018</t>
+  </si>
+  <si>
+    <t>ciiu4Digitos</t>
+  </si>
+  <si>
+    <t>ocupadosACTI2017, ocupadosACTI2018</t>
+  </si>
+  <si>
+    <t>ratioActi2017, ratioActi2018</t>
+  </si>
+  <si>
+    <t>educadosColegio2017, educadosColegio2018</t>
+  </si>
+  <si>
+    <t>educadosSuperior2017, educadosSuperior2018</t>
+  </si>
+  <si>
+    <t>educadosPosgrado2017, educadosPosgrado2018</t>
+  </si>
+  <si>
+    <t>educadosOtro2017, educadosOtro2018</t>
+  </si>
+  <si>
+    <t>ocupadosProduccion, ratioProduccion</t>
+  </si>
+  <si>
+    <t>ocupadosID, ratioID</t>
+  </si>
+  <si>
+    <t>ocupadosAdmin, ratioAdmin</t>
+  </si>
+  <si>
+    <t>ocupadosMarketing, ratioMarketing</t>
+  </si>
+  <si>
+    <t>recursosPropio2017, recursosPropio2018</t>
+  </si>
+  <si>
+    <t>recursosBanca2017, recursosBanca2018</t>
+  </si>
+  <si>
+    <t>recursosConglomerado2017, recursosConglomerado2018</t>
+  </si>
+  <si>
+    <t>recursosPublicos2017,  recursosPublicos2018</t>
+  </si>
+  <si>
+    <t>recursosOtros2017, recursosOtros2018</t>
+  </si>
+  <si>
+    <t xml:space="preserve">recursosEmpresas2017, recursosEmpresas2018 </t>
+  </si>
+  <si>
+    <t>contratoEstado</t>
+  </si>
+  <si>
+    <t>sniSENA</t>
+  </si>
+  <si>
+    <t>sniCamaraComercio</t>
+  </si>
+  <si>
+    <t>sniICONTEC</t>
+  </si>
+  <si>
+    <t>sniUnivSNCTI</t>
+  </si>
+  <si>
+    <t>sniSIC</t>
+  </si>
+  <si>
+    <t>sniMinciencias</t>
+  </si>
+  <si>
+    <t>sniConsultores</t>
+  </si>
+  <si>
+    <t>sniProcolombia</t>
+  </si>
+  <si>
+    <t>sniINNPulsa</t>
+  </si>
+  <si>
+    <t>ascensosGerenciales</t>
+  </si>
+  <si>
+    <t>ascensosNoGerenciales</t>
+  </si>
+  <si>
+    <t>bonosNoGerenciales</t>
+  </si>
+  <si>
+    <t>bonosGerenciales</t>
+  </si>
+  <si>
+    <t>metasProduccion</t>
+  </si>
+  <si>
+    <t>indicadoresDesemp</t>
   </si>
 </sst>
 </file>
@@ -875,7 +1046,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="60">
+  <cellXfs count="59">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -935,9 +1106,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -984,18 +1152,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
@@ -1044,6 +1200,18 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1352,8 +1520,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="C2:I108"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B55" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C62" sqref="C62:C67"/>
+    <sheetView tabSelected="1" topLeftCell="C91" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G106" sqref="G106"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="15.05" x14ac:dyDescent="0.3"/>
@@ -1362,8 +1530,8 @@
     <col min="4" max="4" width="20.77734375" style="2" customWidth="1"/>
     <col min="5" max="5" width="14" style="13" customWidth="1"/>
     <col min="6" max="6" width="15.21875" style="1" customWidth="1"/>
-    <col min="7" max="7" width="15.33203125" style="1" customWidth="1"/>
-    <col min="8" max="8" width="8.88671875" style="28"/>
+    <col min="7" max="7" width="19.88671875" style="1" customWidth="1"/>
+    <col min="8" max="8" width="8.88671875" style="27"/>
   </cols>
   <sheetData>
     <row r="2" spans="3:9" ht="26.2" customHeight="1" x14ac:dyDescent="0.3">
@@ -1396,14 +1564,16 @@
       <c r="D3" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="E3" s="39" t="s">
+      <c r="E3" s="55" t="s">
         <v>122</v>
       </c>
       <c r="F3" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="G3" s="6"/>
-      <c r="H3" s="27" t="s">
+      <c r="G3" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="H3" s="26" t="s">
         <v>211</v>
       </c>
       <c r="I3" s="4"/>
@@ -1415,271 +1585,305 @@
       <c r="D4" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="E4" s="40"/>
+      <c r="E4" s="56"/>
       <c r="F4" s="12" t="s">
         <v>108</v>
       </c>
       <c r="G4" s="6"/>
-      <c r="H4" s="27"/>
+      <c r="H4" s="26"/>
       <c r="I4" s="4"/>
     </row>
     <row r="5" spans="3:9" x14ac:dyDescent="0.3">
-      <c r="C5" s="42" t="s">
+      <c r="C5" s="58" t="s">
         <v>7</v>
       </c>
       <c r="D5" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="E5" s="40"/>
+      <c r="E5" s="56"/>
       <c r="F5" s="9" t="s">
         <v>109</v>
       </c>
-      <c r="G5" s="6"/>
-      <c r="H5" s="27" t="s">
+      <c r="G5" s="6" t="s">
+        <v>226</v>
+      </c>
+      <c r="H5" s="26" t="s">
         <v>211</v>
       </c>
       <c r="I5" s="4"/>
     </row>
     <row r="6" spans="3:9" x14ac:dyDescent="0.3">
-      <c r="C6" s="42"/>
+      <c r="C6" s="58"/>
       <c r="D6" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="E6" s="40"/>
-      <c r="F6" s="52" t="s">
+      <c r="E6" s="56"/>
+      <c r="F6" s="47" t="s">
         <v>111</v>
       </c>
-      <c r="G6" s="57"/>
-      <c r="H6" s="54" t="s">
-        <v>211</v>
-      </c>
-      <c r="I6" s="43"/>
+      <c r="G6" s="52" t="s">
+        <v>227</v>
+      </c>
+      <c r="H6" s="49" t="s">
+        <v>211</v>
+      </c>
+      <c r="I6" s="38"/>
     </row>
     <row r="7" spans="3:9" x14ac:dyDescent="0.3">
-      <c r="C7" s="42"/>
+      <c r="C7" s="58"/>
       <c r="D7" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="E7" s="40"/>
-      <c r="F7" s="53"/>
-      <c r="G7" s="59"/>
-      <c r="H7" s="56"/>
-      <c r="I7" s="44"/>
+      <c r="E7" s="56"/>
+      <c r="F7" s="48"/>
+      <c r="G7" s="54"/>
+      <c r="H7" s="51"/>
+      <c r="I7" s="39"/>
     </row>
     <row r="8" spans="3:9" x14ac:dyDescent="0.3">
-      <c r="C8" s="42"/>
+      <c r="C8" s="58"/>
       <c r="D8" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="E8" s="40"/>
+      <c r="E8" s="56"/>
       <c r="F8" s="11" t="s">
         <v>110</v>
       </c>
-      <c r="G8" s="6"/>
-      <c r="H8" s="27" t="s">
+      <c r="G8" s="6" t="s">
+        <v>228</v>
+      </c>
+      <c r="H8" s="26" t="s">
         <v>211</v>
       </c>
       <c r="I8" s="4"/>
     </row>
     <row r="9" spans="3:9" x14ac:dyDescent="0.3">
-      <c r="C9" s="42" t="s">
+      <c r="C9" s="58" t="s">
         <v>13</v>
       </c>
       <c r="D9" s="7" t="s">
         <v>157</v>
       </c>
-      <c r="E9" s="40"/>
-      <c r="F9" s="24" t="s">
+      <c r="E9" s="56"/>
+      <c r="F9" s="23" t="s">
         <v>182</v>
       </c>
-      <c r="G9" s="6"/>
-      <c r="H9" s="27" t="s">
+      <c r="G9" s="6" t="s">
+        <v>229</v>
+      </c>
+      <c r="H9" s="26" t="s">
         <v>211</v>
       </c>
       <c r="I9" s="4"/>
     </row>
     <row r="10" spans="3:9" x14ac:dyDescent="0.3">
-      <c r="C10" s="42"/>
+      <c r="C10" s="58"/>
       <c r="D10" s="7" t="s">
         <v>158</v>
       </c>
-      <c r="E10" s="40"/>
-      <c r="F10" s="24" t="s">
+      <c r="E10" s="56"/>
+      <c r="F10" s="23" t="s">
         <v>183</v>
       </c>
-      <c r="G10" s="6"/>
-      <c r="H10" s="27" t="s">
+      <c r="G10" s="6" t="s">
+        <v>230</v>
+      </c>
+      <c r="H10" s="26" t="s">
         <v>211</v>
       </c>
       <c r="I10" s="4"/>
     </row>
     <row r="11" spans="3:9" ht="34.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C11" s="42"/>
+      <c r="C11" s="58"/>
       <c r="D11" s="7" t="s">
         <v>159</v>
       </c>
-      <c r="E11" s="40"/>
-      <c r="F11" s="24" t="s">
+      <c r="E11" s="56"/>
+      <c r="F11" s="23" t="s">
         <v>184</v>
       </c>
-      <c r="G11" s="6"/>
-      <c r="H11" s="27" t="s">
+      <c r="G11" s="6" t="s">
+        <v>231</v>
+      </c>
+      <c r="H11" s="26" t="s">
         <v>211</v>
       </c>
       <c r="I11" s="4"/>
     </row>
     <row r="12" spans="3:9" ht="34.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C12" s="42"/>
+      <c r="C12" s="58"/>
       <c r="D12" s="7" t="s">
         <v>160</v>
       </c>
-      <c r="E12" s="40"/>
-      <c r="F12" s="24" t="s">
+      <c r="E12" s="56"/>
+      <c r="F12" s="23" t="s">
         <v>185</v>
       </c>
-      <c r="G12" s="6"/>
-      <c r="H12" s="27" t="s">
+      <c r="G12" s="6" t="s">
+        <v>232</v>
+      </c>
+      <c r="H12" s="26" t="s">
         <v>211</v>
       </c>
       <c r="I12" s="4"/>
     </row>
     <row r="13" spans="3:9" ht="65.45" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C13" s="42"/>
+      <c r="C13" s="58"/>
       <c r="D13" s="7" t="s">
         <v>161</v>
       </c>
-      <c r="E13" s="40"/>
-      <c r="F13" s="24" t="s">
+      <c r="E13" s="56"/>
+      <c r="F13" s="23" t="s">
         <v>186</v>
       </c>
-      <c r="G13" s="6"/>
-      <c r="H13" s="27" t="s">
+      <c r="G13" s="6" t="s">
+        <v>233</v>
+      </c>
+      <c r="H13" s="26" t="s">
         <v>211</v>
       </c>
       <c r="I13" s="4"/>
     </row>
     <row r="14" spans="3:9" ht="46.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C14" s="42"/>
+      <c r="C14" s="58"/>
       <c r="D14" s="7" t="s">
         <v>162</v>
       </c>
-      <c r="E14" s="40"/>
-      <c r="F14" s="24" t="s">
+      <c r="E14" s="56"/>
+      <c r="F14" s="23" t="s">
         <v>187</v>
       </c>
-      <c r="G14" s="6"/>
-      <c r="H14" s="27" t="s">
+      <c r="G14" s="6" t="s">
+        <v>234</v>
+      </c>
+      <c r="H14" s="26" t="s">
         <v>211</v>
       </c>
       <c r="I14" s="4"/>
     </row>
     <row r="15" spans="3:9" ht="66.150000000000006" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C15" s="42"/>
+      <c r="C15" s="58"/>
       <c r="D15" s="7" t="s">
         <v>163</v>
       </c>
-      <c r="E15" s="40"/>
-      <c r="F15" s="24" t="s">
+      <c r="E15" s="56"/>
+      <c r="F15" s="23" t="s">
         <v>188</v>
       </c>
-      <c r="G15" s="6"/>
-      <c r="H15" s="27" t="s">
+      <c r="G15" s="6" t="s">
+        <v>235</v>
+      </c>
+      <c r="H15" s="26" t="s">
         <v>211</v>
       </c>
       <c r="I15" s="4"/>
     </row>
     <row r="16" spans="3:9" x14ac:dyDescent="0.3">
-      <c r="C16" s="42" t="s">
+      <c r="C16" s="58" t="s">
         <v>14</v>
       </c>
       <c r="D16" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="E16" s="40"/>
+      <c r="E16" s="56"/>
       <c r="F16" s="9" t="s">
         <v>112</v>
       </c>
-      <c r="G16" s="6"/>
-      <c r="H16" s="27" t="s">
+      <c r="G16" s="6" t="s">
+        <v>236</v>
+      </c>
+      <c r="H16" s="26" t="s">
         <v>211</v>
       </c>
       <c r="I16" s="4"/>
     </row>
     <row r="17" spans="3:9" x14ac:dyDescent="0.3">
-      <c r="C17" s="42"/>
+      <c r="C17" s="58"/>
       <c r="D17" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="E17" s="40"/>
+      <c r="E17" s="56"/>
       <c r="F17" s="9" t="s">
         <v>113</v>
       </c>
-      <c r="G17" s="6"/>
-      <c r="H17" s="27" t="s">
+      <c r="G17" s="6" t="s">
+        <v>237</v>
+      </c>
+      <c r="H17" s="26" t="s">
         <v>211</v>
       </c>
       <c r="I17" s="4"/>
     </row>
     <row r="18" spans="3:9" ht="15.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C18" s="39" t="s">
+      <c r="C18" s="55" t="s">
         <v>114</v>
       </c>
       <c r="D18" s="7" t="s">
         <v>115</v>
       </c>
-      <c r="E18" s="40"/>
-      <c r="F18" s="39" t="s">
+      <c r="E18" s="56"/>
+      <c r="F18" s="55" t="s">
         <v>202</v>
       </c>
-      <c r="G18" s="57"/>
-      <c r="H18" s="54" t="s">
-        <v>211</v>
-      </c>
-      <c r="I18" s="43"/>
+      <c r="G18" s="6" t="s">
+        <v>240</v>
+      </c>
+      <c r="H18" s="49" t="s">
+        <v>211</v>
+      </c>
+      <c r="I18" s="38"/>
     </row>
     <row r="19" spans="3:9" x14ac:dyDescent="0.3">
-      <c r="C19" s="40"/>
+      <c r="C19" s="56"/>
       <c r="D19" s="7" t="s">
         <v>116</v>
       </c>
-      <c r="E19" s="40"/>
-      <c r="F19" s="40"/>
-      <c r="G19" s="58"/>
-      <c r="H19" s="55"/>
-      <c r="I19" s="45"/>
+      <c r="E19" s="56"/>
+      <c r="F19" s="56"/>
+      <c r="G19" s="6" t="s">
+        <v>238</v>
+      </c>
+      <c r="H19" s="50"/>
+      <c r="I19" s="40"/>
     </row>
     <row r="20" spans="3:9" x14ac:dyDescent="0.3">
-      <c r="C20" s="40"/>
+      <c r="C20" s="56"/>
       <c r="D20" s="7" t="s">
         <v>117</v>
       </c>
-      <c r="E20" s="40"/>
-      <c r="F20" s="40"/>
-      <c r="G20" s="58"/>
-      <c r="H20" s="55"/>
-      <c r="I20" s="45"/>
+      <c r="E20" s="56"/>
+      <c r="F20" s="56"/>
+      <c r="G20" s="6" t="s">
+        <v>241</v>
+      </c>
+      <c r="H20" s="50"/>
+      <c r="I20" s="40"/>
     </row>
     <row r="21" spans="3:9" x14ac:dyDescent="0.3">
-      <c r="C21" s="40"/>
+      <c r="C21" s="56"/>
       <c r="D21" s="7" t="s">
         <v>118</v>
       </c>
-      <c r="E21" s="40"/>
-      <c r="F21" s="40"/>
-      <c r="G21" s="58"/>
-      <c r="H21" s="55"/>
-      <c r="I21" s="45"/>
+      <c r="E21" s="56"/>
+      <c r="F21" s="56"/>
+      <c r="G21" s="6" t="s">
+        <v>239</v>
+      </c>
+      <c r="H21" s="50"/>
+      <c r="I21" s="40"/>
     </row>
     <row r="22" spans="3:9" x14ac:dyDescent="0.3">
-      <c r="C22" s="41"/>
+      <c r="C22" s="57"/>
       <c r="D22" s="7" t="s">
         <v>203</v>
       </c>
-      <c r="E22" s="40"/>
-      <c r="F22" s="41"/>
-      <c r="G22" s="59"/>
-      <c r="H22" s="56"/>
-      <c r="I22" s="44"/>
+      <c r="E22" s="56"/>
+      <c r="F22" s="57"/>
+      <c r="G22" s="6" t="s">
+        <v>242</v>
+      </c>
+      <c r="H22" s="51"/>
+      <c r="I22" s="39"/>
     </row>
     <row r="23" spans="3:9" ht="30.15" x14ac:dyDescent="0.3">
       <c r="C23" s="3" t="s">
@@ -1688,214 +1892,228 @@
       <c r="D23" s="7" t="s">
         <v>62</v>
       </c>
-      <c r="E23" s="40"/>
+      <c r="E23" s="56"/>
       <c r="F23" s="9" t="s">
         <v>119</v>
       </c>
-      <c r="G23" s="6"/>
-      <c r="H23" s="27" t="s">
+      <c r="G23" s="6" t="s">
+        <v>243</v>
+      </c>
+      <c r="H23" s="26" t="s">
         <v>211</v>
       </c>
       <c r="I23" s="4"/>
     </row>
     <row r="24" spans="3:9" x14ac:dyDescent="0.3">
-      <c r="C24" s="42" t="s">
+      <c r="C24" s="58" t="s">
         <v>120</v>
       </c>
       <c r="D24" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="E24" s="40"/>
+      <c r="E24" s="56"/>
       <c r="F24" s="12" t="s">
         <v>221</v>
       </c>
-      <c r="G24" s="6"/>
-      <c r="H24" s="27" t="s">
+      <c r="G24" s="6" t="s">
+        <v>247</v>
+      </c>
+      <c r="H24" s="26" t="s">
         <v>211</v>
       </c>
       <c r="I24" s="4"/>
     </row>
     <row r="25" spans="3:9" ht="135.5" x14ac:dyDescent="0.3">
-      <c r="C25" s="42"/>
+      <c r="C25" s="58"/>
       <c r="D25" s="7" t="s">
         <v>222</v>
       </c>
-      <c r="E25" s="40"/>
+      <c r="E25" s="56"/>
       <c r="F25" s="12" t="s">
         <v>220</v>
       </c>
-      <c r="G25" s="6"/>
-      <c r="H25" s="27" t="s">
+      <c r="G25" s="6" t="s">
+        <v>244</v>
+      </c>
+      <c r="H25" s="26" t="s">
         <v>211</v>
       </c>
       <c r="I25" s="4"/>
     </row>
     <row r="26" spans="3:9" ht="45.2" x14ac:dyDescent="0.3">
-      <c r="C26" s="42"/>
+      <c r="C26" s="58"/>
       <c r="D26" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="E26" s="40"/>
+      <c r="E26" s="56"/>
       <c r="F26" s="12" t="s">
         <v>218</v>
       </c>
-      <c r="G26" s="6"/>
-      <c r="H26" s="27" t="s">
+      <c r="G26" s="6" t="s">
+        <v>245</v>
+      </c>
+      <c r="H26" s="26" t="s">
         <v>211</v>
       </c>
       <c r="I26" s="4"/>
     </row>
     <row r="27" spans="3:9" ht="45.2" x14ac:dyDescent="0.3">
-      <c r="C27" s="42"/>
+      <c r="C27" s="58"/>
       <c r="D27" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="E27" s="41"/>
+      <c r="E27" s="57"/>
       <c r="F27" s="12" t="s">
         <v>217</v>
       </c>
-      <c r="G27" s="6"/>
-      <c r="H27" s="27" t="s">
+      <c r="G27" s="6" t="s">
+        <v>246</v>
+      </c>
+      <c r="H27" s="26" t="s">
         <v>211</v>
       </c>
       <c r="I27" s="4"/>
     </row>
     <row r="28" spans="3:9" x14ac:dyDescent="0.3">
-      <c r="C28" s="42" t="s">
+      <c r="C28" s="58" t="s">
         <v>23</v>
       </c>
       <c r="D28" s="7" t="s">
         <v>21</v>
       </c>
       <c r="E28" s="5"/>
-      <c r="F28" s="46" t="s">
+      <c r="F28" s="41" t="s">
         <v>216</v>
       </c>
-      <c r="G28" s="36"/>
-      <c r="H28" s="37"/>
-      <c r="I28" s="38"/>
+      <c r="G28" s="35"/>
+      <c r="H28" s="36"/>
+      <c r="I28" s="37"/>
     </row>
     <row r="29" spans="3:9" x14ac:dyDescent="0.3">
-      <c r="C29" s="42"/>
+      <c r="C29" s="58"/>
       <c r="D29" s="7" t="s">
         <v>22</v>
       </c>
       <c r="E29" s="5"/>
-      <c r="F29" s="47"/>
-      <c r="G29" s="36"/>
-      <c r="H29" s="37"/>
-      <c r="I29" s="38"/>
+      <c r="F29" s="42"/>
+      <c r="G29" s="35"/>
+      <c r="H29" s="36"/>
+      <c r="I29" s="37"/>
     </row>
     <row r="30" spans="3:9" x14ac:dyDescent="0.3">
-      <c r="C30" s="42" t="s">
+      <c r="C30" s="58" t="s">
         <v>24</v>
       </c>
       <c r="D30" s="7" t="s">
         <v>25</v>
       </c>
       <c r="E30" s="5"/>
-      <c r="F30" s="47"/>
-      <c r="G30" s="36"/>
-      <c r="H30" s="37"/>
-      <c r="I30" s="38"/>
+      <c r="F30" s="42"/>
+      <c r="G30" s="35"/>
+      <c r="H30" s="36"/>
+      <c r="I30" s="37"/>
     </row>
     <row r="31" spans="3:9" x14ac:dyDescent="0.3">
-      <c r="C31" s="42"/>
+      <c r="C31" s="58"/>
       <c r="D31" s="7" t="s">
         <v>26</v>
       </c>
       <c r="E31" s="5"/>
-      <c r="F31" s="47"/>
-      <c r="G31" s="36"/>
-      <c r="H31" s="37"/>
-      <c r="I31" s="38"/>
+      <c r="F31" s="42"/>
+      <c r="G31" s="35"/>
+      <c r="H31" s="36"/>
+      <c r="I31" s="37"/>
     </row>
     <row r="32" spans="3:9" x14ac:dyDescent="0.3">
-      <c r="C32" s="42"/>
+      <c r="C32" s="58"/>
       <c r="D32" s="7" t="s">
         <v>27</v>
       </c>
       <c r="E32" s="5"/>
-      <c r="F32" s="48"/>
-      <c r="G32" s="36"/>
-      <c r="H32" s="37"/>
-      <c r="I32" s="38"/>
+      <c r="F32" s="43"/>
+      <c r="G32" s="35"/>
+      <c r="H32" s="36"/>
+      <c r="I32" s="37"/>
     </row>
     <row r="33" spans="3:9" ht="60.25" x14ac:dyDescent="0.3">
-      <c r="C33" s="39" t="s">
+      <c r="C33" s="55" t="s">
         <v>28</v>
       </c>
       <c r="D33" s="7" t="s">
         <v>125</v>
       </c>
-      <c r="E33" s="39" t="s">
+      <c r="E33" s="55" t="s">
         <v>122</v>
       </c>
-      <c r="F33" s="22" t="s">
+      <c r="F33" s="21" t="s">
         <v>190</v>
       </c>
-      <c r="G33" s="6"/>
-      <c r="H33" s="27" t="s">
+      <c r="G33" s="6" t="s">
+        <v>249</v>
+      </c>
+      <c r="H33" s="26" t="s">
         <v>211</v>
       </c>
       <c r="I33" s="4"/>
     </row>
     <row r="34" spans="3:9" ht="30.15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C34" s="40"/>
+      <c r="C34" s="56"/>
       <c r="D34" s="7">
         <v>10</v>
       </c>
-      <c r="E34" s="40"/>
+      <c r="E34" s="56"/>
       <c r="F34" s="18" t="s">
         <v>191</v>
       </c>
-      <c r="G34" s="21"/>
-      <c r="H34" s="27" t="s">
+      <c r="G34" s="52" t="s">
+        <v>248</v>
+      </c>
+      <c r="H34" s="26" t="s">
         <v>211</v>
       </c>
       <c r="I34" s="4"/>
     </row>
     <row r="35" spans="3:9" ht="30.15" x14ac:dyDescent="0.3">
-      <c r="C35" s="40"/>
+      <c r="C35" s="56"/>
       <c r="D35" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="E35" s="40"/>
+      <c r="E35" s="56"/>
       <c r="F35" s="18" t="s">
         <v>192</v>
       </c>
-      <c r="G35" s="21"/>
-      <c r="H35" s="27" t="s">
+      <c r="G35" s="53"/>
+      <c r="H35" s="26" t="s">
         <v>211</v>
       </c>
       <c r="I35" s="4"/>
     </row>
     <row r="36" spans="3:9" ht="30.15" x14ac:dyDescent="0.3">
-      <c r="C36" s="40"/>
+      <c r="C36" s="56"/>
       <c r="D36" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="E36" s="40"/>
+      <c r="E36" s="56"/>
       <c r="F36" s="18" t="s">
         <v>193</v>
       </c>
-      <c r="G36" s="21"/>
-      <c r="H36" s="27" t="s">
+      <c r="G36" s="53"/>
+      <c r="H36" s="26" t="s">
         <v>211</v>
       </c>
       <c r="I36" s="4"/>
     </row>
     <row r="37" spans="3:9" x14ac:dyDescent="0.3">
-      <c r="C37" s="41"/>
+      <c r="C37" s="57"/>
       <c r="D37" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="E37" s="40"/>
+      <c r="E37" s="56"/>
       <c r="F37" s="18" t="s">
         <v>194</v>
       </c>
-      <c r="G37" s="21"/>
-      <c r="H37" s="27" t="s">
+      <c r="G37" s="54"/>
+      <c r="H37" s="26" t="s">
         <v>211</v>
       </c>
       <c r="I37" s="4"/>
@@ -1907,12 +2125,14 @@
       <c r="D38" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="E38" s="41"/>
+      <c r="E38" s="57"/>
       <c r="F38" s="12" t="s">
         <v>195</v>
       </c>
-      <c r="G38" s="6"/>
-      <c r="H38" s="27" t="s">
+      <c r="G38" s="6" t="s">
+        <v>250</v>
+      </c>
+      <c r="H38" s="26" t="s">
         <v>211</v>
       </c>
       <c r="I38" s="4"/>
@@ -1924,77 +2144,77 @@
       <c r="D39" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="E39" s="42" t="s">
+      <c r="E39" s="58" t="s">
         <v>123</v>
       </c>
       <c r="F39" s="12" t="s">
         <v>154</v>
       </c>
       <c r="G39" s="6"/>
-      <c r="H39" s="27" t="s">
+      <c r="H39" s="26" t="s">
         <v>211</v>
       </c>
       <c r="I39" s="4"/>
     </row>
     <row r="40" spans="3:9" x14ac:dyDescent="0.3">
-      <c r="C40" s="42" t="s">
+      <c r="C40" s="58" t="s">
         <v>36</v>
       </c>
       <c r="D40" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="E40" s="42"/>
-      <c r="F40" s="49" t="s">
+      <c r="E40" s="58"/>
+      <c r="F40" s="44" t="s">
         <v>155</v>
       </c>
       <c r="G40" s="6"/>
-      <c r="H40" s="54" t="s">
+      <c r="H40" s="49" t="s">
         <v>211</v>
       </c>
       <c r="I40" s="4"/>
     </row>
     <row r="41" spans="3:9" x14ac:dyDescent="0.3">
-      <c r="C41" s="42"/>
+      <c r="C41" s="58"/>
       <c r="D41" s="7" t="s">
         <v>38</v>
       </c>
-      <c r="E41" s="42"/>
-      <c r="F41" s="50"/>
+      <c r="E41" s="58"/>
+      <c r="F41" s="45"/>
       <c r="G41" s="6"/>
-      <c r="H41" s="55"/>
+      <c r="H41" s="50"/>
       <c r="I41" s="4"/>
     </row>
     <row r="42" spans="3:9" x14ac:dyDescent="0.3">
-      <c r="C42" s="42"/>
+      <c r="C42" s="58"/>
       <c r="D42" s="7" t="s">
         <v>39</v>
       </c>
-      <c r="E42" s="42"/>
-      <c r="F42" s="50"/>
+      <c r="E42" s="58"/>
+      <c r="F42" s="45"/>
       <c r="G42" s="6"/>
-      <c r="H42" s="55"/>
+      <c r="H42" s="50"/>
       <c r="I42" s="4"/>
     </row>
     <row r="43" spans="3:9" x14ac:dyDescent="0.3">
-      <c r="C43" s="42"/>
+      <c r="C43" s="58"/>
       <c r="D43" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="E43" s="42"/>
-      <c r="F43" s="50"/>
+      <c r="E43" s="58"/>
+      <c r="F43" s="45"/>
       <c r="G43" s="6"/>
-      <c r="H43" s="55"/>
+      <c r="H43" s="50"/>
       <c r="I43" s="4"/>
     </row>
     <row r="44" spans="3:9" x14ac:dyDescent="0.3">
-      <c r="C44" s="42"/>
+      <c r="C44" s="58"/>
       <c r="D44" s="7" t="s">
         <v>41</v>
       </c>
-      <c r="E44" s="42"/>
-      <c r="F44" s="51"/>
+      <c r="E44" s="58"/>
+      <c r="F44" s="46"/>
       <c r="G44" s="6"/>
-      <c r="H44" s="56"/>
+      <c r="H44" s="51"/>
       <c r="I44" s="4"/>
     </row>
     <row r="45" spans="3:9" ht="60.25" x14ac:dyDescent="0.3">
@@ -2004,12 +2224,12 @@
       <c r="D45" s="7" t="s">
         <v>43</v>
       </c>
-      <c r="E45" s="42"/>
-      <c r="F45" s="25" t="s">
+      <c r="E45" s="58"/>
+      <c r="F45" s="24" t="s">
         <v>212</v>
       </c>
       <c r="G45" s="6"/>
-      <c r="H45" s="27" t="s">
+      <c r="H45" s="26" t="s">
         <v>211</v>
       </c>
       <c r="I45" s="4"/>
@@ -2021,12 +2241,12 @@
       <c r="D46" s="7" t="s">
         <v>45</v>
       </c>
-      <c r="E46" s="42"/>
+      <c r="E46" s="58"/>
       <c r="F46" s="12" t="s">
         <v>213</v>
       </c>
       <c r="G46" s="6"/>
-      <c r="H46" s="27" t="s">
+      <c r="H46" s="26" t="s">
         <v>211</v>
       </c>
       <c r="I46" s="4"/>
@@ -2038,12 +2258,12 @@
       <c r="D47" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="E47" s="42"/>
+      <c r="E47" s="58"/>
       <c r="F47" s="12" t="s">
         <v>214</v>
       </c>
       <c r="G47" s="6"/>
-      <c r="H47" s="27" t="s">
+      <c r="H47" s="26" t="s">
         <v>211</v>
       </c>
       <c r="I47" s="4"/>
@@ -2055,12 +2275,12 @@
       <c r="D48" s="7" t="s">
         <v>49</v>
       </c>
-      <c r="E48" s="42"/>
+      <c r="E48" s="58"/>
       <c r="F48" s="12" t="s">
         <v>156</v>
       </c>
       <c r="G48" s="6"/>
-      <c r="H48" s="27" t="s">
+      <c r="H48" s="26" t="s">
         <v>211</v>
       </c>
       <c r="I48" s="4"/>
@@ -2072,187 +2292,209 @@
       <c r="D49" s="7" t="s">
         <v>51</v>
       </c>
-      <c r="E49" s="23" t="s">
+      <c r="E49" s="22" t="s">
         <v>201</v>
       </c>
       <c r="F49" s="12" t="s">
         <v>215</v>
       </c>
       <c r="G49" s="6"/>
-      <c r="H49" s="27" t="s">
+      <c r="H49" s="26" t="s">
         <v>211</v>
       </c>
       <c r="I49" s="4"/>
     </row>
     <row r="50" spans="3:9" ht="45.2" x14ac:dyDescent="0.3">
-      <c r="C50" s="39" t="s">
+      <c r="C50" s="55" t="s">
         <v>52</v>
       </c>
       <c r="D50" s="7" t="s">
         <v>127</v>
       </c>
-      <c r="E50" s="39" t="s">
+      <c r="E50" s="55" t="s">
         <v>122</v>
       </c>
       <c r="F50" s="19" t="s">
         <v>200</v>
       </c>
-      <c r="G50" s="6"/>
-      <c r="H50" s="27" t="s">
+      <c r="G50" s="6" t="s">
+        <v>251</v>
+      </c>
+      <c r="H50" s="26" t="s">
         <v>211</v>
       </c>
       <c r="I50" s="4"/>
     </row>
     <row r="51" spans="3:9" ht="30.15" x14ac:dyDescent="0.3">
-      <c r="C51" s="41"/>
+      <c r="C51" s="57"/>
       <c r="D51" s="7" t="s">
         <v>53</v>
       </c>
-      <c r="E51" s="40"/>
+      <c r="E51" s="56"/>
       <c r="F51" s="19" t="s">
         <v>126</v>
       </c>
-      <c r="G51" s="6"/>
-      <c r="H51" s="27" t="s">
+      <c r="G51" s="6" t="s">
+        <v>252</v>
+      </c>
+      <c r="H51" s="26" t="s">
         <v>211</v>
       </c>
       <c r="I51" s="4"/>
     </row>
     <row r="52" spans="3:9" ht="60.25" x14ac:dyDescent="0.3">
-      <c r="C52" s="39" t="s">
+      <c r="C52" s="55" t="s">
         <v>224</v>
       </c>
       <c r="D52" s="7" t="s">
         <v>125</v>
       </c>
-      <c r="E52" s="40"/>
+      <c r="E52" s="56"/>
       <c r="F52" s="19" t="s">
         <v>223</v>
       </c>
-      <c r="G52" s="6"/>
-      <c r="H52" s="27" t="s">
+      <c r="G52" s="6" t="s">
+        <v>249</v>
+      </c>
+      <c r="H52" s="26" t="s">
         <v>211</v>
       </c>
       <c r="I52" s="4"/>
     </row>
     <row r="53" spans="3:9" ht="60.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C53" s="40"/>
+      <c r="C53" s="56"/>
       <c r="D53" s="7" t="s">
         <v>54</v>
       </c>
-      <c r="E53" s="40"/>
-      <c r="F53" s="24" t="s">
+      <c r="E53" s="56"/>
+      <c r="F53" s="23" t="s">
         <v>196</v>
       </c>
-      <c r="G53" s="6"/>
-      <c r="H53" s="27" t="s">
+      <c r="G53" s="6" t="s">
+        <v>253</v>
+      </c>
+      <c r="H53" s="26" t="s">
         <v>211</v>
       </c>
       <c r="I53" s="4"/>
     </row>
     <row r="54" spans="3:9" ht="120.45" x14ac:dyDescent="0.3">
-      <c r="C54" s="40"/>
+      <c r="C54" s="56"/>
       <c r="D54" s="7" t="s">
         <v>55</v>
       </c>
-      <c r="E54" s="40"/>
-      <c r="F54" s="24" t="s">
+      <c r="E54" s="56"/>
+      <c r="F54" s="23" t="s">
         <v>199</v>
       </c>
-      <c r="G54" s="6"/>
-      <c r="H54" s="27" t="s">
+      <c r="G54" s="6" t="s">
+        <v>254</v>
+      </c>
+      <c r="H54" s="26" t="s">
         <v>211</v>
       </c>
       <c r="I54" s="4"/>
     </row>
     <row r="55" spans="3:9" ht="90.35" x14ac:dyDescent="0.3">
-      <c r="C55" s="40"/>
+      <c r="C55" s="56"/>
       <c r="D55" s="7" t="s">
         <v>56</v>
       </c>
-      <c r="E55" s="40"/>
-      <c r="F55" s="24" t="s">
+      <c r="E55" s="56"/>
+      <c r="F55" s="23" t="s">
         <v>197</v>
       </c>
-      <c r="G55" s="6"/>
-      <c r="H55" s="27" t="s">
+      <c r="G55" s="6" t="s">
+        <v>255</v>
+      </c>
+      <c r="H55" s="26" t="s">
         <v>211</v>
       </c>
       <c r="I55" s="4"/>
     </row>
     <row r="56" spans="3:9" ht="45.2" x14ac:dyDescent="0.3">
-      <c r="C56" s="41"/>
+      <c r="C56" s="57"/>
       <c r="D56" s="7" t="s">
         <v>69</v>
       </c>
-      <c r="E56" s="40"/>
+      <c r="E56" s="56"/>
       <c r="F56" s="12" t="s">
         <v>198</v>
       </c>
-      <c r="G56" s="6"/>
-      <c r="H56" s="27" t="s">
+      <c r="G56" s="6" t="s">
+        <v>256</v>
+      </c>
+      <c r="H56" s="26" t="s">
         <v>211</v>
       </c>
       <c r="I56" s="4"/>
     </row>
     <row r="57" spans="3:9" ht="30.15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C57" s="42" t="s">
+      <c r="C57" s="58" t="s">
         <v>91</v>
       </c>
       <c r="D57" s="7" t="s">
         <v>57</v>
       </c>
-      <c r="E57" s="40"/>
+      <c r="E57" s="56"/>
       <c r="F57" s="9" t="s">
         <v>128</v>
       </c>
-      <c r="G57" s="6"/>
-      <c r="H57" s="27" t="s">
+      <c r="G57" s="6" t="s">
+        <v>257</v>
+      </c>
+      <c r="H57" s="26" t="s">
         <v>211</v>
       </c>
       <c r="I57" s="4"/>
     </row>
     <row r="58" spans="3:9" x14ac:dyDescent="0.3">
-      <c r="C58" s="42"/>
+      <c r="C58" s="58"/>
       <c r="D58" s="7" t="s">
         <v>58</v>
       </c>
-      <c r="E58" s="40"/>
+      <c r="E58" s="56"/>
       <c r="F58" s="9" t="s">
         <v>225</v>
       </c>
-      <c r="G58" s="6"/>
-      <c r="H58" s="27" t="s">
+      <c r="G58" s="6" t="s">
+        <v>258</v>
+      </c>
+      <c r="H58" s="26" t="s">
         <v>211</v>
       </c>
       <c r="I58" s="4"/>
     </row>
     <row r="59" spans="3:9" ht="52.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C59" s="42"/>
+      <c r="C59" s="58"/>
       <c r="D59" s="7" t="s">
         <v>59</v>
       </c>
-      <c r="E59" s="40"/>
+      <c r="E59" s="56"/>
       <c r="F59" s="9" t="s">
         <v>129</v>
       </c>
-      <c r="G59" s="6"/>
-      <c r="H59" s="27" t="s">
+      <c r="G59" s="6" t="s">
+        <v>259</v>
+      </c>
+      <c r="H59" s="26" t="s">
         <v>211</v>
       </c>
       <c r="I59" s="4"/>
     </row>
-    <row r="60" spans="3:9" x14ac:dyDescent="0.3">
-      <c r="C60" s="42"/>
+    <row r="60" spans="3:9" ht="30.15" x14ac:dyDescent="0.3">
+      <c r="C60" s="58"/>
       <c r="D60" s="7" t="s">
         <v>60</v>
       </c>
-      <c r="E60" s="41"/>
+      <c r="E60" s="57"/>
       <c r="F60" s="9" t="s">
         <v>130</v>
       </c>
-      <c r="G60" s="6"/>
-      <c r="H60" s="27" t="s">
+      <c r="G60" s="6" t="s">
+        <v>260</v>
+      </c>
+      <c r="H60" s="26" t="s">
         <v>211</v>
       </c>
       <c r="I60" s="4"/>
@@ -2268,100 +2510,112 @@
       <c r="F61" s="10" t="s">
         <v>131</v>
       </c>
-      <c r="G61" s="36"/>
-      <c r="H61" s="37"/>
-      <c r="I61" s="38"/>
+      <c r="G61" s="35"/>
+      <c r="H61" s="36"/>
+      <c r="I61" s="37"/>
     </row>
     <row r="62" spans="3:9" ht="30.15" x14ac:dyDescent="0.3">
-      <c r="C62" s="42" t="s">
+      <c r="C62" s="58" t="s">
         <v>64</v>
       </c>
       <c r="D62" s="7" t="s">
         <v>65</v>
       </c>
-      <c r="E62" s="39" t="s">
+      <c r="E62" s="55" t="s">
         <v>122</v>
       </c>
       <c r="F62" s="9" t="s">
         <v>204</v>
       </c>
-      <c r="G62" s="6"/>
-      <c r="H62" s="27" t="s">
+      <c r="G62" s="6" t="s">
+        <v>261</v>
+      </c>
+      <c r="H62" s="26" t="s">
         <v>211</v>
       </c>
       <c r="I62" s="4"/>
     </row>
     <row r="63" spans="3:9" ht="60.25" x14ac:dyDescent="0.3">
-      <c r="C63" s="42"/>
+      <c r="C63" s="58"/>
       <c r="D63" s="7" t="s">
         <v>66</v>
       </c>
-      <c r="E63" s="40"/>
+      <c r="E63" s="56"/>
       <c r="F63" s="9" t="s">
         <v>205</v>
       </c>
-      <c r="G63" s="6"/>
-      <c r="H63" s="27" t="s">
+      <c r="G63" s="6" t="s">
+        <v>262</v>
+      </c>
+      <c r="H63" s="26" t="s">
         <v>211</v>
       </c>
       <c r="I63" s="4"/>
     </row>
-    <row r="64" spans="3:9" ht="30.15" x14ac:dyDescent="0.3">
-      <c r="C64" s="42"/>
+    <row r="64" spans="3:9" ht="60.25" x14ac:dyDescent="0.3">
+      <c r="C64" s="58"/>
       <c r="D64" s="7" t="s">
         <v>67</v>
       </c>
-      <c r="E64" s="40"/>
+      <c r="E64" s="56"/>
       <c r="F64" s="9" t="s">
         <v>206</v>
       </c>
-      <c r="G64" s="6"/>
-      <c r="H64" s="27" t="s">
+      <c r="G64" s="6" t="s">
+        <v>263</v>
+      </c>
+      <c r="H64" s="26" t="s">
         <v>211</v>
       </c>
       <c r="I64" s="4"/>
     </row>
     <row r="65" spans="3:9" ht="30.15" x14ac:dyDescent="0.3">
-      <c r="C65" s="42"/>
+      <c r="C65" s="58"/>
       <c r="D65" s="7" t="s">
         <v>68</v>
       </c>
-      <c r="E65" s="40"/>
+      <c r="E65" s="56"/>
       <c r="F65" s="9" t="s">
         <v>207</v>
       </c>
-      <c r="G65" s="6"/>
-      <c r="H65" s="27" t="s">
+      <c r="G65" s="6" t="s">
+        <v>264</v>
+      </c>
+      <c r="H65" s="26" t="s">
         <v>211</v>
       </c>
       <c r="I65" s="4"/>
     </row>
     <row r="66" spans="3:9" ht="60.25" x14ac:dyDescent="0.3">
-      <c r="C66" s="42"/>
+      <c r="C66" s="58"/>
       <c r="D66" s="7" t="s">
         <v>132</v>
       </c>
-      <c r="E66" s="40"/>
+      <c r="E66" s="56"/>
       <c r="F66" s="9" t="s">
         <v>208</v>
       </c>
-      <c r="G66" s="6"/>
-      <c r="H66" s="27" t="s">
+      <c r="G66" s="6" t="s">
+        <v>266</v>
+      </c>
+      <c r="H66" s="26" t="s">
         <v>211</v>
       </c>
       <c r="I66" s="4"/>
     </row>
     <row r="67" spans="3:9" ht="120.45" x14ac:dyDescent="0.3">
-      <c r="C67" s="42"/>
+      <c r="C67" s="58"/>
       <c r="D67" s="2" t="s">
         <v>133</v>
       </c>
-      <c r="E67" s="40"/>
+      <c r="E67" s="56"/>
       <c r="F67" s="9" t="s">
         <v>209</v>
       </c>
-      <c r="G67" s="6"/>
-      <c r="H67" s="27" t="s">
+      <c r="G67" s="6" t="s">
+        <v>265</v>
+      </c>
+      <c r="H67" s="26" t="s">
         <v>211</v>
       </c>
       <c r="I67" s="4"/>
@@ -2373,569 +2627,601 @@
       <c r="D68" s="7" t="s">
         <v>71</v>
       </c>
-      <c r="E68" s="40"/>
-      <c r="F68" s="25" t="s">
+      <c r="E68" s="56"/>
+      <c r="F68" s="24" t="s">
         <v>210</v>
       </c>
-      <c r="G68" s="6"/>
-      <c r="H68" s="27" t="s">
+      <c r="G68" s="6" t="s">
+        <v>267</v>
+      </c>
+      <c r="H68" s="26" t="s">
         <v>211</v>
       </c>
       <c r="I68" s="4"/>
     </row>
     <row r="69" spans="3:9" ht="30.15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C69" s="42" t="s">
+      <c r="C69" s="58" t="s">
         <v>72</v>
       </c>
       <c r="D69" s="7" t="s">
         <v>73</v>
       </c>
-      <c r="E69" s="40"/>
+      <c r="E69" s="56"/>
       <c r="F69" s="9" t="s">
         <v>134</v>
       </c>
-      <c r="G69" s="6"/>
-      <c r="H69" s="27" t="s">
+      <c r="G69" s="6" t="s">
+        <v>268</v>
+      </c>
+      <c r="H69" s="26" t="s">
         <v>211</v>
       </c>
       <c r="I69" s="4"/>
     </row>
     <row r="70" spans="3:9" ht="30.15" x14ac:dyDescent="0.3">
-      <c r="C70" s="42"/>
+      <c r="C70" s="58"/>
       <c r="D70" s="7" t="s">
         <v>74</v>
       </c>
-      <c r="E70" s="40"/>
+      <c r="E70" s="56"/>
       <c r="F70" s="9" t="s">
         <v>140</v>
       </c>
-      <c r="G70" s="6"/>
-      <c r="H70" s="27" t="s">
+      <c r="G70" s="6" t="s">
+        <v>269</v>
+      </c>
+      <c r="H70" s="26" t="s">
         <v>211</v>
       </c>
       <c r="I70" s="4"/>
     </row>
     <row r="71" spans="3:9" x14ac:dyDescent="0.3">
-      <c r="C71" s="42"/>
+      <c r="C71" s="58"/>
       <c r="D71" s="7" t="s">
         <v>75</v>
       </c>
-      <c r="E71" s="40"/>
+      <c r="E71" s="56"/>
       <c r="F71" s="9" t="s">
         <v>136</v>
       </c>
-      <c r="G71" s="6"/>
-      <c r="H71" s="27" t="s">
+      <c r="G71" s="6" t="s">
+        <v>270</v>
+      </c>
+      <c r="H71" s="26" t="s">
         <v>211</v>
       </c>
       <c r="I71" s="4"/>
     </row>
     <row r="72" spans="3:9" ht="30.15" x14ac:dyDescent="0.3">
-      <c r="C72" s="42"/>
+      <c r="C72" s="58"/>
       <c r="D72" s="7" t="s">
         <v>219</v>
       </c>
-      <c r="E72" s="40"/>
+      <c r="E72" s="56"/>
       <c r="F72" s="12" t="s">
         <v>164</v>
       </c>
-      <c r="G72" s="6"/>
-      <c r="H72" s="27" t="s">
+      <c r="G72" s="6" t="s">
+        <v>271</v>
+      </c>
+      <c r="H72" s="26" t="s">
         <v>211</v>
       </c>
       <c r="I72" s="4"/>
     </row>
     <row r="73" spans="3:9" x14ac:dyDescent="0.3">
-      <c r="C73" s="42"/>
+      <c r="C73" s="58"/>
       <c r="D73" s="7" t="s">
         <v>76</v>
       </c>
-      <c r="E73" s="40"/>
+      <c r="E73" s="56"/>
       <c r="F73" s="9" t="s">
         <v>137</v>
       </c>
-      <c r="G73" s="6"/>
-      <c r="H73" s="27" t="s">
+      <c r="G73" s="6" t="s">
+        <v>272</v>
+      </c>
+      <c r="H73" s="26" t="s">
         <v>211</v>
       </c>
       <c r="I73" s="4"/>
     </row>
     <row r="74" spans="3:9" x14ac:dyDescent="0.3">
-      <c r="C74" s="42"/>
+      <c r="C74" s="58"/>
       <c r="D74" s="7" t="s">
         <v>77</v>
       </c>
-      <c r="E74" s="40"/>
+      <c r="E74" s="56"/>
       <c r="F74" s="9" t="s">
         <v>135</v>
       </c>
-      <c r="G74" s="6"/>
-      <c r="H74" s="27" t="s">
+      <c r="G74" s="6" t="s">
+        <v>273</v>
+      </c>
+      <c r="H74" s="26" t="s">
         <v>211</v>
       </c>
       <c r="I74" s="4"/>
     </row>
     <row r="75" spans="3:9" x14ac:dyDescent="0.3">
-      <c r="C75" s="42"/>
+      <c r="C75" s="58"/>
       <c r="D75" s="7" t="s">
         <v>78</v>
       </c>
-      <c r="E75" s="40"/>
+      <c r="E75" s="56"/>
       <c r="F75" s="9" t="s">
         <v>139</v>
       </c>
-      <c r="G75" s="6"/>
-      <c r="H75" s="27" t="s">
+      <c r="G75" s="6" t="s">
+        <v>274</v>
+      </c>
+      <c r="H75" s="26" t="s">
         <v>211</v>
       </c>
       <c r="I75" s="4"/>
     </row>
     <row r="76" spans="3:9" x14ac:dyDescent="0.3">
-      <c r="C76" s="42"/>
+      <c r="C76" s="58"/>
       <c r="D76" s="7" t="s">
         <v>79</v>
       </c>
-      <c r="E76" s="40"/>
+      <c r="E76" s="56"/>
       <c r="F76" s="9" t="s">
         <v>138</v>
       </c>
-      <c r="G76" s="6"/>
-      <c r="H76" s="27" t="s">
+      <c r="G76" s="6" t="s">
+        <v>275</v>
+      </c>
+      <c r="H76" s="26" t="s">
         <v>211</v>
       </c>
       <c r="I76" s="4"/>
     </row>
     <row r="77" spans="3:9" ht="30.15" x14ac:dyDescent="0.3">
-      <c r="C77" s="42"/>
+      <c r="C77" s="58"/>
       <c r="D77" s="7" t="s">
         <v>80</v>
       </c>
-      <c r="E77" s="40"/>
+      <c r="E77" s="56"/>
       <c r="F77" s="12" t="s">
         <v>189</v>
       </c>
-      <c r="G77" s="6"/>
-      <c r="H77" s="27" t="s">
+      <c r="G77" s="6" t="s">
+        <v>276</v>
+      </c>
+      <c r="H77" s="26" t="s">
         <v>211</v>
       </c>
       <c r="I77" s="4"/>
     </row>
     <row r="78" spans="3:9" ht="30.15" x14ac:dyDescent="0.3">
-      <c r="C78" s="42"/>
+      <c r="C78" s="58"/>
       <c r="D78" s="7" t="s">
         <v>81</v>
       </c>
-      <c r="E78" s="40"/>
-      <c r="F78" s="26" t="s">
+      <c r="E78" s="56"/>
+      <c r="F78" s="25" t="s">
         <v>141</v>
       </c>
-      <c r="G78" s="33"/>
-      <c r="H78" s="34"/>
-      <c r="I78" s="35"/>
+      <c r="G78" s="32"/>
+      <c r="H78" s="33"/>
+      <c r="I78" s="34"/>
     </row>
     <row r="79" spans="3:9" ht="30.15" x14ac:dyDescent="0.3">
-      <c r="C79" s="40" t="s">
+      <c r="C79" s="56" t="s">
         <v>83</v>
       </c>
       <c r="D79" s="7" t="s">
         <v>142</v>
       </c>
-      <c r="E79" s="40"/>
+      <c r="E79" s="56"/>
       <c r="F79" s="9" t="s">
         <v>165</v>
       </c>
       <c r="G79" s="6"/>
-      <c r="H79" s="27" t="s">
+      <c r="H79" s="26" t="s">
         <v>211</v>
       </c>
       <c r="I79" s="4"/>
     </row>
     <row r="80" spans="3:9" ht="30.15" x14ac:dyDescent="0.3">
-      <c r="C80" s="40"/>
+      <c r="C80" s="56"/>
       <c r="D80" s="7" t="s">
         <v>82</v>
       </c>
-      <c r="E80" s="40"/>
+      <c r="E80" s="56"/>
       <c r="F80" s="9" t="s">
         <v>166</v>
       </c>
       <c r="G80" s="6"/>
-      <c r="H80" s="27" t="s">
+      <c r="H80" s="26" t="s">
         <v>211</v>
       </c>
       <c r="I80" s="4"/>
     </row>
     <row r="81" spans="3:9" ht="30.15" x14ac:dyDescent="0.3">
-      <c r="C81" s="39" t="s">
+      <c r="C81" s="55" t="s">
         <v>84</v>
       </c>
       <c r="D81" s="7" t="s">
         <v>146</v>
       </c>
-      <c r="E81" s="40"/>
+      <c r="E81" s="56"/>
       <c r="F81" s="9" t="s">
         <v>167</v>
       </c>
       <c r="G81" s="6"/>
-      <c r="H81" s="27" t="s">
+      <c r="H81" s="26" t="s">
         <v>211</v>
       </c>
       <c r="I81" s="4"/>
     </row>
     <row r="82" spans="3:9" ht="69.400000000000006" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C82" s="40"/>
+      <c r="C82" s="56"/>
       <c r="D82" s="7" t="s">
         <v>147</v>
       </c>
-      <c r="E82" s="40"/>
+      <c r="E82" s="56"/>
       <c r="F82" s="9" t="s">
         <v>181</v>
       </c>
       <c r="G82" s="6"/>
-      <c r="H82" s="27" t="s">
+      <c r="H82" s="26" t="s">
         <v>211</v>
       </c>
       <c r="I82" s="4"/>
     </row>
     <row r="83" spans="3:9" x14ac:dyDescent="0.3">
-      <c r="C83" s="40"/>
+      <c r="C83" s="56"/>
       <c r="D83" s="7" t="s">
         <v>85</v>
       </c>
-      <c r="E83" s="40"/>
-      <c r="F83" s="26" t="s">
+      <c r="E83" s="56"/>
+      <c r="F83" s="25" t="s">
         <v>141</v>
       </c>
-      <c r="G83" s="33"/>
-      <c r="H83" s="34"/>
-      <c r="I83" s="35"/>
+      <c r="G83" s="32"/>
+      <c r="H83" s="33"/>
+      <c r="I83" s="34"/>
     </row>
     <row r="84" spans="3:9" x14ac:dyDescent="0.3">
-      <c r="C84" s="40"/>
+      <c r="C84" s="56"/>
       <c r="D84" s="7" t="s">
         <v>86</v>
       </c>
-      <c r="E84" s="40"/>
+      <c r="E84" s="56"/>
       <c r="F84" s="9" t="s">
         <v>168</v>
       </c>
       <c r="G84" s="6"/>
-      <c r="H84" s="27" t="s">
+      <c r="H84" s="26" t="s">
         <v>211</v>
       </c>
       <c r="I84" s="4"/>
     </row>
     <row r="85" spans="3:9" ht="30.15" x14ac:dyDescent="0.3">
-      <c r="C85" s="40"/>
+      <c r="C85" s="56"/>
       <c r="D85" s="7" t="s">
         <v>87</v>
       </c>
-      <c r="E85" s="40"/>
+      <c r="E85" s="56"/>
       <c r="F85" s="9" t="s">
         <v>169</v>
       </c>
       <c r="G85" s="6"/>
-      <c r="H85" s="27" t="s">
+      <c r="H85" s="26" t="s">
         <v>211</v>
       </c>
       <c r="I85" s="4"/>
     </row>
     <row r="86" spans="3:9" ht="30.15" x14ac:dyDescent="0.3">
-      <c r="C86" s="40"/>
+      <c r="C86" s="56"/>
       <c r="D86" s="7" t="s">
         <v>88</v>
       </c>
-      <c r="E86" s="40"/>
+      <c r="E86" s="56"/>
       <c r="F86" s="9" t="s">
         <v>170</v>
       </c>
       <c r="G86" s="6"/>
-      <c r="H86" s="27" t="s">
+      <c r="H86" s="26" t="s">
         <v>211</v>
       </c>
       <c r="I86" s="4"/>
     </row>
     <row r="87" spans="3:9" x14ac:dyDescent="0.3">
-      <c r="C87" s="40"/>
+      <c r="C87" s="56"/>
       <c r="D87" s="7" t="s">
         <v>89</v>
       </c>
-      <c r="E87" s="40"/>
+      <c r="E87" s="56"/>
       <c r="F87" s="9" t="s">
         <v>171</v>
       </c>
       <c r="G87" s="6"/>
-      <c r="H87" s="27" t="s">
+      <c r="H87" s="26" t="s">
         <v>211</v>
       </c>
       <c r="I87" s="4"/>
     </row>
     <row r="88" spans="3:9" x14ac:dyDescent="0.3">
-      <c r="C88" s="40"/>
+      <c r="C88" s="56"/>
       <c r="D88" s="7" t="s">
         <v>90</v>
       </c>
-      <c r="E88" s="40"/>
+      <c r="E88" s="56"/>
       <c r="F88" s="9" t="s">
         <v>172</v>
       </c>
       <c r="G88" s="6"/>
-      <c r="H88" s="27" t="s">
+      <c r="H88" s="26" t="s">
         <v>211</v>
       </c>
       <c r="I88" s="4"/>
     </row>
     <row r="89" spans="3:9" x14ac:dyDescent="0.3">
-      <c r="C89" s="40"/>
+      <c r="C89" s="56"/>
       <c r="D89" s="7" t="s">
         <v>97</v>
       </c>
-      <c r="E89" s="40"/>
-      <c r="F89" s="26" t="s">
+      <c r="E89" s="56"/>
+      <c r="F89" s="25" t="s">
         <v>141</v>
       </c>
-      <c r="G89" s="33"/>
-      <c r="H89" s="34"/>
-      <c r="I89" s="35"/>
+      <c r="G89" s="32"/>
+      <c r="H89" s="33"/>
+      <c r="I89" s="34"/>
     </row>
     <row r="90" spans="3:9" x14ac:dyDescent="0.3">
-      <c r="C90" s="40"/>
+      <c r="C90" s="56"/>
       <c r="D90" s="7" t="s">
         <v>98</v>
       </c>
-      <c r="E90" s="40"/>
+      <c r="E90" s="56"/>
       <c r="F90" s="9" t="s">
         <v>173</v>
       </c>
       <c r="G90" s="6"/>
-      <c r="H90" s="27" t="s">
+      <c r="H90" s="26" t="s">
         <v>211</v>
       </c>
       <c r="I90" s="4"/>
     </row>
     <row r="91" spans="3:9" x14ac:dyDescent="0.3">
-      <c r="C91" s="40"/>
+      <c r="C91" s="56"/>
       <c r="D91" s="7" t="s">
         <v>99</v>
       </c>
-      <c r="E91" s="40"/>
+      <c r="E91" s="56"/>
       <c r="F91" s="9" t="s">
         <v>174</v>
       </c>
       <c r="G91" s="6"/>
-      <c r="H91" s="27" t="s">
+      <c r="H91" s="26" t="s">
         <v>211</v>
       </c>
       <c r="I91" s="4"/>
     </row>
     <row r="92" spans="3:9" ht="30.15" x14ac:dyDescent="0.3">
-      <c r="C92" s="40"/>
+      <c r="C92" s="56"/>
       <c r="D92" s="7" t="s">
         <v>100</v>
       </c>
-      <c r="E92" s="40"/>
+      <c r="E92" s="56"/>
       <c r="F92" s="9" t="s">
         <v>175</v>
       </c>
       <c r="G92" s="6"/>
-      <c r="H92" s="27" t="s">
+      <c r="H92" s="26" t="s">
         <v>211</v>
       </c>
       <c r="I92" s="4"/>
     </row>
     <row r="93" spans="3:9" ht="45.2" x14ac:dyDescent="0.3">
-      <c r="C93" s="40"/>
+      <c r="C93" s="56"/>
       <c r="D93" s="7" t="s">
         <v>144</v>
       </c>
-      <c r="E93" s="40"/>
+      <c r="E93" s="56"/>
       <c r="F93" s="9" t="s">
         <v>176</v>
       </c>
       <c r="G93" s="6"/>
-      <c r="H93" s="27" t="s">
+      <c r="H93" s="26" t="s">
         <v>211</v>
       </c>
       <c r="I93" s="4"/>
     </row>
     <row r="94" spans="3:9" x14ac:dyDescent="0.3">
-      <c r="C94" s="39" t="s">
+      <c r="C94" s="55" t="s">
         <v>92</v>
       </c>
       <c r="D94" s="7" t="s">
         <v>93</v>
       </c>
-      <c r="E94" s="40"/>
+      <c r="E94" s="56"/>
       <c r="F94" s="9" t="s">
         <v>177</v>
       </c>
       <c r="G94" s="6"/>
-      <c r="H94" s="27" t="s">
+      <c r="H94" s="26" t="s">
         <v>211</v>
       </c>
       <c r="I94" s="4"/>
     </row>
     <row r="95" spans="3:9" ht="30.15" x14ac:dyDescent="0.3">
-      <c r="C95" s="40"/>
+      <c r="C95" s="56"/>
       <c r="D95" s="7" t="s">
         <v>94</v>
       </c>
-      <c r="E95" s="40"/>
+      <c r="E95" s="56"/>
       <c r="F95" s="9" t="s">
         <v>178</v>
       </c>
       <c r="G95" s="6"/>
-      <c r="H95" s="27" t="s">
+      <c r="H95" s="26" t="s">
         <v>211</v>
       </c>
       <c r="I95" s="4"/>
     </row>
     <row r="96" spans="3:9" x14ac:dyDescent="0.3">
-      <c r="C96" s="40"/>
+      <c r="C96" s="56"/>
       <c r="D96" s="7" t="s">
         <v>95</v>
       </c>
-      <c r="E96" s="40"/>
-      <c r="F96" s="29" t="s">
+      <c r="E96" s="56"/>
+      <c r="F96" s="28" t="s">
         <v>141</v>
       </c>
-      <c r="G96" s="30"/>
-      <c r="H96" s="31"/>
-      <c r="I96" s="32"/>
+      <c r="G96" s="29"/>
+      <c r="H96" s="30"/>
+      <c r="I96" s="31"/>
     </row>
     <row r="97" spans="3:9" x14ac:dyDescent="0.3">
-      <c r="C97" s="40"/>
+      <c r="C97" s="56"/>
       <c r="D97" s="7" t="s">
         <v>96</v>
       </c>
-      <c r="E97" s="40"/>
+      <c r="E97" s="56"/>
       <c r="F97" s="9" t="s">
         <v>179</v>
       </c>
       <c r="G97" s="6"/>
-      <c r="H97" s="27" t="s">
+      <c r="H97" s="26" t="s">
         <v>211</v>
       </c>
       <c r="I97" s="4"/>
     </row>
     <row r="98" spans="3:9" x14ac:dyDescent="0.3">
-      <c r="C98" s="40"/>
+      <c r="C98" s="56"/>
       <c r="D98" s="7" t="s">
         <v>143</v>
       </c>
-      <c r="E98" s="40"/>
+      <c r="E98" s="56"/>
       <c r="F98" s="9" t="s">
         <v>180</v>
       </c>
       <c r="G98" s="6"/>
-      <c r="H98" s="27" t="s">
+      <c r="H98" s="26" t="s">
         <v>211</v>
       </c>
       <c r="I98" s="4"/>
     </row>
     <row r="99" spans="3:9" ht="30.15" x14ac:dyDescent="0.3">
-      <c r="C99" s="41"/>
+      <c r="C99" s="57"/>
       <c r="D99" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="E99" s="40"/>
+      <c r="E99" s="56"/>
       <c r="F99" s="9" t="s">
         <v>145</v>
       </c>
       <c r="G99" s="6"/>
-      <c r="H99" s="27" t="s">
+      <c r="H99" s="26" t="s">
         <v>211</v>
       </c>
       <c r="I99" s="4"/>
     </row>
     <row r="100" spans="3:9" x14ac:dyDescent="0.3">
-      <c r="C100" s="42" t="s">
+      <c r="C100" s="58" t="s">
         <v>107</v>
       </c>
       <c r="D100" s="7" t="s">
         <v>101</v>
       </c>
-      <c r="E100" s="40"/>
+      <c r="E100" s="56"/>
       <c r="F100" s="9" t="s">
         <v>149</v>
       </c>
-      <c r="G100" s="6"/>
-      <c r="H100" s="27" t="s">
+      <c r="G100" s="6" t="s">
+        <v>280</v>
+      </c>
+      <c r="H100" s="26" t="s">
         <v>211</v>
       </c>
       <c r="I100" s="4"/>
     </row>
     <row r="101" spans="3:9" ht="30.15" x14ac:dyDescent="0.3">
-      <c r="C101" s="42"/>
+      <c r="C101" s="58"/>
       <c r="D101" s="7" t="s">
         <v>102</v>
       </c>
-      <c r="E101" s="40"/>
+      <c r="E101" s="56"/>
       <c r="F101" s="9" t="s">
         <v>148</v>
       </c>
-      <c r="G101" s="6"/>
-      <c r="H101" s="27" t="s">
+      <c r="G101" s="6" t="s">
+        <v>279</v>
+      </c>
+      <c r="H101" s="26" t="s">
         <v>211</v>
       </c>
       <c r="I101" s="4"/>
     </row>
     <row r="102" spans="3:9" x14ac:dyDescent="0.3">
-      <c r="C102" s="42"/>
+      <c r="C102" s="58"/>
       <c r="D102" s="7" t="s">
         <v>103</v>
       </c>
-      <c r="E102" s="40"/>
+      <c r="E102" s="56"/>
       <c r="F102" s="9" t="s">
         <v>151</v>
       </c>
-      <c r="G102" s="6"/>
-      <c r="H102" s="27" t="s">
+      <c r="G102" s="6" t="s">
+        <v>277</v>
+      </c>
+      <c r="H102" s="26" t="s">
         <v>211</v>
       </c>
       <c r="I102" s="4"/>
     </row>
     <row r="103" spans="3:9" ht="30.15" x14ac:dyDescent="0.3">
-      <c r="C103" s="42"/>
+      <c r="C103" s="58"/>
       <c r="D103" s="7" t="s">
         <v>104</v>
       </c>
-      <c r="E103" s="40"/>
+      <c r="E103" s="56"/>
       <c r="F103" s="9" t="s">
         <v>150</v>
       </c>
-      <c r="G103" s="6"/>
-      <c r="H103" s="27" t="s">
+      <c r="G103" s="6" t="s">
+        <v>278</v>
+      </c>
+      <c r="H103" s="26" t="s">
         <v>211</v>
       </c>
       <c r="I103" s="4"/>
     </row>
     <row r="104" spans="3:9" x14ac:dyDescent="0.3">
-      <c r="C104" s="42"/>
+      <c r="C104" s="58"/>
       <c r="D104" s="7" t="s">
         <v>105</v>
       </c>
-      <c r="E104" s="40"/>
+      <c r="E104" s="56"/>
       <c r="F104" s="9" t="s">
         <v>152</v>
       </c>
-      <c r="G104" s="6"/>
-      <c r="H104" s="27" t="s">
+      <c r="G104" s="6" t="s">
+        <v>281</v>
+      </c>
+      <c r="H104" s="26" t="s">
         <v>211</v>
       </c>
       <c r="I104" s="4"/>
     </row>
     <row r="105" spans="3:9" ht="30.15" x14ac:dyDescent="0.3">
-      <c r="C105" s="42"/>
+      <c r="C105" s="58"/>
       <c r="D105" s="8" t="s">
         <v>106</v>
       </c>
-      <c r="E105" s="41"/>
+      <c r="E105" s="57"/>
       <c r="F105" s="9" t="s">
         <v>153</v>
       </c>
-      <c r="G105" s="6"/>
-      <c r="H105" s="27" t="s">
+      <c r="G105" s="6" t="s">
+        <v>282</v>
+      </c>
+      <c r="H105" s="26" t="s">
         <v>211</v>
       </c>
       <c r="I105" s="4"/>
@@ -2951,31 +3237,6 @@
     </row>
   </sheetData>
   <mergeCells count="34">
-    <mergeCell ref="I6:I7"/>
-    <mergeCell ref="I18:I22"/>
-    <mergeCell ref="F28:F32"/>
-    <mergeCell ref="F40:F44"/>
-    <mergeCell ref="F6:F7"/>
-    <mergeCell ref="H40:H44"/>
-    <mergeCell ref="H6:H7"/>
-    <mergeCell ref="H18:H22"/>
-    <mergeCell ref="G18:G22"/>
-    <mergeCell ref="G6:G7"/>
-    <mergeCell ref="E3:E27"/>
-    <mergeCell ref="E33:E38"/>
-    <mergeCell ref="E39:E48"/>
-    <mergeCell ref="F18:F22"/>
-    <mergeCell ref="C30:C32"/>
-    <mergeCell ref="C40:C44"/>
-    <mergeCell ref="C33:C37"/>
-    <mergeCell ref="C50:C51"/>
-    <mergeCell ref="C52:C56"/>
-    <mergeCell ref="C5:C8"/>
-    <mergeCell ref="C9:C15"/>
-    <mergeCell ref="C16:C17"/>
-    <mergeCell ref="C24:C27"/>
-    <mergeCell ref="C28:C29"/>
-    <mergeCell ref="C18:C22"/>
     <mergeCell ref="E50:E60"/>
     <mergeCell ref="E62:E105"/>
     <mergeCell ref="C69:C78"/>
@@ -2985,6 +3246,31 @@
     <mergeCell ref="C100:C105"/>
     <mergeCell ref="C62:C67"/>
     <mergeCell ref="C57:C60"/>
+    <mergeCell ref="C50:C51"/>
+    <mergeCell ref="C52:C56"/>
+    <mergeCell ref="C5:C8"/>
+    <mergeCell ref="C9:C15"/>
+    <mergeCell ref="C16:C17"/>
+    <mergeCell ref="C24:C27"/>
+    <mergeCell ref="C28:C29"/>
+    <mergeCell ref="C18:C22"/>
+    <mergeCell ref="E3:E27"/>
+    <mergeCell ref="E33:E38"/>
+    <mergeCell ref="E39:E48"/>
+    <mergeCell ref="F18:F22"/>
+    <mergeCell ref="C30:C32"/>
+    <mergeCell ref="C40:C44"/>
+    <mergeCell ref="C33:C37"/>
+    <mergeCell ref="I6:I7"/>
+    <mergeCell ref="I18:I22"/>
+    <mergeCell ref="F28:F32"/>
+    <mergeCell ref="F40:F44"/>
+    <mergeCell ref="F6:F7"/>
+    <mergeCell ref="H40:H44"/>
+    <mergeCell ref="H6:H7"/>
+    <mergeCell ref="H18:H22"/>
+    <mergeCell ref="G6:G7"/>
+    <mergeCell ref="G34:G37"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
finished mostly all mutates
</commit_message>
<xml_diff>
--- a/edit_eam/crosscheck.xlsx
+++ b/edit_eam/crosscheck.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="400" uniqueCount="307">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="403" uniqueCount="310">
   <si>
     <t>Nombre</t>
   </si>
@@ -652,9 +652,6 @@
     <t>2017 == VALAGRI17 / Total Capital Humano17,      2018 == VALAGRI18 / Total Capital Humano18</t>
   </si>
   <si>
-    <t xml:space="preserve">2017 == PORCVT17,        2018 == PORCVT18 </t>
-  </si>
-  <si>
     <t>ACTI2017 == II1R10C1,     ACTI2018 == II1R10C2,                   VA17 == VALAGRI17,       VA18 == VALAGRI18</t>
   </si>
   <si>
@@ -935,6 +932,18 @@
   </si>
   <si>
     <t xml:space="preserve">productividadL2017, productividadL2018 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">2017 == PORCVT17/VALORVEN2017,        2018 == PORCVT18/VALORVEN2018 </t>
+  </si>
+  <si>
+    <t>ratioX2017,     ratioX2018</t>
+  </si>
+  <si>
+    <t>ratioM2017, ratioM2018</t>
+  </si>
+  <si>
+    <t>inversion2017, inversion2018</t>
   </si>
 </sst>
 </file>
@@ -1231,6 +1240,18 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
@@ -1270,18 +1291,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1590,8 +1599,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="C2:I107"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C43" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G47" sqref="G47"/>
+    <sheetView tabSelected="1" topLeftCell="C46" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G50" sqref="G50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="15.05" x14ac:dyDescent="0.3"/>
@@ -1634,7 +1643,7 @@
       <c r="D3" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="E3" s="55" t="s">
+      <c r="E3" s="41" t="s">
         <v>122</v>
       </c>
       <c r="F3" s="9" t="s">
@@ -1655,7 +1664,7 @@
       <c r="D4" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="E4" s="56"/>
+      <c r="E4" s="42"/>
       <c r="F4" s="12" t="s">
         <v>108</v>
       </c>
@@ -1664,18 +1673,18 @@
       <c r="I4" s="4"/>
     </row>
     <row r="5" spans="3:9" x14ac:dyDescent="0.3">
-      <c r="C5" s="58" t="s">
+      <c r="C5" s="44" t="s">
         <v>7</v>
       </c>
       <c r="D5" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="E5" s="56"/>
+      <c r="E5" s="42"/>
       <c r="F5" s="9" t="s">
         <v>109</v>
       </c>
       <c r="G5" s="6" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="H5" s="26" t="s">
         <v>209</v>
@@ -1683,44 +1692,44 @@
       <c r="I5" s="4"/>
     </row>
     <row r="6" spans="3:9" x14ac:dyDescent="0.3">
-      <c r="C6" s="58"/>
+      <c r="C6" s="44"/>
       <c r="D6" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="E6" s="56"/>
-      <c r="F6" s="47" t="s">
+      <c r="E6" s="42"/>
+      <c r="F6" s="51" t="s">
         <v>111</v>
       </c>
-      <c r="G6" s="52" t="s">
-        <v>225</v>
-      </c>
-      <c r="H6" s="49" t="s">
-        <v>209</v>
-      </c>
-      <c r="I6" s="41"/>
+      <c r="G6" s="56" t="s">
+        <v>224</v>
+      </c>
+      <c r="H6" s="53" t="s">
+        <v>209</v>
+      </c>
+      <c r="I6" s="45"/>
     </row>
     <row r="7" spans="3:9" x14ac:dyDescent="0.3">
-      <c r="C7" s="58"/>
+      <c r="C7" s="44"/>
       <c r="D7" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="E7" s="56"/>
-      <c r="F7" s="48"/>
-      <c r="G7" s="53"/>
-      <c r="H7" s="51"/>
-      <c r="I7" s="42"/>
+      <c r="E7" s="42"/>
+      <c r="F7" s="52"/>
+      <c r="G7" s="57"/>
+      <c r="H7" s="55"/>
+      <c r="I7" s="46"/>
     </row>
     <row r="8" spans="3:9" x14ac:dyDescent="0.3">
-      <c r="C8" s="58"/>
+      <c r="C8" s="44"/>
       <c r="D8" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="E8" s="56"/>
+      <c r="E8" s="42"/>
       <c r="F8" s="11" t="s">
         <v>110</v>
       </c>
       <c r="G8" s="6" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="H8" s="26" t="s">
         <v>209</v>
@@ -1728,18 +1737,18 @@
       <c r="I8" s="4"/>
     </row>
     <row r="9" spans="3:9" x14ac:dyDescent="0.3">
-      <c r="C9" s="58" t="s">
+      <c r="C9" s="44" t="s">
         <v>13</v>
       </c>
       <c r="D9" s="7" t="s">
         <v>155</v>
       </c>
-      <c r="E9" s="56"/>
+      <c r="E9" s="42"/>
       <c r="F9" s="23" t="s">
         <v>180</v>
       </c>
       <c r="G9" s="6" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="H9" s="26" t="s">
         <v>209</v>
@@ -1747,16 +1756,16 @@
       <c r="I9" s="4"/>
     </row>
     <row r="10" spans="3:9" x14ac:dyDescent="0.3">
-      <c r="C10" s="58"/>
+      <c r="C10" s="44"/>
       <c r="D10" s="7" t="s">
         <v>156</v>
       </c>
-      <c r="E10" s="56"/>
+      <c r="E10" s="42"/>
       <c r="F10" s="23" t="s">
         <v>181</v>
       </c>
       <c r="G10" s="6" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="H10" s="26" t="s">
         <v>209</v>
@@ -1764,16 +1773,16 @@
       <c r="I10" s="4"/>
     </row>
     <row r="11" spans="3:9" ht="34.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C11" s="58"/>
+      <c r="C11" s="44"/>
       <c r="D11" s="7" t="s">
         <v>157</v>
       </c>
-      <c r="E11" s="56"/>
+      <c r="E11" s="42"/>
       <c r="F11" s="23" t="s">
         <v>182</v>
       </c>
       <c r="G11" s="6" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="H11" s="26" t="s">
         <v>209</v>
@@ -1781,16 +1790,16 @@
       <c r="I11" s="4"/>
     </row>
     <row r="12" spans="3:9" ht="34.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C12" s="58"/>
+      <c r="C12" s="44"/>
       <c r="D12" s="7" t="s">
         <v>158</v>
       </c>
-      <c r="E12" s="56"/>
+      <c r="E12" s="42"/>
       <c r="F12" s="23" t="s">
         <v>183</v>
       </c>
       <c r="G12" s="6" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="H12" s="26" t="s">
         <v>209</v>
@@ -1798,16 +1807,16 @@
       <c r="I12" s="4"/>
     </row>
     <row r="13" spans="3:9" ht="65.45" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C13" s="58"/>
+      <c r="C13" s="44"/>
       <c r="D13" s="7" t="s">
         <v>159</v>
       </c>
-      <c r="E13" s="56"/>
+      <c r="E13" s="42"/>
       <c r="F13" s="23" t="s">
         <v>184</v>
       </c>
       <c r="G13" s="6" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="H13" s="26" t="s">
         <v>209</v>
@@ -1815,16 +1824,16 @@
       <c r="I13" s="4"/>
     </row>
     <row r="14" spans="3:9" ht="46.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C14" s="58"/>
+      <c r="C14" s="44"/>
       <c r="D14" s="7" t="s">
         <v>160</v>
       </c>
-      <c r="E14" s="56"/>
+      <c r="E14" s="42"/>
       <c r="F14" s="23" t="s">
         <v>185</v>
       </c>
       <c r="G14" s="6" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="H14" s="26" t="s">
         <v>209</v>
@@ -1832,16 +1841,16 @@
       <c r="I14" s="4"/>
     </row>
     <row r="15" spans="3:9" ht="66.150000000000006" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C15" s="58"/>
+      <c r="C15" s="44"/>
       <c r="D15" s="7" t="s">
         <v>161</v>
       </c>
-      <c r="E15" s="56"/>
+      <c r="E15" s="42"/>
       <c r="F15" s="23" t="s">
         <v>186</v>
       </c>
       <c r="G15" s="6" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="H15" s="26" t="s">
         <v>209</v>
@@ -1849,18 +1858,18 @@
       <c r="I15" s="4"/>
     </row>
     <row r="16" spans="3:9" x14ac:dyDescent="0.3">
-      <c r="C16" s="58" t="s">
+      <c r="C16" s="44" t="s">
         <v>14</v>
       </c>
       <c r="D16" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="E16" s="56"/>
+      <c r="E16" s="42"/>
       <c r="F16" s="9" t="s">
         <v>112</v>
       </c>
       <c r="G16" s="6" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="H16" s="26" t="s">
         <v>209</v>
@@ -1868,16 +1877,16 @@
       <c r="I16" s="4"/>
     </row>
     <row r="17" spans="3:9" x14ac:dyDescent="0.3">
-      <c r="C17" s="58"/>
+      <c r="C17" s="44"/>
       <c r="D17" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="E17" s="56"/>
+      <c r="E17" s="42"/>
       <c r="F17" s="9" t="s">
         <v>113</v>
       </c>
       <c r="G17" s="6" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="H17" s="26" t="s">
         <v>209</v>
@@ -1885,75 +1894,75 @@
       <c r="I17" s="4"/>
     </row>
     <row r="18" spans="3:9" ht="15.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C18" s="55" t="s">
+      <c r="C18" s="41" t="s">
         <v>114</v>
       </c>
       <c r="D18" s="7" t="s">
         <v>115</v>
       </c>
-      <c r="E18" s="56"/>
-      <c r="F18" s="55" t="s">
+      <c r="E18" s="42"/>
+      <c r="F18" s="41" t="s">
         <v>200</v>
       </c>
       <c r="G18" s="6" t="s">
-        <v>238</v>
-      </c>
-      <c r="H18" s="49" t="s">
-        <v>209</v>
-      </c>
-      <c r="I18" s="41"/>
+        <v>237</v>
+      </c>
+      <c r="H18" s="53" t="s">
+        <v>209</v>
+      </c>
+      <c r="I18" s="45"/>
     </row>
     <row r="19" spans="3:9" x14ac:dyDescent="0.3">
-      <c r="C19" s="56"/>
+      <c r="C19" s="42"/>
       <c r="D19" s="7" t="s">
         <v>116</v>
       </c>
-      <c r="E19" s="56"/>
-      <c r="F19" s="56"/>
+      <c r="E19" s="42"/>
+      <c r="F19" s="42"/>
       <c r="G19" s="6" t="s">
-        <v>236</v>
-      </c>
-      <c r="H19" s="50"/>
-      <c r="I19" s="43"/>
+        <v>235</v>
+      </c>
+      <c r="H19" s="54"/>
+      <c r="I19" s="47"/>
     </row>
     <row r="20" spans="3:9" x14ac:dyDescent="0.3">
-      <c r="C20" s="56"/>
+      <c r="C20" s="42"/>
       <c r="D20" s="7" t="s">
         <v>117</v>
       </c>
-      <c r="E20" s="56"/>
-      <c r="F20" s="56"/>
+      <c r="E20" s="42"/>
+      <c r="F20" s="42"/>
       <c r="G20" s="6" t="s">
-        <v>239</v>
-      </c>
-      <c r="H20" s="50"/>
-      <c r="I20" s="43"/>
+        <v>238</v>
+      </c>
+      <c r="H20" s="54"/>
+      <c r="I20" s="47"/>
     </row>
     <row r="21" spans="3:9" x14ac:dyDescent="0.3">
-      <c r="C21" s="56"/>
+      <c r="C21" s="42"/>
       <c r="D21" s="7" t="s">
         <v>118</v>
       </c>
-      <c r="E21" s="56"/>
-      <c r="F21" s="56"/>
+      <c r="E21" s="42"/>
+      <c r="F21" s="42"/>
       <c r="G21" s="6" t="s">
-        <v>237</v>
-      </c>
-      <c r="H21" s="50"/>
-      <c r="I21" s="43"/>
+        <v>236</v>
+      </c>
+      <c r="H21" s="54"/>
+      <c r="I21" s="47"/>
     </row>
     <row r="22" spans="3:9" x14ac:dyDescent="0.3">
-      <c r="C22" s="57"/>
+      <c r="C22" s="43"/>
       <c r="D22" s="7" t="s">
         <v>201</v>
       </c>
-      <c r="E22" s="56"/>
-      <c r="F22" s="57"/>
+      <c r="E22" s="42"/>
+      <c r="F22" s="43"/>
       <c r="G22" s="6" t="s">
-        <v>240</v>
-      </c>
-      <c r="H22" s="51"/>
-      <c r="I22" s="42"/>
+        <v>239</v>
+      </c>
+      <c r="H22" s="55"/>
+      <c r="I22" s="46"/>
     </row>
     <row r="23" spans="3:9" ht="30.15" x14ac:dyDescent="0.3">
       <c r="C23" s="3" t="s">
@@ -1962,12 +1971,12 @@
       <c r="D23" s="7" t="s">
         <v>62</v>
       </c>
-      <c r="E23" s="56"/>
+      <c r="E23" s="42"/>
       <c r="F23" s="9" t="s">
         <v>119</v>
       </c>
       <c r="G23" s="6" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="H23" s="26" t="s">
         <v>209</v>
@@ -1975,35 +1984,35 @@
       <c r="I23" s="4"/>
     </row>
     <row r="24" spans="3:9" x14ac:dyDescent="0.3">
-      <c r="C24" s="58" t="s">
+      <c r="C24" s="44" t="s">
         <v>120</v>
       </c>
       <c r="D24" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="E24" s="56"/>
+      <c r="E24" s="42"/>
       <c r="F24" s="12" t="s">
+        <v>218</v>
+      </c>
+      <c r="G24" s="6" t="s">
+        <v>244</v>
+      </c>
+      <c r="H24" s="26" t="s">
+        <v>209</v>
+      </c>
+      <c r="I24" s="4"/>
+    </row>
+    <row r="25" spans="3:9" ht="135.5" x14ac:dyDescent="0.3">
+      <c r="C25" s="44"/>
+      <c r="D25" s="7" t="s">
         <v>219</v>
       </c>
-      <c r="G24" s="6" t="s">
-        <v>245</v>
-      </c>
-      <c r="H24" s="26" t="s">
-        <v>209</v>
-      </c>
-      <c r="I24" s="4"/>
-    </row>
-    <row r="25" spans="3:9" ht="135.5" x14ac:dyDescent="0.3">
-      <c r="C25" s="58"/>
-      <c r="D25" s="7" t="s">
-        <v>220</v>
-      </c>
-      <c r="E25" s="56"/>
+      <c r="E25" s="42"/>
       <c r="F25" s="12" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="G25" s="6" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="H25" s="26" t="s">
         <v>209</v>
@@ -2011,16 +2020,16 @@
       <c r="I25" s="4"/>
     </row>
     <row r="26" spans="3:9" ht="45.2" x14ac:dyDescent="0.3">
-      <c r="C26" s="58"/>
+      <c r="C26" s="44"/>
       <c r="D26" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="E26" s="56"/>
+      <c r="E26" s="42"/>
       <c r="F26" s="12" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="G26" s="6" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="H26" s="26" t="s">
         <v>209</v>
@@ -2028,16 +2037,16 @@
       <c r="I26" s="4"/>
     </row>
     <row r="27" spans="3:9" ht="45.2" x14ac:dyDescent="0.3">
-      <c r="C27" s="58"/>
+      <c r="C27" s="44"/>
       <c r="D27" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="E27" s="57"/>
+      <c r="E27" s="43"/>
       <c r="F27" s="12" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="G27" s="6" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="H27" s="26" t="s">
         <v>209</v>
@@ -2045,81 +2054,81 @@
       <c r="I27" s="4"/>
     </row>
     <row r="28" spans="3:9" x14ac:dyDescent="0.3">
-      <c r="C28" s="58" t="s">
+      <c r="C28" s="44" t="s">
         <v>23</v>
       </c>
       <c r="D28" s="7" t="s">
         <v>21</v>
       </c>
       <c r="E28" s="5"/>
-      <c r="F28" s="44" t="s">
-        <v>214</v>
+      <c r="F28" s="48" t="s">
+        <v>213</v>
       </c>
       <c r="G28" s="35"/>
       <c r="H28" s="36"/>
       <c r="I28" s="37"/>
     </row>
     <row r="29" spans="3:9" x14ac:dyDescent="0.3">
-      <c r="C29" s="58"/>
+      <c r="C29" s="44"/>
       <c r="D29" s="7" t="s">
         <v>22</v>
       </c>
       <c r="E29" s="5"/>
-      <c r="F29" s="45"/>
+      <c r="F29" s="49"/>
       <c r="G29" s="35"/>
       <c r="H29" s="36"/>
       <c r="I29" s="37"/>
     </row>
     <row r="30" spans="3:9" x14ac:dyDescent="0.3">
-      <c r="C30" s="58" t="s">
+      <c r="C30" s="44" t="s">
         <v>24</v>
       </c>
       <c r="D30" s="7" t="s">
         <v>25</v>
       </c>
       <c r="E30" s="5"/>
-      <c r="F30" s="45"/>
+      <c r="F30" s="49"/>
       <c r="G30" s="35"/>
       <c r="H30" s="36"/>
       <c r="I30" s="37"/>
     </row>
     <row r="31" spans="3:9" x14ac:dyDescent="0.3">
-      <c r="C31" s="58"/>
+      <c r="C31" s="44"/>
       <c r="D31" s="7" t="s">
         <v>26</v>
       </c>
       <c r="E31" s="5"/>
-      <c r="F31" s="45"/>
+      <c r="F31" s="49"/>
       <c r="G31" s="35"/>
       <c r="H31" s="36"/>
       <c r="I31" s="37"/>
     </row>
     <row r="32" spans="3:9" x14ac:dyDescent="0.3">
-      <c r="C32" s="58"/>
+      <c r="C32" s="44"/>
       <c r="D32" s="7" t="s">
         <v>27</v>
       </c>
       <c r="E32" s="5"/>
-      <c r="F32" s="46"/>
+      <c r="F32" s="50"/>
       <c r="G32" s="35"/>
       <c r="H32" s="36"/>
       <c r="I32" s="37"/>
     </row>
     <row r="33" spans="3:9" ht="60.25" x14ac:dyDescent="0.3">
-      <c r="C33" s="55" t="s">
+      <c r="C33" s="41" t="s">
         <v>28</v>
       </c>
       <c r="D33" s="7" t="s">
         <v>125</v>
       </c>
-      <c r="E33" s="55" t="s">
+      <c r="E33" s="41" t="s">
         <v>122</v>
       </c>
       <c r="F33" s="21" t="s">
         <v>188</v>
       </c>
       <c r="G33" s="6" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="H33" s="26" t="s">
         <v>209</v>
@@ -2127,16 +2136,16 @@
       <c r="I33" s="4"/>
     </row>
     <row r="34" spans="3:9" ht="30.15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C34" s="56"/>
+      <c r="C34" s="42"/>
       <c r="D34" s="7">
         <v>10</v>
       </c>
-      <c r="E34" s="56"/>
+      <c r="E34" s="42"/>
       <c r="F34" s="18" t="s">
         <v>189</v>
       </c>
-      <c r="G34" s="52" t="s">
-        <v>246</v>
+      <c r="G34" s="56" t="s">
+        <v>245</v>
       </c>
       <c r="H34" s="26" t="s">
         <v>209</v>
@@ -2144,45 +2153,45 @@
       <c r="I34" s="4"/>
     </row>
     <row r="35" spans="3:9" ht="30.15" x14ac:dyDescent="0.3">
-      <c r="C35" s="56"/>
+      <c r="C35" s="42"/>
       <c r="D35" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="E35" s="56"/>
+      <c r="E35" s="42"/>
       <c r="F35" s="18" t="s">
         <v>190</v>
       </c>
-      <c r="G35" s="54"/>
+      <c r="G35" s="58"/>
       <c r="H35" s="26" t="s">
         <v>209</v>
       </c>
       <c r="I35" s="4"/>
     </row>
     <row r="36" spans="3:9" ht="30.15" x14ac:dyDescent="0.3">
-      <c r="C36" s="56"/>
+      <c r="C36" s="42"/>
       <c r="D36" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="E36" s="56"/>
+      <c r="E36" s="42"/>
       <c r="F36" s="18" t="s">
         <v>191</v>
       </c>
-      <c r="G36" s="54"/>
+      <c r="G36" s="58"/>
       <c r="H36" s="26" t="s">
         <v>209</v>
       </c>
       <c r="I36" s="4"/>
     </row>
     <row r="37" spans="3:9" x14ac:dyDescent="0.3">
-      <c r="C37" s="57"/>
+      <c r="C37" s="43"/>
       <c r="D37" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="E37" s="56"/>
+      <c r="E37" s="42"/>
       <c r="F37" s="18" t="s">
         <v>192</v>
       </c>
-      <c r="G37" s="53"/>
+      <c r="G37" s="57"/>
       <c r="H37" s="26" t="s">
         <v>209</v>
       </c>
@@ -2195,12 +2204,12 @@
       <c r="D38" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="E38" s="57"/>
+      <c r="E38" s="43"/>
       <c r="F38" s="12" t="s">
         <v>193</v>
       </c>
       <c r="G38" s="6" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="H38" s="26" t="s">
         <v>209</v>
@@ -2214,14 +2223,14 @@
       <c r="D39" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="E39" s="58" t="s">
+      <c r="E39" s="44" t="s">
         <v>123</v>
       </c>
       <c r="F39" s="12" t="s">
         <v>153</v>
       </c>
       <c r="G39" s="6" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="H39" s="26" t="s">
         <v>209</v>
@@ -2229,74 +2238,74 @@
       <c r="I39" s="4"/>
     </row>
     <row r="40" spans="3:9" ht="105.4" x14ac:dyDescent="0.3">
-      <c r="C40" s="58" t="s">
+      <c r="C40" s="44" t="s">
         <v>36</v>
       </c>
       <c r="D40" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="E40" s="58"/>
+      <c r="E40" s="44"/>
       <c r="F40" s="6" t="s">
-        <v>299</v>
-      </c>
-      <c r="G40" s="55" t="s">
+        <v>298</v>
+      </c>
+      <c r="G40" s="41" t="s">
         <v>36</v>
       </c>
-      <c r="H40" s="49" t="s">
+      <c r="H40" s="53" t="s">
         <v>209</v>
       </c>
       <c r="I40" s="4"/>
     </row>
     <row r="41" spans="3:9" ht="165.6" x14ac:dyDescent="0.3">
-      <c r="C41" s="58"/>
+      <c r="C41" s="44"/>
       <c r="D41" s="7" t="s">
         <v>38</v>
       </c>
-      <c r="E41" s="58"/>
+      <c r="E41" s="44"/>
       <c r="F41" s="6" t="s">
-        <v>300</v>
-      </c>
-      <c r="G41" s="56"/>
-      <c r="H41" s="50"/>
+        <v>299</v>
+      </c>
+      <c r="G41" s="42"/>
+      <c r="H41" s="54"/>
       <c r="I41" s="4"/>
     </row>
     <row r="42" spans="3:9" ht="60.25" x14ac:dyDescent="0.3">
-      <c r="C42" s="58"/>
+      <c r="C42" s="44"/>
       <c r="D42" s="7" t="s">
         <v>39</v>
       </c>
-      <c r="E42" s="58"/>
+      <c r="E42" s="44"/>
       <c r="F42" s="6" t="s">
-        <v>301</v>
-      </c>
-      <c r="G42" s="56"/>
-      <c r="H42" s="50"/>
+        <v>300</v>
+      </c>
+      <c r="G42" s="42"/>
+      <c r="H42" s="54"/>
       <c r="I42" s="4"/>
     </row>
     <row r="43" spans="3:9" ht="60.25" x14ac:dyDescent="0.3">
-      <c r="C43" s="58"/>
+      <c r="C43" s="44"/>
       <c r="D43" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="E43" s="58"/>
+      <c r="E43" s="44"/>
       <c r="F43" s="6" t="s">
-        <v>303</v>
-      </c>
-      <c r="G43" s="56"/>
-      <c r="H43" s="50"/>
+        <v>302</v>
+      </c>
+      <c r="G43" s="42"/>
+      <c r="H43" s="54"/>
       <c r="I43" s="4"/>
     </row>
     <row r="44" spans="3:9" x14ac:dyDescent="0.3">
-      <c r="C44" s="58"/>
+      <c r="C44" s="44"/>
       <c r="D44" s="7" t="s">
         <v>41</v>
       </c>
-      <c r="E44" s="58"/>
+      <c r="E44" s="44"/>
       <c r="F44" s="38" t="s">
-        <v>302</v>
-      </c>
-      <c r="G44" s="57"/>
-      <c r="H44" s="51"/>
+        <v>301</v>
+      </c>
+      <c r="G44" s="43"/>
+      <c r="H44" s="55"/>
       <c r="I44" s="4"/>
     </row>
     <row r="45" spans="3:9" ht="60.25" x14ac:dyDescent="0.3">
@@ -2306,12 +2315,12 @@
       <c r="D45" s="7" t="s">
         <v>43</v>
       </c>
-      <c r="E45" s="58"/>
+      <c r="E45" s="44"/>
       <c r="F45" s="24" t="s">
         <v>210</v>
       </c>
       <c r="G45" s="6" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="H45" s="26" t="s">
         <v>209</v>
@@ -2325,30 +2334,32 @@
       <c r="D46" s="7" t="s">
         <v>45</v>
       </c>
-      <c r="E46" s="58"/>
+      <c r="E46" s="44"/>
       <c r="F46" s="12" t="s">
         <v>211</v>
       </c>
       <c r="G46" s="6" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="H46" s="26" t="s">
         <v>209</v>
       </c>
       <c r="I46" s="4"/>
     </row>
-    <row r="47" spans="3:9" ht="60.25" x14ac:dyDescent="0.3">
+    <row r="47" spans="3:9" ht="90.35" x14ac:dyDescent="0.3">
       <c r="C47" s="3" t="s">
         <v>46</v>
       </c>
       <c r="D47" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="E47" s="58"/>
+      <c r="E47" s="44"/>
       <c r="F47" s="12" t="s">
-        <v>212</v>
-      </c>
-      <c r="G47" s="6"/>
+        <v>306</v>
+      </c>
+      <c r="G47" s="6" t="s">
+        <v>307</v>
+      </c>
       <c r="H47" s="26" t="s">
         <v>209</v>
       </c>
@@ -2361,11 +2372,13 @@
       <c r="D48" s="7" t="s">
         <v>49</v>
       </c>
-      <c r="E48" s="58"/>
+      <c r="E48" s="44"/>
       <c r="F48" s="12" t="s">
         <v>154</v>
       </c>
-      <c r="G48" s="6"/>
+      <c r="G48" s="6" t="s">
+        <v>308</v>
+      </c>
       <c r="H48" s="26" t="s">
         <v>209</v>
       </c>
@@ -2382,29 +2395,31 @@
         <v>199</v>
       </c>
       <c r="F49" s="12" t="s">
-        <v>213</v>
-      </c>
-      <c r="G49" s="6"/>
+        <v>212</v>
+      </c>
+      <c r="G49" s="6" t="s">
+        <v>309</v>
+      </c>
       <c r="H49" s="26" t="s">
         <v>209</v>
       </c>
       <c r="I49" s="4"/>
     </row>
     <row r="50" spans="3:9" ht="45.2" x14ac:dyDescent="0.3">
-      <c r="C50" s="55" t="s">
+      <c r="C50" s="41" t="s">
         <v>52</v>
       </c>
       <c r="D50" s="7" t="s">
         <v>127</v>
       </c>
-      <c r="E50" s="55" t="s">
+      <c r="E50" s="41" t="s">
         <v>122</v>
       </c>
       <c r="F50" s="19" t="s">
         <v>198</v>
       </c>
       <c r="G50" s="6" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="H50" s="26" t="s">
         <v>209</v>
@@ -2412,16 +2427,16 @@
       <c r="I50" s="4"/>
     </row>
     <row r="51" spans="3:9" ht="30.15" x14ac:dyDescent="0.3">
-      <c r="C51" s="57"/>
+      <c r="C51" s="43"/>
       <c r="D51" s="7" t="s">
         <v>53</v>
       </c>
-      <c r="E51" s="56"/>
+      <c r="E51" s="42"/>
       <c r="F51" s="19" t="s">
         <v>126</v>
       </c>
       <c r="G51" s="6" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="H51" s="26" t="s">
         <v>209</v>
@@ -2429,18 +2444,18 @@
       <c r="I51" s="4"/>
     </row>
     <row r="52" spans="3:9" ht="60.25" x14ac:dyDescent="0.3">
-      <c r="C52" s="55" t="s">
-        <v>222</v>
+      <c r="C52" s="41" t="s">
+        <v>221</v>
       </c>
       <c r="D52" s="7" t="s">
         <v>125</v>
       </c>
-      <c r="E52" s="56"/>
+      <c r="E52" s="42"/>
       <c r="F52" s="19" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="G52" s="6" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="H52" s="26" t="s">
         <v>209</v>
@@ -2448,16 +2463,16 @@
       <c r="I52" s="4"/>
     </row>
     <row r="53" spans="3:9" ht="60.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C53" s="56"/>
+      <c r="C53" s="42"/>
       <c r="D53" s="7" t="s">
         <v>54</v>
       </c>
-      <c r="E53" s="56"/>
+      <c r="E53" s="42"/>
       <c r="F53" s="23" t="s">
         <v>194</v>
       </c>
       <c r="G53" s="6" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="H53" s="26" t="s">
         <v>209</v>
@@ -2465,16 +2480,16 @@
       <c r="I53" s="4"/>
     </row>
     <row r="54" spans="3:9" ht="120.45" x14ac:dyDescent="0.3">
-      <c r="C54" s="56"/>
+      <c r="C54" s="42"/>
       <c r="D54" s="7" t="s">
         <v>55</v>
       </c>
-      <c r="E54" s="56"/>
+      <c r="E54" s="42"/>
       <c r="F54" s="23" t="s">
         <v>197</v>
       </c>
       <c r="G54" s="6" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="H54" s="26" t="s">
         <v>209</v>
@@ -2482,16 +2497,16 @@
       <c r="I54" s="4"/>
     </row>
     <row r="55" spans="3:9" ht="90.35" x14ac:dyDescent="0.3">
-      <c r="C55" s="56"/>
+      <c r="C55" s="42"/>
       <c r="D55" s="7" t="s">
         <v>56</v>
       </c>
-      <c r="E55" s="56"/>
+      <c r="E55" s="42"/>
       <c r="F55" s="23" t="s">
         <v>195</v>
       </c>
       <c r="G55" s="6" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="H55" s="26" t="s">
         <v>209</v>
@@ -2499,16 +2514,16 @@
       <c r="I55" s="4"/>
     </row>
     <row r="56" spans="3:9" ht="45.2" x14ac:dyDescent="0.3">
-      <c r="C56" s="57"/>
+      <c r="C56" s="43"/>
       <c r="D56" s="7" t="s">
         <v>69</v>
       </c>
-      <c r="E56" s="56"/>
+      <c r="E56" s="42"/>
       <c r="F56" s="12" t="s">
         <v>196</v>
       </c>
       <c r="G56" s="6" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="H56" s="26" t="s">
         <v>209</v>
@@ -2516,18 +2531,18 @@
       <c r="I56" s="4"/>
     </row>
     <row r="57" spans="3:9" ht="30.15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C57" s="58" t="s">
+      <c r="C57" s="44" t="s">
         <v>91</v>
       </c>
       <c r="D57" s="7" t="s">
         <v>57</v>
       </c>
-      <c r="E57" s="56"/>
+      <c r="E57" s="42"/>
       <c r="F57" s="9" t="s">
         <v>128</v>
       </c>
       <c r="G57" s="6" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="H57" s="26" t="s">
         <v>209</v>
@@ -2535,16 +2550,16 @@
       <c r="I57" s="4"/>
     </row>
     <row r="58" spans="3:9" x14ac:dyDescent="0.3">
-      <c r="C58" s="58"/>
+      <c r="C58" s="44"/>
       <c r="D58" s="7" t="s">
         <v>58</v>
       </c>
-      <c r="E58" s="56"/>
+      <c r="E58" s="42"/>
       <c r="F58" s="9" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="G58" s="6" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="H58" s="26" t="s">
         <v>209</v>
@@ -2552,16 +2567,16 @@
       <c r="I58" s="4"/>
     </row>
     <row r="59" spans="3:9" ht="52.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C59" s="58"/>
+      <c r="C59" s="44"/>
       <c r="D59" s="7" t="s">
         <v>59</v>
       </c>
-      <c r="E59" s="56"/>
+      <c r="E59" s="42"/>
       <c r="F59" s="9" t="s">
         <v>129</v>
       </c>
       <c r="G59" s="6" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="H59" s="26" t="s">
         <v>209</v>
@@ -2569,16 +2584,16 @@
       <c r="I59" s="4"/>
     </row>
     <row r="60" spans="3:9" ht="30.15" x14ac:dyDescent="0.3">
-      <c r="C60" s="58"/>
+      <c r="C60" s="44"/>
       <c r="D60" s="7" t="s">
         <v>60</v>
       </c>
-      <c r="E60" s="57"/>
+      <c r="E60" s="43"/>
       <c r="F60" s="9" t="s">
         <v>130</v>
       </c>
       <c r="G60" s="6" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="H60" s="26" t="s">
         <v>209</v>
@@ -2601,20 +2616,20 @@
       <c r="I61" s="37"/>
     </row>
     <row r="62" spans="3:9" ht="30.15" x14ac:dyDescent="0.3">
-      <c r="C62" s="58" t="s">
+      <c r="C62" s="44" t="s">
         <v>64</v>
       </c>
       <c r="D62" s="7" t="s">
         <v>65</v>
       </c>
-      <c r="E62" s="55" t="s">
+      <c r="E62" s="41" t="s">
         <v>122</v>
       </c>
       <c r="F62" s="9" t="s">
         <v>202</v>
       </c>
       <c r="G62" s="6" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="H62" s="26" t="s">
         <v>209</v>
@@ -2622,16 +2637,16 @@
       <c r="I62" s="4"/>
     </row>
     <row r="63" spans="3:9" ht="60.25" x14ac:dyDescent="0.3">
-      <c r="C63" s="58"/>
+      <c r="C63" s="44"/>
       <c r="D63" s="7" t="s">
         <v>66</v>
       </c>
-      <c r="E63" s="56"/>
+      <c r="E63" s="42"/>
       <c r="F63" s="9" t="s">
         <v>203</v>
       </c>
       <c r="G63" s="6" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="H63" s="26" t="s">
         <v>209</v>
@@ -2639,16 +2654,16 @@
       <c r="I63" s="4"/>
     </row>
     <row r="64" spans="3:9" ht="60.25" x14ac:dyDescent="0.3">
-      <c r="C64" s="58"/>
+      <c r="C64" s="44"/>
       <c r="D64" s="7" t="s">
         <v>67</v>
       </c>
-      <c r="E64" s="56"/>
+      <c r="E64" s="42"/>
       <c r="F64" s="9" t="s">
         <v>204</v>
       </c>
       <c r="G64" s="6" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="H64" s="26" t="s">
         <v>209</v>
@@ -2656,16 +2671,16 @@
       <c r="I64" s="4"/>
     </row>
     <row r="65" spans="3:9" ht="30.15" x14ac:dyDescent="0.3">
-      <c r="C65" s="58"/>
+      <c r="C65" s="44"/>
       <c r="D65" s="7" t="s">
         <v>68</v>
       </c>
-      <c r="E65" s="56"/>
+      <c r="E65" s="42"/>
       <c r="F65" s="9" t="s">
         <v>205</v>
       </c>
       <c r="G65" s="6" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="H65" s="26" t="s">
         <v>209</v>
@@ -2673,16 +2688,16 @@
       <c r="I65" s="4"/>
     </row>
     <row r="66" spans="3:9" ht="60.25" x14ac:dyDescent="0.3">
-      <c r="C66" s="58"/>
+      <c r="C66" s="44"/>
       <c r="D66" s="7" t="s">
         <v>132</v>
       </c>
-      <c r="E66" s="56"/>
+      <c r="E66" s="42"/>
       <c r="F66" s="9" t="s">
         <v>206</v>
       </c>
       <c r="G66" s="6" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="H66" s="26" t="s">
         <v>209</v>
@@ -2690,16 +2705,16 @@
       <c r="I66" s="4"/>
     </row>
     <row r="67" spans="3:9" ht="120.45" x14ac:dyDescent="0.3">
-      <c r="C67" s="58"/>
+      <c r="C67" s="44"/>
       <c r="D67" s="2" t="s">
         <v>133</v>
       </c>
-      <c r="E67" s="56"/>
+      <c r="E67" s="42"/>
       <c r="F67" s="9" t="s">
         <v>207</v>
       </c>
       <c r="G67" s="6" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="H67" s="26" t="s">
         <v>209</v>
@@ -2713,12 +2728,12 @@
       <c r="D68" s="7" t="s">
         <v>71</v>
       </c>
-      <c r="E68" s="56"/>
+      <c r="E68" s="42"/>
       <c r="F68" s="24" t="s">
         <v>208</v>
       </c>
       <c r="G68" s="6" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="H68" s="26" t="s">
         <v>209</v>
@@ -2726,18 +2741,18 @@
       <c r="I68" s="4"/>
     </row>
     <row r="69" spans="3:9" ht="30.15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C69" s="58" t="s">
+      <c r="C69" s="44" t="s">
         <v>72</v>
       </c>
       <c r="D69" s="7" t="s">
         <v>73</v>
       </c>
-      <c r="E69" s="56"/>
+      <c r="E69" s="42"/>
       <c r="F69" s="9" t="s">
         <v>134</v>
       </c>
       <c r="G69" s="6" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="H69" s="26" t="s">
         <v>209</v>
@@ -2745,16 +2760,16 @@
       <c r="I69" s="4"/>
     </row>
     <row r="70" spans="3:9" ht="30.15" x14ac:dyDescent="0.3">
-      <c r="C70" s="58"/>
+      <c r="C70" s="44"/>
       <c r="D70" s="7" t="s">
         <v>74</v>
       </c>
-      <c r="E70" s="56"/>
+      <c r="E70" s="42"/>
       <c r="F70" s="9" t="s">
         <v>140</v>
       </c>
       <c r="G70" s="6" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="H70" s="26" t="s">
         <v>209</v>
@@ -2762,16 +2777,16 @@
       <c r="I70" s="4"/>
     </row>
     <row r="71" spans="3:9" x14ac:dyDescent="0.3">
-      <c r="C71" s="58"/>
+      <c r="C71" s="44"/>
       <c r="D71" s="7" t="s">
         <v>75</v>
       </c>
-      <c r="E71" s="56"/>
+      <c r="E71" s="42"/>
       <c r="F71" s="9" t="s">
         <v>136</v>
       </c>
       <c r="G71" s="6" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="H71" s="26" t="s">
         <v>209</v>
@@ -2779,16 +2794,16 @@
       <c r="I71" s="4"/>
     </row>
     <row r="72" spans="3:9" ht="30.15" x14ac:dyDescent="0.3">
-      <c r="C72" s="58"/>
+      <c r="C72" s="44"/>
       <c r="D72" s="7" t="s">
-        <v>217</v>
-      </c>
-      <c r="E72" s="56"/>
+        <v>216</v>
+      </c>
+      <c r="E72" s="42"/>
       <c r="F72" s="12" t="s">
         <v>162</v>
       </c>
       <c r="G72" s="6" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="H72" s="26" t="s">
         <v>209</v>
@@ -2796,16 +2811,16 @@
       <c r="I72" s="4"/>
     </row>
     <row r="73" spans="3:9" x14ac:dyDescent="0.3">
-      <c r="C73" s="58"/>
+      <c r="C73" s="44"/>
       <c r="D73" s="7" t="s">
         <v>76</v>
       </c>
-      <c r="E73" s="56"/>
+      <c r="E73" s="42"/>
       <c r="F73" s="9" t="s">
         <v>137</v>
       </c>
       <c r="G73" s="6" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="H73" s="26" t="s">
         <v>209</v>
@@ -2813,16 +2828,16 @@
       <c r="I73" s="4"/>
     </row>
     <row r="74" spans="3:9" x14ac:dyDescent="0.3">
-      <c r="C74" s="58"/>
+      <c r="C74" s="44"/>
       <c r="D74" s="7" t="s">
         <v>77</v>
       </c>
-      <c r="E74" s="56"/>
+      <c r="E74" s="42"/>
       <c r="F74" s="9" t="s">
         <v>135</v>
       </c>
       <c r="G74" s="6" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="H74" s="26" t="s">
         <v>209</v>
@@ -2830,16 +2845,16 @@
       <c r="I74" s="4"/>
     </row>
     <row r="75" spans="3:9" x14ac:dyDescent="0.3">
-      <c r="C75" s="58"/>
+      <c r="C75" s="44"/>
       <c r="D75" s="7" t="s">
         <v>78</v>
       </c>
-      <c r="E75" s="56"/>
+      <c r="E75" s="42"/>
       <c r="F75" s="9" t="s">
         <v>139</v>
       </c>
       <c r="G75" s="6" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="H75" s="26" t="s">
         <v>209</v>
@@ -2847,16 +2862,16 @@
       <c r="I75" s="4"/>
     </row>
     <row r="76" spans="3:9" x14ac:dyDescent="0.3">
-      <c r="C76" s="58"/>
+      <c r="C76" s="44"/>
       <c r="D76" s="7" t="s">
         <v>79</v>
       </c>
-      <c r="E76" s="56"/>
+      <c r="E76" s="42"/>
       <c r="F76" s="9" t="s">
         <v>138</v>
       </c>
       <c r="G76" s="6" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="H76" s="26" t="s">
         <v>209</v>
@@ -2864,16 +2879,16 @@
       <c r="I76" s="4"/>
     </row>
     <row r="77" spans="3:9" ht="30.15" x14ac:dyDescent="0.3">
-      <c r="C77" s="58"/>
+      <c r="C77" s="44"/>
       <c r="D77" s="7" t="s">
         <v>80</v>
       </c>
-      <c r="E77" s="56"/>
+      <c r="E77" s="42"/>
       <c r="F77" s="12" t="s">
         <v>187</v>
       </c>
       <c r="G77" s="6" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="H77" s="26" t="s">
         <v>209</v>
@@ -2881,11 +2896,11 @@
       <c r="I77" s="4"/>
     </row>
     <row r="78" spans="3:9" ht="30.15" x14ac:dyDescent="0.3">
-      <c r="C78" s="58"/>
+      <c r="C78" s="44"/>
       <c r="D78" s="7" t="s">
         <v>81</v>
       </c>
-      <c r="E78" s="56"/>
+      <c r="E78" s="42"/>
       <c r="F78" s="25" t="s">
         <v>141</v>
       </c>
@@ -2894,18 +2909,18 @@
       <c r="I78" s="34"/>
     </row>
     <row r="79" spans="3:9" ht="30.15" x14ac:dyDescent="0.3">
-      <c r="C79" s="56" t="s">
+      <c r="C79" s="42" t="s">
         <v>83</v>
       </c>
       <c r="D79" s="7" t="s">
         <v>142</v>
       </c>
-      <c r="E79" s="56"/>
+      <c r="E79" s="42"/>
       <c r="F79" s="9" t="s">
         <v>163</v>
       </c>
       <c r="G79" s="6" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="H79" s="26" t="s">
         <v>209</v>
@@ -2913,16 +2928,16 @@
       <c r="I79" s="4"/>
     </row>
     <row r="80" spans="3:9" ht="30.15" x14ac:dyDescent="0.3">
-      <c r="C80" s="56"/>
+      <c r="C80" s="42"/>
       <c r="D80" s="7" t="s">
         <v>82</v>
       </c>
-      <c r="E80" s="56"/>
+      <c r="E80" s="42"/>
       <c r="F80" s="9" t="s">
         <v>164</v>
       </c>
       <c r="G80" s="6" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="H80" s="26" t="s">
         <v>209</v>
@@ -2930,18 +2945,18 @@
       <c r="I80" s="4"/>
     </row>
     <row r="81" spans="3:9" ht="30.15" x14ac:dyDescent="0.3">
-      <c r="C81" s="55" t="s">
+      <c r="C81" s="41" t="s">
         <v>84</v>
       </c>
       <c r="D81" s="7" t="s">
         <v>145</v>
       </c>
-      <c r="E81" s="56"/>
+      <c r="E81" s="42"/>
       <c r="F81" s="9" t="s">
         <v>165</v>
       </c>
       <c r="G81" s="6" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="H81" s="26" t="s">
         <v>209</v>
@@ -2949,16 +2964,16 @@
       <c r="I81" s="4"/>
     </row>
     <row r="82" spans="3:9" ht="69.400000000000006" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C82" s="56"/>
+      <c r="C82" s="42"/>
       <c r="D82" s="7" t="s">
         <v>146</v>
       </c>
-      <c r="E82" s="56"/>
+      <c r="E82" s="42"/>
       <c r="F82" s="9" t="s">
         <v>179</v>
       </c>
       <c r="G82" s="6" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="H82" s="26" t="s">
         <v>209</v>
@@ -2966,11 +2981,11 @@
       <c r="I82" s="4"/>
     </row>
     <row r="83" spans="3:9" x14ac:dyDescent="0.3">
-      <c r="C83" s="56"/>
+      <c r="C83" s="42"/>
       <c r="D83" s="7" t="s">
         <v>85</v>
       </c>
-      <c r="E83" s="56"/>
+      <c r="E83" s="42"/>
       <c r="F83" s="25" t="s">
         <v>141</v>
       </c>
@@ -2979,16 +2994,16 @@
       <c r="I83" s="34"/>
     </row>
     <row r="84" spans="3:9" x14ac:dyDescent="0.3">
-      <c r="C84" s="56"/>
+      <c r="C84" s="42"/>
       <c r="D84" s="7" t="s">
         <v>86</v>
       </c>
-      <c r="E84" s="56"/>
+      <c r="E84" s="42"/>
       <c r="F84" s="9" t="s">
         <v>166</v>
       </c>
       <c r="G84" s="6" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="H84" s="26" t="s">
         <v>209</v>
@@ -2996,16 +3011,16 @@
       <c r="I84" s="4"/>
     </row>
     <row r="85" spans="3:9" ht="30.15" x14ac:dyDescent="0.3">
-      <c r="C85" s="56"/>
+      <c r="C85" s="42"/>
       <c r="D85" s="7" t="s">
         <v>87</v>
       </c>
-      <c r="E85" s="56"/>
+      <c r="E85" s="42"/>
       <c r="F85" s="9" t="s">
         <v>167</v>
       </c>
       <c r="G85" s="6" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="H85" s="26" t="s">
         <v>209</v>
@@ -3013,16 +3028,16 @@
       <c r="I85" s="4"/>
     </row>
     <row r="86" spans="3:9" ht="30.15" x14ac:dyDescent="0.3">
-      <c r="C86" s="56"/>
+      <c r="C86" s="42"/>
       <c r="D86" s="7" t="s">
         <v>88</v>
       </c>
-      <c r="E86" s="56"/>
+      <c r="E86" s="42"/>
       <c r="F86" s="9" t="s">
         <v>168</v>
       </c>
       <c r="G86" s="6" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="H86" s="26" t="s">
         <v>209</v>
@@ -3030,16 +3045,16 @@
       <c r="I86" s="4"/>
     </row>
     <row r="87" spans="3:9" x14ac:dyDescent="0.3">
-      <c r="C87" s="56"/>
+      <c r="C87" s="42"/>
       <c r="D87" s="7" t="s">
         <v>89</v>
       </c>
-      <c r="E87" s="56"/>
+      <c r="E87" s="42"/>
       <c r="F87" s="9" t="s">
         <v>169</v>
       </c>
       <c r="G87" s="6" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="H87" s="26" t="s">
         <v>209</v>
@@ -3047,16 +3062,16 @@
       <c r="I87" s="4"/>
     </row>
     <row r="88" spans="3:9" x14ac:dyDescent="0.3">
-      <c r="C88" s="56"/>
+      <c r="C88" s="42"/>
       <c r="D88" s="7" t="s">
         <v>90</v>
       </c>
-      <c r="E88" s="56"/>
+      <c r="E88" s="42"/>
       <c r="F88" s="9" t="s">
         <v>170</v>
       </c>
       <c r="G88" s="6" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="H88" s="26" t="s">
         <v>209</v>
@@ -3064,31 +3079,31 @@
       <c r="I88" s="4"/>
     </row>
     <row r="89" spans="3:9" ht="30.15" x14ac:dyDescent="0.3">
-      <c r="C89" s="56"/>
+      <c r="C89" s="42"/>
       <c r="D89" s="7" t="s">
         <v>97</v>
       </c>
-      <c r="E89" s="56"/>
+      <c r="E89" s="42"/>
       <c r="F89" s="12" t="s">
+        <v>282</v>
+      </c>
+      <c r="G89" s="23" t="s">
         <v>283</v>
-      </c>
-      <c r="G89" s="23" t="s">
-        <v>284</v>
       </c>
       <c r="H89" s="39"/>
       <c r="I89" s="40"/>
     </row>
     <row r="90" spans="3:9" x14ac:dyDescent="0.3">
-      <c r="C90" s="56"/>
+      <c r="C90" s="42"/>
       <c r="D90" s="7" t="s">
         <v>98</v>
       </c>
-      <c r="E90" s="56"/>
+      <c r="E90" s="42"/>
       <c r="F90" s="9" t="s">
         <v>171</v>
       </c>
       <c r="G90" s="6" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="H90" s="26" t="s">
         <v>209</v>
@@ -3096,16 +3111,16 @@
       <c r="I90" s="4"/>
     </row>
     <row r="91" spans="3:9" x14ac:dyDescent="0.3">
-      <c r="C91" s="56"/>
+      <c r="C91" s="42"/>
       <c r="D91" s="7" t="s">
         <v>99</v>
       </c>
-      <c r="E91" s="56"/>
+      <c r="E91" s="42"/>
       <c r="F91" s="9" t="s">
         <v>172</v>
       </c>
       <c r="G91" s="6" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="H91" s="26" t="s">
         <v>209</v>
@@ -3113,16 +3128,16 @@
       <c r="I91" s="4"/>
     </row>
     <row r="92" spans="3:9" ht="30.15" x14ac:dyDescent="0.3">
-      <c r="C92" s="56"/>
+      <c r="C92" s="42"/>
       <c r="D92" s="7" t="s">
         <v>100</v>
       </c>
-      <c r="E92" s="56"/>
+      <c r="E92" s="42"/>
       <c r="F92" s="9" t="s">
         <v>173</v>
       </c>
       <c r="G92" s="6" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="H92" s="26" t="s">
         <v>209</v>
@@ -3130,16 +3145,16 @@
       <c r="I92" s="4"/>
     </row>
     <row r="93" spans="3:9" ht="45.2" x14ac:dyDescent="0.3">
-      <c r="C93" s="56"/>
+      <c r="C93" s="42"/>
       <c r="D93" s="7" t="s">
         <v>144</v>
       </c>
-      <c r="E93" s="56"/>
+      <c r="E93" s="42"/>
       <c r="F93" s="9" t="s">
         <v>174</v>
       </c>
       <c r="G93" s="6" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="H93" s="26" t="s">
         <v>209</v>
@@ -3147,18 +3162,18 @@
       <c r="I93" s="4"/>
     </row>
     <row r="94" spans="3:9" x14ac:dyDescent="0.3">
-      <c r="C94" s="55" t="s">
+      <c r="C94" s="41" t="s">
         <v>92</v>
       </c>
       <c r="D94" s="7" t="s">
         <v>93</v>
       </c>
-      <c r="E94" s="56"/>
+      <c r="E94" s="42"/>
       <c r="F94" s="9" t="s">
         <v>175</v>
       </c>
       <c r="G94" s="6" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="H94" s="26" t="s">
         <v>209</v>
@@ -3166,16 +3181,16 @@
       <c r="I94" s="4"/>
     </row>
     <row r="95" spans="3:9" ht="30.15" x14ac:dyDescent="0.3">
-      <c r="C95" s="56"/>
+      <c r="C95" s="42"/>
       <c r="D95" s="7" t="s">
         <v>94</v>
       </c>
-      <c r="E95" s="56"/>
+      <c r="E95" s="42"/>
       <c r="F95" s="9" t="s">
         <v>176</v>
       </c>
       <c r="G95" s="6" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="H95" s="26" t="s">
         <v>209</v>
@@ -3183,11 +3198,11 @@
       <c r="I95" s="4"/>
     </row>
     <row r="96" spans="3:9" x14ac:dyDescent="0.3">
-      <c r="C96" s="56"/>
+      <c r="C96" s="42"/>
       <c r="D96" s="7" t="s">
         <v>95</v>
       </c>
-      <c r="E96" s="56"/>
+      <c r="E96" s="42"/>
       <c r="F96" s="28" t="s">
         <v>141</v>
       </c>
@@ -3196,16 +3211,16 @@
       <c r="I96" s="31"/>
     </row>
     <row r="97" spans="3:9" x14ac:dyDescent="0.3">
-      <c r="C97" s="56"/>
+      <c r="C97" s="42"/>
       <c r="D97" s="7" t="s">
         <v>96</v>
       </c>
-      <c r="E97" s="56"/>
+      <c r="E97" s="42"/>
       <c r="F97" s="9" t="s">
         <v>177</v>
       </c>
       <c r="G97" s="6" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="H97" s="26" t="s">
         <v>209</v>
@@ -3213,16 +3228,16 @@
       <c r="I97" s="4"/>
     </row>
     <row r="98" spans="3:9" x14ac:dyDescent="0.3">
-      <c r="C98" s="56"/>
+      <c r="C98" s="42"/>
       <c r="D98" s="7" t="s">
         <v>143</v>
       </c>
-      <c r="E98" s="56"/>
+      <c r="E98" s="42"/>
       <c r="F98" s="9" t="s">
         <v>178</v>
       </c>
       <c r="G98" s="6" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="H98" s="26" t="s">
         <v>209</v>
@@ -3230,18 +3245,18 @@
       <c r="I98" s="4"/>
     </row>
     <row r="99" spans="3:9" x14ac:dyDescent="0.3">
-      <c r="C99" s="58" t="s">
+      <c r="C99" s="44" t="s">
         <v>107</v>
       </c>
       <c r="D99" s="7" t="s">
         <v>101</v>
       </c>
-      <c r="E99" s="56"/>
+      <c r="E99" s="42"/>
       <c r="F99" s="9" t="s">
         <v>148</v>
       </c>
       <c r="G99" s="6" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="H99" s="26" t="s">
         <v>209</v>
@@ -3249,16 +3264,16 @@
       <c r="I99" s="4"/>
     </row>
     <row r="100" spans="3:9" ht="30.15" x14ac:dyDescent="0.3">
-      <c r="C100" s="58"/>
+      <c r="C100" s="44"/>
       <c r="D100" s="7" t="s">
         <v>102</v>
       </c>
-      <c r="E100" s="56"/>
+      <c r="E100" s="42"/>
       <c r="F100" s="9" t="s">
         <v>147</v>
       </c>
       <c r="G100" s="6" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="H100" s="26" t="s">
         <v>209</v>
@@ -3266,16 +3281,16 @@
       <c r="I100" s="4"/>
     </row>
     <row r="101" spans="3:9" x14ac:dyDescent="0.3">
-      <c r="C101" s="58"/>
+      <c r="C101" s="44"/>
       <c r="D101" s="7" t="s">
         <v>103</v>
       </c>
-      <c r="E101" s="56"/>
+      <c r="E101" s="42"/>
       <c r="F101" s="9" t="s">
         <v>150</v>
       </c>
       <c r="G101" s="6" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="H101" s="26" t="s">
         <v>209</v>
@@ -3283,16 +3298,16 @@
       <c r="I101" s="4"/>
     </row>
     <row r="102" spans="3:9" ht="30.15" x14ac:dyDescent="0.3">
-      <c r="C102" s="58"/>
+      <c r="C102" s="44"/>
       <c r="D102" s="7" t="s">
         <v>104</v>
       </c>
-      <c r="E102" s="56"/>
+      <c r="E102" s="42"/>
       <c r="F102" s="9" t="s">
         <v>149</v>
       </c>
       <c r="G102" s="6" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="H102" s="26" t="s">
         <v>209</v>
@@ -3300,16 +3315,16 @@
       <c r="I102" s="4"/>
     </row>
     <row r="103" spans="3:9" x14ac:dyDescent="0.3">
-      <c r="C103" s="58"/>
+      <c r="C103" s="44"/>
       <c r="D103" s="7" t="s">
         <v>105</v>
       </c>
-      <c r="E103" s="56"/>
+      <c r="E103" s="42"/>
       <c r="F103" s="9" t="s">
         <v>151</v>
       </c>
       <c r="G103" s="6" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="H103" s="26" t="s">
         <v>209</v>
@@ -3317,16 +3332,16 @@
       <c r="I103" s="4"/>
     </row>
     <row r="104" spans="3:9" ht="30.15" x14ac:dyDescent="0.3">
-      <c r="C104" s="58"/>
+      <c r="C104" s="44"/>
       <c r="D104" s="8" t="s">
         <v>106</v>
       </c>
-      <c r="E104" s="57"/>
+      <c r="E104" s="43"/>
       <c r="F104" s="9" t="s">
         <v>152</v>
       </c>
       <c r="G104" s="6" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="H104" s="26" t="s">
         <v>209</v>
@@ -3344,17 +3359,16 @@
     </row>
   </sheetData>
   <mergeCells count="34">
-    <mergeCell ref="E50:E60"/>
-    <mergeCell ref="E62:E104"/>
-    <mergeCell ref="C69:C78"/>
-    <mergeCell ref="C79:C80"/>
-    <mergeCell ref="C81:C93"/>
-    <mergeCell ref="C94:C98"/>
-    <mergeCell ref="C99:C104"/>
-    <mergeCell ref="C62:C67"/>
-    <mergeCell ref="C57:C60"/>
-    <mergeCell ref="C50:C51"/>
-    <mergeCell ref="C52:C56"/>
+    <mergeCell ref="I6:I7"/>
+    <mergeCell ref="I18:I22"/>
+    <mergeCell ref="F28:F32"/>
+    <mergeCell ref="F6:F7"/>
+    <mergeCell ref="H40:H44"/>
+    <mergeCell ref="H6:H7"/>
+    <mergeCell ref="H18:H22"/>
+    <mergeCell ref="G6:G7"/>
+    <mergeCell ref="G34:G37"/>
+    <mergeCell ref="G40:G44"/>
     <mergeCell ref="E3:E27"/>
     <mergeCell ref="E33:E38"/>
     <mergeCell ref="E39:E48"/>
@@ -3368,16 +3382,17 @@
     <mergeCell ref="C24:C27"/>
     <mergeCell ref="C28:C29"/>
     <mergeCell ref="C18:C22"/>
-    <mergeCell ref="I6:I7"/>
-    <mergeCell ref="I18:I22"/>
-    <mergeCell ref="F28:F32"/>
-    <mergeCell ref="F6:F7"/>
-    <mergeCell ref="H40:H44"/>
-    <mergeCell ref="H6:H7"/>
-    <mergeCell ref="H18:H22"/>
-    <mergeCell ref="G6:G7"/>
-    <mergeCell ref="G34:G37"/>
-    <mergeCell ref="G40:G44"/>
+    <mergeCell ref="E50:E60"/>
+    <mergeCell ref="E62:E104"/>
+    <mergeCell ref="C69:C78"/>
+    <mergeCell ref="C79:C80"/>
+    <mergeCell ref="C81:C93"/>
+    <mergeCell ref="C94:C98"/>
+    <mergeCell ref="C99:C104"/>
+    <mergeCell ref="C62:C67"/>
+    <mergeCell ref="C57:C60"/>
+    <mergeCell ref="C50:C51"/>
+    <mergeCell ref="C52:C56"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
almost ready to create first output
</commit_message>
<xml_diff>
--- a/edit_eam/crosscheck.xlsx
+++ b/edit_eam/crosscheck.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="403" uniqueCount="310">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="406" uniqueCount="313">
   <si>
     <t>Nombre</t>
   </si>
@@ -409,9 +409,6 @@
     <t>IV4R3C3/Total</t>
   </si>
   <si>
-    <t>No se puede desagregar x trabajador. Mas bien =1 si emplea mujeres? O Hacer ratio de mujeres en cada division</t>
-  </si>
-  <si>
     <t>Otras Empresas</t>
   </si>
   <si>
@@ -655,9 +652,6 @@
     <t>ACTI2017 == II1R10C1,     ACTI2018 == II1R10C2,                   VA17 == VALAGRI17,       VA18 == VALAGRI18</t>
   </si>
   <si>
-    <t>VIII1R1C1 != 3 es la mas similar pero no discrimina por nacion/tipo</t>
-  </si>
-  <si>
     <t>V3R4C8 == 1 | V3R2C8 == 1 | V3R1C8 == 1</t>
   </si>
   <si>
@@ -904,9 +898,6 @@
     <t>obsTecnica</t>
   </si>
   <si>
-    <t>obsImitacion</t>
-  </si>
-  <si>
     <t>obsRentabilidad</t>
   </si>
   <si>
@@ -944,6 +935,24 @@
   </si>
   <si>
     <t>inversion2017, inversion2018</t>
+  </si>
+  <si>
+    <t xml:space="preserve">VIII1R1C1 != 3 </t>
+  </si>
+  <si>
+    <t>propietarioActual</t>
+  </si>
+  <si>
+    <t>IV4R11C2 &gt; 0</t>
+  </si>
+  <si>
+    <t>hayMujeres</t>
+  </si>
+  <si>
+    <t>region</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
   </si>
 </sst>
 </file>
@@ -980,18 +989,12 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -1127,7 +1130,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="59">
+  <cellXfs count="61">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1154,112 +1157,126 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1269,29 +1286,23 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1599,40 +1610,40 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="C2:I107"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C46" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G50" sqref="G50"/>
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D107" sqref="D107"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="15.05" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="3" max="3" width="23.21875" style="1" customWidth="1"/>
     <col min="4" max="4" width="20.77734375" style="2" customWidth="1"/>
-    <col min="5" max="5" width="14" style="13" customWidth="1"/>
+    <col min="5" max="5" width="14" style="12" customWidth="1"/>
     <col min="6" max="6" width="15.21875" style="1" customWidth="1"/>
     <col min="7" max="7" width="19.88671875" style="1" customWidth="1"/>
-    <col min="8" max="8" width="8.88671875" style="27"/>
+    <col min="8" max="8" width="8.88671875" style="26"/>
   </cols>
   <sheetData>
     <row r="2" spans="3:9" ht="26.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C2" s="14" t="s">
+      <c r="C2" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="D2" s="15" t="s">
+      <c r="D2" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="E2" s="14" t="s">
+      <c r="E2" s="13" t="s">
         <v>121</v>
       </c>
-      <c r="F2" s="16" t="s">
+      <c r="F2" s="15" t="s">
         <v>1</v>
       </c>
-      <c r="G2" s="14" t="s">
+      <c r="G2" s="13" t="s">
         <v>124</v>
       </c>
-      <c r="H2" s="17" t="s">
+      <c r="H2" s="16" t="s">
         <v>2</v>
       </c>
-      <c r="I2" s="17" t="s">
+      <c r="I2" s="16" t="s">
         <v>3</v>
       </c>
     </row>
@@ -1643,7 +1654,7 @@
       <c r="D3" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="E3" s="41" t="s">
+      <c r="E3" s="48" t="s">
         <v>122</v>
       </c>
       <c r="F3" s="9" t="s">
@@ -1652,8 +1663,8 @@
       <c r="G3" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="H3" s="26" t="s">
-        <v>209</v>
+      <c r="H3" s="25" t="s">
+        <v>208</v>
       </c>
       <c r="I3" s="4"/>
     </row>
@@ -1664,305 +1675,305 @@
       <c r="D4" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="E4" s="42"/>
-      <c r="F4" s="12" t="s">
+      <c r="E4" s="49"/>
+      <c r="F4" s="11" t="s">
         <v>108</v>
       </c>
       <c r="G4" s="6"/>
-      <c r="H4" s="26"/>
+      <c r="H4" s="25"/>
       <c r="I4" s="4"/>
     </row>
     <row r="5" spans="3:9" x14ac:dyDescent="0.3">
-      <c r="C5" s="44" t="s">
+      <c r="C5" s="51" t="s">
         <v>7</v>
       </c>
       <c r="D5" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="E5" s="42"/>
+      <c r="E5" s="49"/>
       <c r="F5" s="9" t="s">
         <v>109</v>
       </c>
       <c r="G5" s="6" t="s">
-        <v>223</v>
-      </c>
-      <c r="H5" s="26" t="s">
-        <v>209</v>
+        <v>221</v>
+      </c>
+      <c r="H5" s="25" t="s">
+        <v>208</v>
       </c>
       <c r="I5" s="4"/>
     </row>
     <row r="6" spans="3:9" x14ac:dyDescent="0.3">
-      <c r="C6" s="44"/>
+      <c r="C6" s="51"/>
       <c r="D6" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="E6" s="42"/>
-      <c r="F6" s="51" t="s">
+      <c r="E6" s="49"/>
+      <c r="F6" s="40" t="s">
         <v>111</v>
       </c>
-      <c r="G6" s="56" t="s">
-        <v>224</v>
-      </c>
-      <c r="H6" s="53" t="s">
-        <v>209</v>
-      </c>
-      <c r="I6" s="45"/>
+      <c r="G6" s="45" t="s">
+        <v>222</v>
+      </c>
+      <c r="H6" s="42" t="s">
+        <v>208</v>
+      </c>
+      <c r="I6" s="37"/>
     </row>
     <row r="7" spans="3:9" x14ac:dyDescent="0.3">
-      <c r="C7" s="44"/>
+      <c r="C7" s="51"/>
       <c r="D7" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="E7" s="42"/>
-      <c r="F7" s="52"/>
-      <c r="G7" s="57"/>
-      <c r="H7" s="55"/>
-      <c r="I7" s="46"/>
+      <c r="E7" s="49"/>
+      <c r="F7" s="41"/>
+      <c r="G7" s="46"/>
+      <c r="H7" s="44"/>
+      <c r="I7" s="38"/>
     </row>
     <row r="8" spans="3:9" x14ac:dyDescent="0.3">
-      <c r="C8" s="44"/>
+      <c r="C8" s="51"/>
       <c r="D8" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="E8" s="42"/>
-      <c r="F8" s="11" t="s">
+      <c r="E8" s="49"/>
+      <c r="F8" s="10" t="s">
         <v>110</v>
       </c>
       <c r="G8" s="6" t="s">
+        <v>223</v>
+      </c>
+      <c r="H8" s="25" t="s">
+        <v>208</v>
+      </c>
+      <c r="I8" s="4"/>
+    </row>
+    <row r="9" spans="3:9" x14ac:dyDescent="0.3">
+      <c r="C9" s="51" t="s">
+        <v>13</v>
+      </c>
+      <c r="D9" s="7" t="s">
+        <v>154</v>
+      </c>
+      <c r="E9" s="49"/>
+      <c r="F9" s="22" t="s">
+        <v>179</v>
+      </c>
+      <c r="G9" s="6" t="s">
+        <v>224</v>
+      </c>
+      <c r="H9" s="25" t="s">
+        <v>208</v>
+      </c>
+      <c r="I9" s="4"/>
+    </row>
+    <row r="10" spans="3:9" x14ac:dyDescent="0.3">
+      <c r="C10" s="51"/>
+      <c r="D10" s="7" t="s">
+        <v>155</v>
+      </c>
+      <c r="E10" s="49"/>
+      <c r="F10" s="22" t="s">
+        <v>180</v>
+      </c>
+      <c r="G10" s="6" t="s">
         <v>225</v>
       </c>
-      <c r="H8" s="26" t="s">
-        <v>209</v>
-      </c>
-      <c r="I8" s="4"/>
-    </row>
-    <row r="9" spans="3:9" x14ac:dyDescent="0.3">
-      <c r="C9" s="44" t="s">
-        <v>13</v>
-      </c>
-      <c r="D9" s="7" t="s">
-        <v>155</v>
-      </c>
-      <c r="E9" s="42"/>
-      <c r="F9" s="23" t="s">
-        <v>180</v>
-      </c>
-      <c r="G9" s="6" t="s">
+      <c r="H10" s="25" t="s">
+        <v>208</v>
+      </c>
+      <c r="I10" s="4"/>
+    </row>
+    <row r="11" spans="3:9" ht="34.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C11" s="51"/>
+      <c r="D11" s="7" t="s">
+        <v>156</v>
+      </c>
+      <c r="E11" s="49"/>
+      <c r="F11" s="22" t="s">
+        <v>181</v>
+      </c>
+      <c r="G11" s="6" t="s">
         <v>226</v>
       </c>
-      <c r="H9" s="26" t="s">
-        <v>209</v>
-      </c>
-      <c r="I9" s="4"/>
-    </row>
-    <row r="10" spans="3:9" x14ac:dyDescent="0.3">
-      <c r="C10" s="44"/>
-      <c r="D10" s="7" t="s">
-        <v>156</v>
-      </c>
-      <c r="E10" s="42"/>
-      <c r="F10" s="23" t="s">
-        <v>181</v>
-      </c>
-      <c r="G10" s="6" t="s">
+      <c r="H11" s="25" t="s">
+        <v>208</v>
+      </c>
+      <c r="I11" s="4"/>
+    </row>
+    <row r="12" spans="3:9" ht="34.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C12" s="51"/>
+      <c r="D12" s="7" t="s">
+        <v>157</v>
+      </c>
+      <c r="E12" s="49"/>
+      <c r="F12" s="22" t="s">
+        <v>182</v>
+      </c>
+      <c r="G12" s="6" t="s">
         <v>227</v>
       </c>
-      <c r="H10" s="26" t="s">
-        <v>209</v>
-      </c>
-      <c r="I10" s="4"/>
-    </row>
-    <row r="11" spans="3:9" ht="34.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C11" s="44"/>
-      <c r="D11" s="7" t="s">
-        <v>157</v>
-      </c>
-      <c r="E11" s="42"/>
-      <c r="F11" s="23" t="s">
-        <v>182</v>
-      </c>
-      <c r="G11" s="6" t="s">
+      <c r="H12" s="25" t="s">
+        <v>208</v>
+      </c>
+      <c r="I12" s="4"/>
+    </row>
+    <row r="13" spans="3:9" ht="65.45" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C13" s="51"/>
+      <c r="D13" s="7" t="s">
+        <v>158</v>
+      </c>
+      <c r="E13" s="49"/>
+      <c r="F13" s="22" t="s">
+        <v>183</v>
+      </c>
+      <c r="G13" s="6" t="s">
         <v>228</v>
       </c>
-      <c r="H11" s="26" t="s">
-        <v>209</v>
-      </c>
-      <c r="I11" s="4"/>
-    </row>
-    <row r="12" spans="3:9" ht="34.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C12" s="44"/>
-      <c r="D12" s="7" t="s">
-        <v>158</v>
-      </c>
-      <c r="E12" s="42"/>
-      <c r="F12" s="23" t="s">
-        <v>183</v>
-      </c>
-      <c r="G12" s="6" t="s">
+      <c r="H13" s="25" t="s">
+        <v>208</v>
+      </c>
+      <c r="I13" s="4"/>
+    </row>
+    <row r="14" spans="3:9" ht="46.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C14" s="51"/>
+      <c r="D14" s="7" t="s">
+        <v>159</v>
+      </c>
+      <c r="E14" s="49"/>
+      <c r="F14" s="22" t="s">
+        <v>184</v>
+      </c>
+      <c r="G14" s="6" t="s">
         <v>229</v>
       </c>
-      <c r="H12" s="26" t="s">
-        <v>209</v>
-      </c>
-      <c r="I12" s="4"/>
-    </row>
-    <row r="13" spans="3:9" ht="65.45" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C13" s="44"/>
-      <c r="D13" s="7" t="s">
-        <v>159</v>
-      </c>
-      <c r="E13" s="42"/>
-      <c r="F13" s="23" t="s">
-        <v>184</v>
-      </c>
-      <c r="G13" s="6" t="s">
+      <c r="H14" s="25" t="s">
+        <v>208</v>
+      </c>
+      <c r="I14" s="4"/>
+    </row>
+    <row r="15" spans="3:9" ht="66.150000000000006" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C15" s="51"/>
+      <c r="D15" s="7" t="s">
+        <v>160</v>
+      </c>
+      <c r="E15" s="49"/>
+      <c r="F15" s="22" t="s">
+        <v>185</v>
+      </c>
+      <c r="G15" s="6" t="s">
         <v>230</v>
       </c>
-      <c r="H13" s="26" t="s">
-        <v>209</v>
-      </c>
-      <c r="I13" s="4"/>
-    </row>
-    <row r="14" spans="3:9" ht="46.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C14" s="44"/>
-      <c r="D14" s="7" t="s">
-        <v>160</v>
-      </c>
-      <c r="E14" s="42"/>
-      <c r="F14" s="23" t="s">
-        <v>185</v>
-      </c>
-      <c r="G14" s="6" t="s">
-        <v>231</v>
-      </c>
-      <c r="H14" s="26" t="s">
-        <v>209</v>
-      </c>
-      <c r="I14" s="4"/>
-    </row>
-    <row r="15" spans="3:9" ht="66.150000000000006" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C15" s="44"/>
-      <c r="D15" s="7" t="s">
-        <v>161</v>
-      </c>
-      <c r="E15" s="42"/>
-      <c r="F15" s="23" t="s">
-        <v>186</v>
-      </c>
-      <c r="G15" s="6" t="s">
-        <v>232</v>
-      </c>
-      <c r="H15" s="26" t="s">
-        <v>209</v>
+      <c r="H15" s="25" t="s">
+        <v>208</v>
       </c>
       <c r="I15" s="4"/>
     </row>
     <row r="16" spans="3:9" x14ac:dyDescent="0.3">
-      <c r="C16" s="44" t="s">
+      <c r="C16" s="51" t="s">
         <v>14</v>
       </c>
       <c r="D16" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="E16" s="42"/>
+      <c r="E16" s="49"/>
       <c r="F16" s="9" t="s">
         <v>112</v>
       </c>
       <c r="G16" s="6" t="s">
-        <v>233</v>
-      </c>
-      <c r="H16" s="26" t="s">
-        <v>209</v>
+        <v>231</v>
+      </c>
+      <c r="H16" s="25" t="s">
+        <v>208</v>
       </c>
       <c r="I16" s="4"/>
     </row>
     <row r="17" spans="3:9" x14ac:dyDescent="0.3">
-      <c r="C17" s="44"/>
+      <c r="C17" s="51"/>
       <c r="D17" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="E17" s="42"/>
+      <c r="E17" s="49"/>
       <c r="F17" s="9" t="s">
         <v>113</v>
       </c>
       <c r="G17" s="6" t="s">
-        <v>234</v>
-      </c>
-      <c r="H17" s="26" t="s">
-        <v>209</v>
+        <v>232</v>
+      </c>
+      <c r="H17" s="25" t="s">
+        <v>208</v>
       </c>
       <c r="I17" s="4"/>
     </row>
     <row r="18" spans="3:9" ht="15.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C18" s="41" t="s">
+      <c r="C18" s="48" t="s">
         <v>114</v>
       </c>
       <c r="D18" s="7" t="s">
         <v>115</v>
       </c>
-      <c r="E18" s="42"/>
-      <c r="F18" s="41" t="s">
-        <v>200</v>
+      <c r="E18" s="49"/>
+      <c r="F18" s="48" t="s">
+        <v>199</v>
       </c>
       <c r="G18" s="6" t="s">
-        <v>237</v>
-      </c>
-      <c r="H18" s="53" t="s">
-        <v>209</v>
-      </c>
-      <c r="I18" s="45"/>
+        <v>235</v>
+      </c>
+      <c r="H18" s="42" t="s">
+        <v>208</v>
+      </c>
+      <c r="I18" s="37"/>
     </row>
     <row r="19" spans="3:9" x14ac:dyDescent="0.3">
-      <c r="C19" s="42"/>
+      <c r="C19" s="49"/>
       <c r="D19" s="7" t="s">
         <v>116</v>
       </c>
-      <c r="E19" s="42"/>
-      <c r="F19" s="42"/>
+      <c r="E19" s="49"/>
+      <c r="F19" s="49"/>
       <c r="G19" s="6" t="s">
-        <v>235</v>
-      </c>
-      <c r="H19" s="54"/>
-      <c r="I19" s="47"/>
+        <v>233</v>
+      </c>
+      <c r="H19" s="43"/>
+      <c r="I19" s="39"/>
     </row>
     <row r="20" spans="3:9" x14ac:dyDescent="0.3">
-      <c r="C20" s="42"/>
+      <c r="C20" s="49"/>
       <c r="D20" s="7" t="s">
         <v>117</v>
       </c>
-      <c r="E20" s="42"/>
-      <c r="F20" s="42"/>
+      <c r="E20" s="49"/>
+      <c r="F20" s="49"/>
       <c r="G20" s="6" t="s">
-        <v>238</v>
-      </c>
-      <c r="H20" s="54"/>
-      <c r="I20" s="47"/>
+        <v>236</v>
+      </c>
+      <c r="H20" s="43"/>
+      <c r="I20" s="39"/>
     </row>
     <row r="21" spans="3:9" x14ac:dyDescent="0.3">
-      <c r="C21" s="42"/>
+      <c r="C21" s="49"/>
       <c r="D21" s="7" t="s">
         <v>118</v>
       </c>
-      <c r="E21" s="42"/>
-      <c r="F21" s="42"/>
+      <c r="E21" s="49"/>
+      <c r="F21" s="49"/>
       <c r="G21" s="6" t="s">
-        <v>236</v>
-      </c>
-      <c r="H21" s="54"/>
-      <c r="I21" s="47"/>
+        <v>234</v>
+      </c>
+      <c r="H21" s="43"/>
+      <c r="I21" s="39"/>
     </row>
     <row r="22" spans="3:9" x14ac:dyDescent="0.3">
-      <c r="C22" s="43"/>
+      <c r="C22" s="50"/>
       <c r="D22" s="7" t="s">
-        <v>201</v>
-      </c>
-      <c r="E22" s="42"/>
-      <c r="F22" s="43"/>
+        <v>200</v>
+      </c>
+      <c r="E22" s="49"/>
+      <c r="F22" s="50"/>
       <c r="G22" s="6" t="s">
-        <v>239</v>
-      </c>
-      <c r="H22" s="55"/>
-      <c r="I22" s="46"/>
+        <v>237</v>
+      </c>
+      <c r="H22" s="44"/>
+      <c r="I22" s="38"/>
     </row>
     <row r="23" spans="3:9" ht="30.15" x14ac:dyDescent="0.3">
       <c r="C23" s="3" t="s">
@@ -1971,229 +1982,233 @@
       <c r="D23" s="7" t="s">
         <v>62</v>
       </c>
-      <c r="E23" s="42"/>
+      <c r="E23" s="49"/>
       <c r="F23" s="9" t="s">
         <v>119</v>
       </c>
       <c r="G23" s="6" t="s">
-        <v>240</v>
-      </c>
-      <c r="H23" s="26" t="s">
-        <v>209</v>
+        <v>238</v>
+      </c>
+      <c r="H23" s="25" t="s">
+        <v>208</v>
       </c>
       <c r="I23" s="4"/>
     </row>
     <row r="24" spans="3:9" x14ac:dyDescent="0.3">
-      <c r="C24" s="44" t="s">
+      <c r="C24" s="51" t="s">
         <v>120</v>
       </c>
       <c r="D24" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="E24" s="42"/>
-      <c r="F24" s="12" t="s">
-        <v>218</v>
+      <c r="E24" s="49"/>
+      <c r="F24" s="11" t="s">
+        <v>216</v>
       </c>
       <c r="G24" s="6" t="s">
-        <v>244</v>
-      </c>
-      <c r="H24" s="26" t="s">
-        <v>209</v>
+        <v>242</v>
+      </c>
+      <c r="H24" s="25" t="s">
+        <v>208</v>
       </c>
       <c r="I24" s="4"/>
     </row>
     <row r="25" spans="3:9" ht="135.5" x14ac:dyDescent="0.3">
-      <c r="C25" s="44"/>
+      <c r="C25" s="51"/>
       <c r="D25" s="7" t="s">
-        <v>219</v>
-      </c>
-      <c r="E25" s="42"/>
-      <c r="F25" s="12" t="s">
         <v>217</v>
       </c>
+      <c r="E25" s="49"/>
+      <c r="F25" s="11" t="s">
+        <v>215</v>
+      </c>
       <c r="G25" s="6" t="s">
-        <v>241</v>
-      </c>
-      <c r="H25" s="26" t="s">
-        <v>209</v>
+        <v>239</v>
+      </c>
+      <c r="H25" s="25" t="s">
+        <v>208</v>
       </c>
       <c r="I25" s="4"/>
     </row>
     <row r="26" spans="3:9" ht="45.2" x14ac:dyDescent="0.3">
-      <c r="C26" s="44"/>
+      <c r="C26" s="51"/>
       <c r="D26" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="E26" s="42"/>
-      <c r="F26" s="12" t="s">
-        <v>215</v>
+      <c r="E26" s="49"/>
+      <c r="F26" s="11" t="s">
+        <v>213</v>
       </c>
       <c r="G26" s="6" t="s">
-        <v>242</v>
-      </c>
-      <c r="H26" s="26" t="s">
-        <v>209</v>
+        <v>240</v>
+      </c>
+      <c r="H26" s="25" t="s">
+        <v>208</v>
       </c>
       <c r="I26" s="4"/>
     </row>
     <row r="27" spans="3:9" ht="45.2" x14ac:dyDescent="0.3">
-      <c r="C27" s="44"/>
+      <c r="C27" s="51"/>
       <c r="D27" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="E27" s="43"/>
-      <c r="F27" s="12" t="s">
-        <v>214</v>
+      <c r="E27" s="50"/>
+      <c r="F27" s="11" t="s">
+        <v>212</v>
       </c>
       <c r="G27" s="6" t="s">
-        <v>243</v>
-      </c>
-      <c r="H27" s="26" t="s">
-        <v>209</v>
+        <v>241</v>
+      </c>
+      <c r="H27" s="25" t="s">
+        <v>208</v>
       </c>
       <c r="I27" s="4"/>
     </row>
     <row r="28" spans="3:9" x14ac:dyDescent="0.3">
-      <c r="C28" s="44" t="s">
+      <c r="C28" s="51" t="s">
         <v>23</v>
       </c>
       <c r="D28" s="7" t="s">
         <v>21</v>
       </c>
       <c r="E28" s="5"/>
-      <c r="F28" s="48" t="s">
-        <v>213</v>
-      </c>
-      <c r="G28" s="35"/>
-      <c r="H28" s="36"/>
-      <c r="I28" s="37"/>
+      <c r="F28" s="52" t="s">
+        <v>307</v>
+      </c>
+      <c r="G28" s="52" t="s">
+        <v>308</v>
+      </c>
+      <c r="H28" s="55" t="s">
+        <v>208</v>
+      </c>
+      <c r="I28" s="58"/>
     </row>
     <row r="29" spans="3:9" x14ac:dyDescent="0.3">
-      <c r="C29" s="44"/>
+      <c r="C29" s="51"/>
       <c r="D29" s="7" t="s">
         <v>22</v>
       </c>
       <c r="E29" s="5"/>
-      <c r="F29" s="49"/>
-      <c r="G29" s="35"/>
-      <c r="H29" s="36"/>
-      <c r="I29" s="37"/>
+      <c r="F29" s="53"/>
+      <c r="G29" s="53"/>
+      <c r="H29" s="56"/>
+      <c r="I29" s="59"/>
     </row>
     <row r="30" spans="3:9" x14ac:dyDescent="0.3">
-      <c r="C30" s="44" t="s">
+      <c r="C30" s="51" t="s">
         <v>24</v>
       </c>
       <c r="D30" s="7" t="s">
         <v>25</v>
       </c>
       <c r="E30" s="5"/>
-      <c r="F30" s="49"/>
-      <c r="G30" s="35"/>
-      <c r="H30" s="36"/>
-      <c r="I30" s="37"/>
+      <c r="F30" s="53"/>
+      <c r="G30" s="53"/>
+      <c r="H30" s="56"/>
+      <c r="I30" s="59"/>
     </row>
     <row r="31" spans="3:9" x14ac:dyDescent="0.3">
-      <c r="C31" s="44"/>
+      <c r="C31" s="51"/>
       <c r="D31" s="7" t="s">
         <v>26</v>
       </c>
       <c r="E31" s="5"/>
-      <c r="F31" s="49"/>
-      <c r="G31" s="35"/>
-      <c r="H31" s="36"/>
-      <c r="I31" s="37"/>
+      <c r="F31" s="53"/>
+      <c r="G31" s="53"/>
+      <c r="H31" s="56"/>
+      <c r="I31" s="59"/>
     </row>
     <row r="32" spans="3:9" x14ac:dyDescent="0.3">
-      <c r="C32" s="44"/>
+      <c r="C32" s="51"/>
       <c r="D32" s="7" t="s">
         <v>27</v>
       </c>
       <c r="E32" s="5"/>
-      <c r="F32" s="50"/>
-      <c r="G32" s="35"/>
-      <c r="H32" s="36"/>
-      <c r="I32" s="37"/>
+      <c r="F32" s="54"/>
+      <c r="G32" s="54"/>
+      <c r="H32" s="57"/>
+      <c r="I32" s="60"/>
     </row>
     <row r="33" spans="3:9" ht="60.25" x14ac:dyDescent="0.3">
-      <c r="C33" s="41" t="s">
+      <c r="C33" s="48" t="s">
         <v>28</v>
       </c>
       <c r="D33" s="7" t="s">
         <v>125</v>
       </c>
-      <c r="E33" s="41" t="s">
+      <c r="E33" s="48" t="s">
         <v>122</v>
       </c>
-      <c r="F33" s="21" t="s">
-        <v>188</v>
+      <c r="F33" s="20" t="s">
+        <v>187</v>
       </c>
       <c r="G33" s="6" t="s">
-        <v>246</v>
-      </c>
-      <c r="H33" s="26" t="s">
-        <v>209</v>
+        <v>244</v>
+      </c>
+      <c r="H33" s="25" t="s">
+        <v>208</v>
       </c>
       <c r="I33" s="4"/>
     </row>
     <row r="34" spans="3:9" ht="30.15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C34" s="42"/>
+      <c r="C34" s="49"/>
       <c r="D34" s="7">
         <v>10</v>
       </c>
-      <c r="E34" s="42"/>
-      <c r="F34" s="18" t="s">
-        <v>189</v>
-      </c>
-      <c r="G34" s="56" t="s">
-        <v>245</v>
-      </c>
-      <c r="H34" s="26" t="s">
-        <v>209</v>
+      <c r="E34" s="49"/>
+      <c r="F34" s="17" t="s">
+        <v>188</v>
+      </c>
+      <c r="G34" s="45" t="s">
+        <v>243</v>
+      </c>
+      <c r="H34" s="25" t="s">
+        <v>208</v>
       </c>
       <c r="I34" s="4"/>
     </row>
     <row r="35" spans="3:9" ht="30.15" x14ac:dyDescent="0.3">
-      <c r="C35" s="42"/>
+      <c r="C35" s="49"/>
       <c r="D35" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="E35" s="42"/>
-      <c r="F35" s="18" t="s">
-        <v>190</v>
-      </c>
-      <c r="G35" s="58"/>
-      <c r="H35" s="26" t="s">
-        <v>209</v>
+      <c r="E35" s="49"/>
+      <c r="F35" s="17" t="s">
+        <v>189</v>
+      </c>
+      <c r="G35" s="47"/>
+      <c r="H35" s="25" t="s">
+        <v>208</v>
       </c>
       <c r="I35" s="4"/>
     </row>
     <row r="36" spans="3:9" ht="30.15" x14ac:dyDescent="0.3">
-      <c r="C36" s="42"/>
+      <c r="C36" s="49"/>
       <c r="D36" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="E36" s="42"/>
-      <c r="F36" s="18" t="s">
-        <v>191</v>
-      </c>
-      <c r="G36" s="58"/>
-      <c r="H36" s="26" t="s">
-        <v>209</v>
+      <c r="E36" s="49"/>
+      <c r="F36" s="17" t="s">
+        <v>190</v>
+      </c>
+      <c r="G36" s="47"/>
+      <c r="H36" s="25" t="s">
+        <v>208</v>
       </c>
       <c r="I36" s="4"/>
     </row>
     <row r="37" spans="3:9" x14ac:dyDescent="0.3">
-      <c r="C37" s="43"/>
+      <c r="C37" s="50"/>
       <c r="D37" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="E37" s="42"/>
-      <c r="F37" s="18" t="s">
-        <v>192</v>
-      </c>
-      <c r="G37" s="57"/>
-      <c r="H37" s="26" t="s">
-        <v>209</v>
+      <c r="E37" s="49"/>
+      <c r="F37" s="17" t="s">
+        <v>191</v>
+      </c>
+      <c r="G37" s="46"/>
+      <c r="H37" s="25" t="s">
+        <v>208</v>
       </c>
       <c r="I37" s="4"/>
     </row>
@@ -2204,15 +2219,15 @@
       <c r="D38" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="E38" s="43"/>
-      <c r="F38" s="12" t="s">
-        <v>193</v>
+      <c r="E38" s="50"/>
+      <c r="F38" s="11" t="s">
+        <v>192</v>
       </c>
       <c r="G38" s="6" t="s">
-        <v>247</v>
-      </c>
-      <c r="H38" s="26" t="s">
-        <v>209</v>
+        <v>245</v>
+      </c>
+      <c r="H38" s="25" t="s">
+        <v>208</v>
       </c>
       <c r="I38" s="4"/>
     </row>
@@ -2223,89 +2238,89 @@
       <c r="D39" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="E39" s="44" t="s">
+      <c r="E39" s="51" t="s">
         <v>123</v>
       </c>
-      <c r="F39" s="12" t="s">
-        <v>153</v>
+      <c r="F39" s="11" t="s">
+        <v>152</v>
       </c>
       <c r="G39" s="6" t="s">
-        <v>303</v>
-      </c>
-      <c r="H39" s="26" t="s">
-        <v>209</v>
+        <v>300</v>
+      </c>
+      <c r="H39" s="25" t="s">
+        <v>208</v>
       </c>
       <c r="I39" s="4"/>
     </row>
     <row r="40" spans="3:9" ht="105.4" x14ac:dyDescent="0.3">
-      <c r="C40" s="44" t="s">
+      <c r="C40" s="51" t="s">
         <v>36</v>
       </c>
       <c r="D40" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="E40" s="44"/>
+      <c r="E40" s="51"/>
       <c r="F40" s="6" t="s">
-        <v>298</v>
-      </c>
-      <c r="G40" s="41" t="s">
-        <v>36</v>
-      </c>
-      <c r="H40" s="53" t="s">
-        <v>209</v>
+        <v>295</v>
+      </c>
+      <c r="G40" s="48" t="s">
+        <v>311</v>
+      </c>
+      <c r="H40" s="42" t="s">
+        <v>208</v>
       </c>
       <c r="I40" s="4"/>
     </row>
     <row r="41" spans="3:9" ht="165.6" x14ac:dyDescent="0.3">
-      <c r="C41" s="44"/>
+      <c r="C41" s="51"/>
       <c r="D41" s="7" t="s">
         <v>38</v>
       </c>
-      <c r="E41" s="44"/>
+      <c r="E41" s="51"/>
       <c r="F41" s="6" t="s">
-        <v>299</v>
-      </c>
-      <c r="G41" s="42"/>
-      <c r="H41" s="54"/>
+        <v>296</v>
+      </c>
+      <c r="G41" s="49"/>
+      <c r="H41" s="43"/>
       <c r="I41" s="4"/>
     </row>
     <row r="42" spans="3:9" ht="60.25" x14ac:dyDescent="0.3">
-      <c r="C42" s="44"/>
+      <c r="C42" s="51"/>
       <c r="D42" s="7" t="s">
         <v>39</v>
       </c>
-      <c r="E42" s="44"/>
+      <c r="E42" s="51"/>
       <c r="F42" s="6" t="s">
-        <v>300</v>
-      </c>
-      <c r="G42" s="42"/>
-      <c r="H42" s="54"/>
+        <v>297</v>
+      </c>
+      <c r="G42" s="49"/>
+      <c r="H42" s="43"/>
       <c r="I42" s="4"/>
     </row>
     <row r="43" spans="3:9" ht="60.25" x14ac:dyDescent="0.3">
-      <c r="C43" s="44"/>
+      <c r="C43" s="51"/>
       <c r="D43" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="E43" s="44"/>
+      <c r="E43" s="51"/>
       <c r="F43" s="6" t="s">
-        <v>302</v>
-      </c>
-      <c r="G43" s="42"/>
-      <c r="H43" s="54"/>
+        <v>299</v>
+      </c>
+      <c r="G43" s="49"/>
+      <c r="H43" s="43"/>
       <c r="I43" s="4"/>
     </row>
     <row r="44" spans="3:9" x14ac:dyDescent="0.3">
-      <c r="C44" s="44"/>
+      <c r="C44" s="51"/>
       <c r="D44" s="7" t="s">
         <v>41</v>
       </c>
-      <c r="E44" s="44"/>
-      <c r="F44" s="38" t="s">
-        <v>301</v>
-      </c>
-      <c r="G44" s="43"/>
-      <c r="H44" s="55"/>
+      <c r="E44" s="51"/>
+      <c r="F44" s="34" t="s">
+        <v>298</v>
+      </c>
+      <c r="G44" s="50"/>
+      <c r="H44" s="44"/>
       <c r="I44" s="4"/>
     </row>
     <row r="45" spans="3:9" ht="60.25" x14ac:dyDescent="0.3">
@@ -2315,15 +2330,15 @@
       <c r="D45" s="7" t="s">
         <v>43</v>
       </c>
-      <c r="E45" s="44"/>
-      <c r="F45" s="24" t="s">
-        <v>210</v>
+      <c r="E45" s="51"/>
+      <c r="F45" s="23" t="s">
+        <v>209</v>
       </c>
       <c r="G45" s="6" t="s">
-        <v>304</v>
-      </c>
-      <c r="H45" s="26" t="s">
-        <v>209</v>
+        <v>301</v>
+      </c>
+      <c r="H45" s="25" t="s">
+        <v>208</v>
       </c>
       <c r="I45" s="4"/>
     </row>
@@ -2334,15 +2349,15 @@
       <c r="D46" s="7" t="s">
         <v>45</v>
       </c>
-      <c r="E46" s="44"/>
-      <c r="F46" s="12" t="s">
-        <v>211</v>
+      <c r="E46" s="51"/>
+      <c r="F46" s="11" t="s">
+        <v>210</v>
       </c>
       <c r="G46" s="6" t="s">
-        <v>305</v>
-      </c>
-      <c r="H46" s="26" t="s">
-        <v>209</v>
+        <v>302</v>
+      </c>
+      <c r="H46" s="25" t="s">
+        <v>208</v>
       </c>
       <c r="I46" s="4"/>
     </row>
@@ -2353,15 +2368,15 @@
       <c r="D47" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="E47" s="44"/>
-      <c r="F47" s="12" t="s">
-        <v>306</v>
+      <c r="E47" s="51"/>
+      <c r="F47" s="11" t="s">
+        <v>303</v>
       </c>
       <c r="G47" s="6" t="s">
-        <v>307</v>
-      </c>
-      <c r="H47" s="26" t="s">
-        <v>209</v>
+        <v>304</v>
+      </c>
+      <c r="H47" s="25" t="s">
+        <v>208</v>
       </c>
       <c r="I47" s="4"/>
     </row>
@@ -2372,15 +2387,15 @@
       <c r="D48" s="7" t="s">
         <v>49</v>
       </c>
-      <c r="E48" s="44"/>
-      <c r="F48" s="12" t="s">
-        <v>154</v>
+      <c r="E48" s="51"/>
+      <c r="F48" s="11" t="s">
+        <v>153</v>
       </c>
       <c r="G48" s="6" t="s">
-        <v>308</v>
-      </c>
-      <c r="H48" s="26" t="s">
-        <v>209</v>
+        <v>305</v>
+      </c>
+      <c r="H48" s="25" t="s">
+        <v>208</v>
       </c>
       <c r="I48" s="4"/>
     </row>
@@ -2391,216 +2406,216 @@
       <c r="D49" s="7" t="s">
         <v>51</v>
       </c>
-      <c r="E49" s="22" t="s">
-        <v>199</v>
-      </c>
-      <c r="F49" s="12" t="s">
-        <v>212</v>
+      <c r="E49" s="21" t="s">
+        <v>198</v>
+      </c>
+      <c r="F49" s="11" t="s">
+        <v>211</v>
       </c>
       <c r="G49" s="6" t="s">
-        <v>309</v>
-      </c>
-      <c r="H49" s="26" t="s">
-        <v>209</v>
+        <v>306</v>
+      </c>
+      <c r="H49" s="25" t="s">
+        <v>208</v>
       </c>
       <c r="I49" s="4"/>
     </row>
     <row r="50" spans="3:9" ht="45.2" x14ac:dyDescent="0.3">
-      <c r="C50" s="41" t="s">
+      <c r="C50" s="48" t="s">
         <v>52</v>
       </c>
       <c r="D50" s="7" t="s">
         <v>127</v>
       </c>
-      <c r="E50" s="41" t="s">
+      <c r="E50" s="48" t="s">
         <v>122</v>
       </c>
-      <c r="F50" s="19" t="s">
-        <v>198</v>
+      <c r="F50" s="18" t="s">
+        <v>197</v>
       </c>
       <c r="G50" s="6" t="s">
-        <v>248</v>
-      </c>
-      <c r="H50" s="26" t="s">
-        <v>209</v>
+        <v>246</v>
+      </c>
+      <c r="H50" s="25" t="s">
+        <v>208</v>
       </c>
       <c r="I50" s="4"/>
     </row>
     <row r="51" spans="3:9" ht="30.15" x14ac:dyDescent="0.3">
-      <c r="C51" s="43"/>
+      <c r="C51" s="50"/>
       <c r="D51" s="7" t="s">
         <v>53</v>
       </c>
-      <c r="E51" s="42"/>
-      <c r="F51" s="19" t="s">
+      <c r="E51" s="49"/>
+      <c r="F51" s="18" t="s">
         <v>126</v>
       </c>
       <c r="G51" s="6" t="s">
-        <v>249</v>
-      </c>
-      <c r="H51" s="26" t="s">
-        <v>209</v>
+        <v>247</v>
+      </c>
+      <c r="H51" s="25" t="s">
+        <v>208</v>
       </c>
       <c r="I51" s="4"/>
     </row>
     <row r="52" spans="3:9" ht="60.25" x14ac:dyDescent="0.3">
-      <c r="C52" s="41" t="s">
-        <v>221</v>
+      <c r="C52" s="48" t="s">
+        <v>219</v>
       </c>
       <c r="D52" s="7" t="s">
         <v>125</v>
       </c>
-      <c r="E52" s="42"/>
-      <c r="F52" s="19" t="s">
-        <v>220</v>
+      <c r="E52" s="49"/>
+      <c r="F52" s="18" t="s">
+        <v>218</v>
       </c>
       <c r="G52" s="6" t="s">
-        <v>246</v>
-      </c>
-      <c r="H52" s="26" t="s">
-        <v>209</v>
+        <v>244</v>
+      </c>
+      <c r="H52" s="25" t="s">
+        <v>208</v>
       </c>
       <c r="I52" s="4"/>
     </row>
     <row r="53" spans="3:9" ht="60.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C53" s="42"/>
+      <c r="C53" s="49"/>
       <c r="D53" s="7" t="s">
         <v>54</v>
       </c>
-      <c r="E53" s="42"/>
-      <c r="F53" s="23" t="s">
-        <v>194</v>
+      <c r="E53" s="49"/>
+      <c r="F53" s="22" t="s">
+        <v>193</v>
       </c>
       <c r="G53" s="6" t="s">
-        <v>250</v>
-      </c>
-      <c r="H53" s="26" t="s">
-        <v>209</v>
+        <v>248</v>
+      </c>
+      <c r="H53" s="25" t="s">
+        <v>208</v>
       </c>
       <c r="I53" s="4"/>
     </row>
     <row r="54" spans="3:9" ht="120.45" x14ac:dyDescent="0.3">
-      <c r="C54" s="42"/>
+      <c r="C54" s="49"/>
       <c r="D54" s="7" t="s">
         <v>55</v>
       </c>
-      <c r="E54" s="42"/>
-      <c r="F54" s="23" t="s">
-        <v>197</v>
+      <c r="E54" s="49"/>
+      <c r="F54" s="22" t="s">
+        <v>196</v>
       </c>
       <c r="G54" s="6" t="s">
-        <v>251</v>
-      </c>
-      <c r="H54" s="26" t="s">
-        <v>209</v>
+        <v>249</v>
+      </c>
+      <c r="H54" s="25" t="s">
+        <v>208</v>
       </c>
       <c r="I54" s="4"/>
     </row>
     <row r="55" spans="3:9" ht="90.35" x14ac:dyDescent="0.3">
-      <c r="C55" s="42"/>
+      <c r="C55" s="49"/>
       <c r="D55" s="7" t="s">
         <v>56</v>
       </c>
-      <c r="E55" s="42"/>
-      <c r="F55" s="23" t="s">
-        <v>195</v>
+      <c r="E55" s="49"/>
+      <c r="F55" s="22" t="s">
+        <v>194</v>
       </c>
       <c r="G55" s="6" t="s">
-        <v>252</v>
-      </c>
-      <c r="H55" s="26" t="s">
-        <v>209</v>
+        <v>250</v>
+      </c>
+      <c r="H55" s="25" t="s">
+        <v>208</v>
       </c>
       <c r="I55" s="4"/>
     </row>
     <row r="56" spans="3:9" ht="45.2" x14ac:dyDescent="0.3">
-      <c r="C56" s="43"/>
+      <c r="C56" s="50"/>
       <c r="D56" s="7" t="s">
         <v>69</v>
       </c>
-      <c r="E56" s="42"/>
-      <c r="F56" s="12" t="s">
-        <v>196</v>
+      <c r="E56" s="49"/>
+      <c r="F56" s="11" t="s">
+        <v>195</v>
       </c>
       <c r="G56" s="6" t="s">
-        <v>253</v>
-      </c>
-      <c r="H56" s="26" t="s">
-        <v>209</v>
+        <v>251</v>
+      </c>
+      <c r="H56" s="25" t="s">
+        <v>208</v>
       </c>
       <c r="I56" s="4"/>
     </row>
     <row r="57" spans="3:9" ht="30.15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C57" s="44" t="s">
+      <c r="C57" s="51" t="s">
         <v>91</v>
       </c>
       <c r="D57" s="7" t="s">
         <v>57</v>
       </c>
-      <c r="E57" s="42"/>
+      <c r="E57" s="49"/>
       <c r="F57" s="9" t="s">
         <v>128</v>
       </c>
       <c r="G57" s="6" t="s">
-        <v>254</v>
-      </c>
-      <c r="H57" s="26" t="s">
-        <v>209</v>
+        <v>252</v>
+      </c>
+      <c r="H57" s="25" t="s">
+        <v>208</v>
       </c>
       <c r="I57" s="4"/>
     </row>
     <row r="58" spans="3:9" x14ac:dyDescent="0.3">
-      <c r="C58" s="44"/>
+      <c r="C58" s="51"/>
       <c r="D58" s="7" t="s">
         <v>58</v>
       </c>
-      <c r="E58" s="42"/>
+      <c r="E58" s="49"/>
       <c r="F58" s="9" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="G58" s="6" t="s">
-        <v>255</v>
-      </c>
-      <c r="H58" s="26" t="s">
-        <v>209</v>
+        <v>253</v>
+      </c>
+      <c r="H58" s="25" t="s">
+        <v>208</v>
       </c>
       <c r="I58" s="4"/>
     </row>
     <row r="59" spans="3:9" ht="52.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C59" s="44"/>
+      <c r="C59" s="51"/>
       <c r="D59" s="7" t="s">
         <v>59</v>
       </c>
-      <c r="E59" s="42"/>
+      <c r="E59" s="49"/>
       <c r="F59" s="9" t="s">
         <v>129</v>
       </c>
       <c r="G59" s="6" t="s">
-        <v>256</v>
-      </c>
-      <c r="H59" s="26" t="s">
-        <v>209</v>
+        <v>254</v>
+      </c>
+      <c r="H59" s="25" t="s">
+        <v>208</v>
       </c>
       <c r="I59" s="4"/>
     </row>
     <row r="60" spans="3:9" ht="30.15" x14ac:dyDescent="0.3">
-      <c r="C60" s="44"/>
+      <c r="C60" s="51"/>
       <c r="D60" s="7" t="s">
         <v>60</v>
       </c>
-      <c r="E60" s="43"/>
+      <c r="E60" s="50"/>
       <c r="F60" s="9" t="s">
         <v>130</v>
       </c>
       <c r="G60" s="6" t="s">
-        <v>257</v>
-      </c>
-      <c r="H60" s="26" t="s">
-        <v>209</v>
+        <v>255</v>
+      </c>
+      <c r="H60" s="25" t="s">
+        <v>208</v>
       </c>
       <c r="I60" s="4"/>
     </row>
-    <row r="61" spans="3:9" ht="105.4" x14ac:dyDescent="0.3">
+    <row r="61" spans="3:9" x14ac:dyDescent="0.3">
       <c r="C61" s="3" t="s">
         <v>61</v>
       </c>
@@ -2608,116 +2623,118 @@
         <v>63</v>
       </c>
       <c r="E61" s="5"/>
-      <c r="F61" s="10" t="s">
-        <v>131</v>
-      </c>
-      <c r="G61" s="35"/>
-      <c r="H61" s="36"/>
-      <c r="I61" s="37"/>
+      <c r="F61" s="11" t="s">
+        <v>309</v>
+      </c>
+      <c r="G61" s="22" t="s">
+        <v>310</v>
+      </c>
+      <c r="H61" s="35"/>
+      <c r="I61" s="36"/>
     </row>
     <row r="62" spans="3:9" ht="30.15" x14ac:dyDescent="0.3">
-      <c r="C62" s="44" t="s">
+      <c r="C62" s="51" t="s">
         <v>64</v>
       </c>
       <c r="D62" s="7" t="s">
         <v>65</v>
       </c>
-      <c r="E62" s="41" t="s">
+      <c r="E62" s="48" t="s">
         <v>122</v>
       </c>
       <c r="F62" s="9" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="G62" s="6" t="s">
-        <v>258</v>
-      </c>
-      <c r="H62" s="26" t="s">
-        <v>209</v>
+        <v>256</v>
+      </c>
+      <c r="H62" s="25" t="s">
+        <v>208</v>
       </c>
       <c r="I62" s="4"/>
     </row>
     <row r="63" spans="3:9" ht="60.25" x14ac:dyDescent="0.3">
-      <c r="C63" s="44"/>
+      <c r="C63" s="51"/>
       <c r="D63" s="7" t="s">
         <v>66</v>
       </c>
-      <c r="E63" s="42"/>
+      <c r="E63" s="49"/>
       <c r="F63" s="9" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="G63" s="6" t="s">
-        <v>259</v>
-      </c>
-      <c r="H63" s="26" t="s">
-        <v>209</v>
+        <v>257</v>
+      </c>
+      <c r="H63" s="25" t="s">
+        <v>208</v>
       </c>
       <c r="I63" s="4"/>
     </row>
     <row r="64" spans="3:9" ht="60.25" x14ac:dyDescent="0.3">
-      <c r="C64" s="44"/>
+      <c r="C64" s="51"/>
       <c r="D64" s="7" t="s">
         <v>67</v>
       </c>
-      <c r="E64" s="42"/>
+      <c r="E64" s="49"/>
       <c r="F64" s="9" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="G64" s="6" t="s">
-        <v>260</v>
-      </c>
-      <c r="H64" s="26" t="s">
-        <v>209</v>
+        <v>258</v>
+      </c>
+      <c r="H64" s="25" t="s">
+        <v>208</v>
       </c>
       <c r="I64" s="4"/>
     </row>
     <row r="65" spans="3:9" ht="30.15" x14ac:dyDescent="0.3">
-      <c r="C65" s="44"/>
+      <c r="C65" s="51"/>
       <c r="D65" s="7" t="s">
         <v>68</v>
       </c>
-      <c r="E65" s="42"/>
+      <c r="E65" s="49"/>
       <c r="F65" s="9" t="s">
+        <v>204</v>
+      </c>
+      <c r="G65" s="6" t="s">
+        <v>259</v>
+      </c>
+      <c r="H65" s="25" t="s">
+        <v>208</v>
+      </c>
+      <c r="I65" s="4"/>
+    </row>
+    <row r="66" spans="3:9" ht="60.25" x14ac:dyDescent="0.3">
+      <c r="C66" s="51"/>
+      <c r="D66" s="7" t="s">
+        <v>131</v>
+      </c>
+      <c r="E66" s="49"/>
+      <c r="F66" s="9" t="s">
         <v>205</v>
       </c>
-      <c r="G65" s="6" t="s">
+      <c r="G66" s="6" t="s">
         <v>261</v>
       </c>
-      <c r="H65" s="26" t="s">
-        <v>209</v>
-      </c>
-      <c r="I65" s="4"/>
-    </row>
-    <row r="66" spans="3:9" ht="60.25" x14ac:dyDescent="0.3">
-      <c r="C66" s="44"/>
-      <c r="D66" s="7" t="s">
+      <c r="H66" s="25" t="s">
+        <v>208</v>
+      </c>
+      <c r="I66" s="4"/>
+    </row>
+    <row r="67" spans="3:9" ht="120.45" x14ac:dyDescent="0.3">
+      <c r="C67" s="51"/>
+      <c r="D67" s="2" t="s">
         <v>132</v>
       </c>
-      <c r="E66" s="42"/>
-      <c r="F66" s="9" t="s">
+      <c r="E67" s="49"/>
+      <c r="F67" s="9" t="s">
         <v>206</v>
       </c>
-      <c r="G66" s="6" t="s">
-        <v>263</v>
-      </c>
-      <c r="H66" s="26" t="s">
-        <v>209</v>
-      </c>
-      <c r="I66" s="4"/>
-    </row>
-    <row r="67" spans="3:9" ht="120.45" x14ac:dyDescent="0.3">
-      <c r="C67" s="44"/>
-      <c r="D67" s="2" t="s">
-        <v>133</v>
-      </c>
-      <c r="E67" s="42"/>
-      <c r="F67" s="9" t="s">
-        <v>207</v>
-      </c>
       <c r="G67" s="6" t="s">
-        <v>262</v>
-      </c>
-      <c r="H67" s="26" t="s">
-        <v>209</v>
+        <v>260</v>
+      </c>
+      <c r="H67" s="25" t="s">
+        <v>208</v>
       </c>
       <c r="I67" s="4"/>
     </row>
@@ -2728,647 +2745,648 @@
       <c r="D68" s="7" t="s">
         <v>71</v>
       </c>
-      <c r="E68" s="42"/>
-      <c r="F68" s="24" t="s">
-        <v>208</v>
+      <c r="E68" s="49"/>
+      <c r="F68" s="23" t="s">
+        <v>207</v>
       </c>
       <c r="G68" s="6" t="s">
-        <v>264</v>
-      </c>
-      <c r="H68" s="26" t="s">
-        <v>209</v>
+        <v>262</v>
+      </c>
+      <c r="H68" s="25" t="s">
+        <v>208</v>
       </c>
       <c r="I68" s="4"/>
     </row>
     <row r="69" spans="3:9" ht="30.15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C69" s="44" t="s">
+      <c r="C69" s="51" t="s">
         <v>72</v>
       </c>
       <c r="D69" s="7" t="s">
         <v>73</v>
       </c>
-      <c r="E69" s="42"/>
+      <c r="E69" s="49"/>
       <c r="F69" s="9" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="G69" s="6" t="s">
-        <v>265</v>
-      </c>
-      <c r="H69" s="26" t="s">
-        <v>209</v>
+        <v>263</v>
+      </c>
+      <c r="H69" s="25" t="s">
+        <v>208</v>
       </c>
       <c r="I69" s="4"/>
     </row>
     <row r="70" spans="3:9" ht="30.15" x14ac:dyDescent="0.3">
-      <c r="C70" s="44"/>
+      <c r="C70" s="51"/>
       <c r="D70" s="7" t="s">
         <v>74</v>
       </c>
-      <c r="E70" s="42"/>
+      <c r="E70" s="49"/>
       <c r="F70" s="9" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="G70" s="6" t="s">
-        <v>266</v>
-      </c>
-      <c r="H70" s="26" t="s">
-        <v>209</v>
+        <v>264</v>
+      </c>
+      <c r="H70" s="25" t="s">
+        <v>208</v>
       </c>
       <c r="I70" s="4"/>
     </row>
     <row r="71" spans="3:9" x14ac:dyDescent="0.3">
-      <c r="C71" s="44"/>
+      <c r="C71" s="51"/>
       <c r="D71" s="7" t="s">
         <v>75</v>
       </c>
-      <c r="E71" s="42"/>
+      <c r="E71" s="49"/>
       <c r="F71" s="9" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="G71" s="6" t="s">
-        <v>267</v>
-      </c>
-      <c r="H71" s="26" t="s">
-        <v>209</v>
+        <v>265</v>
+      </c>
+      <c r="H71" s="25" t="s">
+        <v>208</v>
       </c>
       <c r="I71" s="4"/>
     </row>
     <row r="72" spans="3:9" ht="30.15" x14ac:dyDescent="0.3">
-      <c r="C72" s="44"/>
+      <c r="C72" s="51"/>
       <c r="D72" s="7" t="s">
-        <v>216</v>
-      </c>
-      <c r="E72" s="42"/>
-      <c r="F72" s="12" t="s">
-        <v>162</v>
+        <v>214</v>
+      </c>
+      <c r="E72" s="49"/>
+      <c r="F72" s="11" t="s">
+        <v>161</v>
       </c>
       <c r="G72" s="6" t="s">
-        <v>268</v>
-      </c>
-      <c r="H72" s="26" t="s">
-        <v>209</v>
+        <v>266</v>
+      </c>
+      <c r="H72" s="25" t="s">
+        <v>208</v>
       </c>
       <c r="I72" s="4"/>
     </row>
     <row r="73" spans="3:9" x14ac:dyDescent="0.3">
-      <c r="C73" s="44"/>
+      <c r="C73" s="51"/>
       <c r="D73" s="7" t="s">
         <v>76</v>
       </c>
-      <c r="E73" s="42"/>
+      <c r="E73" s="49"/>
       <c r="F73" s="9" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="G73" s="6" t="s">
-        <v>269</v>
-      </c>
-      <c r="H73" s="26" t="s">
-        <v>209</v>
+        <v>267</v>
+      </c>
+      <c r="H73" s="25" t="s">
+        <v>208</v>
       </c>
       <c r="I73" s="4"/>
     </row>
     <row r="74" spans="3:9" x14ac:dyDescent="0.3">
-      <c r="C74" s="44"/>
+      <c r="C74" s="51"/>
       <c r="D74" s="7" t="s">
         <v>77</v>
       </c>
-      <c r="E74" s="42"/>
+      <c r="E74" s="49"/>
       <c r="F74" s="9" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="G74" s="6" t="s">
-        <v>270</v>
-      </c>
-      <c r="H74" s="26" t="s">
-        <v>209</v>
+        <v>268</v>
+      </c>
+      <c r="H74" s="25" t="s">
+        <v>208</v>
       </c>
       <c r="I74" s="4"/>
     </row>
     <row r="75" spans="3:9" x14ac:dyDescent="0.3">
-      <c r="C75" s="44"/>
+      <c r="C75" s="51"/>
       <c r="D75" s="7" t="s">
         <v>78</v>
       </c>
-      <c r="E75" s="42"/>
+      <c r="E75" s="49"/>
       <c r="F75" s="9" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="G75" s="6" t="s">
-        <v>271</v>
-      </c>
-      <c r="H75" s="26" t="s">
-        <v>209</v>
+        <v>269</v>
+      </c>
+      <c r="H75" s="25" t="s">
+        <v>208</v>
       </c>
       <c r="I75" s="4"/>
     </row>
     <row r="76" spans="3:9" x14ac:dyDescent="0.3">
-      <c r="C76" s="44"/>
+      <c r="C76" s="51"/>
       <c r="D76" s="7" t="s">
         <v>79</v>
       </c>
-      <c r="E76" s="42"/>
+      <c r="E76" s="49"/>
       <c r="F76" s="9" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="G76" s="6" t="s">
-        <v>272</v>
-      </c>
-      <c r="H76" s="26" t="s">
-        <v>209</v>
+        <v>270</v>
+      </c>
+      <c r="H76" s="25" t="s">
+        <v>208</v>
       </c>
       <c r="I76" s="4"/>
     </row>
     <row r="77" spans="3:9" ht="30.15" x14ac:dyDescent="0.3">
-      <c r="C77" s="44"/>
+      <c r="C77" s="51"/>
       <c r="D77" s="7" t="s">
         <v>80</v>
       </c>
-      <c r="E77" s="42"/>
-      <c r="F77" s="12" t="s">
-        <v>187</v>
+      <c r="E77" s="49"/>
+      <c r="F77" s="11" t="s">
+        <v>186</v>
       </c>
       <c r="G77" s="6" t="s">
-        <v>273</v>
-      </c>
-      <c r="H77" s="26" t="s">
-        <v>209</v>
+        <v>271</v>
+      </c>
+      <c r="H77" s="25" t="s">
+        <v>208</v>
       </c>
       <c r="I77" s="4"/>
     </row>
     <row r="78" spans="3:9" ht="30.15" x14ac:dyDescent="0.3">
-      <c r="C78" s="44"/>
+      <c r="C78" s="51"/>
       <c r="D78" s="7" t="s">
         <v>81</v>
       </c>
-      <c r="E78" s="42"/>
-      <c r="F78" s="25" t="s">
+      <c r="E78" s="49"/>
+      <c r="F78" s="24" t="s">
+        <v>140</v>
+      </c>
+      <c r="G78" s="31"/>
+      <c r="H78" s="32"/>
+      <c r="I78" s="33"/>
+    </row>
+    <row r="79" spans="3:9" ht="30.15" x14ac:dyDescent="0.3">
+      <c r="C79" s="49" t="s">
+        <v>83</v>
+      </c>
+      <c r="D79" s="7" t="s">
         <v>141</v>
       </c>
-      <c r="G78" s="32"/>
-      <c r="H78" s="33"/>
-      <c r="I78" s="34"/>
-    </row>
-    <row r="79" spans="3:9" ht="30.15" x14ac:dyDescent="0.3">
-      <c r="C79" s="42" t="s">
-        <v>83</v>
-      </c>
-      <c r="D79" s="7" t="s">
-        <v>142</v>
-      </c>
-      <c r="E79" s="42"/>
+      <c r="E79" s="49"/>
       <c r="F79" s="9" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="G79" s="6" t="s">
-        <v>280</v>
-      </c>
-      <c r="H79" s="26" t="s">
-        <v>209</v>
+        <v>278</v>
+      </c>
+      <c r="H79" s="25" t="s">
+        <v>208</v>
       </c>
       <c r="I79" s="4"/>
     </row>
     <row r="80" spans="3:9" ht="30.15" x14ac:dyDescent="0.3">
-      <c r="C80" s="42"/>
+      <c r="C80" s="49"/>
       <c r="D80" s="7" t="s">
         <v>82</v>
       </c>
-      <c r="E80" s="42"/>
+      <c r="E80" s="49"/>
       <c r="F80" s="9" t="s">
+        <v>163</v>
+      </c>
+      <c r="G80" s="6" t="s">
+        <v>279</v>
+      </c>
+      <c r="H80" s="25" t="s">
+        <v>208</v>
+      </c>
+      <c r="I80" s="4"/>
+    </row>
+    <row r="81" spans="3:9" ht="30.15" x14ac:dyDescent="0.3">
+      <c r="C81" s="48" t="s">
+        <v>84</v>
+      </c>
+      <c r="D81" s="7" t="s">
+        <v>144</v>
+      </c>
+      <c r="E81" s="49"/>
+      <c r="F81" s="9" t="s">
         <v>164</v>
       </c>
-      <c r="G80" s="6" t="s">
+      <c r="G81" s="6" t="s">
         <v>281</v>
       </c>
-      <c r="H80" s="26" t="s">
-        <v>209</v>
-      </c>
-      <c r="I80" s="4"/>
-    </row>
-    <row r="81" spans="3:9" ht="30.15" x14ac:dyDescent="0.3">
-      <c r="C81" s="41" t="s">
-        <v>84</v>
-      </c>
-      <c r="D81" s="7" t="s">
+      <c r="H81" s="25" t="s">
+        <v>208</v>
+      </c>
+      <c r="I81" s="4"/>
+    </row>
+    <row r="82" spans="3:9" ht="69.400000000000006" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C82" s="49"/>
+      <c r="D82" s="7" t="s">
         <v>145</v>
       </c>
-      <c r="E81" s="42"/>
-      <c r="F81" s="9" t="s">
-        <v>165</v>
-      </c>
-      <c r="G81" s="6" t="s">
-        <v>283</v>
-      </c>
-      <c r="H81" s="26" t="s">
-        <v>209</v>
-      </c>
-      <c r="I81" s="4"/>
-    </row>
-    <row r="82" spans="3:9" ht="69.400000000000006" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C82" s="42"/>
-      <c r="D82" s="7" t="s">
-        <v>146</v>
-      </c>
-      <c r="E82" s="42"/>
+      <c r="E82" s="49"/>
       <c r="F82" s="9" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="G82" s="6" t="s">
-        <v>284</v>
-      </c>
-      <c r="H82" s="26" t="s">
-        <v>209</v>
+        <v>282</v>
+      </c>
+      <c r="H82" s="25" t="s">
+        <v>208</v>
       </c>
       <c r="I82" s="4"/>
     </row>
     <row r="83" spans="3:9" x14ac:dyDescent="0.3">
-      <c r="C83" s="42"/>
+      <c r="C83" s="49"/>
       <c r="D83" s="7" t="s">
         <v>85</v>
       </c>
-      <c r="E83" s="42"/>
-      <c r="F83" s="25" t="s">
-        <v>141</v>
-      </c>
-      <c r="G83" s="32"/>
-      <c r="H83" s="33"/>
-      <c r="I83" s="34"/>
+      <c r="E83" s="49"/>
+      <c r="F83" s="24" t="s">
+        <v>140</v>
+      </c>
+      <c r="G83" s="31"/>
+      <c r="H83" s="32"/>
+      <c r="I83" s="33"/>
     </row>
     <row r="84" spans="3:9" x14ac:dyDescent="0.3">
-      <c r="C84" s="42"/>
+      <c r="C84" s="49"/>
       <c r="D84" s="7" t="s">
         <v>86</v>
       </c>
-      <c r="E84" s="42"/>
+      <c r="E84" s="49"/>
       <c r="F84" s="9" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="G84" s="6" t="s">
-        <v>285</v>
-      </c>
-      <c r="H84" s="26" t="s">
-        <v>209</v>
+        <v>283</v>
+      </c>
+      <c r="H84" s="25" t="s">
+        <v>208</v>
       </c>
       <c r="I84" s="4"/>
     </row>
     <row r="85" spans="3:9" ht="30.15" x14ac:dyDescent="0.3">
-      <c r="C85" s="42"/>
+      <c r="C85" s="49"/>
       <c r="D85" s="7" t="s">
         <v>87</v>
       </c>
-      <c r="E85" s="42"/>
+      <c r="E85" s="49"/>
       <c r="F85" s="9" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="G85" s="6" t="s">
-        <v>286</v>
-      </c>
-      <c r="H85" s="26" t="s">
-        <v>209</v>
+        <v>284</v>
+      </c>
+      <c r="H85" s="25" t="s">
+        <v>208</v>
       </c>
       <c r="I85" s="4"/>
     </row>
     <row r="86" spans="3:9" ht="30.15" x14ac:dyDescent="0.3">
-      <c r="C86" s="42"/>
+      <c r="C86" s="49"/>
       <c r="D86" s="7" t="s">
         <v>88</v>
       </c>
-      <c r="E86" s="42"/>
+      <c r="E86" s="49"/>
       <c r="F86" s="9" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="G86" s="6" t="s">
-        <v>287</v>
-      </c>
-      <c r="H86" s="26" t="s">
-        <v>209</v>
+        <v>285</v>
+      </c>
+      <c r="H86" s="25" t="s">
+        <v>208</v>
       </c>
       <c r="I86" s="4"/>
     </row>
     <row r="87" spans="3:9" x14ac:dyDescent="0.3">
-      <c r="C87" s="42"/>
+      <c r="C87" s="49"/>
       <c r="D87" s="7" t="s">
         <v>89</v>
       </c>
-      <c r="E87" s="42"/>
+      <c r="E87" s="49"/>
       <c r="F87" s="9" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="G87" s="6" t="s">
-        <v>288</v>
-      </c>
-      <c r="H87" s="26" t="s">
-        <v>209</v>
+        <v>286</v>
+      </c>
+      <c r="H87" s="25" t="s">
+        <v>208</v>
       </c>
       <c r="I87" s="4"/>
     </row>
     <row r="88" spans="3:9" x14ac:dyDescent="0.3">
-      <c r="C88" s="42"/>
+      <c r="C88" s="49"/>
       <c r="D88" s="7" t="s">
         <v>90</v>
       </c>
-      <c r="E88" s="42"/>
+      <c r="E88" s="49"/>
       <c r="F88" s="9" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="G88" s="6" t="s">
-        <v>289</v>
-      </c>
-      <c r="H88" s="26" t="s">
-        <v>209</v>
+        <v>287</v>
+      </c>
+      <c r="H88" s="25" t="s">
+        <v>208</v>
       </c>
       <c r="I88" s="4"/>
     </row>
     <row r="89" spans="3:9" ht="30.15" x14ac:dyDescent="0.3">
-      <c r="C89" s="42"/>
+      <c r="C89" s="49"/>
       <c r="D89" s="7" t="s">
         <v>97</v>
       </c>
-      <c r="E89" s="42"/>
-      <c r="F89" s="12" t="s">
-        <v>282</v>
-      </c>
-      <c r="G89" s="23" t="s">
-        <v>283</v>
-      </c>
-      <c r="H89" s="39"/>
-      <c r="I89" s="40"/>
+      <c r="E89" s="49"/>
+      <c r="F89" s="11" t="s">
+        <v>280</v>
+      </c>
+      <c r="G89" s="22" t="s">
+        <v>281</v>
+      </c>
+      <c r="H89" s="35"/>
+      <c r="I89" s="36"/>
     </row>
     <row r="90" spans="3:9" x14ac:dyDescent="0.3">
-      <c r="C90" s="42"/>
+      <c r="C90" s="49"/>
       <c r="D90" s="7" t="s">
         <v>98</v>
       </c>
-      <c r="E90" s="42"/>
+      <c r="E90" s="49"/>
       <c r="F90" s="9" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="G90" s="6" t="s">
-        <v>290</v>
-      </c>
-      <c r="H90" s="26" t="s">
-        <v>209</v>
+        <v>288</v>
+      </c>
+      <c r="H90" s="25" t="s">
+        <v>208</v>
       </c>
       <c r="I90" s="4"/>
     </row>
     <row r="91" spans="3:9" x14ac:dyDescent="0.3">
-      <c r="C91" s="42"/>
+      <c r="C91" s="49"/>
       <c r="D91" s="7" t="s">
         <v>99</v>
       </c>
-      <c r="E91" s="42"/>
+      <c r="E91" s="49"/>
       <c r="F91" s="9" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="G91" s="6" t="s">
-        <v>291</v>
-      </c>
-      <c r="H91" s="26" t="s">
-        <v>209</v>
+        <v>289</v>
+      </c>
+      <c r="H91" s="25" t="s">
+        <v>208</v>
       </c>
       <c r="I91" s="4"/>
     </row>
     <row r="92" spans="3:9" ht="30.15" x14ac:dyDescent="0.3">
-      <c r="C92" s="42"/>
+      <c r="C92" s="49"/>
       <c r="D92" s="7" t="s">
         <v>100</v>
       </c>
-      <c r="E92" s="42"/>
+      <c r="E92" s="49"/>
       <c r="F92" s="9" t="s">
+        <v>172</v>
+      </c>
+      <c r="G92" s="6" t="s">
+        <v>290</v>
+      </c>
+      <c r="H92" s="25" t="s">
+        <v>208</v>
+      </c>
+      <c r="I92" s="4"/>
+    </row>
+    <row r="93" spans="3:9" ht="45.2" x14ac:dyDescent="0.3">
+      <c r="C93" s="49"/>
+      <c r="D93" s="7" t="s">
+        <v>143</v>
+      </c>
+      <c r="E93" s="49"/>
+      <c r="F93" s="9" t="s">
         <v>173</v>
       </c>
-      <c r="G92" s="6" t="s">
-        <v>292</v>
-      </c>
-      <c r="H92" s="26" t="s">
-        <v>209</v>
-      </c>
-      <c r="I92" s="4"/>
-    </row>
-    <row r="93" spans="3:9" ht="45.2" x14ac:dyDescent="0.3">
-      <c r="C93" s="42"/>
-      <c r="D93" s="7" t="s">
-        <v>144</v>
-      </c>
-      <c r="E93" s="42"/>
-      <c r="F93" s="9" t="s">
-        <v>174</v>
-      </c>
       <c r="G93" s="6" t="s">
-        <v>293</v>
-      </c>
-      <c r="H93" s="26" t="s">
-        <v>209</v>
+        <v>291</v>
+      </c>
+      <c r="H93" s="25" t="s">
+        <v>208</v>
       </c>
       <c r="I93" s="4"/>
     </row>
     <row r="94" spans="3:9" x14ac:dyDescent="0.3">
-      <c r="C94" s="41" t="s">
+      <c r="C94" s="48" t="s">
         <v>92</v>
       </c>
       <c r="D94" s="7" t="s">
         <v>93</v>
       </c>
-      <c r="E94" s="42"/>
+      <c r="E94" s="49"/>
       <c r="F94" s="9" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="G94" s="6" t="s">
-        <v>294</v>
-      </c>
-      <c r="H94" s="26" t="s">
-        <v>209</v>
+        <v>292</v>
+      </c>
+      <c r="H94" s="25" t="s">
+        <v>208</v>
       </c>
       <c r="I94" s="4"/>
     </row>
     <row r="95" spans="3:9" ht="30.15" x14ac:dyDescent="0.3">
-      <c r="C95" s="42"/>
+      <c r="C95" s="49"/>
       <c r="D95" s="7" t="s">
         <v>94</v>
       </c>
-      <c r="E95" s="42"/>
+      <c r="E95" s="49"/>
       <c r="F95" s="9" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="G95" s="6" t="s">
-        <v>295</v>
-      </c>
-      <c r="H95" s="26" t="s">
-        <v>209</v>
+        <v>293</v>
+      </c>
+      <c r="H95" s="25" t="s">
+        <v>208</v>
       </c>
       <c r="I95" s="4"/>
     </row>
     <row r="96" spans="3:9" x14ac:dyDescent="0.3">
-      <c r="C96" s="42"/>
+      <c r="C96" s="49"/>
       <c r="D96" s="7" t="s">
         <v>95</v>
       </c>
-      <c r="E96" s="42"/>
-      <c r="F96" s="28" t="s">
-        <v>141</v>
-      </c>
-      <c r="G96" s="29"/>
-      <c r="H96" s="30"/>
-      <c r="I96" s="31"/>
+      <c r="E96" s="49"/>
+      <c r="F96" s="27" t="s">
+        <v>140</v>
+      </c>
+      <c r="G96" s="28"/>
+      <c r="H96" s="29"/>
+      <c r="I96" s="30"/>
     </row>
     <row r="97" spans="3:9" x14ac:dyDescent="0.3">
-      <c r="C97" s="42"/>
+      <c r="C97" s="49"/>
       <c r="D97" s="7" t="s">
         <v>96</v>
       </c>
-      <c r="E97" s="42"/>
+      <c r="E97" s="49"/>
       <c r="F97" s="9" t="s">
+        <v>176</v>
+      </c>
+      <c r="G97" s="6" t="s">
+        <v>312</v>
+      </c>
+      <c r="H97" s="25" t="s">
+        <v>208</v>
+      </c>
+      <c r="I97" s="4"/>
+    </row>
+    <row r="98" spans="3:9" x14ac:dyDescent="0.3">
+      <c r="C98" s="49"/>
+      <c r="D98" s="7" t="s">
+        <v>142</v>
+      </c>
+      <c r="E98" s="49"/>
+      <c r="F98" s="9" t="s">
         <v>177</v>
       </c>
-      <c r="G97" s="6" t="s">
-        <v>296</v>
-      </c>
-      <c r="H97" s="26" t="s">
-        <v>209</v>
-      </c>
-      <c r="I97" s="4"/>
-    </row>
-    <row r="98" spans="3:9" x14ac:dyDescent="0.3">
-      <c r="C98" s="42"/>
-      <c r="D98" s="7" t="s">
-        <v>143</v>
-      </c>
-      <c r="E98" s="42"/>
-      <c r="F98" s="9" t="s">
-        <v>178</v>
-      </c>
       <c r="G98" s="6" t="s">
-        <v>297</v>
-      </c>
-      <c r="H98" s="26" t="s">
-        <v>209</v>
+        <v>294</v>
+      </c>
+      <c r="H98" s="25" t="s">
+        <v>208</v>
       </c>
       <c r="I98" s="4"/>
     </row>
     <row r="99" spans="3:9" x14ac:dyDescent="0.3">
-      <c r="C99" s="44" t="s">
+      <c r="C99" s="51" t="s">
         <v>107</v>
       </c>
       <c r="D99" s="7" t="s">
         <v>101</v>
       </c>
-      <c r="E99" s="42"/>
+      <c r="E99" s="49"/>
       <c r="F99" s="9" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="G99" s="6" t="s">
-        <v>277</v>
-      </c>
-      <c r="H99" s="26" t="s">
-        <v>209</v>
+        <v>275</v>
+      </c>
+      <c r="H99" s="25" t="s">
+        <v>208</v>
       </c>
       <c r="I99" s="4"/>
     </row>
     <row r="100" spans="3:9" ht="30.15" x14ac:dyDescent="0.3">
-      <c r="C100" s="44"/>
+      <c r="C100" s="51"/>
       <c r="D100" s="7" t="s">
         <v>102</v>
       </c>
-      <c r="E100" s="42"/>
+      <c r="E100" s="49"/>
       <c r="F100" s="9" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="G100" s="6" t="s">
-        <v>276</v>
-      </c>
-      <c r="H100" s="26" t="s">
-        <v>209</v>
+        <v>274</v>
+      </c>
+      <c r="H100" s="25" t="s">
+        <v>208</v>
       </c>
       <c r="I100" s="4"/>
     </row>
     <row r="101" spans="3:9" x14ac:dyDescent="0.3">
-      <c r="C101" s="44"/>
+      <c r="C101" s="51"/>
       <c r="D101" s="7" t="s">
         <v>103</v>
       </c>
-      <c r="E101" s="42"/>
+      <c r="E101" s="49"/>
       <c r="F101" s="9" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="G101" s="6" t="s">
-        <v>274</v>
-      </c>
-      <c r="H101" s="26" t="s">
-        <v>209</v>
+        <v>272</v>
+      </c>
+      <c r="H101" s="25" t="s">
+        <v>208</v>
       </c>
       <c r="I101" s="4"/>
     </row>
     <row r="102" spans="3:9" ht="30.15" x14ac:dyDescent="0.3">
-      <c r="C102" s="44"/>
+      <c r="C102" s="51"/>
       <c r="D102" s="7" t="s">
         <v>104</v>
       </c>
-      <c r="E102" s="42"/>
+      <c r="E102" s="49"/>
       <c r="F102" s="9" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="G102" s="6" t="s">
-        <v>275</v>
-      </c>
-      <c r="H102" s="26" t="s">
-        <v>209</v>
+        <v>273</v>
+      </c>
+      <c r="H102" s="25" t="s">
+        <v>208</v>
       </c>
       <c r="I102" s="4"/>
     </row>
     <row r="103" spans="3:9" x14ac:dyDescent="0.3">
-      <c r="C103" s="44"/>
+      <c r="C103" s="51"/>
       <c r="D103" s="7" t="s">
         <v>105</v>
       </c>
-      <c r="E103" s="42"/>
+      <c r="E103" s="49"/>
       <c r="F103" s="9" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="G103" s="6" t="s">
-        <v>278</v>
-      </c>
-      <c r="H103" s="26" t="s">
-        <v>209</v>
+        <v>276</v>
+      </c>
+      <c r="H103" s="25" t="s">
+        <v>208</v>
       </c>
       <c r="I103" s="4"/>
     </row>
     <row r="104" spans="3:9" ht="30.15" x14ac:dyDescent="0.3">
-      <c r="C104" s="44"/>
+      <c r="C104" s="51"/>
       <c r="D104" s="8" t="s">
         <v>106</v>
       </c>
-      <c r="E104" s="43"/>
+      <c r="E104" s="50"/>
       <c r="F104" s="9" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="G104" s="6" t="s">
-        <v>279</v>
-      </c>
-      <c r="H104" s="26" t="s">
-        <v>209</v>
+        <v>277</v>
+      </c>
+      <c r="H104" s="25" t="s">
+        <v>208</v>
       </c>
       <c r="I104" s="4"/>
     </row>
     <row r="105" spans="3:9" x14ac:dyDescent="0.3">
-      <c r="E105" s="20"/>
+      <c r="E105" s="19"/>
     </row>
     <row r="106" spans="3:9" x14ac:dyDescent="0.3">
-      <c r="E106" s="20"/>
+      <c r="E106" s="19"/>
     </row>
     <row r="107" spans="3:9" x14ac:dyDescent="0.3">
-      <c r="E107" s="20"/>
+      <c r="E107" s="19"/>
     </row>
   </sheetData>
-  <mergeCells count="34">
-    <mergeCell ref="I6:I7"/>
-    <mergeCell ref="I18:I22"/>
-    <mergeCell ref="F28:F32"/>
-    <mergeCell ref="F6:F7"/>
-    <mergeCell ref="H40:H44"/>
-    <mergeCell ref="H6:H7"/>
-    <mergeCell ref="H18:H22"/>
-    <mergeCell ref="G6:G7"/>
-    <mergeCell ref="G34:G37"/>
-    <mergeCell ref="G40:G44"/>
+  <mergeCells count="37">
+    <mergeCell ref="E50:E60"/>
+    <mergeCell ref="E62:E104"/>
+    <mergeCell ref="C69:C78"/>
+    <mergeCell ref="C79:C80"/>
+    <mergeCell ref="C81:C93"/>
+    <mergeCell ref="C94:C98"/>
+    <mergeCell ref="C99:C104"/>
+    <mergeCell ref="C62:C67"/>
+    <mergeCell ref="C57:C60"/>
+    <mergeCell ref="C50:C51"/>
+    <mergeCell ref="C52:C56"/>
     <mergeCell ref="E3:E27"/>
     <mergeCell ref="E33:E38"/>
     <mergeCell ref="E39:E48"/>
@@ -3382,17 +3400,19 @@
     <mergeCell ref="C24:C27"/>
     <mergeCell ref="C28:C29"/>
     <mergeCell ref="C18:C22"/>
-    <mergeCell ref="E50:E60"/>
-    <mergeCell ref="E62:E104"/>
-    <mergeCell ref="C69:C78"/>
-    <mergeCell ref="C79:C80"/>
-    <mergeCell ref="C81:C93"/>
-    <mergeCell ref="C94:C98"/>
-    <mergeCell ref="C99:C104"/>
-    <mergeCell ref="C62:C67"/>
-    <mergeCell ref="C57:C60"/>
-    <mergeCell ref="C50:C51"/>
-    <mergeCell ref="C52:C56"/>
+    <mergeCell ref="I6:I7"/>
+    <mergeCell ref="I18:I22"/>
+    <mergeCell ref="F28:F32"/>
+    <mergeCell ref="F6:F7"/>
+    <mergeCell ref="H40:H44"/>
+    <mergeCell ref="H6:H7"/>
+    <mergeCell ref="H18:H22"/>
+    <mergeCell ref="G6:G7"/>
+    <mergeCell ref="G34:G37"/>
+    <mergeCell ref="G40:G44"/>
+    <mergeCell ref="G28:G32"/>
+    <mergeCell ref="H28:H32"/>
+    <mergeCell ref="I28:I32"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
modified read functions preparing for 19/20
</commit_message>
<xml_diff>
--- a/edit_eam/crosscheck.xlsx
+++ b/edit_eam/crosscheck.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="406" uniqueCount="313">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="479" uniqueCount="314">
   <si>
     <t>Nombre</t>
   </si>
@@ -388,9 +388,6 @@
     <t>EAM</t>
   </si>
   <si>
-    <t>Nombre asignado</t>
-  </si>
-  <si>
     <t>Total</t>
   </si>
   <si>
@@ -953,6 +950,12 @@
   </si>
   <si>
     <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>Nombre asignado 17/18</t>
+  </si>
+  <si>
+    <t>Nombre asignado 19/20</t>
   </si>
 </sst>
 </file>
@@ -1241,6 +1244,33 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1265,44 +1295,17 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1608,10 +1611,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="C2:I107"/>
+  <dimension ref="C2:J107"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D107" sqref="D107"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E39" sqref="E39:E48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="15.05" x14ac:dyDescent="0.3"/>
@@ -1620,11 +1623,11 @@
     <col min="4" max="4" width="20.77734375" style="2" customWidth="1"/>
     <col min="5" max="5" width="14" style="12" customWidth="1"/>
     <col min="6" max="6" width="15.21875" style="1" customWidth="1"/>
-    <col min="7" max="7" width="19.88671875" style="1" customWidth="1"/>
-    <col min="8" max="8" width="8.88671875" style="26"/>
+    <col min="7" max="8" width="19.88671875" style="1" customWidth="1"/>
+    <col min="9" max="9" width="8.88671875" style="26"/>
   </cols>
   <sheetData>
-    <row r="2" spans="3:9" ht="26.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="3:10" ht="26.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C2" s="13" t="s">
         <v>0</v>
       </c>
@@ -1638,23 +1641,26 @@
         <v>1</v>
       </c>
       <c r="G2" s="13" t="s">
-        <v>124</v>
-      </c>
-      <c r="H2" s="16" t="s">
+        <v>312</v>
+      </c>
+      <c r="H2" s="13" t="s">
+        <v>313</v>
+      </c>
+      <c r="I2" s="16" t="s">
         <v>2</v>
       </c>
-      <c r="I2" s="16" t="s">
+      <c r="J2" s="16" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="3:9" x14ac:dyDescent="0.3">
+    <row r="3" spans="3:10" x14ac:dyDescent="0.3">
       <c r="C3" s="3" t="s">
         <v>4</v>
       </c>
       <c r="D3" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="E3" s="48" t="s">
+      <c r="E3" s="43" t="s">
         <v>122</v>
       </c>
       <c r="F3" s="9" t="s">
@@ -1663,743 +1669,855 @@
       <c r="G3" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="H3" s="25" t="s">
-        <v>208</v>
-      </c>
-      <c r="I3" s="4"/>
-    </row>
-    <row r="4" spans="3:9" x14ac:dyDescent="0.3">
+      <c r="H3" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="I3" s="25" t="s">
+        <v>207</v>
+      </c>
+      <c r="J3" s="4"/>
+    </row>
+    <row r="4" spans="3:10" x14ac:dyDescent="0.3">
       <c r="C4" s="3" t="s">
         <v>6</v>
       </c>
       <c r="D4" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="E4" s="49"/>
+      <c r="E4" s="44"/>
       <c r="F4" s="11" t="s">
         <v>108</v>
       </c>
       <c r="G4" s="6"/>
-      <c r="H4" s="25"/>
-      <c r="I4" s="4"/>
-    </row>
-    <row r="5" spans="3:9" x14ac:dyDescent="0.3">
-      <c r="C5" s="51" t="s">
+      <c r="H4" s="6"/>
+      <c r="I4" s="25"/>
+      <c r="J4" s="4"/>
+    </row>
+    <row r="5" spans="3:10" x14ac:dyDescent="0.3">
+      <c r="C5" s="60" t="s">
         <v>7</v>
       </c>
       <c r="D5" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="E5" s="49"/>
+      <c r="E5" s="44"/>
       <c r="F5" s="9" t="s">
         <v>109</v>
       </c>
       <c r="G5" s="6" t="s">
-        <v>221</v>
-      </c>
-      <c r="H5" s="25" t="s">
-        <v>208</v>
-      </c>
-      <c r="I5" s="4"/>
-    </row>
-    <row r="6" spans="3:9" x14ac:dyDescent="0.3">
-      <c r="C6" s="51"/>
+        <v>220</v>
+      </c>
+      <c r="H5" s="6" t="s">
+        <v>220</v>
+      </c>
+      <c r="I5" s="25" t="s">
+        <v>207</v>
+      </c>
+      <c r="J5" s="4"/>
+    </row>
+    <row r="6" spans="3:10" x14ac:dyDescent="0.3">
+      <c r="C6" s="60"/>
       <c r="D6" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="E6" s="49"/>
-      <c r="F6" s="40" t="s">
+      <c r="E6" s="44"/>
+      <c r="F6" s="49" t="s">
         <v>111</v>
       </c>
-      <c r="G6" s="45" t="s">
-        <v>222</v>
-      </c>
-      <c r="H6" s="42" t="s">
-        <v>208</v>
-      </c>
-      <c r="I6" s="37"/>
-    </row>
-    <row r="7" spans="3:9" x14ac:dyDescent="0.3">
-      <c r="C7" s="51"/>
+      <c r="G6" s="54" t="s">
+        <v>221</v>
+      </c>
+      <c r="H6" s="54" t="s">
+        <v>221</v>
+      </c>
+      <c r="I6" s="51" t="s">
+        <v>207</v>
+      </c>
+      <c r="J6" s="37"/>
+    </row>
+    <row r="7" spans="3:10" x14ac:dyDescent="0.3">
+      <c r="C7" s="60"/>
       <c r="D7" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="E7" s="49"/>
-      <c r="F7" s="41"/>
-      <c r="G7" s="46"/>
-      <c r="H7" s="44"/>
-      <c r="I7" s="38"/>
-    </row>
-    <row r="8" spans="3:9" x14ac:dyDescent="0.3">
-      <c r="C8" s="51"/>
+      <c r="E7" s="44"/>
+      <c r="F7" s="50"/>
+      <c r="G7" s="55"/>
+      <c r="H7" s="55"/>
+      <c r="I7" s="53"/>
+      <c r="J7" s="38"/>
+    </row>
+    <row r="8" spans="3:10" x14ac:dyDescent="0.3">
+      <c r="C8" s="60"/>
       <c r="D8" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="E8" s="49"/>
+      <c r="E8" s="44"/>
       <c r="F8" s="10" t="s">
         <v>110</v>
       </c>
       <c r="G8" s="6" t="s">
+        <v>222</v>
+      </c>
+      <c r="H8" s="6" t="s">
+        <v>222</v>
+      </c>
+      <c r="I8" s="25" t="s">
+        <v>207</v>
+      </c>
+      <c r="J8" s="4"/>
+    </row>
+    <row r="9" spans="3:10" x14ac:dyDescent="0.3">
+      <c r="C9" s="60" t="s">
+        <v>13</v>
+      </c>
+      <c r="D9" s="7" t="s">
+        <v>153</v>
+      </c>
+      <c r="E9" s="44"/>
+      <c r="F9" s="22" t="s">
+        <v>178</v>
+      </c>
+      <c r="G9" s="6" t="s">
         <v>223</v>
       </c>
-      <c r="H8" s="25" t="s">
-        <v>208</v>
-      </c>
-      <c r="I8" s="4"/>
-    </row>
-    <row r="9" spans="3:9" x14ac:dyDescent="0.3">
-      <c r="C9" s="51" t="s">
-        <v>13</v>
-      </c>
-      <c r="D9" s="7" t="s">
+      <c r="H9" s="6" t="s">
+        <v>223</v>
+      </c>
+      <c r="I9" s="25" t="s">
+        <v>207</v>
+      </c>
+      <c r="J9" s="4"/>
+    </row>
+    <row r="10" spans="3:10" x14ac:dyDescent="0.3">
+      <c r="C10" s="60"/>
+      <c r="D10" s="7" t="s">
         <v>154</v>
       </c>
-      <c r="E9" s="49"/>
-      <c r="F9" s="22" t="s">
+      <c r="E10" s="44"/>
+      <c r="F10" s="22" t="s">
         <v>179</v>
       </c>
-      <c r="G9" s="6" t="s">
+      <c r="G10" s="6" t="s">
         <v>224</v>
       </c>
-      <c r="H9" s="25" t="s">
-        <v>208</v>
-      </c>
-      <c r="I9" s="4"/>
-    </row>
-    <row r="10" spans="3:9" x14ac:dyDescent="0.3">
-      <c r="C10" s="51"/>
-      <c r="D10" s="7" t="s">
+      <c r="H10" s="6" t="s">
+        <v>224</v>
+      </c>
+      <c r="I10" s="25" t="s">
+        <v>207</v>
+      </c>
+      <c r="J10" s="4"/>
+    </row>
+    <row r="11" spans="3:10" ht="34.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C11" s="60"/>
+      <c r="D11" s="7" t="s">
         <v>155</v>
       </c>
-      <c r="E10" s="49"/>
-      <c r="F10" s="22" t="s">
+      <c r="E11" s="44"/>
+      <c r="F11" s="22" t="s">
         <v>180</v>
       </c>
-      <c r="G10" s="6" t="s">
+      <c r="G11" s="6" t="s">
         <v>225</v>
       </c>
-      <c r="H10" s="25" t="s">
-        <v>208</v>
-      </c>
-      <c r="I10" s="4"/>
-    </row>
-    <row r="11" spans="3:9" ht="34.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C11" s="51"/>
-      <c r="D11" s="7" t="s">
+      <c r="H11" s="6" t="s">
+        <v>225</v>
+      </c>
+      <c r="I11" s="25" t="s">
+        <v>207</v>
+      </c>
+      <c r="J11" s="4"/>
+    </row>
+    <row r="12" spans="3:10" ht="34.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C12" s="60"/>
+      <c r="D12" s="7" t="s">
         <v>156</v>
       </c>
-      <c r="E11" s="49"/>
-      <c r="F11" s="22" t="s">
+      <c r="E12" s="44"/>
+      <c r="F12" s="22" t="s">
         <v>181</v>
       </c>
-      <c r="G11" s="6" t="s">
+      <c r="G12" s="6" t="s">
         <v>226</v>
       </c>
-      <c r="H11" s="25" t="s">
-        <v>208</v>
-      </c>
-      <c r="I11" s="4"/>
-    </row>
-    <row r="12" spans="3:9" ht="34.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C12" s="51"/>
-      <c r="D12" s="7" t="s">
+      <c r="H12" s="6" t="s">
+        <v>226</v>
+      </c>
+      <c r="I12" s="25" t="s">
+        <v>207</v>
+      </c>
+      <c r="J12" s="4"/>
+    </row>
+    <row r="13" spans="3:10" ht="65.45" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C13" s="60"/>
+      <c r="D13" s="7" t="s">
         <v>157</v>
       </c>
-      <c r="E12" s="49"/>
-      <c r="F12" s="22" t="s">
+      <c r="E13" s="44"/>
+      <c r="F13" s="22" t="s">
         <v>182</v>
       </c>
-      <c r="G12" s="6" t="s">
+      <c r="G13" s="6" t="s">
         <v>227</v>
       </c>
-      <c r="H12" s="25" t="s">
-        <v>208</v>
-      </c>
-      <c r="I12" s="4"/>
-    </row>
-    <row r="13" spans="3:9" ht="65.45" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C13" s="51"/>
-      <c r="D13" s="7" t="s">
+      <c r="H13" s="6" t="s">
+        <v>227</v>
+      </c>
+      <c r="I13" s="25" t="s">
+        <v>207</v>
+      </c>
+      <c r="J13" s="4"/>
+    </row>
+    <row r="14" spans="3:10" ht="46.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C14" s="60"/>
+      <c r="D14" s="7" t="s">
         <v>158</v>
       </c>
-      <c r="E13" s="49"/>
-      <c r="F13" s="22" t="s">
+      <c r="E14" s="44"/>
+      <c r="F14" s="22" t="s">
         <v>183</v>
       </c>
-      <c r="G13" s="6" t="s">
+      <c r="G14" s="6" t="s">
         <v>228</v>
       </c>
-      <c r="H13" s="25" t="s">
-        <v>208</v>
-      </c>
-      <c r="I13" s="4"/>
-    </row>
-    <row r="14" spans="3:9" ht="46.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C14" s="51"/>
-      <c r="D14" s="7" t="s">
+      <c r="H14" s="6" t="s">
+        <v>228</v>
+      </c>
+      <c r="I14" s="25" t="s">
+        <v>207</v>
+      </c>
+      <c r="J14" s="4"/>
+    </row>
+    <row r="15" spans="3:10" ht="66.150000000000006" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C15" s="60"/>
+      <c r="D15" s="7" t="s">
         <v>159</v>
       </c>
-      <c r="E14" s="49"/>
-      <c r="F14" s="22" t="s">
+      <c r="E15" s="44"/>
+      <c r="F15" s="22" t="s">
         <v>184</v>
       </c>
-      <c r="G14" s="6" t="s">
+      <c r="G15" s="6" t="s">
         <v>229</v>
       </c>
-      <c r="H14" s="25" t="s">
-        <v>208</v>
-      </c>
-      <c r="I14" s="4"/>
-    </row>
-    <row r="15" spans="3:9" ht="66.150000000000006" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C15" s="51"/>
-      <c r="D15" s="7" t="s">
-        <v>160</v>
-      </c>
-      <c r="E15" s="49"/>
-      <c r="F15" s="22" t="s">
-        <v>185</v>
-      </c>
-      <c r="G15" s="6" t="s">
-        <v>230</v>
-      </c>
-      <c r="H15" s="25" t="s">
-        <v>208</v>
-      </c>
-      <c r="I15" s="4"/>
-    </row>
-    <row r="16" spans="3:9" x14ac:dyDescent="0.3">
-      <c r="C16" s="51" t="s">
+      <c r="H15" s="6" t="s">
+        <v>229</v>
+      </c>
+      <c r="I15" s="25" t="s">
+        <v>207</v>
+      </c>
+      <c r="J15" s="4"/>
+    </row>
+    <row r="16" spans="3:10" x14ac:dyDescent="0.3">
+      <c r="C16" s="60" t="s">
         <v>14</v>
       </c>
       <c r="D16" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="E16" s="49"/>
+      <c r="E16" s="44"/>
       <c r="F16" s="9" t="s">
         <v>112</v>
       </c>
       <c r="G16" s="6" t="s">
-        <v>231</v>
-      </c>
-      <c r="H16" s="25" t="s">
-        <v>208</v>
-      </c>
-      <c r="I16" s="4"/>
-    </row>
-    <row r="17" spans="3:9" x14ac:dyDescent="0.3">
-      <c r="C17" s="51"/>
+        <v>230</v>
+      </c>
+      <c r="H16" s="6" t="s">
+        <v>230</v>
+      </c>
+      <c r="I16" s="25" t="s">
+        <v>207</v>
+      </c>
+      <c r="J16" s="4"/>
+    </row>
+    <row r="17" spans="3:10" x14ac:dyDescent="0.3">
+      <c r="C17" s="60"/>
       <c r="D17" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="E17" s="49"/>
+      <c r="E17" s="44"/>
       <c r="F17" s="9" t="s">
         <v>113</v>
       </c>
       <c r="G17" s="6" t="s">
-        <v>232</v>
-      </c>
-      <c r="H17" s="25" t="s">
-        <v>208</v>
-      </c>
-      <c r="I17" s="4"/>
-    </row>
-    <row r="18" spans="3:9" ht="15.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C18" s="48" t="s">
+        <v>231</v>
+      </c>
+      <c r="H17" s="6" t="s">
+        <v>231</v>
+      </c>
+      <c r="I17" s="25" t="s">
+        <v>207</v>
+      </c>
+      <c r="J17" s="4"/>
+    </row>
+    <row r="18" spans="3:10" ht="15.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C18" s="43" t="s">
         <v>114</v>
       </c>
       <c r="D18" s="7" t="s">
         <v>115</v>
       </c>
-      <c r="E18" s="49"/>
-      <c r="F18" s="48" t="s">
-        <v>199</v>
+      <c r="E18" s="44"/>
+      <c r="F18" s="43" t="s">
+        <v>198</v>
       </c>
       <c r="G18" s="6" t="s">
-        <v>235</v>
-      </c>
-      <c r="H18" s="42" t="s">
-        <v>208</v>
-      </c>
-      <c r="I18" s="37"/>
-    </row>
-    <row r="19" spans="3:9" x14ac:dyDescent="0.3">
-      <c r="C19" s="49"/>
+        <v>234</v>
+      </c>
+      <c r="H18" s="6" t="s">
+        <v>234</v>
+      </c>
+      <c r="I18" s="51" t="s">
+        <v>207</v>
+      </c>
+      <c r="J18" s="37"/>
+    </row>
+    <row r="19" spans="3:10" x14ac:dyDescent="0.3">
+      <c r="C19" s="44"/>
       <c r="D19" s="7" t="s">
         <v>116</v>
       </c>
-      <c r="E19" s="49"/>
-      <c r="F19" s="49"/>
+      <c r="E19" s="44"/>
+      <c r="F19" s="44"/>
       <c r="G19" s="6" t="s">
-        <v>233</v>
-      </c>
-      <c r="H19" s="43"/>
-      <c r="I19" s="39"/>
-    </row>
-    <row r="20" spans="3:9" x14ac:dyDescent="0.3">
-      <c r="C20" s="49"/>
+        <v>232</v>
+      </c>
+      <c r="H19" s="6" t="s">
+        <v>232</v>
+      </c>
+      <c r="I19" s="52"/>
+      <c r="J19" s="39"/>
+    </row>
+    <row r="20" spans="3:10" x14ac:dyDescent="0.3">
+      <c r="C20" s="44"/>
       <c r="D20" s="7" t="s">
         <v>117</v>
       </c>
-      <c r="E20" s="49"/>
-      <c r="F20" s="49"/>
+      <c r="E20" s="44"/>
+      <c r="F20" s="44"/>
       <c r="G20" s="6" t="s">
-        <v>236</v>
-      </c>
-      <c r="H20" s="43"/>
-      <c r="I20" s="39"/>
-    </row>
-    <row r="21" spans="3:9" x14ac:dyDescent="0.3">
-      <c r="C21" s="49"/>
+        <v>235</v>
+      </c>
+      <c r="H20" s="6" t="s">
+        <v>235</v>
+      </c>
+      <c r="I20" s="52"/>
+      <c r="J20" s="39"/>
+    </row>
+    <row r="21" spans="3:10" x14ac:dyDescent="0.3">
+      <c r="C21" s="44"/>
       <c r="D21" s="7" t="s">
         <v>118</v>
       </c>
-      <c r="E21" s="49"/>
-      <c r="F21" s="49"/>
+      <c r="E21" s="44"/>
+      <c r="F21" s="44"/>
       <c r="G21" s="6" t="s">
-        <v>234</v>
-      </c>
-      <c r="H21" s="43"/>
-      <c r="I21" s="39"/>
-    </row>
-    <row r="22" spans="3:9" x14ac:dyDescent="0.3">
-      <c r="C22" s="50"/>
+        <v>233</v>
+      </c>
+      <c r="H21" s="6" t="s">
+        <v>233</v>
+      </c>
+      <c r="I21" s="52"/>
+      <c r="J21" s="39"/>
+    </row>
+    <row r="22" spans="3:10" x14ac:dyDescent="0.3">
+      <c r="C22" s="45"/>
       <c r="D22" s="7" t="s">
-        <v>200</v>
-      </c>
-      <c r="E22" s="49"/>
-      <c r="F22" s="50"/>
+        <v>199</v>
+      </c>
+      <c r="E22" s="44"/>
+      <c r="F22" s="45"/>
       <c r="G22" s="6" t="s">
-        <v>237</v>
-      </c>
-      <c r="H22" s="44"/>
-      <c r="I22" s="38"/>
-    </row>
-    <row r="23" spans="3:9" ht="30.15" x14ac:dyDescent="0.3">
+        <v>236</v>
+      </c>
+      <c r="H22" s="6" t="s">
+        <v>236</v>
+      </c>
+      <c r="I22" s="53"/>
+      <c r="J22" s="38"/>
+    </row>
+    <row r="23" spans="3:10" ht="30.15" x14ac:dyDescent="0.3">
       <c r="C23" s="3" t="s">
         <v>17</v>
       </c>
       <c r="D23" s="7" t="s">
         <v>62</v>
       </c>
-      <c r="E23" s="49"/>
+      <c r="E23" s="44"/>
       <c r="F23" s="9" t="s">
         <v>119</v>
       </c>
       <c r="G23" s="6" t="s">
-        <v>238</v>
-      </c>
-      <c r="H23" s="25" t="s">
-        <v>208</v>
-      </c>
-      <c r="I23" s="4"/>
-    </row>
-    <row r="24" spans="3:9" x14ac:dyDescent="0.3">
-      <c r="C24" s="51" t="s">
+        <v>237</v>
+      </c>
+      <c r="H23" s="6" t="s">
+        <v>237</v>
+      </c>
+      <c r="I23" s="25" t="s">
+        <v>207</v>
+      </c>
+      <c r="J23" s="4"/>
+    </row>
+    <row r="24" spans="3:10" x14ac:dyDescent="0.3">
+      <c r="C24" s="60" t="s">
         <v>120</v>
       </c>
       <c r="D24" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="E24" s="49"/>
+      <c r="E24" s="44"/>
       <c r="F24" s="11" t="s">
+        <v>215</v>
+      </c>
+      <c r="G24" s="6" t="s">
+        <v>241</v>
+      </c>
+      <c r="H24" s="6" t="s">
+        <v>241</v>
+      </c>
+      <c r="I24" s="25" t="s">
+        <v>207</v>
+      </c>
+      <c r="J24" s="4"/>
+    </row>
+    <row r="25" spans="3:10" ht="135.5" x14ac:dyDescent="0.3">
+      <c r="C25" s="60"/>
+      <c r="D25" s="7" t="s">
         <v>216</v>
       </c>
-      <c r="G24" s="6" t="s">
-        <v>242</v>
-      </c>
-      <c r="H24" s="25" t="s">
-        <v>208</v>
-      </c>
-      <c r="I24" s="4"/>
-    </row>
-    <row r="25" spans="3:9" ht="135.5" x14ac:dyDescent="0.3">
-      <c r="C25" s="51"/>
-      <c r="D25" s="7" t="s">
-        <v>217</v>
-      </c>
-      <c r="E25" s="49"/>
+      <c r="E25" s="44"/>
       <c r="F25" s="11" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="G25" s="6" t="s">
-        <v>239</v>
-      </c>
-      <c r="H25" s="25" t="s">
-        <v>208</v>
-      </c>
-      <c r="I25" s="4"/>
-    </row>
-    <row r="26" spans="3:9" ht="45.2" x14ac:dyDescent="0.3">
-      <c r="C26" s="51"/>
+        <v>238</v>
+      </c>
+      <c r="H25" s="6" t="s">
+        <v>238</v>
+      </c>
+      <c r="I25" s="25" t="s">
+        <v>207</v>
+      </c>
+      <c r="J25" s="4"/>
+    </row>
+    <row r="26" spans="3:10" ht="45.2" x14ac:dyDescent="0.3">
+      <c r="C26" s="60"/>
       <c r="D26" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="E26" s="49"/>
+      <c r="E26" s="44"/>
       <c r="F26" s="11" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="G26" s="6" t="s">
-        <v>240</v>
-      </c>
-      <c r="H26" s="25" t="s">
-        <v>208</v>
-      </c>
-      <c r="I26" s="4"/>
-    </row>
-    <row r="27" spans="3:9" ht="45.2" x14ac:dyDescent="0.3">
-      <c r="C27" s="51"/>
+        <v>239</v>
+      </c>
+      <c r="H26" s="6" t="s">
+        <v>239</v>
+      </c>
+      <c r="I26" s="25" t="s">
+        <v>207</v>
+      </c>
+      <c r="J26" s="4"/>
+    </row>
+    <row r="27" spans="3:10" ht="45.2" x14ac:dyDescent="0.3">
+      <c r="C27" s="60"/>
       <c r="D27" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="E27" s="50"/>
+      <c r="E27" s="45"/>
       <c r="F27" s="11" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="G27" s="6" t="s">
-        <v>241</v>
-      </c>
-      <c r="H27" s="25" t="s">
-        <v>208</v>
-      </c>
-      <c r="I27" s="4"/>
-    </row>
-    <row r="28" spans="3:9" x14ac:dyDescent="0.3">
-      <c r="C28" s="51" t="s">
+        <v>240</v>
+      </c>
+      <c r="H27" s="6" t="s">
+        <v>240</v>
+      </c>
+      <c r="I27" s="25" t="s">
+        <v>207</v>
+      </c>
+      <c r="J27" s="4"/>
+    </row>
+    <row r="28" spans="3:10" x14ac:dyDescent="0.3">
+      <c r="C28" s="60" t="s">
         <v>23</v>
       </c>
       <c r="D28" s="7" t="s">
         <v>21</v>
       </c>
       <c r="E28" s="5"/>
-      <c r="F28" s="52" t="s">
+      <c r="F28" s="46" t="s">
+        <v>306</v>
+      </c>
+      <c r="G28" s="46" t="s">
         <v>307</v>
       </c>
-      <c r="G28" s="52" t="s">
-        <v>308</v>
-      </c>
-      <c r="H28" s="55" t="s">
-        <v>208</v>
-      </c>
-      <c r="I28" s="58"/>
-    </row>
-    <row r="29" spans="3:9" x14ac:dyDescent="0.3">
-      <c r="C29" s="51"/>
+      <c r="H28" s="46" t="s">
+        <v>307</v>
+      </c>
+      <c r="I28" s="57" t="s">
+        <v>207</v>
+      </c>
+      <c r="J28" s="40"/>
+    </row>
+    <row r="29" spans="3:10" x14ac:dyDescent="0.3">
+      <c r="C29" s="60"/>
       <c r="D29" s="7" t="s">
         <v>22</v>
       </c>
       <c r="E29" s="5"/>
-      <c r="F29" s="53"/>
-      <c r="G29" s="53"/>
-      <c r="H29" s="56"/>
-      <c r="I29" s="59"/>
-    </row>
-    <row r="30" spans="3:9" x14ac:dyDescent="0.3">
-      <c r="C30" s="51" t="s">
+      <c r="F29" s="47"/>
+      <c r="G29" s="47"/>
+      <c r="H29" s="47"/>
+      <c r="I29" s="58"/>
+      <c r="J29" s="41"/>
+    </row>
+    <row r="30" spans="3:10" x14ac:dyDescent="0.3">
+      <c r="C30" s="60" t="s">
         <v>24</v>
       </c>
       <c r="D30" s="7" t="s">
         <v>25</v>
       </c>
       <c r="E30" s="5"/>
-      <c r="F30" s="53"/>
-      <c r="G30" s="53"/>
-      <c r="H30" s="56"/>
-      <c r="I30" s="59"/>
-    </row>
-    <row r="31" spans="3:9" x14ac:dyDescent="0.3">
-      <c r="C31" s="51"/>
+      <c r="F30" s="47"/>
+      <c r="G30" s="47"/>
+      <c r="H30" s="47"/>
+      <c r="I30" s="58"/>
+      <c r="J30" s="41"/>
+    </row>
+    <row r="31" spans="3:10" x14ac:dyDescent="0.3">
+      <c r="C31" s="60"/>
       <c r="D31" s="7" t="s">
         <v>26</v>
       </c>
       <c r="E31" s="5"/>
-      <c r="F31" s="53"/>
-      <c r="G31" s="53"/>
-      <c r="H31" s="56"/>
-      <c r="I31" s="59"/>
-    </row>
-    <row r="32" spans="3:9" x14ac:dyDescent="0.3">
-      <c r="C32" s="51"/>
+      <c r="F31" s="47"/>
+      <c r="G31" s="47"/>
+      <c r="H31" s="47"/>
+      <c r="I31" s="58"/>
+      <c r="J31" s="41"/>
+    </row>
+    <row r="32" spans="3:10" x14ac:dyDescent="0.3">
+      <c r="C32" s="60"/>
       <c r="D32" s="7" t="s">
         <v>27</v>
       </c>
       <c r="E32" s="5"/>
-      <c r="F32" s="54"/>
-      <c r="G32" s="54"/>
-      <c r="H32" s="57"/>
-      <c r="I32" s="60"/>
-    </row>
-    <row r="33" spans="3:9" ht="60.25" x14ac:dyDescent="0.3">
-      <c r="C33" s="48" t="s">
+      <c r="F32" s="48"/>
+      <c r="G32" s="48"/>
+      <c r="H32" s="48"/>
+      <c r="I32" s="59"/>
+      <c r="J32" s="42"/>
+    </row>
+    <row r="33" spans="3:10" ht="60.25" x14ac:dyDescent="0.3">
+      <c r="C33" s="43" t="s">
         <v>28</v>
       </c>
       <c r="D33" s="7" t="s">
-        <v>125</v>
-      </c>
-      <c r="E33" s="48" t="s">
+        <v>124</v>
+      </c>
+      <c r="E33" s="43" t="s">
         <v>122</v>
       </c>
       <c r="F33" s="20" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="G33" s="6" t="s">
-        <v>244</v>
-      </c>
-      <c r="H33" s="25" t="s">
-        <v>208</v>
-      </c>
-      <c r="I33" s="4"/>
-    </row>
-    <row r="34" spans="3:9" ht="30.15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C34" s="49"/>
+        <v>243</v>
+      </c>
+      <c r="H33" s="6"/>
+      <c r="I33" s="25" t="s">
+        <v>207</v>
+      </c>
+      <c r="J33" s="4"/>
+    </row>
+    <row r="34" spans="3:10" ht="30.15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C34" s="44"/>
       <c r="D34" s="7">
         <v>10</v>
       </c>
-      <c r="E34" s="49"/>
+      <c r="E34" s="44"/>
       <c r="F34" s="17" t="s">
-        <v>188</v>
-      </c>
-      <c r="G34" s="45" t="s">
-        <v>243</v>
-      </c>
-      <c r="H34" s="25" t="s">
-        <v>208</v>
-      </c>
-      <c r="I34" s="4"/>
-    </row>
-    <row r="35" spans="3:9" ht="30.15" x14ac:dyDescent="0.3">
-      <c r="C35" s="49"/>
+        <v>187</v>
+      </c>
+      <c r="G34" s="54" t="s">
+        <v>242</v>
+      </c>
+      <c r="H34" s="54"/>
+      <c r="I34" s="25" t="s">
+        <v>207</v>
+      </c>
+      <c r="J34" s="4"/>
+    </row>
+    <row r="35" spans="3:10" ht="30.15" x14ac:dyDescent="0.3">
+      <c r="C35" s="44"/>
       <c r="D35" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="E35" s="49"/>
+      <c r="E35" s="44"/>
       <c r="F35" s="17" t="s">
-        <v>189</v>
-      </c>
-      <c r="G35" s="47"/>
-      <c r="H35" s="25" t="s">
-        <v>208</v>
-      </c>
-      <c r="I35" s="4"/>
-    </row>
-    <row r="36" spans="3:9" ht="30.15" x14ac:dyDescent="0.3">
-      <c r="C36" s="49"/>
+        <v>188</v>
+      </c>
+      <c r="G35" s="56"/>
+      <c r="H35" s="56"/>
+      <c r="I35" s="25" t="s">
+        <v>207</v>
+      </c>
+      <c r="J35" s="4"/>
+    </row>
+    <row r="36" spans="3:10" ht="30.15" x14ac:dyDescent="0.3">
+      <c r="C36" s="44"/>
       <c r="D36" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="E36" s="49"/>
+      <c r="E36" s="44"/>
       <c r="F36" s="17" t="s">
-        <v>190</v>
-      </c>
-      <c r="G36" s="47"/>
-      <c r="H36" s="25" t="s">
-        <v>208</v>
-      </c>
-      <c r="I36" s="4"/>
-    </row>
-    <row r="37" spans="3:9" x14ac:dyDescent="0.3">
-      <c r="C37" s="50"/>
+        <v>189</v>
+      </c>
+      <c r="G36" s="56"/>
+      <c r="H36" s="56"/>
+      <c r="I36" s="25" t="s">
+        <v>207</v>
+      </c>
+      <c r="J36" s="4"/>
+    </row>
+    <row r="37" spans="3:10" x14ac:dyDescent="0.3">
+      <c r="C37" s="45"/>
       <c r="D37" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="E37" s="49"/>
+      <c r="E37" s="44"/>
       <c r="F37" s="17" t="s">
-        <v>191</v>
-      </c>
-      <c r="G37" s="46"/>
-      <c r="H37" s="25" t="s">
-        <v>208</v>
-      </c>
-      <c r="I37" s="4"/>
-    </row>
-    <row r="38" spans="3:9" ht="30.15" x14ac:dyDescent="0.3">
+        <v>190</v>
+      </c>
+      <c r="G37" s="55"/>
+      <c r="H37" s="55"/>
+      <c r="I37" s="25" t="s">
+        <v>207</v>
+      </c>
+      <c r="J37" s="4"/>
+    </row>
+    <row r="38" spans="3:10" ht="30.15" x14ac:dyDescent="0.3">
       <c r="C38" s="3" t="s">
         <v>32</v>
       </c>
       <c r="D38" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="E38" s="50"/>
+      <c r="E38" s="45"/>
       <c r="F38" s="11" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="G38" s="6" t="s">
-        <v>245</v>
-      </c>
-      <c r="H38" s="25" t="s">
-        <v>208</v>
-      </c>
-      <c r="I38" s="4"/>
-    </row>
-    <row r="39" spans="3:9" x14ac:dyDescent="0.3">
+        <v>244</v>
+      </c>
+      <c r="H38" s="6" t="s">
+        <v>244</v>
+      </c>
+      <c r="I38" s="25" t="s">
+        <v>207</v>
+      </c>
+      <c r="J38" s="4"/>
+    </row>
+    <row r="39" spans="3:10" x14ac:dyDescent="0.3">
       <c r="C39" s="3" t="s">
         <v>34</v>
       </c>
       <c r="D39" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="E39" s="51" t="s">
+      <c r="E39" s="60" t="s">
         <v>123</v>
       </c>
       <c r="F39" s="11" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="G39" s="6" t="s">
-        <v>300</v>
-      </c>
-      <c r="H39" s="25" t="s">
-        <v>208</v>
-      </c>
-      <c r="I39" s="4"/>
-    </row>
-    <row r="40" spans="3:9" ht="105.4" x14ac:dyDescent="0.3">
-      <c r="C40" s="51" t="s">
+        <v>299</v>
+      </c>
+      <c r="H39" s="6" t="s">
+        <v>299</v>
+      </c>
+      <c r="I39" s="25" t="s">
+        <v>207</v>
+      </c>
+      <c r="J39" s="25" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="40" spans="3:10" ht="105.4" x14ac:dyDescent="0.3">
+      <c r="C40" s="60" t="s">
         <v>36</v>
       </c>
       <c r="D40" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="E40" s="51"/>
+      <c r="E40" s="60"/>
       <c r="F40" s="6" t="s">
-        <v>295</v>
-      </c>
-      <c r="G40" s="48" t="s">
-        <v>311</v>
-      </c>
-      <c r="H40" s="42" t="s">
-        <v>208</v>
-      </c>
-      <c r="I40" s="4"/>
-    </row>
-    <row r="41" spans="3:9" ht="165.6" x14ac:dyDescent="0.3">
-      <c r="C41" s="51"/>
+        <v>294</v>
+      </c>
+      <c r="G40" s="43" t="s">
+        <v>310</v>
+      </c>
+      <c r="H40" s="43" t="s">
+        <v>310</v>
+      </c>
+      <c r="I40" s="51" t="s">
+        <v>207</v>
+      </c>
+      <c r="J40" s="51" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="41" spans="3:10" ht="165.6" x14ac:dyDescent="0.3">
+      <c r="C41" s="60"/>
       <c r="D41" s="7" t="s">
         <v>38</v>
       </c>
-      <c r="E41" s="51"/>
+      <c r="E41" s="60"/>
       <c r="F41" s="6" t="s">
-        <v>296</v>
-      </c>
-      <c r="G41" s="49"/>
-      <c r="H41" s="43"/>
-      <c r="I41" s="4"/>
-    </row>
-    <row r="42" spans="3:9" ht="60.25" x14ac:dyDescent="0.3">
-      <c r="C42" s="51"/>
+        <v>295</v>
+      </c>
+      <c r="G41" s="44"/>
+      <c r="H41" s="44"/>
+      <c r="I41" s="52"/>
+      <c r="J41" s="52"/>
+    </row>
+    <row r="42" spans="3:10" ht="60.25" x14ac:dyDescent="0.3">
+      <c r="C42" s="60"/>
       <c r="D42" s="7" t="s">
         <v>39</v>
       </c>
-      <c r="E42" s="51"/>
+      <c r="E42" s="60"/>
       <c r="F42" s="6" t="s">
-        <v>297</v>
-      </c>
-      <c r="G42" s="49"/>
-      <c r="H42" s="43"/>
-      <c r="I42" s="4"/>
-    </row>
-    <row r="43" spans="3:9" ht="60.25" x14ac:dyDescent="0.3">
-      <c r="C43" s="51"/>
+        <v>296</v>
+      </c>
+      <c r="G42" s="44"/>
+      <c r="H42" s="44"/>
+      <c r="I42" s="52"/>
+      <c r="J42" s="52"/>
+    </row>
+    <row r="43" spans="3:10" ht="60.25" x14ac:dyDescent="0.3">
+      <c r="C43" s="60"/>
       <c r="D43" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="E43" s="51"/>
+      <c r="E43" s="60"/>
       <c r="F43" s="6" t="s">
-        <v>299</v>
-      </c>
-      <c r="G43" s="49"/>
-      <c r="H43" s="43"/>
-      <c r="I43" s="4"/>
-    </row>
-    <row r="44" spans="3:9" x14ac:dyDescent="0.3">
-      <c r="C44" s="51"/>
+        <v>298</v>
+      </c>
+      <c r="G43" s="44"/>
+      <c r="H43" s="44"/>
+      <c r="I43" s="52"/>
+      <c r="J43" s="52"/>
+    </row>
+    <row r="44" spans="3:10" x14ac:dyDescent="0.3">
+      <c r="C44" s="60"/>
       <c r="D44" s="7" t="s">
         <v>41</v>
       </c>
-      <c r="E44" s="51"/>
+      <c r="E44" s="60"/>
       <c r="F44" s="34" t="s">
-        <v>298</v>
-      </c>
-      <c r="G44" s="50"/>
-      <c r="H44" s="44"/>
-      <c r="I44" s="4"/>
-    </row>
-    <row r="45" spans="3:9" ht="60.25" x14ac:dyDescent="0.3">
+        <v>297</v>
+      </c>
+      <c r="G44" s="45"/>
+      <c r="H44" s="45"/>
+      <c r="I44" s="53"/>
+      <c r="J44" s="53"/>
+    </row>
+    <row r="45" spans="3:10" ht="60.25" x14ac:dyDescent="0.3">
       <c r="C45" s="3" t="s">
         <v>42</v>
       </c>
       <c r="D45" s="7" t="s">
         <v>43</v>
       </c>
-      <c r="E45" s="51"/>
+      <c r="E45" s="60"/>
       <c r="F45" s="23" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="G45" s="6" t="s">
-        <v>301</v>
-      </c>
-      <c r="H45" s="25" t="s">
-        <v>208</v>
-      </c>
-      <c r="I45" s="4"/>
-    </row>
-    <row r="46" spans="3:9" ht="120.45" x14ac:dyDescent="0.3">
+        <v>300</v>
+      </c>
+      <c r="H45" s="6"/>
+      <c r="I45" s="25" t="s">
+        <v>207</v>
+      </c>
+      <c r="J45" s="25" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="46" spans="3:10" ht="120.45" x14ac:dyDescent="0.3">
       <c r="C46" s="3" t="s">
         <v>44</v>
       </c>
       <c r="D46" s="7" t="s">
         <v>45</v>
       </c>
-      <c r="E46" s="51"/>
+      <c r="E46" s="60"/>
       <c r="F46" s="11" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="G46" s="6" t="s">
-        <v>302</v>
-      </c>
-      <c r="H46" s="25" t="s">
-        <v>208</v>
-      </c>
-      <c r="I46" s="4"/>
-    </row>
-    <row r="47" spans="3:9" ht="90.35" x14ac:dyDescent="0.3">
+        <v>301</v>
+      </c>
+      <c r="H46" s="6"/>
+      <c r="I46" s="25" t="s">
+        <v>207</v>
+      </c>
+      <c r="J46" s="25" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="47" spans="3:10" ht="90.35" x14ac:dyDescent="0.3">
       <c r="C47" s="3" t="s">
         <v>46</v>
       </c>
       <c r="D47" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="E47" s="51"/>
+      <c r="E47" s="60"/>
       <c r="F47" s="11" t="s">
+        <v>302</v>
+      </c>
+      <c r="G47" s="6" t="s">
         <v>303</v>
       </c>
-      <c r="G47" s="6" t="s">
-        <v>304</v>
-      </c>
-      <c r="H47" s="25" t="s">
-        <v>208</v>
-      </c>
-      <c r="I47" s="4"/>
-    </row>
-    <row r="48" spans="3:9" ht="30.15" x14ac:dyDescent="0.3">
+      <c r="H47" s="6"/>
+      <c r="I47" s="25" t="s">
+        <v>207</v>
+      </c>
+      <c r="J47" s="25" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="48" spans="3:10" ht="30.15" x14ac:dyDescent="0.3">
       <c r="C48" s="3" t="s">
         <v>47</v>
       </c>
       <c r="D48" s="7" t="s">
         <v>49</v>
       </c>
-      <c r="E48" s="51"/>
+      <c r="E48" s="60"/>
       <c r="F48" s="11" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="G48" s="6" t="s">
-        <v>305</v>
-      </c>
-      <c r="H48" s="25" t="s">
-        <v>208</v>
-      </c>
-      <c r="I48" s="4"/>
-    </row>
-    <row r="49" spans="3:9" ht="120.45" x14ac:dyDescent="0.3">
+        <v>304</v>
+      </c>
+      <c r="H48" s="6"/>
+      <c r="I48" s="25" t="s">
+        <v>207</v>
+      </c>
+      <c r="J48" s="25" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="49" spans="3:10" ht="120.45" x14ac:dyDescent="0.3">
       <c r="C49" s="3" t="s">
         <v>50</v>
       </c>
@@ -2407,215 +2525,235 @@
         <v>51</v>
       </c>
       <c r="E49" s="21" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="F49" s="11" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="G49" s="6" t="s">
-        <v>306</v>
-      </c>
-      <c r="H49" s="25" t="s">
-        <v>208</v>
-      </c>
-      <c r="I49" s="4"/>
-    </row>
-    <row r="50" spans="3:9" ht="45.2" x14ac:dyDescent="0.3">
-      <c r="C50" s="48" t="s">
+        <v>305</v>
+      </c>
+      <c r="H49" s="6"/>
+      <c r="I49" s="25" t="s">
+        <v>207</v>
+      </c>
+      <c r="J49" s="4"/>
+    </row>
+    <row r="50" spans="3:10" ht="45.2" x14ac:dyDescent="0.3">
+      <c r="C50" s="43" t="s">
         <v>52</v>
       </c>
       <c r="D50" s="7" t="s">
-        <v>127</v>
-      </c>
-      <c r="E50" s="48" t="s">
+        <v>126</v>
+      </c>
+      <c r="E50" s="43" t="s">
         <v>122</v>
       </c>
       <c r="F50" s="18" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="G50" s="6" t="s">
-        <v>246</v>
-      </c>
-      <c r="H50" s="25" t="s">
-        <v>208</v>
-      </c>
-      <c r="I50" s="4"/>
-    </row>
-    <row r="51" spans="3:9" ht="30.15" x14ac:dyDescent="0.3">
-      <c r="C51" s="50"/>
+        <v>245</v>
+      </c>
+      <c r="H50" s="6"/>
+      <c r="I50" s="25" t="s">
+        <v>207</v>
+      </c>
+      <c r="J50" s="4"/>
+    </row>
+    <row r="51" spans="3:10" ht="30.15" x14ac:dyDescent="0.3">
+      <c r="C51" s="45"/>
       <c r="D51" s="7" t="s">
         <v>53</v>
       </c>
-      <c r="E51" s="49"/>
+      <c r="E51" s="44"/>
       <c r="F51" s="18" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="G51" s="6" t="s">
-        <v>247</v>
-      </c>
-      <c r="H51" s="25" t="s">
-        <v>208</v>
-      </c>
-      <c r="I51" s="4"/>
-    </row>
-    <row r="52" spans="3:9" ht="60.25" x14ac:dyDescent="0.3">
-      <c r="C52" s="48" t="s">
-        <v>219</v>
+        <v>246</v>
+      </c>
+      <c r="H51" s="6"/>
+      <c r="I51" s="25" t="s">
+        <v>207</v>
+      </c>
+      <c r="J51" s="4"/>
+    </row>
+    <row r="52" spans="3:10" ht="60.25" x14ac:dyDescent="0.3">
+      <c r="C52" s="43" t="s">
+        <v>218</v>
       </c>
       <c r="D52" s="7" t="s">
-        <v>125</v>
-      </c>
-      <c r="E52" s="49"/>
+        <v>124</v>
+      </c>
+      <c r="E52" s="44"/>
       <c r="F52" s="18" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="G52" s="6" t="s">
-        <v>244</v>
-      </c>
-      <c r="H52" s="25" t="s">
-        <v>208</v>
-      </c>
-      <c r="I52" s="4"/>
-    </row>
-    <row r="53" spans="3:9" ht="60.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C53" s="49"/>
+        <v>243</v>
+      </c>
+      <c r="H52" s="6"/>
+      <c r="I52" s="25" t="s">
+        <v>207</v>
+      </c>
+      <c r="J52" s="4"/>
+    </row>
+    <row r="53" spans="3:10" ht="60.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C53" s="44"/>
       <c r="D53" s="7" t="s">
         <v>54</v>
       </c>
-      <c r="E53" s="49"/>
+      <c r="E53" s="44"/>
       <c r="F53" s="22" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="G53" s="6" t="s">
-        <v>248</v>
-      </c>
-      <c r="H53" s="25" t="s">
-        <v>208</v>
-      </c>
-      <c r="I53" s="4"/>
-    </row>
-    <row r="54" spans="3:9" ht="120.45" x14ac:dyDescent="0.3">
-      <c r="C54" s="49"/>
+        <v>247</v>
+      </c>
+      <c r="H53" s="6"/>
+      <c r="I53" s="25" t="s">
+        <v>207</v>
+      </c>
+      <c r="J53" s="4"/>
+    </row>
+    <row r="54" spans="3:10" ht="120.45" x14ac:dyDescent="0.3">
+      <c r="C54" s="44"/>
       <c r="D54" s="7" t="s">
         <v>55</v>
       </c>
-      <c r="E54" s="49"/>
+      <c r="E54" s="44"/>
       <c r="F54" s="22" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="G54" s="6" t="s">
-        <v>249</v>
-      </c>
-      <c r="H54" s="25" t="s">
-        <v>208</v>
-      </c>
-      <c r="I54" s="4"/>
-    </row>
-    <row r="55" spans="3:9" ht="90.35" x14ac:dyDescent="0.3">
-      <c r="C55" s="49"/>
+        <v>248</v>
+      </c>
+      <c r="H54" s="6"/>
+      <c r="I54" s="25" t="s">
+        <v>207</v>
+      </c>
+      <c r="J54" s="4"/>
+    </row>
+    <row r="55" spans="3:10" ht="90.35" x14ac:dyDescent="0.3">
+      <c r="C55" s="44"/>
       <c r="D55" s="7" t="s">
         <v>56</v>
       </c>
-      <c r="E55" s="49"/>
+      <c r="E55" s="44"/>
       <c r="F55" s="22" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="G55" s="6" t="s">
-        <v>250</v>
-      </c>
-      <c r="H55" s="25" t="s">
-        <v>208</v>
-      </c>
-      <c r="I55" s="4"/>
-    </row>
-    <row r="56" spans="3:9" ht="45.2" x14ac:dyDescent="0.3">
-      <c r="C56" s="50"/>
+        <v>249</v>
+      </c>
+      <c r="H55" s="6"/>
+      <c r="I55" s="25" t="s">
+        <v>207</v>
+      </c>
+      <c r="J55" s="4"/>
+    </row>
+    <row r="56" spans="3:10" ht="45.2" x14ac:dyDescent="0.3">
+      <c r="C56" s="45"/>
       <c r="D56" s="7" t="s">
         <v>69</v>
       </c>
-      <c r="E56" s="49"/>
+      <c r="E56" s="44"/>
       <c r="F56" s="11" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="G56" s="6" t="s">
-        <v>251</v>
-      </c>
-      <c r="H56" s="25" t="s">
-        <v>208</v>
-      </c>
-      <c r="I56" s="4"/>
-    </row>
-    <row r="57" spans="3:9" ht="30.15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C57" s="51" t="s">
+        <v>250</v>
+      </c>
+      <c r="H56" s="6"/>
+      <c r="I56" s="25" t="s">
+        <v>207</v>
+      </c>
+      <c r="J56" s="4"/>
+    </row>
+    <row r="57" spans="3:10" ht="30.15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C57" s="60" t="s">
         <v>91</v>
       </c>
       <c r="D57" s="7" t="s">
         <v>57</v>
       </c>
-      <c r="E57" s="49"/>
+      <c r="E57" s="44"/>
       <c r="F57" s="9" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="G57" s="6" t="s">
-        <v>252</v>
-      </c>
-      <c r="H57" s="25" t="s">
-        <v>208</v>
-      </c>
-      <c r="I57" s="4"/>
-    </row>
-    <row r="58" spans="3:9" x14ac:dyDescent="0.3">
-      <c r="C58" s="51"/>
+        <v>251</v>
+      </c>
+      <c r="H57" s="6" t="s">
+        <v>251</v>
+      </c>
+      <c r="I57" s="25" t="s">
+        <v>207</v>
+      </c>
+      <c r="J57" s="4"/>
+    </row>
+    <row r="58" spans="3:10" x14ac:dyDescent="0.3">
+      <c r="C58" s="60"/>
       <c r="D58" s="7" t="s">
         <v>58</v>
       </c>
-      <c r="E58" s="49"/>
+      <c r="E58" s="44"/>
       <c r="F58" s="9" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="G58" s="6" t="s">
-        <v>253</v>
-      </c>
-      <c r="H58" s="25" t="s">
-        <v>208</v>
-      </c>
-      <c r="I58" s="4"/>
-    </row>
-    <row r="59" spans="3:9" ht="52.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C59" s="51"/>
+        <v>252</v>
+      </c>
+      <c r="H58" s="6" t="s">
+        <v>252</v>
+      </c>
+      <c r="I58" s="25" t="s">
+        <v>207</v>
+      </c>
+      <c r="J58" s="4"/>
+    </row>
+    <row r="59" spans="3:10" ht="52.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C59" s="60"/>
       <c r="D59" s="7" t="s">
         <v>59</v>
       </c>
-      <c r="E59" s="49"/>
+      <c r="E59" s="44"/>
       <c r="F59" s="9" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="G59" s="6" t="s">
-        <v>254</v>
-      </c>
-      <c r="H59" s="25" t="s">
-        <v>208</v>
-      </c>
-      <c r="I59" s="4"/>
-    </row>
-    <row r="60" spans="3:9" ht="30.15" x14ac:dyDescent="0.3">
-      <c r="C60" s="51"/>
+        <v>253</v>
+      </c>
+      <c r="H59" s="6" t="s">
+        <v>253</v>
+      </c>
+      <c r="I59" s="25" t="s">
+        <v>207</v>
+      </c>
+      <c r="J59" s="4"/>
+    </row>
+    <row r="60" spans="3:10" ht="30.15" x14ac:dyDescent="0.3">
+      <c r="C60" s="60"/>
       <c r="D60" s="7" t="s">
         <v>60</v>
       </c>
-      <c r="E60" s="50"/>
+      <c r="E60" s="45"/>
       <c r="F60" s="9" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="G60" s="6" t="s">
-        <v>255</v>
-      </c>
-      <c r="H60" s="25" t="s">
-        <v>208</v>
-      </c>
-      <c r="I60" s="4"/>
-    </row>
-    <row r="61" spans="3:9" x14ac:dyDescent="0.3">
+        <v>254</v>
+      </c>
+      <c r="H60" s="6" t="s">
+        <v>254</v>
+      </c>
+      <c r="I60" s="25" t="s">
+        <v>207</v>
+      </c>
+      <c r="J60" s="4"/>
+    </row>
+    <row r="61" spans="3:10" x14ac:dyDescent="0.3">
       <c r="C61" s="3" t="s">
         <v>61</v>
       </c>
@@ -2624,758 +2762,873 @@
       </c>
       <c r="E61" s="5"/>
       <c r="F61" s="11" t="s">
+        <v>308</v>
+      </c>
+      <c r="G61" s="22" t="s">
         <v>309</v>
       </c>
-      <c r="G61" s="22" t="s">
-        <v>310</v>
-      </c>
-      <c r="H61" s="35"/>
-      <c r="I61" s="36"/>
-    </row>
-    <row r="62" spans="3:9" ht="30.15" x14ac:dyDescent="0.3">
-      <c r="C62" s="51" t="s">
+      <c r="H61" s="22" t="s">
+        <v>309</v>
+      </c>
+      <c r="I61" s="35"/>
+      <c r="J61" s="36"/>
+    </row>
+    <row r="62" spans="3:10" ht="30.15" x14ac:dyDescent="0.3">
+      <c r="C62" s="60" t="s">
         <v>64</v>
       </c>
       <c r="D62" s="7" t="s">
         <v>65</v>
       </c>
-      <c r="E62" s="48" t="s">
+      <c r="E62" s="43" t="s">
         <v>122</v>
       </c>
       <c r="F62" s="9" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="G62" s="6" t="s">
-        <v>256</v>
-      </c>
-      <c r="H62" s="25" t="s">
-        <v>208</v>
-      </c>
-      <c r="I62" s="4"/>
-    </row>
-    <row r="63" spans="3:9" ht="60.25" x14ac:dyDescent="0.3">
-      <c r="C63" s="51"/>
+        <v>255</v>
+      </c>
+      <c r="H62" s="6"/>
+      <c r="I62" s="25" t="s">
+        <v>207</v>
+      </c>
+      <c r="J62" s="4"/>
+    </row>
+    <row r="63" spans="3:10" ht="60.25" x14ac:dyDescent="0.3">
+      <c r="C63" s="60"/>
       <c r="D63" s="7" t="s">
         <v>66</v>
       </c>
-      <c r="E63" s="49"/>
+      <c r="E63" s="44"/>
       <c r="F63" s="9" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="G63" s="6" t="s">
-        <v>257</v>
-      </c>
-      <c r="H63" s="25" t="s">
-        <v>208</v>
-      </c>
-      <c r="I63" s="4"/>
-    </row>
-    <row r="64" spans="3:9" ht="60.25" x14ac:dyDescent="0.3">
-      <c r="C64" s="51"/>
+        <v>256</v>
+      </c>
+      <c r="H63" s="6"/>
+      <c r="I63" s="25" t="s">
+        <v>207</v>
+      </c>
+      <c r="J63" s="4"/>
+    </row>
+    <row r="64" spans="3:10" ht="60.25" x14ac:dyDescent="0.3">
+      <c r="C64" s="60"/>
       <c r="D64" s="7" t="s">
         <v>67</v>
       </c>
-      <c r="E64" s="49"/>
+      <c r="E64" s="44"/>
       <c r="F64" s="9" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="G64" s="6" t="s">
-        <v>258</v>
-      </c>
-      <c r="H64" s="25" t="s">
-        <v>208</v>
-      </c>
-      <c r="I64" s="4"/>
-    </row>
-    <row r="65" spans="3:9" ht="30.15" x14ac:dyDescent="0.3">
-      <c r="C65" s="51"/>
+        <v>257</v>
+      </c>
+      <c r="H64" s="6"/>
+      <c r="I64" s="25" t="s">
+        <v>207</v>
+      </c>
+      <c r="J64" s="4"/>
+    </row>
+    <row r="65" spans="3:10" ht="30.15" x14ac:dyDescent="0.3">
+      <c r="C65" s="60"/>
       <c r="D65" s="7" t="s">
         <v>68</v>
       </c>
-      <c r="E65" s="49"/>
+      <c r="E65" s="44"/>
       <c r="F65" s="9" t="s">
+        <v>203</v>
+      </c>
+      <c r="G65" s="6" t="s">
+        <v>258</v>
+      </c>
+      <c r="H65" s="6"/>
+      <c r="I65" s="25" t="s">
+        <v>207</v>
+      </c>
+      <c r="J65" s="4"/>
+    </row>
+    <row r="66" spans="3:10" ht="60.25" x14ac:dyDescent="0.3">
+      <c r="C66" s="60"/>
+      <c r="D66" s="7" t="s">
+        <v>130</v>
+      </c>
+      <c r="E66" s="44"/>
+      <c r="F66" s="9" t="s">
         <v>204</v>
       </c>
-      <c r="G65" s="6" t="s">
+      <c r="G66" s="6" t="s">
+        <v>260</v>
+      </c>
+      <c r="H66" s="6"/>
+      <c r="I66" s="25" t="s">
+        <v>207</v>
+      </c>
+      <c r="J66" s="4"/>
+    </row>
+    <row r="67" spans="3:10" ht="120.45" x14ac:dyDescent="0.3">
+      <c r="C67" s="60"/>
+      <c r="D67" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="E67" s="44"/>
+      <c r="F67" s="9" t="s">
+        <v>205</v>
+      </c>
+      <c r="G67" s="6" t="s">
         <v>259</v>
       </c>
-      <c r="H65" s="25" t="s">
-        <v>208</v>
-      </c>
-      <c r="I65" s="4"/>
-    </row>
-    <row r="66" spans="3:9" ht="60.25" x14ac:dyDescent="0.3">
-      <c r="C66" s="51"/>
-      <c r="D66" s="7" t="s">
-        <v>131</v>
-      </c>
-      <c r="E66" s="49"/>
-      <c r="F66" s="9" t="s">
-        <v>205</v>
-      </c>
-      <c r="G66" s="6" t="s">
-        <v>261</v>
-      </c>
-      <c r="H66" s="25" t="s">
-        <v>208</v>
-      </c>
-      <c r="I66" s="4"/>
-    </row>
-    <row r="67" spans="3:9" ht="120.45" x14ac:dyDescent="0.3">
-      <c r="C67" s="51"/>
-      <c r="D67" s="2" t="s">
-        <v>132</v>
-      </c>
-      <c r="E67" s="49"/>
-      <c r="F67" s="9" t="s">
-        <v>206</v>
-      </c>
-      <c r="G67" s="6" t="s">
-        <v>260</v>
-      </c>
-      <c r="H67" s="25" t="s">
-        <v>208</v>
-      </c>
-      <c r="I67" s="4"/>
-    </row>
-    <row r="68" spans="3:9" x14ac:dyDescent="0.3">
+      <c r="H67" s="6"/>
+      <c r="I67" s="25" t="s">
+        <v>207</v>
+      </c>
+      <c r="J67" s="4"/>
+    </row>
+    <row r="68" spans="3:10" x14ac:dyDescent="0.3">
       <c r="C68" s="3" t="s">
         <v>70</v>
       </c>
       <c r="D68" s="7" t="s">
         <v>71</v>
       </c>
-      <c r="E68" s="49"/>
+      <c r="E68" s="44"/>
       <c r="F68" s="23" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="G68" s="6" t="s">
-        <v>262</v>
-      </c>
-      <c r="H68" s="25" t="s">
-        <v>208</v>
-      </c>
-      <c r="I68" s="4"/>
-    </row>
-    <row r="69" spans="3:9" ht="30.15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C69" s="51" t="s">
+        <v>261</v>
+      </c>
+      <c r="H68" s="6" t="s">
+        <v>261</v>
+      </c>
+      <c r="I68" s="25" t="s">
+        <v>207</v>
+      </c>
+      <c r="J68" s="4"/>
+    </row>
+    <row r="69" spans="3:10" ht="30.15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C69" s="60" t="s">
         <v>72</v>
       </c>
       <c r="D69" s="7" t="s">
         <v>73</v>
       </c>
-      <c r="E69" s="49"/>
+      <c r="E69" s="44"/>
       <c r="F69" s="9" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="G69" s="6" t="s">
-        <v>263</v>
-      </c>
-      <c r="H69" s="25" t="s">
-        <v>208</v>
-      </c>
-      <c r="I69" s="4"/>
-    </row>
-    <row r="70" spans="3:9" ht="30.15" x14ac:dyDescent="0.3">
-      <c r="C70" s="51"/>
+        <v>262</v>
+      </c>
+      <c r="H69" s="6" t="s">
+        <v>262</v>
+      </c>
+      <c r="I69" s="25" t="s">
+        <v>207</v>
+      </c>
+      <c r="J69" s="4"/>
+    </row>
+    <row r="70" spans="3:10" ht="30.15" x14ac:dyDescent="0.3">
+      <c r="C70" s="60"/>
       <c r="D70" s="7" t="s">
         <v>74</v>
       </c>
-      <c r="E70" s="49"/>
+      <c r="E70" s="44"/>
       <c r="F70" s="9" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="G70" s="6" t="s">
-        <v>264</v>
-      </c>
-      <c r="H70" s="25" t="s">
-        <v>208</v>
-      </c>
-      <c r="I70" s="4"/>
-    </row>
-    <row r="71" spans="3:9" x14ac:dyDescent="0.3">
-      <c r="C71" s="51"/>
+        <v>263</v>
+      </c>
+      <c r="H70" s="6" t="s">
+        <v>263</v>
+      </c>
+      <c r="I70" s="25" t="s">
+        <v>207</v>
+      </c>
+      <c r="J70" s="4"/>
+    </row>
+    <row r="71" spans="3:10" x14ac:dyDescent="0.3">
+      <c r="C71" s="60"/>
       <c r="D71" s="7" t="s">
         <v>75</v>
       </c>
-      <c r="E71" s="49"/>
+      <c r="E71" s="44"/>
       <c r="F71" s="9" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="G71" s="6" t="s">
+        <v>264</v>
+      </c>
+      <c r="H71" s="6" t="s">
+        <v>264</v>
+      </c>
+      <c r="I71" s="25" t="s">
+        <v>207</v>
+      </c>
+      <c r="J71" s="4"/>
+    </row>
+    <row r="72" spans="3:10" ht="30.15" x14ac:dyDescent="0.3">
+      <c r="C72" s="60"/>
+      <c r="D72" s="7" t="s">
+        <v>213</v>
+      </c>
+      <c r="E72" s="44"/>
+      <c r="F72" s="11" t="s">
+        <v>160</v>
+      </c>
+      <c r="G72" s="6" t="s">
         <v>265</v>
       </c>
-      <c r="H71" s="25" t="s">
-        <v>208</v>
-      </c>
-      <c r="I71" s="4"/>
-    </row>
-    <row r="72" spans="3:9" ht="30.15" x14ac:dyDescent="0.3">
-      <c r="C72" s="51"/>
-      <c r="D72" s="7" t="s">
-        <v>214</v>
-      </c>
-      <c r="E72" s="49"/>
-      <c r="F72" s="11" t="s">
-        <v>161</v>
-      </c>
-      <c r="G72" s="6" t="s">
-        <v>266</v>
-      </c>
-      <c r="H72" s="25" t="s">
-        <v>208</v>
-      </c>
-      <c r="I72" s="4"/>
-    </row>
-    <row r="73" spans="3:9" x14ac:dyDescent="0.3">
-      <c r="C73" s="51"/>
+      <c r="H72" s="6" t="s">
+        <v>265</v>
+      </c>
+      <c r="I72" s="25" t="s">
+        <v>207</v>
+      </c>
+      <c r="J72" s="4"/>
+    </row>
+    <row r="73" spans="3:10" x14ac:dyDescent="0.3">
+      <c r="C73" s="60"/>
       <c r="D73" s="7" t="s">
         <v>76</v>
       </c>
-      <c r="E73" s="49"/>
+      <c r="E73" s="44"/>
       <c r="F73" s="9" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="G73" s="6" t="s">
-        <v>267</v>
-      </c>
-      <c r="H73" s="25" t="s">
-        <v>208</v>
-      </c>
-      <c r="I73" s="4"/>
-    </row>
-    <row r="74" spans="3:9" x14ac:dyDescent="0.3">
-      <c r="C74" s="51"/>
+        <v>266</v>
+      </c>
+      <c r="H73" s="6" t="s">
+        <v>266</v>
+      </c>
+      <c r="I73" s="25" t="s">
+        <v>207</v>
+      </c>
+      <c r="J73" s="4"/>
+    </row>
+    <row r="74" spans="3:10" x14ac:dyDescent="0.3">
+      <c r="C74" s="60"/>
       <c r="D74" s="7" t="s">
         <v>77</v>
       </c>
-      <c r="E74" s="49"/>
+      <c r="E74" s="44"/>
       <c r="F74" s="9" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="G74" s="6" t="s">
-        <v>268</v>
-      </c>
-      <c r="H74" s="25" t="s">
-        <v>208</v>
-      </c>
-      <c r="I74" s="4"/>
-    </row>
-    <row r="75" spans="3:9" x14ac:dyDescent="0.3">
-      <c r="C75" s="51"/>
+        <v>267</v>
+      </c>
+      <c r="H74" s="6" t="s">
+        <v>267</v>
+      </c>
+      <c r="I74" s="25" t="s">
+        <v>207</v>
+      </c>
+      <c r="J74" s="4"/>
+    </row>
+    <row r="75" spans="3:10" x14ac:dyDescent="0.3">
+      <c r="C75" s="60"/>
       <c r="D75" s="7" t="s">
         <v>78</v>
       </c>
-      <c r="E75" s="49"/>
+      <c r="E75" s="44"/>
       <c r="F75" s="9" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="G75" s="6" t="s">
-        <v>269</v>
-      </c>
-      <c r="H75" s="25" t="s">
-        <v>208</v>
-      </c>
-      <c r="I75" s="4"/>
-    </row>
-    <row r="76" spans="3:9" x14ac:dyDescent="0.3">
-      <c r="C76" s="51"/>
+        <v>268</v>
+      </c>
+      <c r="H75" s="6" t="s">
+        <v>268</v>
+      </c>
+      <c r="I75" s="25" t="s">
+        <v>207</v>
+      </c>
+      <c r="J75" s="4"/>
+    </row>
+    <row r="76" spans="3:10" x14ac:dyDescent="0.3">
+      <c r="C76" s="60"/>
       <c r="D76" s="7" t="s">
         <v>79</v>
       </c>
-      <c r="E76" s="49"/>
+      <c r="E76" s="44"/>
       <c r="F76" s="9" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="G76" s="6" t="s">
-        <v>270</v>
-      </c>
-      <c r="H76" s="25" t="s">
-        <v>208</v>
-      </c>
-      <c r="I76" s="4"/>
-    </row>
-    <row r="77" spans="3:9" ht="30.15" x14ac:dyDescent="0.3">
-      <c r="C77" s="51"/>
+        <v>269</v>
+      </c>
+      <c r="H76" s="6" t="s">
+        <v>269</v>
+      </c>
+      <c r="I76" s="25" t="s">
+        <v>207</v>
+      </c>
+      <c r="J76" s="4"/>
+    </row>
+    <row r="77" spans="3:10" ht="30.15" x14ac:dyDescent="0.3">
+      <c r="C77" s="60"/>
       <c r="D77" s="7" t="s">
         <v>80</v>
       </c>
-      <c r="E77" s="49"/>
+      <c r="E77" s="44"/>
       <c r="F77" s="11" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="G77" s="6" t="s">
-        <v>271</v>
-      </c>
-      <c r="H77" s="25" t="s">
-        <v>208</v>
-      </c>
-      <c r="I77" s="4"/>
-    </row>
-    <row r="78" spans="3:9" ht="30.15" x14ac:dyDescent="0.3">
-      <c r="C78" s="51"/>
+        <v>270</v>
+      </c>
+      <c r="H77" s="6" t="s">
+        <v>270</v>
+      </c>
+      <c r="I77" s="25" t="s">
+        <v>207</v>
+      </c>
+      <c r="J77" s="4"/>
+    </row>
+    <row r="78" spans="3:10" ht="30.15" x14ac:dyDescent="0.3">
+      <c r="C78" s="60"/>
       <c r="D78" s="7" t="s">
         <v>81</v>
       </c>
-      <c r="E78" s="49"/>
+      <c r="E78" s="44"/>
       <c r="F78" s="24" t="s">
+        <v>139</v>
+      </c>
+      <c r="G78" s="31"/>
+      <c r="H78" s="31"/>
+      <c r="I78" s="32"/>
+      <c r="J78" s="33"/>
+    </row>
+    <row r="79" spans="3:10" ht="30.15" x14ac:dyDescent="0.3">
+      <c r="C79" s="44" t="s">
+        <v>83</v>
+      </c>
+      <c r="D79" s="7" t="s">
         <v>140</v>
       </c>
-      <c r="G78" s="31"/>
-      <c r="H78" s="32"/>
-      <c r="I78" s="33"/>
-    </row>
-    <row r="79" spans="3:9" ht="30.15" x14ac:dyDescent="0.3">
-      <c r="C79" s="49" t="s">
-        <v>83</v>
-      </c>
-      <c r="D79" s="7" t="s">
-        <v>141</v>
-      </c>
-      <c r="E79" s="49"/>
+      <c r="E79" s="44"/>
       <c r="F79" s="9" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="G79" s="6" t="s">
-        <v>278</v>
-      </c>
-      <c r="H79" s="25" t="s">
-        <v>208</v>
-      </c>
-      <c r="I79" s="4"/>
-    </row>
-    <row r="80" spans="3:9" ht="30.15" x14ac:dyDescent="0.3">
-      <c r="C80" s="49"/>
+        <v>277</v>
+      </c>
+      <c r="H79" s="6" t="s">
+        <v>277</v>
+      </c>
+      <c r="I79" s="25" t="s">
+        <v>207</v>
+      </c>
+      <c r="J79" s="4"/>
+    </row>
+    <row r="80" spans="3:10" ht="30.15" x14ac:dyDescent="0.3">
+      <c r="C80" s="44"/>
       <c r="D80" s="7" t="s">
         <v>82</v>
       </c>
-      <c r="E80" s="49"/>
+      <c r="E80" s="44"/>
       <c r="F80" s="9" t="s">
+        <v>162</v>
+      </c>
+      <c r="G80" s="6" t="s">
+        <v>278</v>
+      </c>
+      <c r="H80" s="6" t="s">
+        <v>278</v>
+      </c>
+      <c r="I80" s="25" t="s">
+        <v>207</v>
+      </c>
+      <c r="J80" s="4"/>
+    </row>
+    <row r="81" spans="3:10" ht="30.15" x14ac:dyDescent="0.3">
+      <c r="C81" s="43" t="s">
+        <v>84</v>
+      </c>
+      <c r="D81" s="7" t="s">
+        <v>143</v>
+      </c>
+      <c r="E81" s="44"/>
+      <c r="F81" s="9" t="s">
         <v>163</v>
       </c>
-      <c r="G80" s="6" t="s">
-        <v>279</v>
-      </c>
-      <c r="H80" s="25" t="s">
-        <v>208</v>
-      </c>
-      <c r="I80" s="4"/>
-    </row>
-    <row r="81" spans="3:9" ht="30.15" x14ac:dyDescent="0.3">
-      <c r="C81" s="48" t="s">
-        <v>84</v>
-      </c>
-      <c r="D81" s="7" t="s">
+      <c r="G81" s="6" t="s">
+        <v>280</v>
+      </c>
+      <c r="H81" s="6" t="s">
+        <v>280</v>
+      </c>
+      <c r="I81" s="25" t="s">
+        <v>207</v>
+      </c>
+      <c r="J81" s="4"/>
+    </row>
+    <row r="82" spans="3:10" ht="69.400000000000006" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C82" s="44"/>
+      <c r="D82" s="7" t="s">
         <v>144</v>
       </c>
-      <c r="E81" s="49"/>
-      <c r="F81" s="9" t="s">
-        <v>164</v>
-      </c>
-      <c r="G81" s="6" t="s">
+      <c r="E82" s="44"/>
+      <c r="F82" s="9" t="s">
+        <v>177</v>
+      </c>
+      <c r="G82" s="6" t="s">
         <v>281</v>
       </c>
-      <c r="H81" s="25" t="s">
-        <v>208</v>
-      </c>
-      <c r="I81" s="4"/>
-    </row>
-    <row r="82" spans="3:9" ht="69.400000000000006" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C82" s="49"/>
-      <c r="D82" s="7" t="s">
-        <v>145</v>
-      </c>
-      <c r="E82" s="49"/>
-      <c r="F82" s="9" t="s">
-        <v>178</v>
-      </c>
-      <c r="G82" s="6" t="s">
-        <v>282</v>
-      </c>
-      <c r="H82" s="25" t="s">
-        <v>208</v>
-      </c>
-      <c r="I82" s="4"/>
-    </row>
-    <row r="83" spans="3:9" x14ac:dyDescent="0.3">
-      <c r="C83" s="49"/>
+      <c r="H82" s="6" t="s">
+        <v>281</v>
+      </c>
+      <c r="I82" s="25" t="s">
+        <v>207</v>
+      </c>
+      <c r="J82" s="4"/>
+    </row>
+    <row r="83" spans="3:10" x14ac:dyDescent="0.3">
+      <c r="C83" s="44"/>
       <c r="D83" s="7" t="s">
         <v>85</v>
       </c>
-      <c r="E83" s="49"/>
+      <c r="E83" s="44"/>
       <c r="F83" s="24" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="G83" s="31"/>
-      <c r="H83" s="32"/>
-      <c r="I83" s="33"/>
-    </row>
-    <row r="84" spans="3:9" x14ac:dyDescent="0.3">
-      <c r="C84" s="49"/>
+      <c r="H83" s="31"/>
+      <c r="I83" s="32"/>
+      <c r="J83" s="33"/>
+    </row>
+    <row r="84" spans="3:10" x14ac:dyDescent="0.3">
+      <c r="C84" s="44"/>
       <c r="D84" s="7" t="s">
         <v>86</v>
       </c>
-      <c r="E84" s="49"/>
+      <c r="E84" s="44"/>
       <c r="F84" s="9" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="G84" s="6" t="s">
-        <v>283</v>
-      </c>
-      <c r="H84" s="25" t="s">
-        <v>208</v>
-      </c>
-      <c r="I84" s="4"/>
-    </row>
-    <row r="85" spans="3:9" ht="30.15" x14ac:dyDescent="0.3">
-      <c r="C85" s="49"/>
+        <v>282</v>
+      </c>
+      <c r="H84" s="6" t="s">
+        <v>282</v>
+      </c>
+      <c r="I84" s="25" t="s">
+        <v>207</v>
+      </c>
+      <c r="J84" s="4"/>
+    </row>
+    <row r="85" spans="3:10" ht="30.15" x14ac:dyDescent="0.3">
+      <c r="C85" s="44"/>
       <c r="D85" s="7" t="s">
         <v>87</v>
       </c>
-      <c r="E85" s="49"/>
+      <c r="E85" s="44"/>
       <c r="F85" s="9" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="G85" s="6" t="s">
-        <v>284</v>
-      </c>
-      <c r="H85" s="25" t="s">
-        <v>208</v>
-      </c>
-      <c r="I85" s="4"/>
-    </row>
-    <row r="86" spans="3:9" ht="30.15" x14ac:dyDescent="0.3">
-      <c r="C86" s="49"/>
+        <v>283</v>
+      </c>
+      <c r="H85" s="6" t="s">
+        <v>283</v>
+      </c>
+      <c r="I85" s="25" t="s">
+        <v>207</v>
+      </c>
+      <c r="J85" s="4"/>
+    </row>
+    <row r="86" spans="3:10" ht="30.15" x14ac:dyDescent="0.3">
+      <c r="C86" s="44"/>
       <c r="D86" s="7" t="s">
         <v>88</v>
       </c>
-      <c r="E86" s="49"/>
+      <c r="E86" s="44"/>
       <c r="F86" s="9" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="G86" s="6" t="s">
-        <v>285</v>
-      </c>
-      <c r="H86" s="25" t="s">
-        <v>208</v>
-      </c>
-      <c r="I86" s="4"/>
-    </row>
-    <row r="87" spans="3:9" x14ac:dyDescent="0.3">
-      <c r="C87" s="49"/>
+        <v>284</v>
+      </c>
+      <c r="H86" s="6" t="s">
+        <v>284</v>
+      </c>
+      <c r="I86" s="25" t="s">
+        <v>207</v>
+      </c>
+      <c r="J86" s="4"/>
+    </row>
+    <row r="87" spans="3:10" x14ac:dyDescent="0.3">
+      <c r="C87" s="44"/>
       <c r="D87" s="7" t="s">
         <v>89</v>
       </c>
-      <c r="E87" s="49"/>
+      <c r="E87" s="44"/>
       <c r="F87" s="9" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="G87" s="6" t="s">
-        <v>286</v>
-      </c>
-      <c r="H87" s="25" t="s">
-        <v>208</v>
-      </c>
-      <c r="I87" s="4"/>
-    </row>
-    <row r="88" spans="3:9" x14ac:dyDescent="0.3">
-      <c r="C88" s="49"/>
+        <v>285</v>
+      </c>
+      <c r="H87" s="6" t="s">
+        <v>285</v>
+      </c>
+      <c r="I87" s="25" t="s">
+        <v>207</v>
+      </c>
+      <c r="J87" s="4"/>
+    </row>
+    <row r="88" spans="3:10" x14ac:dyDescent="0.3">
+      <c r="C88" s="44"/>
       <c r="D88" s="7" t="s">
         <v>90</v>
       </c>
-      <c r="E88" s="49"/>
+      <c r="E88" s="44"/>
       <c r="F88" s="9" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="G88" s="6" t="s">
-        <v>287</v>
-      </c>
-      <c r="H88" s="25" t="s">
-        <v>208</v>
-      </c>
-      <c r="I88" s="4"/>
-    </row>
-    <row r="89" spans="3:9" ht="30.15" x14ac:dyDescent="0.3">
-      <c r="C89" s="49"/>
+        <v>286</v>
+      </c>
+      <c r="H88" s="6" t="s">
+        <v>286</v>
+      </c>
+      <c r="I88" s="25" t="s">
+        <v>207</v>
+      </c>
+      <c r="J88" s="4"/>
+    </row>
+    <row r="89" spans="3:10" ht="30.15" x14ac:dyDescent="0.3">
+      <c r="C89" s="44"/>
       <c r="D89" s="7" t="s">
         <v>97</v>
       </c>
-      <c r="E89" s="49"/>
+      <c r="E89" s="44"/>
       <c r="F89" s="11" t="s">
+        <v>279</v>
+      </c>
+      <c r="G89" s="22" t="s">
         <v>280</v>
       </c>
-      <c r="G89" s="22" t="s">
-        <v>281</v>
-      </c>
-      <c r="H89" s="35"/>
-      <c r="I89" s="36"/>
-    </row>
-    <row r="90" spans="3:9" x14ac:dyDescent="0.3">
-      <c r="C90" s="49"/>
+      <c r="H89" s="22" t="s">
+        <v>280</v>
+      </c>
+      <c r="I89" s="35"/>
+      <c r="J89" s="36"/>
+    </row>
+    <row r="90" spans="3:10" x14ac:dyDescent="0.3">
+      <c r="C90" s="44"/>
       <c r="D90" s="7" t="s">
         <v>98</v>
       </c>
-      <c r="E90" s="49"/>
+      <c r="E90" s="44"/>
       <c r="F90" s="9" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="G90" s="6" t="s">
-        <v>288</v>
-      </c>
-      <c r="H90" s="25" t="s">
-        <v>208</v>
-      </c>
-      <c r="I90" s="4"/>
-    </row>
-    <row r="91" spans="3:9" x14ac:dyDescent="0.3">
-      <c r="C91" s="49"/>
+        <v>287</v>
+      </c>
+      <c r="H90" s="6" t="s">
+        <v>287</v>
+      </c>
+      <c r="I90" s="25" t="s">
+        <v>207</v>
+      </c>
+      <c r="J90" s="4"/>
+    </row>
+    <row r="91" spans="3:10" x14ac:dyDescent="0.3">
+      <c r="C91" s="44"/>
       <c r="D91" s="7" t="s">
         <v>99</v>
       </c>
-      <c r="E91" s="49"/>
+      <c r="E91" s="44"/>
       <c r="F91" s="9" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="G91" s="6" t="s">
-        <v>289</v>
-      </c>
-      <c r="H91" s="25" t="s">
-        <v>208</v>
-      </c>
-      <c r="I91" s="4"/>
-    </row>
-    <row r="92" spans="3:9" ht="30.15" x14ac:dyDescent="0.3">
-      <c r="C92" s="49"/>
+        <v>288</v>
+      </c>
+      <c r="H91" s="6" t="s">
+        <v>288</v>
+      </c>
+      <c r="I91" s="25" t="s">
+        <v>207</v>
+      </c>
+      <c r="J91" s="4"/>
+    </row>
+    <row r="92" spans="3:10" ht="30.15" x14ac:dyDescent="0.3">
+      <c r="C92" s="44"/>
       <c r="D92" s="7" t="s">
         <v>100</v>
       </c>
-      <c r="E92" s="49"/>
+      <c r="E92" s="44"/>
       <c r="F92" s="9" t="s">
+        <v>171</v>
+      </c>
+      <c r="G92" s="6" t="s">
+        <v>289</v>
+      </c>
+      <c r="H92" s="6" t="s">
+        <v>289</v>
+      </c>
+      <c r="I92" s="25" t="s">
+        <v>207</v>
+      </c>
+      <c r="J92" s="4"/>
+    </row>
+    <row r="93" spans="3:10" ht="45.2" x14ac:dyDescent="0.3">
+      <c r="C93" s="44"/>
+      <c r="D93" s="7" t="s">
+        <v>142</v>
+      </c>
+      <c r="E93" s="44"/>
+      <c r="F93" s="9" t="s">
         <v>172</v>
       </c>
-      <c r="G92" s="6" t="s">
+      <c r="G93" s="6" t="s">
         <v>290</v>
       </c>
-      <c r="H92" s="25" t="s">
-        <v>208</v>
-      </c>
-      <c r="I92" s="4"/>
-    </row>
-    <row r="93" spans="3:9" ht="45.2" x14ac:dyDescent="0.3">
-      <c r="C93" s="49"/>
-      <c r="D93" s="7" t="s">
-        <v>143</v>
-      </c>
-      <c r="E93" s="49"/>
-      <c r="F93" s="9" t="s">
-        <v>173</v>
-      </c>
-      <c r="G93" s="6" t="s">
-        <v>291</v>
-      </c>
-      <c r="H93" s="25" t="s">
-        <v>208</v>
-      </c>
-      <c r="I93" s="4"/>
-    </row>
-    <row r="94" spans="3:9" x14ac:dyDescent="0.3">
-      <c r="C94" s="48" t="s">
+      <c r="H93" s="6" t="s">
+        <v>290</v>
+      </c>
+      <c r="I93" s="25" t="s">
+        <v>207</v>
+      </c>
+      <c r="J93" s="4"/>
+    </row>
+    <row r="94" spans="3:10" x14ac:dyDescent="0.3">
+      <c r="C94" s="43" t="s">
         <v>92</v>
       </c>
       <c r="D94" s="7" t="s">
         <v>93</v>
       </c>
-      <c r="E94" s="49"/>
+      <c r="E94" s="44"/>
       <c r="F94" s="9" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="G94" s="6" t="s">
-        <v>292</v>
-      </c>
-      <c r="H94" s="25" t="s">
-        <v>208</v>
-      </c>
-      <c r="I94" s="4"/>
-    </row>
-    <row r="95" spans="3:9" ht="30.15" x14ac:dyDescent="0.3">
-      <c r="C95" s="49"/>
+        <v>291</v>
+      </c>
+      <c r="H94" s="6" t="s">
+        <v>291</v>
+      </c>
+      <c r="I94" s="25" t="s">
+        <v>207</v>
+      </c>
+      <c r="J94" s="4"/>
+    </row>
+    <row r="95" spans="3:10" ht="30.15" x14ac:dyDescent="0.3">
+      <c r="C95" s="44"/>
       <c r="D95" s="7" t="s">
         <v>94</v>
       </c>
-      <c r="E95" s="49"/>
+      <c r="E95" s="44"/>
       <c r="F95" s="9" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="G95" s="6" t="s">
-        <v>293</v>
-      </c>
-      <c r="H95" s="25" t="s">
-        <v>208</v>
-      </c>
-      <c r="I95" s="4"/>
-    </row>
-    <row r="96" spans="3:9" x14ac:dyDescent="0.3">
-      <c r="C96" s="49"/>
+        <v>292</v>
+      </c>
+      <c r="H95" s="6" t="s">
+        <v>292</v>
+      </c>
+      <c r="I95" s="25" t="s">
+        <v>207</v>
+      </c>
+      <c r="J95" s="4"/>
+    </row>
+    <row r="96" spans="3:10" x14ac:dyDescent="0.3">
+      <c r="C96" s="44"/>
       <c r="D96" s="7" t="s">
         <v>95</v>
       </c>
-      <c r="E96" s="49"/>
+      <c r="E96" s="44"/>
       <c r="F96" s="27" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="G96" s="28"/>
-      <c r="H96" s="29"/>
-      <c r="I96" s="30"/>
-    </row>
-    <row r="97" spans="3:9" x14ac:dyDescent="0.3">
-      <c r="C97" s="49"/>
+      <c r="H96" s="28"/>
+      <c r="I96" s="29"/>
+      <c r="J96" s="30"/>
+    </row>
+    <row r="97" spans="3:10" x14ac:dyDescent="0.3">
+      <c r="C97" s="44"/>
       <c r="D97" s="7" t="s">
         <v>96</v>
       </c>
-      <c r="E97" s="49"/>
+      <c r="E97" s="44"/>
       <c r="F97" s="9" t="s">
+        <v>175</v>
+      </c>
+      <c r="G97" s="6" t="s">
+        <v>311</v>
+      </c>
+      <c r="H97" s="6" t="s">
+        <v>311</v>
+      </c>
+      <c r="I97" s="25" t="s">
+        <v>207</v>
+      </c>
+      <c r="J97" s="4"/>
+    </row>
+    <row r="98" spans="3:10" x14ac:dyDescent="0.3">
+      <c r="C98" s="44"/>
+      <c r="D98" s="7" t="s">
+        <v>141</v>
+      </c>
+      <c r="E98" s="44"/>
+      <c r="F98" s="9" t="s">
         <v>176</v>
       </c>
-      <c r="G97" s="6" t="s">
-        <v>312</v>
-      </c>
-      <c r="H97" s="25" t="s">
-        <v>208</v>
-      </c>
-      <c r="I97" s="4"/>
-    </row>
-    <row r="98" spans="3:9" x14ac:dyDescent="0.3">
-      <c r="C98" s="49"/>
-      <c r="D98" s="7" t="s">
-        <v>142</v>
-      </c>
-      <c r="E98" s="49"/>
-      <c r="F98" s="9" t="s">
-        <v>177</v>
-      </c>
       <c r="G98" s="6" t="s">
-        <v>294</v>
-      </c>
-      <c r="H98" s="25" t="s">
-        <v>208</v>
-      </c>
-      <c r="I98" s="4"/>
-    </row>
-    <row r="99" spans="3:9" x14ac:dyDescent="0.3">
-      <c r="C99" s="51" t="s">
+        <v>293</v>
+      </c>
+      <c r="H98" s="6" t="s">
+        <v>293</v>
+      </c>
+      <c r="I98" s="25" t="s">
+        <v>207</v>
+      </c>
+      <c r="J98" s="4"/>
+    </row>
+    <row r="99" spans="3:10" x14ac:dyDescent="0.3">
+      <c r="C99" s="60" t="s">
         <v>107</v>
       </c>
       <c r="D99" s="7" t="s">
         <v>101</v>
       </c>
-      <c r="E99" s="49"/>
+      <c r="E99" s="44"/>
       <c r="F99" s="9" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="G99" s="6" t="s">
-        <v>275</v>
-      </c>
-      <c r="H99" s="25" t="s">
-        <v>208</v>
-      </c>
-      <c r="I99" s="4"/>
-    </row>
-    <row r="100" spans="3:9" ht="30.15" x14ac:dyDescent="0.3">
-      <c r="C100" s="51"/>
+        <v>274</v>
+      </c>
+      <c r="H99" s="6" t="s">
+        <v>274</v>
+      </c>
+      <c r="I99" s="25" t="s">
+        <v>207</v>
+      </c>
+      <c r="J99" s="4"/>
+    </row>
+    <row r="100" spans="3:10" ht="30.15" x14ac:dyDescent="0.3">
+      <c r="C100" s="60"/>
       <c r="D100" s="7" t="s">
         <v>102</v>
       </c>
-      <c r="E100" s="49"/>
+      <c r="E100" s="44"/>
       <c r="F100" s="9" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="G100" s="6" t="s">
-        <v>274</v>
-      </c>
-      <c r="H100" s="25" t="s">
-        <v>208</v>
-      </c>
-      <c r="I100" s="4"/>
-    </row>
-    <row r="101" spans="3:9" x14ac:dyDescent="0.3">
-      <c r="C101" s="51"/>
+        <v>273</v>
+      </c>
+      <c r="H100" s="6" t="s">
+        <v>273</v>
+      </c>
+      <c r="I100" s="25" t="s">
+        <v>207</v>
+      </c>
+      <c r="J100" s="4"/>
+    </row>
+    <row r="101" spans="3:10" x14ac:dyDescent="0.3">
+      <c r="C101" s="60"/>
       <c r="D101" s="7" t="s">
         <v>103</v>
       </c>
-      <c r="E101" s="49"/>
+      <c r="E101" s="44"/>
       <c r="F101" s="9" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="G101" s="6" t="s">
-        <v>272</v>
-      </c>
-      <c r="H101" s="25" t="s">
-        <v>208</v>
-      </c>
-      <c r="I101" s="4"/>
-    </row>
-    <row r="102" spans="3:9" ht="30.15" x14ac:dyDescent="0.3">
-      <c r="C102" s="51"/>
+        <v>271</v>
+      </c>
+      <c r="H101" s="6" t="s">
+        <v>271</v>
+      </c>
+      <c r="I101" s="25" t="s">
+        <v>207</v>
+      </c>
+      <c r="J101" s="4"/>
+    </row>
+    <row r="102" spans="3:10" ht="30.15" x14ac:dyDescent="0.3">
+      <c r="C102" s="60"/>
       <c r="D102" s="7" t="s">
         <v>104</v>
       </c>
-      <c r="E102" s="49"/>
+      <c r="E102" s="44"/>
       <c r="F102" s="9" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="G102" s="6" t="s">
-        <v>273</v>
-      </c>
-      <c r="H102" s="25" t="s">
-        <v>208</v>
-      </c>
-      <c r="I102" s="4"/>
-    </row>
-    <row r="103" spans="3:9" x14ac:dyDescent="0.3">
-      <c r="C103" s="51"/>
+        <v>272</v>
+      </c>
+      <c r="H102" s="6" t="s">
+        <v>272</v>
+      </c>
+      <c r="I102" s="25" t="s">
+        <v>207</v>
+      </c>
+      <c r="J102" s="4"/>
+    </row>
+    <row r="103" spans="3:10" x14ac:dyDescent="0.3">
+      <c r="C103" s="60"/>
       <c r="D103" s="7" t="s">
         <v>105</v>
       </c>
-      <c r="E103" s="49"/>
+      <c r="E103" s="44"/>
       <c r="F103" s="9" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="G103" s="6" t="s">
-        <v>276</v>
-      </c>
-      <c r="H103" s="25" t="s">
-        <v>208</v>
-      </c>
-      <c r="I103" s="4"/>
-    </row>
-    <row r="104" spans="3:9" ht="30.15" x14ac:dyDescent="0.3">
-      <c r="C104" s="51"/>
+        <v>275</v>
+      </c>
+      <c r="H103" s="6" t="s">
+        <v>275</v>
+      </c>
+      <c r="I103" s="25" t="s">
+        <v>207</v>
+      </c>
+      <c r="J103" s="4"/>
+    </row>
+    <row r="104" spans="3:10" ht="30.15" x14ac:dyDescent="0.3">
+      <c r="C104" s="60"/>
       <c r="D104" s="8" t="s">
         <v>106</v>
       </c>
-      <c r="E104" s="50"/>
+      <c r="E104" s="45"/>
       <c r="F104" s="9" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="G104" s="6" t="s">
-        <v>277</v>
-      </c>
-      <c r="H104" s="25" t="s">
-        <v>208</v>
-      </c>
-      <c r="I104" s="4"/>
-    </row>
-    <row r="105" spans="3:9" x14ac:dyDescent="0.3">
+        <v>276</v>
+      </c>
+      <c r="H104" s="6" t="s">
+        <v>276</v>
+      </c>
+      <c r="I104" s="25" t="s">
+        <v>207</v>
+      </c>
+      <c r="J104" s="4"/>
+    </row>
+    <row r="105" spans="3:10" x14ac:dyDescent="0.3">
       <c r="E105" s="19"/>
     </row>
-    <row r="106" spans="3:9" x14ac:dyDescent="0.3">
+    <row r="106" spans="3:10" x14ac:dyDescent="0.3">
       <c r="E106" s="19"/>
     </row>
-    <row r="107" spans="3:9" x14ac:dyDescent="0.3">
+    <row r="107" spans="3:10" x14ac:dyDescent="0.3">
       <c r="E107" s="19"/>
     </row>
   </sheetData>
-  <mergeCells count="37">
+  <mergeCells count="39">
+    <mergeCell ref="J40:J44"/>
     <mergeCell ref="E50:E60"/>
     <mergeCell ref="E62:E104"/>
     <mergeCell ref="C69:C78"/>
@@ -3400,19 +3653,20 @@
     <mergeCell ref="C24:C27"/>
     <mergeCell ref="C28:C29"/>
     <mergeCell ref="C18:C22"/>
+    <mergeCell ref="H40:H44"/>
+    <mergeCell ref="F28:F32"/>
+    <mergeCell ref="F6:F7"/>
+    <mergeCell ref="I40:I44"/>
     <mergeCell ref="I6:I7"/>
     <mergeCell ref="I18:I22"/>
-    <mergeCell ref="F28:F32"/>
-    <mergeCell ref="F6:F7"/>
-    <mergeCell ref="H40:H44"/>
-    <mergeCell ref="H6:H7"/>
-    <mergeCell ref="H18:H22"/>
     <mergeCell ref="G6:G7"/>
     <mergeCell ref="G34:G37"/>
     <mergeCell ref="G40:G44"/>
     <mergeCell ref="G28:G32"/>
+    <mergeCell ref="I28:I32"/>
+    <mergeCell ref="H6:H7"/>
     <mergeCell ref="H28:H32"/>
-    <mergeCell ref="I28:I32"/>
+    <mergeCell ref="H34:H37"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
added more to the data dict and fixed one bug
</commit_message>
<xml_diff>
--- a/edit_eam/crosscheck.xlsx
+++ b/edit_eam/crosscheck.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="572" uniqueCount="334">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="574" uniqueCount="334">
   <si>
     <t>Nombre</t>
   </si>
@@ -1022,7 +1022,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1047,6 +1047,14 @@
     </font>
     <font>
       <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -1193,7 +1201,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="51">
+  <cellXfs count="52">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1294,11 +1302,47 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1309,40 +1353,7 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1651,8 +1662,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="C2:J107"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C31" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="G33" sqref="G33"/>
+    <sheetView tabSelected="1" topLeftCell="D83" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="I105" sqref="I105"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="15.05" x14ac:dyDescent="0.3"/>
@@ -1698,7 +1709,7 @@
       <c r="D3" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="E3" s="42" t="s">
+      <c r="E3" s="36" t="s">
         <v>122</v>
       </c>
       <c r="F3" s="8" t="s">
@@ -1724,7 +1735,7 @@
       <c r="D4" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="E4" s="43"/>
+      <c r="E4" s="37"/>
       <c r="F4" s="10" t="s">
         <v>108</v>
       </c>
@@ -1734,13 +1745,13 @@
       <c r="J4" s="24"/>
     </row>
     <row r="5" spans="3:10" x14ac:dyDescent="0.3">
-      <c r="C5" s="48" t="s">
+      <c r="C5" s="39" t="s">
         <v>7</v>
       </c>
       <c r="D5" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="E5" s="43"/>
+      <c r="E5" s="37"/>
       <c r="F5" s="8" t="s">
         <v>109</v>
       </c>
@@ -1758,18 +1769,18 @@
       </c>
     </row>
     <row r="6" spans="3:10" x14ac:dyDescent="0.3">
-      <c r="C6" s="48"/>
+      <c r="C6" s="39"/>
       <c r="D6" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="E6" s="43"/>
-      <c r="F6" s="49" t="s">
+      <c r="E6" s="37"/>
+      <c r="F6" s="43" t="s">
         <v>111</v>
       </c>
-      <c r="G6" s="39" t="s">
+      <c r="G6" s="45" t="s">
         <v>221</v>
       </c>
-      <c r="H6" s="39" t="s">
+      <c r="H6" s="45" t="s">
         <v>221</v>
       </c>
       <c r="I6" s="33" t="s">
@@ -1780,23 +1791,23 @@
       </c>
     </row>
     <row r="7" spans="3:10" x14ac:dyDescent="0.3">
-      <c r="C7" s="48"/>
+      <c r="C7" s="39"/>
       <c r="D7" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="E7" s="43"/>
-      <c r="F7" s="50"/>
-      <c r="G7" s="40"/>
-      <c r="H7" s="40"/>
-      <c r="I7" s="34"/>
-      <c r="J7" s="34"/>
+      <c r="E7" s="37"/>
+      <c r="F7" s="44"/>
+      <c r="G7" s="46"/>
+      <c r="H7" s="46"/>
+      <c r="I7" s="35"/>
+      <c r="J7" s="35"/>
     </row>
     <row r="8" spans="3:10" x14ac:dyDescent="0.3">
-      <c r="C8" s="48"/>
+      <c r="C8" s="39"/>
       <c r="D8" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="E8" s="43"/>
+      <c r="E8" s="37"/>
       <c r="F8" s="9" t="s">
         <v>110</v>
       </c>
@@ -1814,13 +1825,13 @@
       </c>
     </row>
     <row r="9" spans="3:10" x14ac:dyDescent="0.3">
-      <c r="C9" s="48" t="s">
+      <c r="C9" s="39" t="s">
         <v>13</v>
       </c>
       <c r="D9" s="6" t="s">
         <v>153</v>
       </c>
-      <c r="E9" s="43"/>
+      <c r="E9" s="37"/>
       <c r="F9" s="21" t="s">
         <v>178</v>
       </c>
@@ -1838,11 +1849,11 @@
       </c>
     </row>
     <row r="10" spans="3:10" x14ac:dyDescent="0.3">
-      <c r="C10" s="48"/>
+      <c r="C10" s="39"/>
       <c r="D10" s="6" t="s">
         <v>154</v>
       </c>
-      <c r="E10" s="43"/>
+      <c r="E10" s="37"/>
       <c r="F10" s="21" t="s">
         <v>179</v>
       </c>
@@ -1860,11 +1871,11 @@
       </c>
     </row>
     <row r="11" spans="3:10" ht="34.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C11" s="48"/>
+      <c r="C11" s="39"/>
       <c r="D11" s="6" t="s">
         <v>155</v>
       </c>
-      <c r="E11" s="43"/>
+      <c r="E11" s="37"/>
       <c r="F11" s="21" t="s">
         <v>180</v>
       </c>
@@ -1882,11 +1893,11 @@
       </c>
     </row>
     <row r="12" spans="3:10" ht="34.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C12" s="48"/>
+      <c r="C12" s="39"/>
       <c r="D12" s="6" t="s">
         <v>156</v>
       </c>
-      <c r="E12" s="43"/>
+      <c r="E12" s="37"/>
       <c r="F12" s="21" t="s">
         <v>181</v>
       </c>
@@ -1904,11 +1915,11 @@
       </c>
     </row>
     <row r="13" spans="3:10" ht="65.45" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C13" s="48"/>
+      <c r="C13" s="39"/>
       <c r="D13" s="6" t="s">
         <v>157</v>
       </c>
-      <c r="E13" s="43"/>
+      <c r="E13" s="37"/>
       <c r="F13" s="21" t="s">
         <v>182</v>
       </c>
@@ -1926,11 +1937,11 @@
       </c>
     </row>
     <row r="14" spans="3:10" ht="46.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C14" s="48"/>
+      <c r="C14" s="39"/>
       <c r="D14" s="6" t="s">
         <v>158</v>
       </c>
-      <c r="E14" s="43"/>
+      <c r="E14" s="37"/>
       <c r="F14" s="21" t="s">
         <v>183</v>
       </c>
@@ -1948,11 +1959,11 @@
       </c>
     </row>
     <row r="15" spans="3:10" ht="66.150000000000006" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C15" s="48"/>
+      <c r="C15" s="39"/>
       <c r="D15" s="6" t="s">
         <v>159</v>
       </c>
-      <c r="E15" s="43"/>
+      <c r="E15" s="37"/>
       <c r="F15" s="21" t="s">
         <v>184</v>
       </c>
@@ -1970,13 +1981,13 @@
       </c>
     </row>
     <row r="16" spans="3:10" x14ac:dyDescent="0.3">
-      <c r="C16" s="48" t="s">
+      <c r="C16" s="39" t="s">
         <v>14</v>
       </c>
       <c r="D16" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="E16" s="43"/>
+      <c r="E16" s="37"/>
       <c r="F16" s="8" t="s">
         <v>112</v>
       </c>
@@ -1994,11 +2005,11 @@
       </c>
     </row>
     <row r="17" spans="3:10" x14ac:dyDescent="0.3">
-      <c r="C17" s="48"/>
+      <c r="C17" s="39"/>
       <c r="D17" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="E17" s="43"/>
+      <c r="E17" s="37"/>
       <c r="F17" s="8" t="s">
         <v>113</v>
       </c>
@@ -2016,14 +2027,14 @@
       </c>
     </row>
     <row r="18" spans="3:10" ht="15.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C18" s="42" t="s">
+      <c r="C18" s="36" t="s">
         <v>114</v>
       </c>
       <c r="D18" s="6" t="s">
         <v>115</v>
       </c>
-      <c r="E18" s="43"/>
-      <c r="F18" s="42" t="s">
+      <c r="E18" s="37"/>
+      <c r="F18" s="36" t="s">
         <v>198</v>
       </c>
       <c r="G18" s="5" t="s">
@@ -2040,68 +2051,68 @@
       </c>
     </row>
     <row r="19" spans="3:10" x14ac:dyDescent="0.3">
-      <c r="C19" s="43"/>
+      <c r="C19" s="37"/>
       <c r="D19" s="6" t="s">
         <v>116</v>
       </c>
-      <c r="E19" s="43"/>
-      <c r="F19" s="43"/>
+      <c r="E19" s="37"/>
+      <c r="F19" s="37"/>
       <c r="G19" s="5" t="s">
         <v>232</v>
       </c>
       <c r="H19" s="5" t="s">
         <v>232</v>
       </c>
-      <c r="I19" s="35"/>
-      <c r="J19" s="35"/>
+      <c r="I19" s="34"/>
+      <c r="J19" s="34"/>
     </row>
     <row r="20" spans="3:10" x14ac:dyDescent="0.3">
-      <c r="C20" s="43"/>
+      <c r="C20" s="37"/>
       <c r="D20" s="6" t="s">
         <v>117</v>
       </c>
-      <c r="E20" s="43"/>
-      <c r="F20" s="43"/>
+      <c r="E20" s="37"/>
+      <c r="F20" s="37"/>
       <c r="G20" s="5" t="s">
         <v>235</v>
       </c>
       <c r="H20" s="5" t="s">
         <v>235</v>
       </c>
-      <c r="I20" s="35"/>
-      <c r="J20" s="35"/>
+      <c r="I20" s="34"/>
+      <c r="J20" s="34"/>
     </row>
     <row r="21" spans="3:10" x14ac:dyDescent="0.3">
-      <c r="C21" s="43"/>
+      <c r="C21" s="37"/>
       <c r="D21" s="6" t="s">
         <v>118</v>
       </c>
-      <c r="E21" s="43"/>
-      <c r="F21" s="43"/>
+      <c r="E21" s="37"/>
+      <c r="F21" s="37"/>
       <c r="G21" s="5" t="s">
         <v>233</v>
       </c>
       <c r="H21" s="5" t="s">
         <v>233</v>
       </c>
-      <c r="I21" s="35"/>
-      <c r="J21" s="35"/>
+      <c r="I21" s="34"/>
+      <c r="J21" s="34"/>
     </row>
     <row r="22" spans="3:10" x14ac:dyDescent="0.3">
-      <c r="C22" s="44"/>
+      <c r="C22" s="38"/>
       <c r="D22" s="6" t="s">
         <v>199</v>
       </c>
-      <c r="E22" s="43"/>
-      <c r="F22" s="44"/>
+      <c r="E22" s="37"/>
+      <c r="F22" s="38"/>
       <c r="G22" s="5" t="s">
         <v>236</v>
       </c>
       <c r="H22" s="5" t="s">
         <v>236</v>
       </c>
-      <c r="I22" s="34"/>
-      <c r="J22" s="34"/>
+      <c r="I22" s="35"/>
+      <c r="J22" s="35"/>
     </row>
     <row r="23" spans="3:10" ht="30.15" x14ac:dyDescent="0.3">
       <c r="C23" s="3" t="s">
@@ -2110,7 +2121,7 @@
       <c r="D23" s="6" t="s">
         <v>62</v>
       </c>
-      <c r="E23" s="43"/>
+      <c r="E23" s="37"/>
       <c r="F23" s="8" t="s">
         <v>119</v>
       </c>
@@ -2128,13 +2139,13 @@
       </c>
     </row>
     <row r="24" spans="3:10" x14ac:dyDescent="0.3">
-      <c r="C24" s="48" t="s">
+      <c r="C24" s="39" t="s">
         <v>120</v>
       </c>
       <c r="D24" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="E24" s="43"/>
+      <c r="E24" s="37"/>
       <c r="F24" s="10" t="s">
         <v>215</v>
       </c>
@@ -2152,11 +2163,11 @@
       </c>
     </row>
     <row r="25" spans="3:10" ht="135.5" x14ac:dyDescent="0.3">
-      <c r="C25" s="48"/>
+      <c r="C25" s="39"/>
       <c r="D25" s="6" t="s">
         <v>216</v>
       </c>
-      <c r="E25" s="43"/>
+      <c r="E25" s="37"/>
       <c r="F25" s="10" t="s">
         <v>214</v>
       </c>
@@ -2174,11 +2185,11 @@
       </c>
     </row>
     <row r="26" spans="3:10" ht="45.2" x14ac:dyDescent="0.3">
-      <c r="C26" s="48"/>
+      <c r="C26" s="39"/>
       <c r="D26" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="E26" s="43"/>
+      <c r="E26" s="37"/>
       <c r="F26" s="10" t="s">
         <v>212</v>
       </c>
@@ -2196,11 +2207,11 @@
       </c>
     </row>
     <row r="27" spans="3:10" ht="45.2" x14ac:dyDescent="0.3">
-      <c r="C27" s="48"/>
+      <c r="C27" s="39"/>
       <c r="D27" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="E27" s="44"/>
+      <c r="E27" s="38"/>
       <c r="F27" s="10" t="s">
         <v>211</v>
       </c>
@@ -2218,93 +2229,93 @@
       </c>
     </row>
     <row r="28" spans="3:10" x14ac:dyDescent="0.3">
-      <c r="C28" s="48" t="s">
+      <c r="C28" s="39" t="s">
         <v>23</v>
       </c>
       <c r="D28" s="6" t="s">
         <v>21</v>
       </c>
       <c r="E28" s="4"/>
-      <c r="F28" s="45" t="s">
+      <c r="F28" s="40" t="s">
         <v>306</v>
       </c>
-      <c r="G28" s="45" t="s">
+      <c r="G28" s="40" t="s">
         <v>307</v>
       </c>
-      <c r="H28" s="45" t="s">
+      <c r="H28" s="40" t="s">
         <v>307</v>
       </c>
-      <c r="I28" s="36" t="s">
-        <v>207</v>
-      </c>
-      <c r="J28" s="36" t="s">
+      <c r="I28" s="48" t="s">
+        <v>207</v>
+      </c>
+      <c r="J28" s="48" t="s">
         <v>207</v>
       </c>
     </row>
     <row r="29" spans="3:10" x14ac:dyDescent="0.3">
-      <c r="C29" s="48"/>
+      <c r="C29" s="39"/>
       <c r="D29" s="6" t="s">
         <v>22</v>
       </c>
       <c r="E29" s="4"/>
-      <c r="F29" s="46"/>
-      <c r="G29" s="46"/>
-      <c r="H29" s="46"/>
-      <c r="I29" s="37"/>
-      <c r="J29" s="37"/>
+      <c r="F29" s="41"/>
+      <c r="G29" s="41"/>
+      <c r="H29" s="41"/>
+      <c r="I29" s="49"/>
+      <c r="J29" s="49"/>
     </row>
     <row r="30" spans="3:10" x14ac:dyDescent="0.3">
-      <c r="C30" s="48" t="s">
+      <c r="C30" s="39" t="s">
         <v>24</v>
       </c>
       <c r="D30" s="6" t="s">
         <v>25</v>
       </c>
       <c r="E30" s="4"/>
-      <c r="F30" s="46"/>
-      <c r="G30" s="46"/>
-      <c r="H30" s="46"/>
-      <c r="I30" s="37"/>
-      <c r="J30" s="37"/>
+      <c r="F30" s="41"/>
+      <c r="G30" s="41"/>
+      <c r="H30" s="41"/>
+      <c r="I30" s="49"/>
+      <c r="J30" s="49"/>
     </row>
     <row r="31" spans="3:10" x14ac:dyDescent="0.3">
-      <c r="C31" s="48"/>
+      <c r="C31" s="39"/>
       <c r="D31" s="6" t="s">
         <v>26</v>
       </c>
       <c r="E31" s="4"/>
-      <c r="F31" s="46"/>
-      <c r="G31" s="46"/>
-      <c r="H31" s="46"/>
-      <c r="I31" s="37"/>
-      <c r="J31" s="37"/>
+      <c r="F31" s="41"/>
+      <c r="G31" s="41"/>
+      <c r="H31" s="41"/>
+      <c r="I31" s="49"/>
+      <c r="J31" s="49"/>
     </row>
     <row r="32" spans="3:10" x14ac:dyDescent="0.3">
-      <c r="C32" s="48"/>
+      <c r="C32" s="39"/>
       <c r="D32" s="6" t="s">
         <v>27</v>
       </c>
       <c r="E32" s="4"/>
-      <c r="F32" s="47"/>
-      <c r="G32" s="47"/>
-      <c r="H32" s="47"/>
-      <c r="I32" s="38"/>
-      <c r="J32" s="38"/>
+      <c r="F32" s="42"/>
+      <c r="G32" s="42"/>
+      <c r="H32" s="42"/>
+      <c r="I32" s="50"/>
+      <c r="J32" s="50"/>
     </row>
     <row r="33" spans="3:10" ht="60.25" x14ac:dyDescent="0.3">
-      <c r="C33" s="42" t="s">
+      <c r="C33" s="36" t="s">
         <v>28</v>
       </c>
       <c r="D33" s="6" t="s">
         <v>124</v>
       </c>
-      <c r="E33" s="42" t="s">
+      <c r="E33" s="36" t="s">
         <v>122</v>
       </c>
       <c r="F33" s="19" t="s">
         <v>186</v>
       </c>
-      <c r="G33" s="5" t="s">
+      <c r="G33" s="51" t="s">
         <v>243</v>
       </c>
       <c r="H33" s="5" t="s">
@@ -2318,18 +2329,18 @@
       </c>
     </row>
     <row r="34" spans="3:10" ht="30.15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C34" s="43"/>
+      <c r="C34" s="37"/>
       <c r="D34" s="6">
         <v>10</v>
       </c>
-      <c r="E34" s="43"/>
+      <c r="E34" s="37"/>
       <c r="F34" s="16" t="s">
         <v>187</v>
       </c>
-      <c r="G34" s="39" t="s">
+      <c r="G34" s="45" t="s">
         <v>242</v>
       </c>
-      <c r="H34" s="39" t="s">
+      <c r="H34" s="45" t="s">
         <v>314</v>
       </c>
       <c r="I34" s="33" t="s">
@@ -2340,46 +2351,46 @@
       </c>
     </row>
     <row r="35" spans="3:10" ht="30.15" x14ac:dyDescent="0.3">
-      <c r="C35" s="43"/>
+      <c r="C35" s="37"/>
       <c r="D35" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="E35" s="43"/>
+      <c r="E35" s="37"/>
       <c r="F35" s="16" t="s">
         <v>188</v>
       </c>
-      <c r="G35" s="41"/>
-      <c r="H35" s="41"/>
-      <c r="I35" s="35"/>
-      <c r="J35" s="35"/>
+      <c r="G35" s="47"/>
+      <c r="H35" s="47"/>
+      <c r="I35" s="34"/>
+      <c r="J35" s="34"/>
     </row>
     <row r="36" spans="3:10" ht="30.15" x14ac:dyDescent="0.3">
-      <c r="C36" s="43"/>
+      <c r="C36" s="37"/>
       <c r="D36" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="E36" s="43"/>
+      <c r="E36" s="37"/>
       <c r="F36" s="16" t="s">
         <v>189</v>
       </c>
-      <c r="G36" s="41"/>
-      <c r="H36" s="41"/>
-      <c r="I36" s="35"/>
-      <c r="J36" s="35"/>
+      <c r="G36" s="47"/>
+      <c r="H36" s="47"/>
+      <c r="I36" s="34"/>
+      <c r="J36" s="34"/>
     </row>
     <row r="37" spans="3:10" x14ac:dyDescent="0.3">
-      <c r="C37" s="44"/>
+      <c r="C37" s="38"/>
       <c r="D37" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="E37" s="43"/>
+      <c r="E37" s="37"/>
       <c r="F37" s="16" t="s">
         <v>190</v>
       </c>
-      <c r="G37" s="40"/>
-      <c r="H37" s="40"/>
-      <c r="I37" s="34"/>
-      <c r="J37" s="34"/>
+      <c r="G37" s="46"/>
+      <c r="H37" s="46"/>
+      <c r="I37" s="35"/>
+      <c r="J37" s="35"/>
     </row>
     <row r="38" spans="3:10" ht="30.15" x14ac:dyDescent="0.3">
       <c r="C38" s="3" t="s">
@@ -2388,7 +2399,7 @@
       <c r="D38" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="E38" s="44"/>
+      <c r="E38" s="38"/>
       <c r="F38" s="10" t="s">
         <v>191</v>
       </c>
@@ -2412,7 +2423,7 @@
       <c r="D39" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="E39" s="48" t="s">
+      <c r="E39" s="39" t="s">
         <v>123</v>
       </c>
       <c r="F39" s="10" t="s">
@@ -2427,23 +2438,25 @@
       <c r="I39" s="24" t="s">
         <v>207</v>
       </c>
-      <c r="J39" s="24"/>
+      <c r="J39" s="24" t="s">
+        <v>207</v>
+      </c>
     </row>
     <row r="40" spans="3:10" ht="105.4" x14ac:dyDescent="0.3">
-      <c r="C40" s="48" t="s">
+      <c r="C40" s="39" t="s">
         <v>36</v>
       </c>
       <c r="D40" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="E40" s="48"/>
+      <c r="E40" s="39"/>
       <c r="F40" s="5" t="s">
         <v>294</v>
       </c>
-      <c r="G40" s="42" t="s">
+      <c r="G40" s="36" t="s">
         <v>310</v>
       </c>
-      <c r="H40" s="42" t="s">
+      <c r="H40" s="36" t="s">
         <v>310</v>
       </c>
       <c r="I40" s="33" t="s">
@@ -2454,60 +2467,60 @@
       </c>
     </row>
     <row r="41" spans="3:10" ht="165.6" x14ac:dyDescent="0.3">
-      <c r="C41" s="48"/>
+      <c r="C41" s="39"/>
       <c r="D41" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="E41" s="48"/>
+      <c r="E41" s="39"/>
       <c r="F41" s="5" t="s">
         <v>295</v>
       </c>
-      <c r="G41" s="43"/>
-      <c r="H41" s="43"/>
-      <c r="I41" s="35"/>
-      <c r="J41" s="35"/>
+      <c r="G41" s="37"/>
+      <c r="H41" s="37"/>
+      <c r="I41" s="34"/>
+      <c r="J41" s="34"/>
     </row>
     <row r="42" spans="3:10" ht="60.25" x14ac:dyDescent="0.3">
-      <c r="C42" s="48"/>
+      <c r="C42" s="39"/>
       <c r="D42" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="E42" s="48"/>
+      <c r="E42" s="39"/>
       <c r="F42" s="5" t="s">
         <v>296</v>
       </c>
-      <c r="G42" s="43"/>
-      <c r="H42" s="43"/>
-      <c r="I42" s="35"/>
-      <c r="J42" s="35"/>
+      <c r="G42" s="37"/>
+      <c r="H42" s="37"/>
+      <c r="I42" s="34"/>
+      <c r="J42" s="34"/>
     </row>
     <row r="43" spans="3:10" ht="60.25" x14ac:dyDescent="0.3">
-      <c r="C43" s="48"/>
+      <c r="C43" s="39"/>
       <c r="D43" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="E43" s="48"/>
+      <c r="E43" s="39"/>
       <c r="F43" s="5" t="s">
         <v>298</v>
       </c>
-      <c r="G43" s="43"/>
-      <c r="H43" s="43"/>
-      <c r="I43" s="35"/>
-      <c r="J43" s="35"/>
+      <c r="G43" s="37"/>
+      <c r="H43" s="37"/>
+      <c r="I43" s="34"/>
+      <c r="J43" s="34"/>
     </row>
     <row r="44" spans="3:10" x14ac:dyDescent="0.3">
-      <c r="C44" s="48"/>
+      <c r="C44" s="39"/>
       <c r="D44" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="E44" s="48"/>
+      <c r="E44" s="39"/>
       <c r="F44" s="31" t="s">
         <v>297</v>
       </c>
-      <c r="G44" s="44"/>
-      <c r="H44" s="44"/>
-      <c r="I44" s="34"/>
-      <c r="J44" s="34"/>
+      <c r="G44" s="38"/>
+      <c r="H44" s="38"/>
+      <c r="I44" s="35"/>
+      <c r="J44" s="35"/>
     </row>
     <row r="45" spans="3:10" ht="60.25" x14ac:dyDescent="0.3">
       <c r="C45" s="3" t="s">
@@ -2516,7 +2529,7 @@
       <c r="D45" s="6" t="s">
         <v>43</v>
       </c>
-      <c r="E45" s="48"/>
+      <c r="E45" s="39"/>
       <c r="F45" s="22" t="s">
         <v>208</v>
       </c>
@@ -2540,7 +2553,7 @@
       <c r="D46" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="E46" s="48"/>
+      <c r="E46" s="39"/>
       <c r="F46" s="10" t="s">
         <v>209</v>
       </c>
@@ -2564,7 +2577,7 @@
       <c r="D47" s="6" t="s">
         <v>48</v>
       </c>
-      <c r="E47" s="48"/>
+      <c r="E47" s="39"/>
       <c r="F47" s="10" t="s">
         <v>302</v>
       </c>
@@ -2588,7 +2601,7 @@
       <c r="D48" s="6" t="s">
         <v>49</v>
       </c>
-      <c r="E48" s="48"/>
+      <c r="E48" s="39"/>
       <c r="F48" s="10" t="s">
         <v>152</v>
       </c>
@@ -2632,13 +2645,13 @@
       </c>
     </row>
     <row r="50" spans="3:10" ht="45.2" x14ac:dyDescent="0.3">
-      <c r="C50" s="42" t="s">
+      <c r="C50" s="36" t="s">
         <v>52</v>
       </c>
       <c r="D50" s="6" t="s">
         <v>126</v>
       </c>
-      <c r="E50" s="42" t="s">
+      <c r="E50" s="36" t="s">
         <v>122</v>
       </c>
       <c r="F50" s="17" t="s">
@@ -2658,11 +2671,11 @@
       </c>
     </row>
     <row r="51" spans="3:10" ht="30.15" x14ac:dyDescent="0.3">
-      <c r="C51" s="44"/>
+      <c r="C51" s="38"/>
       <c r="D51" s="6" t="s">
         <v>53</v>
       </c>
-      <c r="E51" s="43"/>
+      <c r="E51" s="37"/>
       <c r="F51" s="17" t="s">
         <v>125</v>
       </c>
@@ -2680,13 +2693,13 @@
       </c>
     </row>
     <row r="52" spans="3:10" ht="60.25" x14ac:dyDescent="0.3">
-      <c r="C52" s="42" t="s">
+      <c r="C52" s="36" t="s">
         <v>218</v>
       </c>
       <c r="D52" s="6" t="s">
         <v>124</v>
       </c>
-      <c r="E52" s="43"/>
+      <c r="E52" s="37"/>
       <c r="F52" s="17" t="s">
         <v>217</v>
       </c>
@@ -2704,11 +2717,11 @@
       </c>
     </row>
     <row r="53" spans="3:10" ht="60.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C53" s="43"/>
+      <c r="C53" s="37"/>
       <c r="D53" s="6" t="s">
         <v>54</v>
       </c>
-      <c r="E53" s="43"/>
+      <c r="E53" s="37"/>
       <c r="F53" s="21" t="s">
         <v>192</v>
       </c>
@@ -2726,11 +2739,11 @@
       </c>
     </row>
     <row r="54" spans="3:10" ht="120.45" x14ac:dyDescent="0.3">
-      <c r="C54" s="43"/>
+      <c r="C54" s="37"/>
       <c r="D54" s="6" t="s">
         <v>55</v>
       </c>
-      <c r="E54" s="43"/>
+      <c r="E54" s="37"/>
       <c r="F54" s="21" t="s">
         <v>195</v>
       </c>
@@ -2748,11 +2761,11 @@
       </c>
     </row>
     <row r="55" spans="3:10" ht="90.35" x14ac:dyDescent="0.3">
-      <c r="C55" s="43"/>
+      <c r="C55" s="37"/>
       <c r="D55" s="6" t="s">
         <v>56</v>
       </c>
-      <c r="E55" s="43"/>
+      <c r="E55" s="37"/>
       <c r="F55" s="21" t="s">
         <v>193</v>
       </c>
@@ -2770,11 +2783,11 @@
       </c>
     </row>
     <row r="56" spans="3:10" ht="45.2" x14ac:dyDescent="0.3">
-      <c r="C56" s="44"/>
+      <c r="C56" s="38"/>
       <c r="D56" s="6" t="s">
         <v>69</v>
       </c>
-      <c r="E56" s="43"/>
+      <c r="E56" s="37"/>
       <c r="F56" s="10" t="s">
         <v>194</v>
       </c>
@@ -2792,13 +2805,13 @@
       </c>
     </row>
     <row r="57" spans="3:10" ht="30.15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C57" s="48" t="s">
+      <c r="C57" s="39" t="s">
         <v>91</v>
       </c>
       <c r="D57" s="6" t="s">
         <v>57</v>
       </c>
-      <c r="E57" s="43"/>
+      <c r="E57" s="37"/>
       <c r="F57" s="8" t="s">
         <v>127</v>
       </c>
@@ -2816,11 +2829,11 @@
       </c>
     </row>
     <row r="58" spans="3:10" x14ac:dyDescent="0.3">
-      <c r="C58" s="48"/>
+      <c r="C58" s="39"/>
       <c r="D58" s="6" t="s">
         <v>58</v>
       </c>
-      <c r="E58" s="43"/>
+      <c r="E58" s="37"/>
       <c r="F58" s="8" t="s">
         <v>219</v>
       </c>
@@ -2838,11 +2851,11 @@
       </c>
     </row>
     <row r="59" spans="3:10" ht="52.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C59" s="48"/>
+      <c r="C59" s="39"/>
       <c r="D59" s="6" t="s">
         <v>59</v>
       </c>
-      <c r="E59" s="43"/>
+      <c r="E59" s="37"/>
       <c r="F59" s="8" t="s">
         <v>128</v>
       </c>
@@ -2860,11 +2873,11 @@
       </c>
     </row>
     <row r="60" spans="3:10" ht="30.15" x14ac:dyDescent="0.3">
-      <c r="C60" s="48"/>
+      <c r="C60" s="39"/>
       <c r="D60" s="6" t="s">
         <v>60</v>
       </c>
-      <c r="E60" s="44"/>
+      <c r="E60" s="38"/>
       <c r="F60" s="8" t="s">
         <v>129</v>
       </c>
@@ -2906,13 +2919,13 @@
       </c>
     </row>
     <row r="62" spans="3:10" ht="30.15" x14ac:dyDescent="0.3">
-      <c r="C62" s="48" t="s">
+      <c r="C62" s="39" t="s">
         <v>64</v>
       </c>
       <c r="D62" s="6" t="s">
         <v>65</v>
       </c>
-      <c r="E62" s="42" t="s">
+      <c r="E62" s="36" t="s">
         <v>122</v>
       </c>
       <c r="F62" s="8" t="s">
@@ -2932,11 +2945,11 @@
       </c>
     </row>
     <row r="63" spans="3:10" ht="60.25" x14ac:dyDescent="0.3">
-      <c r="C63" s="48"/>
+      <c r="C63" s="39"/>
       <c r="D63" s="6" t="s">
         <v>66</v>
       </c>
-      <c r="E63" s="43"/>
+      <c r="E63" s="37"/>
       <c r="F63" s="8" t="s">
         <v>201</v>
       </c>
@@ -2954,11 +2967,11 @@
       </c>
     </row>
     <row r="64" spans="3:10" ht="60.25" x14ac:dyDescent="0.3">
-      <c r="C64" s="48"/>
+      <c r="C64" s="39"/>
       <c r="D64" s="6" t="s">
         <v>67</v>
       </c>
-      <c r="E64" s="43"/>
+      <c r="E64" s="37"/>
       <c r="F64" s="8" t="s">
         <v>202</v>
       </c>
@@ -2976,11 +2989,11 @@
       </c>
     </row>
     <row r="65" spans="3:10" ht="30.15" x14ac:dyDescent="0.3">
-      <c r="C65" s="48"/>
+      <c r="C65" s="39"/>
       <c r="D65" s="6" t="s">
         <v>68</v>
       </c>
-      <c r="E65" s="43"/>
+      <c r="E65" s="37"/>
       <c r="F65" s="8" t="s">
         <v>203</v>
       </c>
@@ -2998,11 +3011,11 @@
       </c>
     </row>
     <row r="66" spans="3:10" ht="60.25" x14ac:dyDescent="0.3">
-      <c r="C66" s="48"/>
+      <c r="C66" s="39"/>
       <c r="D66" s="6" t="s">
         <v>130</v>
       </c>
-      <c r="E66" s="43"/>
+      <c r="E66" s="37"/>
       <c r="F66" s="8" t="s">
         <v>204</v>
       </c>
@@ -3020,11 +3033,11 @@
       </c>
     </row>
     <row r="67" spans="3:10" ht="120.45" x14ac:dyDescent="0.3">
-      <c r="C67" s="48"/>
+      <c r="C67" s="39"/>
       <c r="D67" s="2" t="s">
         <v>131</v>
       </c>
-      <c r="E67" s="43"/>
+      <c r="E67" s="37"/>
       <c r="F67" s="8" t="s">
         <v>205</v>
       </c>
@@ -3048,7 +3061,7 @@
       <c r="D68" s="6" t="s">
         <v>71</v>
       </c>
-      <c r="E68" s="43"/>
+      <c r="E68" s="37"/>
       <c r="F68" s="22" t="s">
         <v>206</v>
       </c>
@@ -3066,13 +3079,13 @@
       </c>
     </row>
     <row r="69" spans="3:10" ht="30.15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C69" s="48" t="s">
+      <c r="C69" s="39" t="s">
         <v>72</v>
       </c>
       <c r="D69" s="6" t="s">
         <v>73</v>
       </c>
-      <c r="E69" s="43"/>
+      <c r="E69" s="37"/>
       <c r="F69" s="8" t="s">
         <v>132</v>
       </c>
@@ -3090,11 +3103,11 @@
       </c>
     </row>
     <row r="70" spans="3:10" ht="30.15" x14ac:dyDescent="0.3">
-      <c r="C70" s="48"/>
+      <c r="C70" s="39"/>
       <c r="D70" s="6" t="s">
         <v>74</v>
       </c>
-      <c r="E70" s="43"/>
+      <c r="E70" s="37"/>
       <c r="F70" s="8" t="s">
         <v>138</v>
       </c>
@@ -3112,11 +3125,11 @@
       </c>
     </row>
     <row r="71" spans="3:10" x14ac:dyDescent="0.3">
-      <c r="C71" s="48"/>
+      <c r="C71" s="39"/>
       <c r="D71" s="6" t="s">
         <v>75</v>
       </c>
-      <c r="E71" s="43"/>
+      <c r="E71" s="37"/>
       <c r="F71" s="8" t="s">
         <v>134</v>
       </c>
@@ -3134,11 +3147,11 @@
       </c>
     </row>
     <row r="72" spans="3:10" ht="30.15" x14ac:dyDescent="0.3">
-      <c r="C72" s="48"/>
+      <c r="C72" s="39"/>
       <c r="D72" s="6" t="s">
         <v>213</v>
       </c>
-      <c r="E72" s="43"/>
+      <c r="E72" s="37"/>
       <c r="F72" s="10" t="s">
         <v>160</v>
       </c>
@@ -3156,11 +3169,11 @@
       </c>
     </row>
     <row r="73" spans="3:10" x14ac:dyDescent="0.3">
-      <c r="C73" s="48"/>
+      <c r="C73" s="39"/>
       <c r="D73" s="6" t="s">
         <v>76</v>
       </c>
-      <c r="E73" s="43"/>
+      <c r="E73" s="37"/>
       <c r="F73" s="8" t="s">
         <v>135</v>
       </c>
@@ -3178,11 +3191,11 @@
       </c>
     </row>
     <row r="74" spans="3:10" x14ac:dyDescent="0.3">
-      <c r="C74" s="48"/>
+      <c r="C74" s="39"/>
       <c r="D74" s="6" t="s">
         <v>77</v>
       </c>
-      <c r="E74" s="43"/>
+      <c r="E74" s="37"/>
       <c r="F74" s="8" t="s">
         <v>133</v>
       </c>
@@ -3200,11 +3213,11 @@
       </c>
     </row>
     <row r="75" spans="3:10" x14ac:dyDescent="0.3">
-      <c r="C75" s="48"/>
+      <c r="C75" s="39"/>
       <c r="D75" s="6" t="s">
         <v>78</v>
       </c>
-      <c r="E75" s="43"/>
+      <c r="E75" s="37"/>
       <c r="F75" s="8" t="s">
         <v>137</v>
       </c>
@@ -3222,11 +3235,11 @@
       </c>
     </row>
     <row r="76" spans="3:10" x14ac:dyDescent="0.3">
-      <c r="C76" s="48"/>
+      <c r="C76" s="39"/>
       <c r="D76" s="6" t="s">
         <v>79</v>
       </c>
-      <c r="E76" s="43"/>
+      <c r="E76" s="37"/>
       <c r="F76" s="8" t="s">
         <v>136</v>
       </c>
@@ -3244,11 +3257,11 @@
       </c>
     </row>
     <row r="77" spans="3:10" ht="30.15" x14ac:dyDescent="0.3">
-      <c r="C77" s="48"/>
+      <c r="C77" s="39"/>
       <c r="D77" s="6" t="s">
         <v>80</v>
       </c>
-      <c r="E77" s="43"/>
+      <c r="E77" s="37"/>
       <c r="F77" s="10" t="s">
         <v>185</v>
       </c>
@@ -3266,11 +3279,11 @@
       </c>
     </row>
     <row r="78" spans="3:10" ht="30.15" x14ac:dyDescent="0.3">
-      <c r="C78" s="48"/>
+      <c r="C78" s="39"/>
       <c r="D78" s="6" t="s">
         <v>81</v>
       </c>
-      <c r="E78" s="43"/>
+      <c r="E78" s="37"/>
       <c r="F78" s="23" t="s">
         <v>139</v>
       </c>
@@ -3280,13 +3293,13 @@
       <c r="J78" s="30"/>
     </row>
     <row r="79" spans="3:10" ht="30.15" x14ac:dyDescent="0.3">
-      <c r="C79" s="43" t="s">
+      <c r="C79" s="37" t="s">
         <v>83</v>
       </c>
       <c r="D79" s="6" t="s">
         <v>140</v>
       </c>
-      <c r="E79" s="43"/>
+      <c r="E79" s="37"/>
       <c r="F79" s="8" t="s">
         <v>161</v>
       </c>
@@ -3304,11 +3317,11 @@
       </c>
     </row>
     <row r="80" spans="3:10" ht="30.15" x14ac:dyDescent="0.3">
-      <c r="C80" s="43"/>
+      <c r="C80" s="37"/>
       <c r="D80" s="6" t="s">
         <v>82</v>
       </c>
-      <c r="E80" s="43"/>
+      <c r="E80" s="37"/>
       <c r="F80" s="8" t="s">
         <v>162</v>
       </c>
@@ -3326,13 +3339,13 @@
       </c>
     </row>
     <row r="81" spans="3:10" ht="30.15" x14ac:dyDescent="0.3">
-      <c r="C81" s="42" t="s">
+      <c r="C81" s="36" t="s">
         <v>84</v>
       </c>
       <c r="D81" s="6" t="s">
         <v>143</v>
       </c>
-      <c r="E81" s="43"/>
+      <c r="E81" s="37"/>
       <c r="F81" s="8" t="s">
         <v>163</v>
       </c>
@@ -3350,11 +3363,11 @@
       </c>
     </row>
     <row r="82" spans="3:10" ht="69.400000000000006" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C82" s="43"/>
+      <c r="C82" s="37"/>
       <c r="D82" s="6" t="s">
         <v>144</v>
       </c>
-      <c r="E82" s="43"/>
+      <c r="E82" s="37"/>
       <c r="F82" s="8" t="s">
         <v>177</v>
       </c>
@@ -3372,11 +3385,11 @@
       </c>
     </row>
     <row r="83" spans="3:10" x14ac:dyDescent="0.3">
-      <c r="C83" s="43"/>
+      <c r="C83" s="37"/>
       <c r="D83" s="6" t="s">
         <v>85</v>
       </c>
-      <c r="E83" s="43"/>
+      <c r="E83" s="37"/>
       <c r="F83" s="23" t="s">
         <v>139</v>
       </c>
@@ -3386,11 +3399,11 @@
       <c r="J83" s="30"/>
     </row>
     <row r="84" spans="3:10" x14ac:dyDescent="0.3">
-      <c r="C84" s="43"/>
+      <c r="C84" s="37"/>
       <c r="D84" s="6" t="s">
         <v>86</v>
       </c>
-      <c r="E84" s="43"/>
+      <c r="E84" s="37"/>
       <c r="F84" s="8" t="s">
         <v>164</v>
       </c>
@@ -3408,11 +3421,11 @@
       </c>
     </row>
     <row r="85" spans="3:10" ht="30.15" x14ac:dyDescent="0.3">
-      <c r="C85" s="43"/>
+      <c r="C85" s="37"/>
       <c r="D85" s="6" t="s">
         <v>87</v>
       </c>
-      <c r="E85" s="43"/>
+      <c r="E85" s="37"/>
       <c r="F85" s="8" t="s">
         <v>165</v>
       </c>
@@ -3430,11 +3443,11 @@
       </c>
     </row>
     <row r="86" spans="3:10" ht="30.15" x14ac:dyDescent="0.3">
-      <c r="C86" s="43"/>
+      <c r="C86" s="37"/>
       <c r="D86" s="6" t="s">
         <v>88</v>
       </c>
-      <c r="E86" s="43"/>
+      <c r="E86" s="37"/>
       <c r="F86" s="8" t="s">
         <v>166</v>
       </c>
@@ -3452,11 +3465,11 @@
       </c>
     </row>
     <row r="87" spans="3:10" x14ac:dyDescent="0.3">
-      <c r="C87" s="43"/>
+      <c r="C87" s="37"/>
       <c r="D87" s="6" t="s">
         <v>89</v>
       </c>
-      <c r="E87" s="43"/>
+      <c r="E87" s="37"/>
       <c r="F87" s="8" t="s">
         <v>167</v>
       </c>
@@ -3474,11 +3487,11 @@
       </c>
     </row>
     <row r="88" spans="3:10" x14ac:dyDescent="0.3">
-      <c r="C88" s="43"/>
+      <c r="C88" s="37"/>
       <c r="D88" s="6" t="s">
         <v>90</v>
       </c>
-      <c r="E88" s="43"/>
+      <c r="E88" s="37"/>
       <c r="F88" s="8" t="s">
         <v>168</v>
       </c>
@@ -3496,11 +3509,11 @@
       </c>
     </row>
     <row r="89" spans="3:10" ht="30.15" x14ac:dyDescent="0.3">
-      <c r="C89" s="43"/>
+      <c r="C89" s="37"/>
       <c r="D89" s="6" t="s">
         <v>97</v>
       </c>
-      <c r="E89" s="43"/>
+      <c r="E89" s="37"/>
       <c r="F89" s="10" t="s">
         <v>279</v>
       </c>
@@ -3510,17 +3523,19 @@
       <c r="H89" s="21" t="s">
         <v>280</v>
       </c>
-      <c r="I89" s="32"/>
+      <c r="I89" s="32" t="s">
+        <v>207</v>
+      </c>
       <c r="J89" s="32" t="s">
         <v>207</v>
       </c>
     </row>
     <row r="90" spans="3:10" x14ac:dyDescent="0.3">
-      <c r="C90" s="43"/>
+      <c r="C90" s="37"/>
       <c r="D90" s="6" t="s">
         <v>98</v>
       </c>
-      <c r="E90" s="43"/>
+      <c r="E90" s="37"/>
       <c r="F90" s="8" t="s">
         <v>169</v>
       </c>
@@ -3538,11 +3553,11 @@
       </c>
     </row>
     <row r="91" spans="3:10" x14ac:dyDescent="0.3">
-      <c r="C91" s="43"/>
+      <c r="C91" s="37"/>
       <c r="D91" s="6" t="s">
         <v>99</v>
       </c>
-      <c r="E91" s="43"/>
+      <c r="E91" s="37"/>
       <c r="F91" s="8" t="s">
         <v>170</v>
       </c>
@@ -3560,11 +3575,11 @@
       </c>
     </row>
     <row r="92" spans="3:10" ht="30.15" x14ac:dyDescent="0.3">
-      <c r="C92" s="43"/>
+      <c r="C92" s="37"/>
       <c r="D92" s="6" t="s">
         <v>100</v>
       </c>
-      <c r="E92" s="43"/>
+      <c r="E92" s="37"/>
       <c r="F92" s="8" t="s">
         <v>171</v>
       </c>
@@ -3582,11 +3597,11 @@
       </c>
     </row>
     <row r="93" spans="3:10" ht="45.2" x14ac:dyDescent="0.3">
-      <c r="C93" s="43"/>
+      <c r="C93" s="37"/>
       <c r="D93" s="6" t="s">
         <v>142</v>
       </c>
-      <c r="E93" s="43"/>
+      <c r="E93" s="37"/>
       <c r="F93" s="8" t="s">
         <v>172</v>
       </c>
@@ -3604,13 +3619,13 @@
       </c>
     </row>
     <row r="94" spans="3:10" x14ac:dyDescent="0.3">
-      <c r="C94" s="42" t="s">
+      <c r="C94" s="36" t="s">
         <v>92</v>
       </c>
       <c r="D94" s="6" t="s">
         <v>93</v>
       </c>
-      <c r="E94" s="43"/>
+      <c r="E94" s="37"/>
       <c r="F94" s="8" t="s">
         <v>173</v>
       </c>
@@ -3628,11 +3643,11 @@
       </c>
     </row>
     <row r="95" spans="3:10" ht="30.15" x14ac:dyDescent="0.3">
-      <c r="C95" s="43"/>
+      <c r="C95" s="37"/>
       <c r="D95" s="6" t="s">
         <v>94</v>
       </c>
-      <c r="E95" s="43"/>
+      <c r="E95" s="37"/>
       <c r="F95" s="8" t="s">
         <v>174</v>
       </c>
@@ -3650,11 +3665,11 @@
       </c>
     </row>
     <row r="96" spans="3:10" x14ac:dyDescent="0.3">
-      <c r="C96" s="43"/>
+      <c r="C96" s="37"/>
       <c r="D96" s="6" t="s">
         <v>95</v>
       </c>
-      <c r="E96" s="43"/>
+      <c r="E96" s="37"/>
       <c r="F96" s="26" t="s">
         <v>139</v>
       </c>
@@ -3664,11 +3679,11 @@
       <c r="J96" s="28"/>
     </row>
     <row r="97" spans="3:10" x14ac:dyDescent="0.3">
-      <c r="C97" s="43"/>
+      <c r="C97" s="37"/>
       <c r="D97" s="6" t="s">
         <v>96</v>
       </c>
-      <c r="E97" s="43"/>
+      <c r="E97" s="37"/>
       <c r="F97" s="8" t="s">
         <v>175</v>
       </c>
@@ -3686,11 +3701,11 @@
       </c>
     </row>
     <row r="98" spans="3:10" x14ac:dyDescent="0.3">
-      <c r="C98" s="43"/>
+      <c r="C98" s="37"/>
       <c r="D98" s="6" t="s">
         <v>141</v>
       </c>
-      <c r="E98" s="43"/>
+      <c r="E98" s="37"/>
       <c r="F98" s="8" t="s">
         <v>176</v>
       </c>
@@ -3708,13 +3723,13 @@
       </c>
     </row>
     <row r="99" spans="3:10" x14ac:dyDescent="0.3">
-      <c r="C99" s="48" t="s">
+      <c r="C99" s="39" t="s">
         <v>107</v>
       </c>
       <c r="D99" s="6" t="s">
         <v>101</v>
       </c>
-      <c r="E99" s="43"/>
+      <c r="E99" s="37"/>
       <c r="F99" s="8" t="s">
         <v>146</v>
       </c>
@@ -3732,11 +3747,11 @@
       </c>
     </row>
     <row r="100" spans="3:10" ht="30.15" x14ac:dyDescent="0.3">
-      <c r="C100" s="48"/>
+      <c r="C100" s="39"/>
       <c r="D100" s="6" t="s">
         <v>102</v>
       </c>
-      <c r="E100" s="43"/>
+      <c r="E100" s="37"/>
       <c r="F100" s="8" t="s">
         <v>145</v>
       </c>
@@ -3754,11 +3769,11 @@
       </c>
     </row>
     <row r="101" spans="3:10" x14ac:dyDescent="0.3">
-      <c r="C101" s="48"/>
+      <c r="C101" s="39"/>
       <c r="D101" s="6" t="s">
         <v>103</v>
       </c>
-      <c r="E101" s="43"/>
+      <c r="E101" s="37"/>
       <c r="F101" s="8" t="s">
         <v>148</v>
       </c>
@@ -3776,11 +3791,11 @@
       </c>
     </row>
     <row r="102" spans="3:10" ht="30.15" x14ac:dyDescent="0.3">
-      <c r="C102" s="48"/>
+      <c r="C102" s="39"/>
       <c r="D102" s="6" t="s">
         <v>104</v>
       </c>
-      <c r="E102" s="43"/>
+      <c r="E102" s="37"/>
       <c r="F102" s="8" t="s">
         <v>147</v>
       </c>
@@ -3798,11 +3813,11 @@
       </c>
     </row>
     <row r="103" spans="3:10" x14ac:dyDescent="0.3">
-      <c r="C103" s="48"/>
+      <c r="C103" s="39"/>
       <c r="D103" s="6" t="s">
         <v>105</v>
       </c>
-      <c r="E103" s="43"/>
+      <c r="E103" s="37"/>
       <c r="F103" s="8" t="s">
         <v>149</v>
       </c>
@@ -3820,11 +3835,11 @@
       </c>
     </row>
     <row r="104" spans="3:10" ht="30.15" x14ac:dyDescent="0.3">
-      <c r="C104" s="48"/>
+      <c r="C104" s="39"/>
       <c r="D104" s="7" t="s">
         <v>106</v>
       </c>
-      <c r="E104" s="44"/>
+      <c r="E104" s="38"/>
       <c r="F104" s="8" t="s">
         <v>150</v>
       </c>
@@ -3852,20 +3867,21 @@
     </row>
   </sheetData>
   <mergeCells count="44">
-    <mergeCell ref="J40:J44"/>
-    <mergeCell ref="E50:E60"/>
-    <mergeCell ref="E62:E104"/>
-    <mergeCell ref="C69:C78"/>
-    <mergeCell ref="C79:C80"/>
-    <mergeCell ref="C81:C93"/>
-    <mergeCell ref="C94:C98"/>
-    <mergeCell ref="C99:C104"/>
-    <mergeCell ref="C62:C67"/>
-    <mergeCell ref="C57:C60"/>
-    <mergeCell ref="C50:C51"/>
-    <mergeCell ref="C52:C56"/>
-    <mergeCell ref="H40:H44"/>
-    <mergeCell ref="I40:I44"/>
+    <mergeCell ref="J6:J7"/>
+    <mergeCell ref="J18:J22"/>
+    <mergeCell ref="J28:J32"/>
+    <mergeCell ref="I34:I37"/>
+    <mergeCell ref="J34:J37"/>
+    <mergeCell ref="I6:I7"/>
+    <mergeCell ref="I18:I22"/>
+    <mergeCell ref="G6:G7"/>
+    <mergeCell ref="G34:G37"/>
+    <mergeCell ref="G40:G44"/>
+    <mergeCell ref="G28:G32"/>
+    <mergeCell ref="I28:I32"/>
+    <mergeCell ref="H6:H7"/>
+    <mergeCell ref="H28:H32"/>
+    <mergeCell ref="H34:H37"/>
     <mergeCell ref="E3:E27"/>
     <mergeCell ref="E33:E38"/>
     <mergeCell ref="E39:E48"/>
@@ -3881,21 +3897,20 @@
     <mergeCell ref="C18:C22"/>
     <mergeCell ref="F28:F32"/>
     <mergeCell ref="F6:F7"/>
-    <mergeCell ref="G6:G7"/>
-    <mergeCell ref="G34:G37"/>
-    <mergeCell ref="G40:G44"/>
-    <mergeCell ref="G28:G32"/>
-    <mergeCell ref="I28:I32"/>
-    <mergeCell ref="H6:H7"/>
-    <mergeCell ref="H28:H32"/>
-    <mergeCell ref="H34:H37"/>
-    <mergeCell ref="J6:J7"/>
-    <mergeCell ref="J18:J22"/>
-    <mergeCell ref="J28:J32"/>
-    <mergeCell ref="I34:I37"/>
-    <mergeCell ref="J34:J37"/>
-    <mergeCell ref="I6:I7"/>
-    <mergeCell ref="I18:I22"/>
+    <mergeCell ref="J40:J44"/>
+    <mergeCell ref="E50:E60"/>
+    <mergeCell ref="E62:E104"/>
+    <mergeCell ref="C69:C78"/>
+    <mergeCell ref="C79:C80"/>
+    <mergeCell ref="C81:C93"/>
+    <mergeCell ref="C94:C98"/>
+    <mergeCell ref="C99:C104"/>
+    <mergeCell ref="C62:C67"/>
+    <mergeCell ref="C57:C60"/>
+    <mergeCell ref="C50:C51"/>
+    <mergeCell ref="C52:C56"/>
+    <mergeCell ref="H40:H44"/>
+    <mergeCell ref="I40:I44"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>